<commit_message>
WristRot in Zylindrisch und Kugelig
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Bezugsquellen" sheetId="2" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Rotary Encoder" sheetId="6" r:id="rId6"/>
     <sheet name="BOM" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="692">
   <si>
     <t>Bauteilnummer</t>
   </si>
@@ -2038,12 +2038,6 @@
     <t>Lager  zum Grippermount</t>
   </si>
   <si>
-    <t>https://www.conrad.de/de/senkschrauben-m3-16-mm-innensechskant-din-7991-iso-10642-edelstahl-100-st-toolcraft-401632-401632.html?sc.queryFromSuggest=true</t>
-  </si>
-  <si>
-    <t>Senkschraube Innensechskant M3 16mm</t>
-  </si>
-  <si>
     <t>Befestigung Lagerdeckel</t>
   </si>
   <si>
@@ -2090,6 +2084,18 @@
   </si>
   <si>
     <t>Gewindestift M3 20mm</t>
+  </si>
+  <si>
+    <t>http://www.dswaelzlager.de/Miniaturlager-MR105-ZZ</t>
+  </si>
+  <si>
+    <t>http://www.dswaelzlager.de/Rillenkugellager-686-ZZ-beidseitig-Stahldeckscheiben-6x13x5mm-</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/senkschrauben-m3-14-mm-innensechskant-iso-10642-edelstahl-a2-100-st-1069038.html</t>
+  </si>
+  <si>
+    <t>Senkschraube Innensechskant M3 14mm</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2165,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2206,9 +2212,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2217,13 +2220,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
@@ -2465,9 +2470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2505,9 +2510,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2542,7 +2547,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2577,7 +2582,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2751,10 +2756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E41"/>
+  <dimension ref="A2:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,98 +2869,108 @@
         <v>558</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>688</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="E28" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>560</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>565</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D30" t="s">
         <v>561</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
         <v>564</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E31" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>566</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E32" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>650</v>
       </c>
-      <c r="E32" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>650</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>650</v>
+      </c>
+      <c r="E35" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>236</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E37" t="s">
         <v>640</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>659</v>
-      </c>
-      <c r="E36" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E38" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>684</v>
-      </c>
-      <c r="E39" t="s">
-        <v>685</v>
+        <v>660</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
       <c r="E40" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="E41" t="s">
-        <v>688</v>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>684</v>
+      </c>
+      <c r="E42" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>687</v>
+      </c>
+      <c r="E43" t="s">
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -2967,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M88" sqref="M88"/>
+    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3368,7 +3383,7 @@
       </c>
       <c r="C36" s="5">
         <f>C40/C38*(C44/C42)</f>
-        <v>10.453333333333333</v>
+        <v>3.7333333333333334</v>
       </c>
       <c r="D36" t="s">
         <v>325</v>
@@ -3413,7 +3428,7 @@
         <v>342</v>
       </c>
       <c r="C40" s="7">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
         <v>338</v>
@@ -3425,7 +3440,7 @@
       </c>
       <c r="C41" s="4">
         <f>C40*C37/PI()</f>
-        <v>33.422538049298019</v>
+        <v>11.93662073189215</v>
       </c>
       <c r="D41" t="s">
         <v>340</v>
@@ -3483,7 +3498,7 @@
       </c>
       <c r="C46" s="5">
         <f>C50/C48*(C54/C52)</f>
-        <v>10.453333333333333</v>
+        <v>3.7333333333333334</v>
       </c>
       <c r="D46" t="s">
         <v>325</v>
@@ -3528,7 +3543,7 @@
         <v>342</v>
       </c>
       <c r="C50" s="7">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
         <v>338</v>
@@ -3540,7 +3555,7 @@
       </c>
       <c r="C51" s="4">
         <f>C50*C47/PI()</f>
-        <v>33.422538049298019</v>
+        <v>11.93662073189215</v>
       </c>
       <c r="D51" t="s">
         <v>340</v>
@@ -3737,7 +3752,7 @@
       </c>
       <c r="C70" s="2">
         <f>C65/C36</f>
-        <v>0.12809933035714285</v>
+        <v>0.35867812499999996</v>
       </c>
       <c r="D70" t="s">
         <v>322</v>
@@ -3749,7 +3764,7 @@
       </c>
       <c r="C71" s="2">
         <f>C66/C36</f>
-        <v>4.2699776785714287E-2</v>
+        <v>0.119559375</v>
       </c>
       <c r="D71" t="s">
         <v>322</v>
@@ -3974,7 +3989,7 @@
       </c>
       <c r="C77" s="2">
         <f>C70*(1+C57)</f>
-        <v>0.16652912946428572</v>
+        <v>0.46628156249999997</v>
       </c>
       <c r="D77" t="s">
         <v>322</v>
@@ -3982,31 +3997,31 @@
       <c r="E77" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="F77" s="28">
+      <c r="F77" s="27">
         <v>1.8</v>
       </c>
-      <c r="G77" s="28" t="s">
+      <c r="G77" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="H77" s="28" t="s">
+      <c r="H77" s="27" t="s">
         <v>423</v>
       </c>
-      <c r="I77" s="28" t="s">
+      <c r="I77" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="J77" s="28">
+      <c r="J77" s="27">
         <v>5</v>
       </c>
       <c r="K77" s="15">
         <v>45</v>
       </c>
-      <c r="L77" s="28">
+      <c r="L77" s="27">
         <v>2</v>
       </c>
-      <c r="M77" s="28" t="s">
+      <c r="M77" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N77" s="28">
+      <c r="N77" s="27">
         <v>0.31</v>
       </c>
       <c r="O77" s="17">
@@ -4035,7 +4050,7 @@
       </c>
       <c r="C78" s="2">
         <f>C71*(1+C57)</f>
-        <v>5.5509709821428575E-2</v>
+        <v>0.15542718750000001</v>
       </c>
       <c r="D78" t="s">
         <v>322</v>
@@ -4043,31 +4058,31 @@
       <c r="E78" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="F78" s="28">
+      <c r="F78" s="27">
         <v>1.8</v>
       </c>
-      <c r="G78" s="28" t="s">
+      <c r="G78" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="H78" s="28" t="s">
+      <c r="H78" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="I78" s="28" t="s">
+      <c r="I78" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J78" s="28">
+      <c r="J78" s="27">
         <v>5</v>
       </c>
-      <c r="K78" s="28">
+      <c r="K78" s="27">
         <v>18</v>
       </c>
-      <c r="L78" s="28">
+      <c r="L78" s="27">
         <v>0.8</v>
       </c>
-      <c r="M78" s="28" t="s">
+      <c r="M78" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N78" s="28">
+      <c r="N78" s="27">
         <v>0.17</v>
       </c>
       <c r="O78" s="17">
@@ -4394,31 +4409,31 @@
       <c r="E87" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="F87" s="28">
+      <c r="F87" s="27">
         <v>1.8</v>
       </c>
-      <c r="G87" s="28" t="s">
+      <c r="G87" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="H87" s="28" t="s">
+      <c r="H87" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="I87" s="28" t="s">
+      <c r="I87" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="J87" s="28">
+      <c r="J87" s="27">
         <v>5</v>
       </c>
-      <c r="K87" s="28">
+      <c r="K87" s="27">
         <v>23</v>
       </c>
-      <c r="L87" s="28">
+      <c r="L87" s="27">
         <v>0.5</v>
       </c>
-      <c r="M87" s="28" t="s">
+      <c r="M87" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N87" s="28">
+      <c r="N87" s="27">
         <v>0.22</v>
       </c>
       <c r="O87" s="17">
@@ -4430,28 +4445,28 @@
       <c r="E88" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="F88" s="28">
+      <c r="F88" s="27">
         <v>0.9</v>
       </c>
-      <c r="G88" s="28" t="s">
+      <c r="G88" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="H88" s="28" t="s">
+      <c r="H88" s="27" t="s">
         <v>423</v>
       </c>
-      <c r="I88" s="28" t="s">
+      <c r="I88" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="K88" s="28">
+      <c r="K88" s="27">
         <v>23</v>
       </c>
-      <c r="L88" s="28">
+      <c r="L88" s="27">
         <v>0.31</v>
       </c>
-      <c r="M88" s="28" t="s">
+      <c r="M88" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N88" s="28">
+      <c r="N88" s="27">
         <v>0.28000000000000003</v>
       </c>
       <c r="O88" s="18">
@@ -4463,31 +4478,31 @@
       <c r="E89" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="F89" s="28">
+      <c r="F89" s="27">
         <v>1.8</v>
       </c>
-      <c r="G89" s="28" t="s">
+      <c r="G89" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="H89" s="28" t="s">
+      <c r="H89" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="I89" s="28" t="s">
+      <c r="I89" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J89" s="28">
+      <c r="J89" s="27">
         <v>5</v>
       </c>
-      <c r="K89" s="28">
+      <c r="K89" s="27">
         <v>18</v>
       </c>
-      <c r="L89" s="28">
+      <c r="L89" s="27">
         <v>0.8</v>
       </c>
-      <c r="M89" s="28" t="s">
+      <c r="M89" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N89" s="28">
+      <c r="N89" s="27">
         <v>0.17</v>
       </c>
       <c r="O89" s="17">
@@ -4535,31 +4550,31 @@
       <c r="E91" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="F91" s="28">
+      <c r="F91" s="27">
         <v>1.8</v>
       </c>
-      <c r="G91" s="28" t="s">
+      <c r="G91" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="H91" s="28" t="s">
+      <c r="H91" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="I91" s="28" t="s">
+      <c r="I91" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="J91" s="28">
+      <c r="J91" s="27">
         <v>5</v>
       </c>
-      <c r="K91" s="28">
+      <c r="K91" s="27">
         <v>14</v>
       </c>
-      <c r="L91" s="28">
+      <c r="L91" s="27">
         <v>0.4</v>
       </c>
-      <c r="M91" s="28" t="s">
+      <c r="M91" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="N91" s="28">
+      <c r="N91" s="27">
         <v>0.12</v>
       </c>
       <c r="O91" s="18">
@@ -7251,8 +7266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7450,8 +7465,8 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -7467,10 +7482,10 @@
       <c r="C4" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="10" t="s">
         <v>361</v>
       </c>
@@ -10917,8 +10932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10927,7 +10942,7 @@
     <col min="2" max="2" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="54.88671875" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -10940,7 +10955,7 @@
       <c r="D1" t="s">
         <v>602</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="28" t="s">
         <v>599</v>
       </c>
       <c r="F1" t="s">
@@ -10968,8 +10983,11 @@
       <c r="D3" t="s">
         <v>666</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="28" t="s">
         <v>664</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -10982,8 +11000,11 @@
       <c r="D4" t="s">
         <v>668</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="28" t="s">
         <v>662</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -11001,8 +11022,11 @@
       <c r="D6" t="s">
         <v>671</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="28" t="s">
         <v>557</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -11010,13 +11034,16 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>673</v>
+        <v>691</v>
       </c>
       <c r="D7" t="s">
-        <v>674</v>
-      </c>
-      <c r="E7" t="s">
         <v>672</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>690</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -11024,13 +11051,16 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D8" t="s">
-        <v>677</v>
-      </c>
-      <c r="E8" t="s">
         <v>675</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -11038,13 +11068,16 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>676</v>
+      </c>
+      <c r="D9" t="s">
         <v>678</v>
       </c>
-      <c r="D9" t="s">
-        <v>680</v>
-      </c>
-      <c r="E9" t="s">
-        <v>679</v>
+      <c r="E9" s="28" t="s">
+        <v>677</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -11052,13 +11085,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>679</v>
+      </c>
+      <c r="D10" t="s">
+        <v>680</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>681</v>
       </c>
-      <c r="D10" t="s">
-        <v>682</v>
-      </c>
-      <c r="E10" t="s">
-        <v>683</v>
+      <c r="F10">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -11071,7 +11107,7 @@
       <c r="D12" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="28" t="s">
         <v>554</v>
       </c>
       <c r="F12">
@@ -11095,7 +11131,7 @@
       <c r="D13" t="s">
         <v>622</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="28" t="s">
         <v>613</v>
       </c>
       <c r="F13">
@@ -11119,7 +11155,7 @@
       <c r="D14" t="s">
         <v>617</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="29" t="s">
         <v>615</v>
       </c>
       <c r="F14">
@@ -11143,7 +11179,7 @@
       <c r="D15" t="s">
         <v>618</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="28" t="s">
         <v>619</v>
       </c>
       <c r="F15">
@@ -11167,7 +11203,7 @@
       <c r="D16" t="s">
         <v>623</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="26" t="s">
         <v>473</v>
       </c>
       <c r="F16">
@@ -11182,7 +11218,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E17" s="25"/>
+      <c r="E17" s="26"/>
       <c r="H17" s="22"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -11195,7 +11231,7 @@
       <c r="D18" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="26" t="s">
         <v>544</v>
       </c>
       <c r="F18">
@@ -11219,8 +11255,11 @@
       <c r="D19" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="28" t="s">
         <v>649</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
       <c r="H19" s="22"/>
     </row>
@@ -11234,8 +11273,11 @@
       <c r="D20" t="s">
         <v>641</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>657</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="H20" s="22"/>
     </row>
@@ -11249,8 +11291,11 @@
       <c r="D21" t="s">
         <v>642</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="29" t="s">
         <v>615</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
       <c r="H21" s="22"/>
     </row>
@@ -11264,8 +11309,11 @@
       <c r="D22" t="s">
         <v>655</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="26" t="s">
         <v>643</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
       </c>
       <c r="H22" s="22"/>
     </row>
@@ -11273,20 +11321,23 @@
       <c r="D23" t="s">
         <v>656</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="28" t="s">
         <v>654</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="27"/>
+      <c r="E24" s="26"/>
       <c r="H24" s="22"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D25" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="E25" s="27"/>
+      <c r="E25" s="26"/>
       <c r="H25" s="22"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
@@ -11299,7 +11350,7 @@
       <c r="D26" t="s">
         <v>635</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>627</v>
       </c>
       <c r="F26">
@@ -11323,7 +11374,7 @@
       <c r="D27" t="s">
         <v>631</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>632</v>
       </c>
       <c r="F27">
@@ -11341,8 +11392,11 @@
       <c r="D28" t="s">
         <v>634</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="25" t="s">
         <v>633</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
       <c r="H28" s="22"/>
     </row>
@@ -11356,8 +11410,11 @@
       <c r="D29" t="s">
         <v>653</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>652</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
       </c>
       <c r="H29" s="22"/>
     </row>
@@ -11371,8 +11428,11 @@
       <c r="D30" t="s">
         <v>646</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="25" t="s">
         <v>647</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
       </c>
       <c r="H30" s="22"/>
     </row>
@@ -11386,7 +11446,7 @@
       <c r="D31" t="s">
         <v>631</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="25" t="s">
         <v>627</v>
       </c>
       <c r="F31">
@@ -11395,11 +11455,11 @@
       <c r="H31" s="22"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E32" s="26"/>
+      <c r="E32" s="25"/>
       <c r="H32" s="22"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E33" s="11"/>
+      <c r="E33" s="25"/>
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
@@ -11412,7 +11472,7 @@
       <c r="D34" t="s">
         <v>604</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="28" t="s">
         <v>608</v>
       </c>
       <c r="F34">
@@ -11436,7 +11496,7 @@
       <c r="D35" t="s">
         <v>611</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="28" t="s">
         <v>605</v>
       </c>
       <c r="G35" s="23">

</xml_diff>

<commit_message>
Wrist2 begonnen mit engerem Bogen an der Weltraumkugel
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="693">
   <si>
     <t>Bauteilnummer</t>
   </si>
@@ -2096,6 +2096,9 @@
   </si>
   <si>
     <t>Senkschraube Innensechskant M3 14mm</t>
+  </si>
+  <si>
+    <t>Wrist</t>
   </si>
 </sst>
 </file>
@@ -2165,7 +2168,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2216,6 +2219,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2759,7 +2765,7 @@
   <dimension ref="A2:E43"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2980,10 +2986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AD109"/>
+  <dimension ref="A3:AD110"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3060,7 +3066,7 @@
       </c>
       <c r="C8">
         <f>N78+N77 +0.4</f>
-        <v>0.88</v>
+        <v>0.72</v>
       </c>
       <c r="D8" t="s">
         <v>315</v>
@@ -3072,7 +3078,7 @@
       </c>
       <c r="C9">
         <f>N77+0.1</f>
-        <v>0.41000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="D9" t="s">
         <v>315</v>
@@ -3656,7 +3662,7 @@
       </c>
       <c r="C62" s="4">
         <f>((C3+C4+C5)*(C7+C8+C9)*(C59))/1000</f>
-        <v>10.992105000000002</v>
+        <v>9.5794650000000008</v>
       </c>
       <c r="D62" t="s">
         <v>322</v>
@@ -3668,7 +3674,7 @@
       </c>
       <c r="C63" s="4">
         <f>((C3+C4+C5)*(C7+C8+C9)*(C58+C59))/1000</f>
-        <v>32.976315</v>
+        <v>28.738395000000001</v>
       </c>
       <c r="D63" t="s">
         <v>322</v>
@@ -3680,7 +3686,7 @@
       </c>
       <c r="C64" s="2">
         <f>((C4+C5)*(C8+C9)*(C58+C59))/1000</f>
-        <v>9.4911750000000001</v>
+        <v>7.1367749999999992</v>
       </c>
       <c r="D64" t="s">
         <v>322</v>
@@ -3691,8 +3697,8 @@
         <v>575</v>
       </c>
       <c r="C65" s="2">
-        <f>((C5)*(C9+C6)*(C58+C59))/1000</f>
-        <v>1.3390649999999999</v>
+        <f>((C5)*(C9+C6)*(C59))/1000</f>
+        <v>0.36787500000000001</v>
       </c>
       <c r="D65" t="s">
         <v>322</v>
@@ -3704,7 +3710,7 @@
       </c>
       <c r="C66" s="2">
         <f>((C5)*(C9+C6)*(C59))/1000</f>
-        <v>0.446355</v>
+        <v>0.36787500000000001</v>
       </c>
       <c r="D66" t="s">
         <v>322</v>
@@ -3716,7 +3722,7 @@
       </c>
       <c r="C67" s="2">
         <f>C62/C10</f>
-        <v>1.8320175000000003</v>
+        <v>1.5965775000000002</v>
       </c>
       <c r="D67" t="s">
         <v>322</v>
@@ -3728,7 +3734,7 @@
       </c>
       <c r="C68" s="2">
         <f>C63/C16</f>
-        <v>1.93220595703125</v>
+        <v>1.6838903320312502</v>
       </c>
       <c r="D68" t="s">
         <v>322</v>
@@ -3740,7 +3746,7 @@
       </c>
       <c r="C69" s="2">
         <f>C64/C26</f>
-        <v>1.334696484375</v>
+        <v>1.003608984375</v>
       </c>
       <c r="D69" t="s">
         <v>322</v>
@@ -3752,7 +3758,7 @@
       </c>
       <c r="C70" s="2">
         <f>C65/C36</f>
-        <v>0.35867812499999996</v>
+        <v>9.853794642857143E-2</v>
       </c>
       <c r="D70" t="s">
         <v>322</v>
@@ -3764,7 +3770,7 @@
       </c>
       <c r="C71" s="2">
         <f>C66/C36</f>
-        <v>0.119559375</v>
+        <v>9.853794642857143E-2</v>
       </c>
       <c r="D71" t="s">
         <v>322</v>
@@ -3841,7 +3847,7 @@
       </c>
       <c r="C74" s="2">
         <f>C67*(1+C57)</f>
-        <v>2.3816227500000005</v>
+        <v>2.0755507500000006</v>
       </c>
       <c r="D74" t="s">
         <v>322</v>
@@ -3887,7 +3893,7 @@
       </c>
       <c r="C75" s="2">
         <f>C68*(1+C57)</f>
-        <v>2.5118677441406252</v>
+        <v>2.1890574316406255</v>
       </c>
       <c r="D75" t="s">
         <v>322</v>
@@ -3933,7 +3939,7 @@
       </c>
       <c r="C76" s="2">
         <f>C69*(1+C57)</f>
-        <v>1.7351054296875001</v>
+        <v>1.3046916796875001</v>
       </c>
       <c r="D76" t="s">
         <v>322</v>
@@ -3989,44 +3995,44 @@
       </c>
       <c r="C77" s="2">
         <f>C70*(1+C57)</f>
-        <v>0.46628156249999997</v>
+        <v>0.12809933035714285</v>
       </c>
       <c r="D77" t="s">
         <v>322</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="F77" s="27">
-        <v>1.8</v>
-      </c>
-      <c r="G77" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="F77" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="G77" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="H77" s="27" t="s">
+      <c r="H77" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="I77" s="27" t="s">
-        <v>433</v>
-      </c>
-      <c r="J77" s="27">
+      <c r="I77" s="28" t="s">
+        <v>424</v>
+      </c>
+      <c r="J77" s="28">
         <v>5</v>
       </c>
-      <c r="K77" s="15">
-        <v>45</v>
-      </c>
-      <c r="L77" s="27">
-        <v>2</v>
-      </c>
-      <c r="M77" s="27" t="s">
+      <c r="K77" s="28">
+        <v>11</v>
+      </c>
+      <c r="L77" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="M77" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="N77" s="27">
-        <v>0.31</v>
-      </c>
-      <c r="O77" s="17">
+      <c r="N77" s="28">
+        <v>0.15</v>
+      </c>
+      <c r="O77" s="18">
         <f t="shared" si="0"/>
-        <v>145.16129032258064</v>
+        <v>73.333333333333343</v>
       </c>
       <c r="P77" s="11"/>
       <c r="Q77" s="14"/>
@@ -4050,7 +4056,7 @@
       </c>
       <c r="C78" s="2">
         <f>C71*(1+C57)</f>
-        <v>0.15542718750000001</v>
+        <v>0.12809933035714285</v>
       </c>
       <c r="D78" t="s">
         <v>322</v>
@@ -4619,161 +4625,197 @@
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>581</v>
+      <c r="E93" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="F93" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="G93" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="H93" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="I93" s="28" t="s">
+        <v>424</v>
+      </c>
+      <c r="J93" s="28">
+        <v>5</v>
+      </c>
+      <c r="K93" s="28">
+        <v>11</v>
+      </c>
+      <c r="L93" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="M93" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="N93" s="28">
+        <v>0.15</v>
+      </c>
+      <c r="O93" s="18">
+        <f t="shared" ref="O93" si="4">K93/N93</f>
+        <v>73.333333333333343</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>584</v>
       </c>
-      <c r="C94" s="19">
+      <c r="C95" s="19">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>589</v>
       </c>
-      <c r="C95" s="19">
+      <c r="C96" s="19">
         <f>(C15/1000/2)</f>
         <v>7.1619724391352904E-2</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>590</v>
-      </c>
-    </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>585</v>
-      </c>
-      <c r="C96" s="19">
-        <f>C62/C95</f>
-        <v>153.47873917994505</v>
-      </c>
-      <c r="D96" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>585</v>
+      </c>
+      <c r="C97" s="19">
+        <f>C62/C96</f>
+        <v>133.75456386364689</v>
+      </c>
+      <c r="D97" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>586</v>
       </c>
-      <c r="C97" s="19">
-        <f>(C94)*C96*2*PI()</f>
-        <v>964.33535897987861</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C98" s="19">
+        <f>(C95)*C97*2*PI()</f>
+        <v>840.40471043627974</v>
+      </c>
+      <c r="D98" t="s">
         <v>583</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>584</v>
-      </c>
-      <c r="C100" s="20">
-        <v>1</v>
-      </c>
-      <c r="D100" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>584</v>
+      </c>
+      <c r="C101" s="20">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>589</v>
       </c>
-      <c r="C101" s="20">
+      <c r="C102" s="20">
         <f>(C21/1000/2)</f>
         <v>3.8197186342054885E-2</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>585</v>
-      </c>
-      <c r="C102" s="20">
-        <f>C63/C101</f>
-        <v>863.3179078871907</v>
-      </c>
-      <c r="D102" t="s">
-        <v>582</v>
-      </c>
-      <c r="E102" s="20"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>585</v>
+      </c>
+      <c r="C103" s="20">
+        <f>C63/C102</f>
+        <v>752.36942173301361</v>
+      </c>
+      <c r="D103" t="s">
+        <v>582</v>
+      </c>
+      <c r="E103" s="20"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>586</v>
       </c>
-      <c r="C103" s="20">
-        <f>(C100)*C102*2*PI()</f>
-        <v>5424.3863942618163</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C104" s="20">
+        <f>(C101)*C103*2*PI()</f>
+        <v>4727.2764962040728</v>
+      </c>
+      <c r="D104" t="s">
         <v>583</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>584</v>
       </c>
-      <c r="C106" s="20">
+      <c r="C107" s="20">
         <f>60*C18/C20</f>
         <v>18.75</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>589</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C108" s="20">
         <f>(C25/1000/2)</f>
         <v>6.3661977236758135E-2</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>590</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>585</v>
-      </c>
-      <c r="C108" s="20">
-        <f>C63/(C20/C18)/C107</f>
-        <v>161.87210772884828</v>
-      </c>
-      <c r="D108" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>585</v>
+      </c>
+      <c r="C109" s="20">
+        <f>C63/(C20/C18)/C108</f>
+        <v>141.06926657494006</v>
+      </c>
+      <c r="D109" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>586</v>
       </c>
-      <c r="C109" s="20">
-        <f>(C106/60)*C108*2*PI()</f>
-        <v>317.83514028877835</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C110" s="20">
+        <f>(C107/60)*C109*2*PI()</f>
+        <v>276.98885719945736</v>
+      </c>
+      <c r="D110" t="s">
         <v>583</v>
       </c>
     </row>
@@ -4795,11 +4837,12 @@
     <hyperlink ref="E89" r:id="rId14" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-54v-08a-18ncm255ozin-14hs130804s-p-93.html"/>
     <hyperlink ref="E91" r:id="rId15" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-12v-04a-14ncm20ozin-14hs100404s-p-90.html"/>
     <hyperlink ref="E78" r:id="rId16" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-54v-08a-18ncm255ozin-14hs130804s-p-93.html"/>
-    <hyperlink ref="E77" r:id="rId17" display="http://www.omc-stepperonline.com/3d-printer-nema-17-stepper-motor-2a-45ncm64ozin-17hs162004s-p-16.html"/>
-    <hyperlink ref="E88" r:id="rId18" display="http://www.omc-stepperonline.com/9deg-nema-17-unipolar-stepper-motor-12v-031a-16ncm227ozin-17hm130316s-p-262.html"/>
+    <hyperlink ref="E88" r:id="rId17" display="http://www.omc-stepperonline.com/9deg-nema-17-unipolar-stepper-motor-12v-031a-16ncm227ozin-17hm130316s-p-262.html"/>
+    <hyperlink ref="E93" r:id="rId18" display="http://www.omc-stepperonline.com/09-nema-17-bipolar-stepper-12a-11ncm156ozin-17hm081204s-p-99.html"/>
+    <hyperlink ref="E77" r:id="rId19" display="http://www.omc-stepperonline.com/09-nema-17-bipolar-stepper-12a-11ncm156ozin-17hm081204s-p-99.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -7444,8 +7487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J36" sqref="A36:J36"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J33" sqref="A33:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7465,8 +7508,8 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -7482,10 +7525,10 @@
       <c r="C4" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="10" t="s">
         <v>361</v>
       </c>
@@ -10933,7 +10976,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10942,7 +10985,7 @@
     <col min="2" max="2" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="54.88671875" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -10955,7 +10998,7 @@
       <c r="D1" t="s">
         <v>602</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>599</v>
       </c>
       <c r="F1" t="s">
@@ -10983,7 +11026,7 @@
       <c r="D3" t="s">
         <v>666</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="29" t="s">
         <v>664</v>
       </c>
       <c r="F3">
@@ -11000,7 +11043,7 @@
       <c r="D4" t="s">
         <v>668</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="29" t="s">
         <v>662</v>
       </c>
       <c r="F4">
@@ -11022,7 +11065,7 @@
       <c r="D6" t="s">
         <v>671</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="29" t="s">
         <v>557</v>
       </c>
       <c r="F6">
@@ -11039,7 +11082,7 @@
       <c r="D7" t="s">
         <v>672</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="29" t="s">
         <v>690</v>
       </c>
       <c r="F7">
@@ -11056,7 +11099,7 @@
       <c r="D8" t="s">
         <v>675</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="29" t="s">
         <v>673</v>
       </c>
       <c r="F8">
@@ -11073,7 +11116,7 @@
       <c r="D9" t="s">
         <v>678</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>677</v>
       </c>
       <c r="F9">
@@ -11090,7 +11133,7 @@
       <c r="D10" t="s">
         <v>680</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="29" t="s">
         <v>681</v>
       </c>
       <c r="F10">
@@ -11098,6 +11141,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>692</v>
+      </c>
       <c r="B12">
         <v>1</v>
       </c>
@@ -11107,7 +11153,7 @@
       <c r="D12" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="29" t="s">
         <v>554</v>
       </c>
       <c r="F12">
@@ -11131,7 +11177,7 @@
       <c r="D13" t="s">
         <v>622</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="29" t="s">
         <v>613</v>
       </c>
       <c r="F13">
@@ -11155,7 +11201,7 @@
       <c r="D14" t="s">
         <v>617</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="30" t="s">
         <v>615</v>
       </c>
       <c r="F14">
@@ -11179,7 +11225,7 @@
       <c r="D15" t="s">
         <v>618</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="29" t="s">
         <v>619</v>
       </c>
       <c r="F15">
@@ -11255,7 +11301,7 @@
       <c r="D19" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="29" t="s">
         <v>649</v>
       </c>
       <c r="F19">
@@ -11291,7 +11337,7 @@
       <c r="D21" t="s">
         <v>642</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="30" t="s">
         <v>615</v>
       </c>
       <c r="F21">
@@ -11321,7 +11367,7 @@
       <c r="D23" t="s">
         <v>656</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="29" t="s">
         <v>654</v>
       </c>
       <c r="F23">
@@ -11472,7 +11518,7 @@
       <c r="D34" t="s">
         <v>604</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="29" t="s">
         <v>608</v>
       </c>
       <c r="F34">
@@ -11496,7 +11542,7 @@
       <c r="D35" t="s">
         <v>611</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="29" t="s">
         <v>605</v>
       </c>
       <c r="G35" s="23">

</xml_diff>

<commit_message>
kleine verbesserungen an Forearm
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11294,7 +11294,7 @@
   <dimension ref="A1:K138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K106" sqref="K71:K106"/>
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12005,7 +12005,7 @@
     </row>
     <row r="53" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C53" s="32" t="str">
         <f>C73</f>
@@ -12020,7 +12020,7 @@
     </row>
     <row r="54" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C54" s="32" t="str">
         <f>C84</f>
@@ -12296,11 +12296,11 @@
       </c>
       <c r="I73" s="18">
         <f>SUMIF(C$1:C$69,"="&amp;C73,B$1:B$69)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J73" s="33">
         <f>G73*B73-I73</f>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K73" s="35">
         <f t="shared" ref="K73" si="4">B73*H73</f>
@@ -12611,7 +12611,7 @@
     <row r="84" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="33">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C84" s="32" t="s">
         <v>725</v>
@@ -12627,7 +12627,7 @@
       </c>
       <c r="I84" s="18">
         <f>SUMIF(C$1:C$69,"="&amp;C84,B$1:B$69)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J84" s="33">
         <f t="shared" si="5"/>
@@ -12635,7 +12635,7 @@
       </c>
       <c r="K84" s="35">
         <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1.3499999999999999</v>
       </c>
     </row>
     <row r="85" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Schraubenlänge  im Grippermount korrigiert
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11958,8 +11958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11996,11 +11996,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f>C170</f>
-        <v>XXXXX Zylinderkopfschraube Innensechskant M3 22mm</v>
+        <f>C168</f>
+        <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D3" t="s">
         <v>610</v>
@@ -12011,7 +12011,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>611</v>
@@ -14447,11 +14447,11 @@
       </c>
       <c r="I168" s="18">
         <f>SUMIF(C$1:C$163,"="&amp;C168,B$1:B$163)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J168" s="33">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K168" s="34">
         <f>B168*H168</f>
@@ -14507,11 +14507,11 @@
       </c>
       <c r="I170" s="18">
         <f>SUMIF(C$1:C$163,"="&amp;C170,B$1:B$163)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J170" s="33">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K170" s="34">
         <f t="shared" ref="K170:K235" si="6">B170*H170</f>

</xml_diff>

<commit_message>
zahnriemen für Hüfte jetzt drin
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -17,12 +17,16 @@
     <sheet name="Drehkranz" sheetId="9" r:id="rId8"/>
     <sheet name="BOM" sheetId="7" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="Kaufstatus">BOM!$L:$L</definedName>
+    <definedName name="ShoppingStatus">BOM!$L:$L</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="841">
   <si>
     <t>Bauteilnummer</t>
   </si>
@@ -2028,9 +2032,6 @@
     <t>Rillenkugellager  3.967 x 7.938 x 3.175 mm</t>
   </si>
   <si>
-    <t>https://www.reichelt.de/DI-20MM/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=7121&amp;artnr=DI+20MM&amp;SEARCH=distanzbolzen</t>
-  </si>
-  <si>
     <t>Gabelbefestigung</t>
   </si>
   <si>
@@ -2061,9 +2062,6 @@
     <t>http://www.cncshop.at/index.php?a=10273</t>
   </si>
   <si>
-    <t>https://www.reichelt.de/Distanzhuelsen-etc-/DI-5MM/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=7123&amp;GROUPID=3365&amp;artnr=DI+5MM</t>
-  </si>
-  <si>
     <t>Übersetzung HandgelenkNicker</t>
   </si>
   <si>
@@ -2376,9 +2374,6 @@
     <t>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</t>
   </si>
   <si>
-    <t>Distanzbolzen M3 5mm, , Schlüsselweite 5mm</t>
-  </si>
-  <si>
     <t>Shoulder</t>
   </si>
   <si>
@@ -2463,9 +2458,6 @@
     <t>Bestellmenge [VPE]</t>
   </si>
   <si>
-    <t>XXXX Distanzbolzen M3 20mm, Schlüsselweite 5mm</t>
-  </si>
-  <si>
     <t>Senkkopfschraube Innensechskant M6 16mm</t>
   </si>
   <si>
@@ -2481,9 +2473,6 @@
     <t>Befestigung DrehlagerDeckel/Drehlager/Basis</t>
   </si>
   <si>
-    <t>gekauft</t>
-  </si>
-  <si>
     <t>Befestigung HüftMotorBasis</t>
   </si>
   <si>
@@ -2527,6 +2516,39 @@
   </si>
   <si>
     <t>GehäuseVerbindung Oben</t>
+  </si>
+  <si>
+    <t>Hüftmotor Zahnriemen original 564mm</t>
+  </si>
+  <si>
+    <t>http://www.cncshop.at/index.php?a=10331</t>
+  </si>
+  <si>
+    <t>Zahnriemen T5 560mm 10mm Breite</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Got it</t>
+  </si>
+  <si>
+    <t>ordered not yet delivered</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Still Open</t>
+  </si>
+  <si>
+    <t>http://www.3d-drucker-experte.de/</t>
+  </si>
+  <si>
+    <t>returned</t>
   </si>
 </sst>
 </file>
@@ -2541,7 +2563,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2587,6 +2609,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2611,7 +2641,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2682,6 +2712,10 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3723,7 +3757,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="E42" t="s">
         <v>624</v>
@@ -4266,7 +4300,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C46" s="5">
         <f>C50/C48*(C54/C52)</f>
@@ -4520,7 +4554,7 @@
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C70" s="2">
         <f>C66/C46</f>
@@ -4532,7 +4566,7 @@
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C71" s="2">
         <f>C65/C46</f>
@@ -4818,7 +4852,7 @@
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C78" s="2">
         <f>C71*(1+C57)</f>
@@ -8326,7 +8360,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -11935,10 +11969,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L269"/>
+  <dimension ref="A1:M269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11949,9 +11983,10 @@
     <col min="4" max="4" width="42.33203125" customWidth="1"/>
     <col min="5" max="5" width="25.21875" style="29" customWidth="1"/>
     <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>597</v>
       </c>
@@ -11967,18 +12002,27 @@
       <c r="F1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>833</v>
+      </c>
+      <c r="M1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D3" t="s">
@@ -11987,8 +12031,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
@@ -12001,13 +12048,16 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1</v>
       </c>
@@ -12022,12 +12072,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="str">
-        <f>C170</f>
+        <f>C171</f>
         <v>Zylinderkopfschraube Innensechskant M3 12mm</v>
       </c>
       <c r="D7" t="s">
@@ -12037,31 +12087,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D8" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="str">
-        <f>C178</f>
+        <f>C179</f>
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D9" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2</v>
       </c>
@@ -12073,7 +12123,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -12082,20 +12132,20 @@
         <v xml:space="preserve">Herkulex Servo DRS - 0201 </v>
       </c>
       <c r="D11" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="str">
-        <f>C197</f>
+        <f>C196</f>
         <v>Zahnriemenscheibe T2,5, 16 Zähne</v>
       </c>
       <c r="D13" t="s">
@@ -12104,12 +12154,12 @@
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="str">
-        <f>C199</f>
+        <f>C198</f>
         <v>Zahnriemenscheibe T2,5, 44 Zähne</v>
       </c>
       <c r="D14" t="s">
@@ -12118,12 +12168,12 @@
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="str">
-        <f>C197</f>
+        <f>C196</f>
         <v>Zahnriemenscheibe T2,5, 16 Zähne</v>
       </c>
       <c r="D15" t="s">
@@ -12132,12 +12182,12 @@
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="str">
-        <f>C207</f>
+        <f>C206</f>
         <v>Zahnriemen T2,5 160mm 6mm Breite</v>
       </c>
       <c r="D16" t="s">
@@ -12151,7 +12201,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="str">
-        <f>C187</f>
+        <f>C188</f>
         <v>Silberstahlwelle 6mm Durchmesser</v>
       </c>
       <c r="D17" t="s">
@@ -12241,7 +12291,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="32" t="str">
-        <f>C169</f>
+        <f>C170</f>
         <v>Zylinderkopfschraube Innensechskant M3 14mm</v>
       </c>
       <c r="D23" s="32" t="s">
@@ -12255,7 +12305,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D24" s="32" t="s">
@@ -12269,7 +12319,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="32" t="str">
-        <f>C206</f>
+        <f>C205</f>
         <v>Zahnriemen T2,5 230mm 6mm Breite</v>
       </c>
       <c r="D25" s="32" t="s">
@@ -12283,7 +12333,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="32" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D26" s="32" t="s">
@@ -12297,7 +12347,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D27" s="32" t="s">
@@ -12325,7 +12375,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="32" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D29" s="32" t="s">
@@ -12340,7 +12390,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="32" t="str">
-        <f>C171</f>
+        <f>C172</f>
         <v>Zylinderkopfschraube Innensechskant M2 6mm</v>
       </c>
       <c r="D30" s="32" t="s">
@@ -12355,7 +12405,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="32" t="str">
-        <f>C179</f>
+        <f>C180</f>
         <v>Muttern M2</v>
       </c>
       <c r="D31" s="32" t="s">
@@ -12385,11 +12435,11 @@
         <v>4</v>
       </c>
       <c r="C33" s="32" t="str">
-        <f>C174</f>
+        <f>C175</f>
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="E33" s="9"/>
       <c r="H33" s="22"/>
@@ -12400,11 +12450,11 @@
         <v>4</v>
       </c>
       <c r="C34" s="32" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="E34" s="9"/>
       <c r="H34" s="22"/>
@@ -12415,7 +12465,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="32" t="str">
-        <f>C184</f>
+        <f>C185</f>
         <v>Unterlegscheiben M2 Dicke 0,5mm</v>
       </c>
       <c r="D35" s="32" t="s">
@@ -12434,7 +12484,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E36" s="9"/>
       <c r="H36" s="22"/>
@@ -12445,11 +12495,11 @@
         <v>4</v>
       </c>
       <c r="C37" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
@@ -12463,7 +12513,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
@@ -12473,11 +12523,11 @@
         <v>4</v>
       </c>
       <c r="C39" s="32" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E39" s="9"/>
       <c r="H39" s="22"/>
@@ -12488,11 +12538,11 @@
         <v>4</v>
       </c>
       <c r="C40" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="22"/>
@@ -12502,11 +12552,11 @@
         <v>2</v>
       </c>
       <c r="C41" s="32" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="22"/>
@@ -12516,11 +12566,11 @@
         <v>2</v>
       </c>
       <c r="C42" s="32" t="str">
-        <f>C174</f>
+        <f>C175</f>
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
@@ -12533,7 +12583,7 @@
     </row>
     <row r="44" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -12543,7 +12593,7 @@
         <v>Rillenkugellager DIN 625 SKF - 61807 35x47x7mm</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E44" s="9"/>
       <c r="H44" s="22"/>
@@ -12558,7 +12608,7 @@
         <v>RillenKugellager 6x19x6</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="22"/>
@@ -12572,7 +12622,7 @@
         <v>Rillenkugellager 6x10x3</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E46" s="9"/>
       <c r="H46" s="22"/>
@@ -12587,7 +12637,7 @@
         <v>Rillenkugellager 3x10x4</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E47" s="9"/>
       <c r="H47" s="22"/>
@@ -12598,11 +12648,11 @@
         <v>2</v>
       </c>
       <c r="C48" s="32" t="str">
-        <f>C194</f>
+        <f>C193</f>
         <v>Distanzhülsen M6 10mm</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
@@ -12612,11 +12662,11 @@
         <v>40</v>
       </c>
       <c r="C49" s="32" t="str">
-        <f>C187</f>
+        <f>C188</f>
         <v>Silberstahlwelle 6mm Durchmesser</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="22"/>
@@ -12627,11 +12677,11 @@
         <v>50</v>
       </c>
       <c r="C50" s="32" t="str">
-        <f>C187</f>
+        <f>C188</f>
         <v>Silberstahlwelle 6mm Durchmesser</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
@@ -12641,11 +12691,11 @@
         <v>50</v>
       </c>
       <c r="C51" s="32" t="str">
-        <f>C188</f>
+        <f>C189</f>
         <v>Silberstahlwelle 3mm Durchmesser</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E51" s="9"/>
       <c r="H51" s="22"/>
@@ -12701,11 +12751,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="32" t="str">
-        <f>C208</f>
+        <f>C207</f>
         <v>Zahnriemen T2,5 200mm 6mm Breite</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H55" s="22"/>
       <c r="I55" s="22"/>
@@ -12715,11 +12765,11 @@
         <v>1</v>
       </c>
       <c r="C56" s="32" t="str">
-        <f>C208</f>
+        <f>C207</f>
         <v>Zahnriemen T2,5 200mm 6mm Breite</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H56" s="22"/>
       <c r="I56" s="22"/>
@@ -12729,11 +12779,11 @@
         <v>4</v>
       </c>
       <c r="C57" s="32" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="22"/>
@@ -12743,11 +12793,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="32" t="str">
-        <f>C178</f>
+        <f>C179</f>
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E58" s="9"/>
       <c r="H58" s="22"/>
@@ -12758,11 +12808,11 @@
         <v>8</v>
       </c>
       <c r="C59" s="32" t="str">
-        <f>C167</f>
+        <f>C168</f>
         <v>Zylinderkopfschraube Innensechskant M3 25mm</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E59" s="9"/>
       <c r="H59" s="22"/>
@@ -12777,7 +12827,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E60" s="9"/>
       <c r="H60" s="22"/>
@@ -12788,11 +12838,11 @@
         <v>2</v>
       </c>
       <c r="C61" s="32" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="E61" s="9"/>
       <c r="H61" s="22"/>
@@ -12807,7 +12857,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="E62" s="9"/>
       <c r="H62" s="22"/>
@@ -12833,11 +12883,11 @@
         <v>1</v>
       </c>
       <c r="C64" s="32" t="str">
-        <f>C197</f>
+        <f>C196</f>
         <v>Zahnriemenscheibe T2,5, 16 Zähne</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E64" s="9"/>
       <c r="H64" s="22"/>
@@ -12848,11 +12898,11 @@
         <v>1</v>
       </c>
       <c r="C65" s="32" t="str">
-        <f>C197</f>
+        <f>C196</f>
         <v>Zahnriemenscheibe T2,5, 16 Zähne</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E65" s="9"/>
       <c r="H65" s="22"/>
@@ -12863,11 +12913,11 @@
         <v>1</v>
       </c>
       <c r="C66" s="32" t="str">
-        <f>C202</f>
+        <f>C201</f>
         <v>Zahnriemenscheibe T2,5, 60 Zähne</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E66" s="9"/>
       <c r="H66" s="22"/>
@@ -12897,13 +12947,13 @@
     </row>
     <row r="69" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" s="32" t="str">
-        <f>C171</f>
+        <f>C172</f>
         <v>Zylinderkopfschraube Innensechskant M2 6mm</v>
       </c>
       <c r="D69" s="32" t="s">
@@ -12918,7 +12968,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="32" t="str">
-        <f>C179</f>
+        <f>C180</f>
         <v>Muttern M2</v>
       </c>
       <c r="D70" s="32" t="s">
@@ -12948,7 +12998,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="32" t="str">
-        <f>C184</f>
+        <f>C185</f>
         <v>Unterlegscheiben M2 Dicke 0,5mm</v>
       </c>
       <c r="D72" s="32" t="s">
@@ -12967,7 +13017,7 @@
         <v>Rillenkugellager DIN 625 SKF - 61807 35x47x7mm</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E73" s="9"/>
       <c r="H73" s="22"/>
@@ -12978,11 +13028,11 @@
         <v>4</v>
       </c>
       <c r="C74" t="str">
-        <f>C174</f>
+        <f>C175</f>
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D74" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E74" s="9"/>
       <c r="H74" s="22"/>
@@ -12993,11 +13043,11 @@
         <v>4</v>
       </c>
       <c r="C75" t="str">
-        <f>C174</f>
+        <f>C175</f>
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D75" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E75" s="9"/>
       <c r="H75" s="22"/>
@@ -13008,11 +13058,11 @@
         <v>4</v>
       </c>
       <c r="C76" s="32" t="str">
-        <f>C164</f>
+        <f>C165</f>
         <v>Zylinderkopfschraube Innensechskant M3 40mm</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E76" s="9"/>
       <c r="H76" s="22"/>
@@ -13023,11 +13073,11 @@
         <v>4</v>
       </c>
       <c r="C77" s="32" t="str">
-        <f>C165</f>
+        <f>C166</f>
         <v>Zylinderkopfschraube Innensechskant M3 30mm</v>
       </c>
       <c r="D77" s="32" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E77" s="9"/>
       <c r="H77" s="22"/>
@@ -13038,11 +13088,11 @@
         <v>8</v>
       </c>
       <c r="C78" s="32" t="str">
-        <f>C178</f>
+        <f>C179</f>
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D78" s="32" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E78" s="9"/>
       <c r="H78" s="22"/>
@@ -13053,11 +13103,11 @@
         <v>12</v>
       </c>
       <c r="C79" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D79" s="32" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E79" s="9"/>
       <c r="H79" s="22"/>
@@ -13068,11 +13118,11 @@
         <v>4</v>
       </c>
       <c r="C80" s="32" t="str">
-        <f>C163</f>
+        <f>C164</f>
         <v>Zylinderkopfschraube Innensechskant M3 45mm</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E80" s="9"/>
       <c r="H80" s="22"/>
@@ -13087,7 +13137,7 @@
         <v>Rillenkugellager  4 x13 x 5 mm mit Flansch</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E81" s="9"/>
       <c r="H81" s="22"/>
@@ -13098,11 +13148,11 @@
         <v>12</v>
       </c>
       <c r="C82" s="32" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D82" s="32" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E82" s="9"/>
       <c r="H82" s="22"/>
@@ -13113,11 +13163,11 @@
         <v>1</v>
       </c>
       <c r="C83" s="32" t="str">
-        <f>C181</f>
+        <f>C182</f>
         <v>Madenschraube M3 16mm</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E83" s="9"/>
       <c r="H83" s="22"/>
@@ -13128,11 +13178,11 @@
         <v>72</v>
       </c>
       <c r="C84" s="32" t="str">
-        <f>C189</f>
+        <f>C190</f>
         <v>Silberstahlwelle 8mm Durchmesser</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E84" s="9"/>
       <c r="H84" s="22"/>
@@ -13143,11 +13193,11 @@
         <v>1</v>
       </c>
       <c r="C85" s="32" t="str">
-        <f>C203</f>
+        <f>C202</f>
         <v>Zahnriemenscheibe T5, 48 Zähne</v>
       </c>
       <c r="D85" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E85" s="9"/>
       <c r="H85" s="22"/>
@@ -13158,11 +13208,11 @@
         <v>1</v>
       </c>
       <c r="C86" s="32" t="str">
-        <f>C204</f>
+        <f>C203</f>
         <v>Zahnriemenscheibe T5, 16 Zähne</v>
       </c>
       <c r="D86" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E86" s="9"/>
       <c r="H86" s="22"/>
@@ -13177,7 +13227,7 @@
         <v>Metallbohrer 8mm</v>
       </c>
       <c r="D87" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E87" s="9"/>
       <c r="H87" s="22"/>
@@ -13192,7 +13242,7 @@
         <v>Gewindeschneider M3</v>
       </c>
       <c r="D88" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E88" s="9"/>
       <c r="H88" s="22"/>
@@ -13207,7 +13257,7 @@
         <v>Metallbohrer 2.3mm (für M3 Gewinde)</v>
       </c>
       <c r="D89" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E89" s="9"/>
       <c r="H89" s="22"/>
@@ -13218,11 +13268,11 @@
         <v>2</v>
       </c>
       <c r="C90" t="str">
-        <f>C182</f>
+        <f>C183</f>
         <v>Madenschraube M3 5mm</v>
       </c>
       <c r="D90" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E90" s="9"/>
       <c r="H90" s="22"/>
@@ -13237,7 +13287,7 @@
         <v>Rillenkugellager 8x22x7</v>
       </c>
       <c r="D91" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E91" s="9"/>
       <c r="H91" s="22"/>
@@ -13248,11 +13298,11 @@
         <v>4</v>
       </c>
       <c r="C92" t="str">
-        <f>C185</f>
+        <f>C186</f>
         <v>Unterlegscheiben 8mm Innendurchmesser</v>
       </c>
       <c r="D92" s="32" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E92" s="9"/>
       <c r="H92" s="22"/>
@@ -13263,11 +13313,11 @@
         <v>4</v>
       </c>
       <c r="C93" t="str">
-        <f>C163</f>
+        <f>C164</f>
         <v>Zylinderkopfschraube Innensechskant M3 45mm</v>
       </c>
       <c r="D93" s="32" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E93" s="9"/>
       <c r="H93" s="22"/>
@@ -13278,11 +13328,11 @@
         <v>4</v>
       </c>
       <c r="C94" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D94" s="32" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E94" s="9"/>
       <c r="H94" s="22"/>
@@ -13293,11 +13343,11 @@
         <v>4</v>
       </c>
       <c r="C95" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D95" s="32" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E95" s="9"/>
       <c r="H95" s="22"/>
@@ -13308,11 +13358,11 @@
         <v>1</v>
       </c>
       <c r="C96" t="str">
-        <f>C163</f>
+        <f>C164</f>
         <v>Zylinderkopfschraube Innensechskant M3 45mm</v>
       </c>
       <c r="D96" s="32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E96" s="9"/>
       <c r="H96" s="22"/>
@@ -13323,11 +13373,11 @@
         <v>4</v>
       </c>
       <c r="C97" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E97" s="9"/>
       <c r="H97" s="22"/>
@@ -13338,11 +13388,11 @@
         <v>1</v>
       </c>
       <c r="C98" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E98" s="9"/>
       <c r="H98" s="22"/>
@@ -13357,7 +13407,7 @@
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D99" s="32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E99" s="9"/>
       <c r="H99" s="22"/>
@@ -13368,11 +13418,11 @@
         <v>4</v>
       </c>
       <c r="C100" t="str">
-        <f>C186</f>
+        <f>C187</f>
         <v>Unterlegscheiben M3 Kunststoff 0,8mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D100" s="32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E100" s="9"/>
       <c r="H100" s="22"/>
@@ -13383,7 +13433,7 @@
         <v>4</v>
       </c>
       <c r="C101" t="str">
-        <f>C175</f>
+        <f>C176</f>
         <v>Senkkopfschraube Innensechskant M3 25mm</v>
       </c>
       <c r="D101" s="32" t="s">
@@ -13398,11 +13448,11 @@
         <v>8</v>
       </c>
       <c r="C102" t="str">
-        <f>C167</f>
+        <f>C168</f>
         <v>Zylinderkopfschraube Innensechskant M3 25mm</v>
       </c>
       <c r="D102" s="32" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E102" s="9"/>
       <c r="H102" s="22"/>
@@ -13417,7 +13467,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D103" s="32" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E103" s="9"/>
       <c r="H103" s="22"/>
@@ -13428,11 +13478,11 @@
         <v>8</v>
       </c>
       <c r="C104" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D104" s="32" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E104" s="9"/>
       <c r="H104" s="22"/>
@@ -13443,11 +13493,11 @@
         <v>4</v>
       </c>
       <c r="C105" t="str">
-        <f>C165</f>
+        <f>C166</f>
         <v>Zylinderkopfschraube Innensechskant M3 30mm</v>
       </c>
       <c r="D105" s="32" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E105" s="9"/>
       <c r="H105" s="22"/>
@@ -13458,11 +13508,11 @@
         <v>4</v>
       </c>
       <c r="C106" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D106" s="32" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E106" s="9"/>
       <c r="H106" s="22"/>
@@ -13473,11 +13523,11 @@
         <v>1</v>
       </c>
       <c r="C107" t="str">
-        <f>C209</f>
+        <f>C208</f>
         <v>Zahnriemen T5 340mm 10mm Breite</v>
       </c>
       <c r="D107" s="32" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E107" s="9"/>
       <c r="H107" s="22"/>
@@ -13488,11 +13538,11 @@
         <v>1</v>
       </c>
       <c r="C108" t="str">
-        <f>C204</f>
+        <f>C203</f>
         <v>Zahnriemenscheibe T5, 16 Zähne</v>
       </c>
       <c r="D108" s="32" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E108" s="9"/>
       <c r="H108" s="22"/>
@@ -13503,11 +13553,11 @@
         <v>1</v>
       </c>
       <c r="C109" t="str">
-        <f>C210</f>
+        <f>C209</f>
         <v>Zahnriemen T5 510mm 10mm Breite</v>
       </c>
       <c r="D109" s="32" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E109" s="9"/>
       <c r="H109" s="22"/>
@@ -13536,13 +13586,13 @@
     </row>
     <row r="112" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="B112">
         <v>4</v>
       </c>
       <c r="C112" t="str">
-        <f>C171</f>
+        <f>C172</f>
         <v>Zylinderkopfschraube Innensechskant M2 6mm</v>
       </c>
       <c r="D112" s="32" t="s">
@@ -13557,7 +13607,7 @@
         <v>4</v>
       </c>
       <c r="C113" t="str">
-        <f>C179</f>
+        <f>C180</f>
         <v>Muttern M2</v>
       </c>
       <c r="D113" s="32" t="s">
@@ -13587,7 +13637,7 @@
         <v>2</v>
       </c>
       <c r="C115" t="str">
-        <f>C184</f>
+        <f>C185</f>
         <v>Unterlegscheiben M2 Dicke 0,5mm</v>
       </c>
       <c r="D115" s="32" t="s">
@@ -13606,7 +13656,7 @@
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D116" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E116" s="9"/>
       <c r="H116" s="22"/>
@@ -13617,11 +13667,11 @@
         <v>4</v>
       </c>
       <c r="C117" t="str">
-        <f>C186</f>
+        <f>C187</f>
         <v>Unterlegscheiben M3 Kunststoff 0,8mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D117" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E117" s="9"/>
       <c r="H117" s="22"/>
@@ -13632,11 +13682,11 @@
         <v>4</v>
       </c>
       <c r="C118" t="str">
-        <f>C177</f>
+        <f>C178</f>
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D118" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E118" s="9"/>
       <c r="H118" s="22"/>
@@ -13647,11 +13697,11 @@
         <v>2</v>
       </c>
       <c r="C119" t="str">
-        <f>C168</f>
+        <f>C169</f>
         <v>XXXXX Zylinderkopfschraube Innensechskant M3 22mm</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E119" s="9"/>
       <c r="H119" s="22"/>
@@ -13662,11 +13712,11 @@
         <v>3</v>
       </c>
       <c r="C120" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D120" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E120" s="9"/>
       <c r="H120" s="22"/>
@@ -13677,11 +13727,11 @@
         <v>1</v>
       </c>
       <c r="C121" t="str">
-        <f>C164</f>
+        <f>C165</f>
         <v>Zylinderkopfschraube Innensechskant M3 40mm</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E121" s="9"/>
       <c r="H121" s="22"/>
@@ -13692,11 +13742,11 @@
         <v>1</v>
       </c>
       <c r="C122" t="str">
-        <f>C163</f>
+        <f>C164</f>
         <v>Zylinderkopfschraube Innensechskant M3 45mm</v>
       </c>
       <c r="D122" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E122" s="9"/>
       <c r="H122" s="22"/>
@@ -13707,11 +13757,11 @@
         <v>1</v>
       </c>
       <c r="C123" t="str">
-        <f>C167</f>
+        <f>C168</f>
         <v>Zylinderkopfschraube Innensechskant M3 25mm</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E123" s="9"/>
       <c r="H123" s="22"/>
@@ -13726,7 +13776,7 @@
         <v>Rillenkugellager 8x22x7</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E124" s="9"/>
       <c r="H124" s="22"/>
@@ -13737,11 +13787,11 @@
         <v>110</v>
       </c>
       <c r="C125" t="str">
-        <f>C189</f>
+        <f>C190</f>
         <v>Silberstahlwelle 8mm Durchmesser</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E125" s="9"/>
       <c r="H125" s="22"/>
@@ -13752,11 +13802,11 @@
         <v>1</v>
       </c>
       <c r="C126" t="str">
-        <f>C203</f>
+        <f>C202</f>
         <v>Zahnriemenscheibe T5, 48 Zähne</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E126" s="9"/>
       <c r="H126" s="22"/>
@@ -13767,11 +13817,11 @@
         <v>1</v>
       </c>
       <c r="C127" t="str">
-        <f>C204</f>
+        <f>C203</f>
         <v>Zahnriemenscheibe T5, 16 Zähne</v>
       </c>
       <c r="D127" s="32" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E127" s="9"/>
       <c r="H127" s="22"/>
@@ -13782,11 +13832,11 @@
         <v>1</v>
       </c>
       <c r="C128" t="str">
-        <f>C211</f>
+        <f>C210</f>
         <v>Zahnriemen T5 500mm 10mm Breite</v>
       </c>
       <c r="D128" s="32" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E128" s="9"/>
       <c r="H128" s="22"/>
@@ -13797,11 +13847,11 @@
         <v>1</v>
       </c>
       <c r="C129" t="str">
-        <f>C212</f>
+        <f>C211</f>
         <v>Zahnriemen T5 480mm 10mm Breite</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E129" s="9"/>
       <c r="H129" s="22"/>
@@ -13812,11 +13862,11 @@
         <v>1</v>
       </c>
       <c r="C130" t="str">
-        <f>C204</f>
+        <f>C203</f>
         <v>Zahnriemenscheibe T5, 16 Zähne</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="E130" s="9"/>
       <c r="H130" s="22"/>
@@ -13827,11 +13877,11 @@
         <v>1</v>
       </c>
       <c r="C131" t="str">
-        <f>C213</f>
+        <f>C212</f>
         <v>Zahnriemen T5 340mm 10mm Breite</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="E131" s="9"/>
       <c r="H131" s="22"/>
@@ -13842,11 +13892,11 @@
         <v>4</v>
       </c>
       <c r="C132" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D132" s="32" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E132" s="9"/>
       <c r="H132" s="22"/>
@@ -13857,11 +13907,11 @@
         <v>4</v>
       </c>
       <c r="C133" t="str">
-        <f>C178</f>
+        <f>C179</f>
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D133" s="32" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E133" s="9"/>
       <c r="H133" s="22"/>
@@ -13872,11 +13922,11 @@
         <v>4</v>
       </c>
       <c r="C134" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E134" s="9"/>
       <c r="H134" s="22"/>
@@ -13887,11 +13937,11 @@
         <v>4</v>
       </c>
       <c r="C135" t="str">
-        <f>C163</f>
+        <f>C164</f>
         <v>Zylinderkopfschraube Innensechskant M3 45mm</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E135" s="9"/>
       <c r="H135" s="22"/>
@@ -13902,11 +13952,11 @@
         <v>4</v>
       </c>
       <c r="C136" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E136" s="9"/>
       <c r="H136" s="22"/>
@@ -13921,7 +13971,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E137" s="9"/>
       <c r="H137" s="22"/>
@@ -13933,11 +13983,11 @@
         <v>300</v>
       </c>
       <c r="C138" t="str">
-        <f>C195</f>
+        <f>C194</f>
         <v>Gewindestange M3</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E138" s="9"/>
       <c r="H138" s="22"/>
@@ -13948,11 +13998,11 @@
         <v>6</v>
       </c>
       <c r="C139" t="str">
-        <f>C190</f>
+        <f>C191</f>
         <v>Unterlegscheiben M3 Stahl  0,8mm, Außendurchmesser 9mm</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E139" s="9"/>
       <c r="H139" s="22"/>
@@ -13967,7 +14017,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E140" s="9"/>
       <c r="H140" s="22"/>
@@ -13997,7 +14047,7 @@
         <v>Rillenkugellager DIN 625 SKF - SKF 61818 - 90x115x13</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="E142" s="9"/>
       <c r="H142" s="22"/>
@@ -14011,7 +14061,7 @@
     </row>
     <row r="144" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -14021,7 +14071,7 @@
         <v>Rillenkugellager DIN 625 SKF - SKF 61818 - 85x110x13</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E144" s="9"/>
       <c r="H144" s="22"/>
@@ -14032,11 +14082,11 @@
         <v>6</v>
       </c>
       <c r="C145" t="str">
-        <f>C164</f>
+        <f>C165</f>
         <v>Zylinderkopfschraube Innensechskant M3 40mm</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E145" s="9"/>
       <c r="H145" s="22"/>
@@ -14047,11 +14097,11 @@
         <v>6</v>
       </c>
       <c r="C146" t="str">
-        <f>C190</f>
+        <f>C191</f>
         <v>Unterlegscheiben M3 Stahl  0,8mm, Außendurchmesser 9mm</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E146" s="9"/>
       <c r="H146" s="22"/>
@@ -14062,11 +14112,11 @@
         <v>8</v>
       </c>
       <c r="C147" t="str">
-        <f>C174</f>
+        <f>C175</f>
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E147" s="9"/>
       <c r="H147" s="22"/>
@@ -14081,7 +14131,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D148" s="32" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E148" s="9"/>
       <c r="H148" s="22"/>
@@ -14092,11 +14142,11 @@
         <v>8</v>
       </c>
       <c r="C149" t="str">
-        <f>C165</f>
+        <f>C166</f>
         <v>Zylinderkopfschraube Innensechskant M3 30mm</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E149" s="9"/>
       <c r="H149" s="22"/>
@@ -14122,7 +14172,7 @@
         <v>4</v>
       </c>
       <c r="C151" t="str">
-        <f>C171</f>
+        <f>C172</f>
         <v>Zylinderkopfschraube Innensechskant M2 6mm</v>
       </c>
       <c r="D151" s="32" t="s">
@@ -14137,7 +14187,7 @@
         <v>4</v>
       </c>
       <c r="C152" t="str">
-        <f>C179</f>
+        <f>C180</f>
         <v>Muttern M2</v>
       </c>
       <c r="D152" s="32" t="s">
@@ -14152,11 +14202,11 @@
         <v>4</v>
       </c>
       <c r="C153" t="str">
-        <f>C178</f>
+        <f>C179</f>
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="E153" s="9"/>
       <c r="H153" s="22"/>
@@ -14167,11 +14217,11 @@
         <v>4</v>
       </c>
       <c r="C154" t="str">
-        <f>C166</f>
+        <f>C167</f>
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="E154" s="9"/>
       <c r="H154" s="22"/>
@@ -14182,11 +14232,11 @@
         <v>4</v>
       </c>
       <c r="C155" t="str">
-        <f>C183</f>
+        <f>C184</f>
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="E155" s="9"/>
       <c r="H155" s="22"/>
@@ -14201,7 +14251,7 @@
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="E156" s="9"/>
       <c r="H156" s="22"/>
@@ -14212,11 +14262,11 @@
         <v>8</v>
       </c>
       <c r="C157" t="str">
-        <f>C186</f>
+        <f>C187</f>
         <v>Unterlegscheiben M3 Kunststoff 0,8mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="E157" s="9"/>
       <c r="H157" s="22"/>
@@ -14227,11 +14277,11 @@
         <v>1</v>
       </c>
       <c r="C158" t="str">
-        <f>C198</f>
+        <f>C197</f>
         <v>Zahnriemenscheibe T2,5, 12 Zähne</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="E158" s="9"/>
       <c r="H158" s="22"/>
@@ -14246,135 +14296,120 @@
         <v>NEMA 24 - 57x57x56 - 1,26Nm - 6,35mm Achse</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="E159" s="9"/>
       <c r="H159" s="22"/>
       <c r="I159" s="22"/>
     </row>
     <row r="160" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D160" s="32"/>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160" t="str">
+        <f>C213</f>
+        <v>Zahnriemen T5 560mm 10mm Breite</v>
+      </c>
+      <c r="D160" s="32" t="s">
+        <v>830</v>
+      </c>
       <c r="E160" s="9"/>
       <c r="H160" s="22"/>
       <c r="I160" s="22"/>
     </row>
     <row r="161" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C161" s="32"/>
+      <c r="D161" s="32"/>
       <c r="E161" s="9"/>
       <c r="H161" s="22"/>
       <c r="I161" s="22"/>
     </row>
     <row r="162" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B162" t="s">
-        <v>812</v>
-      </c>
-      <c r="C162" s="32" t="s">
+      <c r="A162" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162" s="32"/>
+      <c r="E162" s="9"/>
+      <c r="H162" s="22"/>
+      <c r="I162" s="22"/>
+    </row>
+    <row r="163" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
+        <v>809</v>
+      </c>
+      <c r="C163" s="32" t="s">
         <v>663</v>
       </c>
-      <c r="E162" s="9"/>
-      <c r="G162" t="s">
+      <c r="E163" s="9"/>
+      <c r="G163" t="s">
         <v>660</v>
       </c>
-      <c r="H162" s="22" t="s">
+      <c r="H163" s="22" t="s">
+        <v>671</v>
+      </c>
+      <c r="I163" s="22" t="s">
         <v>672</v>
       </c>
-      <c r="I162" s="22" t="s">
+      <c r="J163" t="s">
         <v>673</v>
       </c>
-      <c r="J162" t="s">
-        <v>674</v>
-      </c>
-      <c r="K162" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="33">
-        <f t="shared" ref="B163:B192" si="0">ROUNDUP(I163/G163,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C163" s="32" t="s">
-        <v>734</v>
-      </c>
-      <c r="E163" t="s">
-        <v>787</v>
-      </c>
-      <c r="G163">
-        <v>25</v>
-      </c>
-      <c r="H163" s="22">
-        <v>7.45</v>
-      </c>
-      <c r="I163" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C163,B$1:B$161)</f>
-        <v>14</v>
-      </c>
-      <c r="J163" s="33">
-        <f t="shared" ref="J163:J168" si="1">G163*B163-I163</f>
-        <v>11</v>
-      </c>
-      <c r="K163" s="34">
-        <f>B163*H163</f>
-        <v>7.45</v>
+      <c r="K163" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="164" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="33">
+        <f t="shared" ref="B164:B192" si="0">ROUNDUP(I164/G164,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C164" s="32" t="s">
+        <v>732</v>
+      </c>
+      <c r="E164" t="s">
+        <v>784</v>
+      </c>
+      <c r="G164">
+        <v>25</v>
+      </c>
+      <c r="H164" s="22">
+        <v>7.45</v>
+      </c>
+      <c r="I164" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C164,B$1:B$162)</f>
+        <v>14</v>
+      </c>
+      <c r="J164" s="33">
+        <f t="shared" ref="J164:J169" si="1">G164*B164-I164</f>
+        <v>11</v>
+      </c>
+      <c r="K164" s="34">
+        <f>B164*H164</f>
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C164" s="32" t="s">
-        <v>728</v>
-      </c>
-      <c r="E164" s="9" t="s">
-        <v>671</v>
-      </c>
-      <c r="G164">
+      <c r="C165" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="E165" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="G165">
         <v>100</v>
       </c>
-      <c r="H164" s="22">
+      <c r="H165" s="22">
         <v>2.63</v>
       </c>
-      <c r="I164" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C164,B$1:B$161)</f>
+      <c r="I165" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C165,B$1:B$162)</f>
         <v>11</v>
       </c>
-      <c r="J164" s="33">
+      <c r="J165" s="33">
         <f t="shared" si="1"/>
         <v>89</v>
-      </c>
-      <c r="K164" s="34">
-        <f>B164*H164</f>
-        <v>2.63</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="33">
-        <f t="shared" ref="B165" si="2">ROUNDUP(I165/G165,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C165" s="32" t="s">
-        <v>729</v>
-      </c>
-      <c r="E165" s="9" t="s">
-        <v>671</v>
-      </c>
-      <c r="G165">
-        <v>100</v>
-      </c>
-      <c r="H165" s="22">
-        <v>2.63</v>
-      </c>
-      <c r="I165" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C165,B$1:B$161)</f>
-        <v>16</v>
-      </c>
-      <c r="J165" s="33">
-        <f t="shared" si="1"/>
-        <v>84</v>
       </c>
       <c r="K165" s="34">
         <f>B165*H165</f>
@@ -14383,74 +14418,74 @@
     </row>
     <row r="166" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B166" si="2">ROUNDUP(I166/G166,0)</f>
         <v>1</v>
       </c>
       <c r="C166" s="32" t="s">
-        <v>616</v>
+        <v>727</v>
       </c>
       <c r="E166" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G166">
         <v>100</v>
       </c>
       <c r="H166" s="22">
-        <v>1.79</v>
+        <v>2.63</v>
       </c>
       <c r="I166" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C166,B$1:B$161)</f>
-        <v>26</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C166,B$1:B$162)</f>
+        <v>16</v>
       </c>
       <c r="J166" s="33">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="K166" s="34">
         <f>B166*H166</f>
-        <v>1.79</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="33">
-        <f t="shared" ref="B167" si="3">ROUNDUP(I167/G167,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C167" s="32" t="s">
-        <v>707</v>
+        <v>616</v>
       </c>
       <c r="E167" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G167">
         <v>100</v>
       </c>
       <c r="H167" s="22">
-        <v>1.71</v>
+        <v>1.79</v>
       </c>
       <c r="I167" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C167,B$1:B$161)</f>
-        <v>17</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C167,B$1:B$162)</f>
+        <v>26</v>
       </c>
       <c r="J167" s="33">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K167" s="34">
-        <f t="shared" ref="K167" si="4">B167*H167</f>
-        <v>1.71</v>
+        <f>B167*H167</f>
+        <v>1.79</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="33">
-        <f t="shared" ref="B168" si="5">ROUNDUP(I168/G168,0)</f>
+        <f t="shared" ref="B168" si="3">ROUNDUP(I168/G168,0)</f>
         <v>1</v>
       </c>
       <c r="C168" s="32" t="s">
-        <v>822</v>
+        <v>705</v>
       </c>
       <c r="E168" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G168">
         <v>100</v>
@@ -14459,222 +14494,223 @@
         <v>1.71</v>
       </c>
       <c r="I168" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C168,B$1:B$161)</f>
-        <v>2</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C168,B$1:B$162)</f>
+        <v>17</v>
       </c>
       <c r="J168" s="33">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K168" s="34">
-        <f t="shared" ref="K168:K230" si="6">B168*H168</f>
+        <f t="shared" ref="K168" si="4">B168*H168</f>
         <v>1.71</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B169" si="5">ROUNDUP(I169/G169,0)</f>
         <v>1</v>
       </c>
       <c r="C169" s="32" t="s">
-        <v>649</v>
-      </c>
-      <c r="E169" t="s">
-        <v>705</v>
+        <v>817</v>
+      </c>
+      <c r="E169" s="9" t="s">
+        <v>670</v>
       </c>
       <c r="G169">
         <v>100</v>
       </c>
       <c r="H169" s="22">
+        <v>1.71</v>
+      </c>
+      <c r="I169" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C169,B$1:B$162)</f>
+        <v>2</v>
+      </c>
+      <c r="J169" s="33">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="K169" s="34">
+        <f t="shared" ref="K169:K230" si="6">B169*H169</f>
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C170" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="E170" t="s">
+        <v>703</v>
+      </c>
+      <c r="G170">
+        <v>100</v>
+      </c>
+      <c r="H170" s="22">
         <v>1.79</v>
       </c>
-      <c r="I169" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C169,B$1:B$161)</f>
+      <c r="I170" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C170,B$1:B$162)</f>
         <v>2</v>
       </c>
-      <c r="J169" s="33">
-        <f t="shared" ref="J169" si="7">G169*B169-I169</f>
+      <c r="J170" s="33">
+        <f t="shared" ref="J170" si="7">G170*B170-I170</f>
         <v>98</v>
       </c>
-      <c r="K169" s="34">
+      <c r="K170" s="34">
         <f t="shared" si="6"/>
         <v>1.79</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="33">
-        <f t="shared" ref="B170:B173" si="8">ROUNDUP(I170/G170,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C170" s="32" t="s">
-        <v>704</v>
-      </c>
-      <c r="E170" t="s">
-        <v>705</v>
-      </c>
-      <c r="G170">
+    <row r="171" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="33">
+        <f t="shared" ref="B171:B174" si="8">ROUNDUP(I171/G171,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C171" s="32" t="s">
+        <v>702</v>
+      </c>
+      <c r="E171" t="s">
+        <v>703</v>
+      </c>
+      <c r="G171">
         <v>100</v>
       </c>
-      <c r="H170" s="22">
+      <c r="H171" s="22">
         <v>1.63</v>
       </c>
-      <c r="I170" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C170,B$1:B$161)</f>
+      <c r="I171" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C171,B$1:B$162)</f>
         <v>4</v>
       </c>
-      <c r="J170" s="33">
-        <f t="shared" ref="J170:J173" si="9">G170*B170-I170</f>
+      <c r="J171" s="33">
+        <f t="shared" ref="J171:J174" si="9">G171*B171-I171</f>
         <v>96</v>
       </c>
-      <c r="K170" s="34">
+      <c r="K171" s="34">
         <f t="shared" si="6"/>
         <v>1.63</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="33">
-        <f>ROUNDUP(I171/G171,0)</f>
+    <row r="172" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="33">
+        <f>ROUNDUP(I172/G172,0)</f>
         <v>2</v>
       </c>
-      <c r="C171" s="32" t="s">
+      <c r="C172" s="32" t="s">
         <v>655</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E172" t="s">
         <v>658</v>
       </c>
-      <c r="G171">
+      <c r="G172">
         <v>10</v>
       </c>
-      <c r="H171" s="22">
+      <c r="H172" s="22">
         <v>0.99</v>
       </c>
-      <c r="I171" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C171,B$1:B$161)</f>
+      <c r="I172" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C172,B$1:B$162)</f>
         <v>16</v>
       </c>
-      <c r="J171" s="33">
-        <f>G171*B171-I171</f>
+      <c r="J172" s="33">
+        <f>G172*B172-I172</f>
         <v>4</v>
       </c>
-      <c r="K171" s="34">
-        <f>B171*H171</f>
+      <c r="K172" s="34">
+        <f>B172*H172</f>
         <v>1.98</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="33"/>
-      <c r="C172" s="32"/>
-      <c r="E172"/>
-      <c r="H172" s="22"/>
-      <c r="I172" s="18"/>
-      <c r="J172" s="33"/>
-      <c r="K172" s="34"/>
-    </row>
     <row r="173" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="33">
+      <c r="B173" s="33"/>
+      <c r="C173" s="32"/>
+      <c r="E173"/>
+      <c r="H173" s="22"/>
+      <c r="I173" s="18"/>
+      <c r="J173" s="33"/>
+      <c r="K173" s="34"/>
+    </row>
+    <row r="174" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="33">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="C173" s="32" t="s">
-        <v>716</v>
-      </c>
-      <c r="E173" t="s">
-        <v>715</v>
-      </c>
-      <c r="G173">
+      <c r="C174" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="E174" t="s">
+        <v>713</v>
+      </c>
+      <c r="G174">
         <v>10</v>
       </c>
-      <c r="H173" s="22">
+      <c r="H174" s="22">
         <v>2.35</v>
       </c>
-      <c r="I173" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C173,B$1:B$161)</f>
+      <c r="I174" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C174,B$1:B$162)</f>
         <v>0</v>
       </c>
-      <c r="J173" s="33">
+      <c r="J174" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K173" s="34">
+      <c r="K174" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="33">
-        <f t="shared" ref="B174" si="10">ROUNDUP(I174/G174,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C174" s="32" t="s">
-        <v>724</v>
-      </c>
-      <c r="E174" t="s">
-        <v>725</v>
-      </c>
-      <c r="F174" t="s">
-        <v>727</v>
-      </c>
-      <c r="G174">
-        <v>50</v>
-      </c>
-      <c r="H174" s="22">
-        <v>3.65</v>
-      </c>
-      <c r="I174" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C174,B$1:B$161)</f>
-        <v>22</v>
-      </c>
-      <c r="J174" s="33">
-        <f t="shared" ref="J174" si="11">G174*B174-I174</f>
-        <v>28</v>
-      </c>
-      <c r="K174" s="34">
-        <f t="shared" ref="K174" si="12">B174*H174</f>
-        <v>3.65</v>
-      </c>
-    </row>
     <row r="175" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B175" s="33">
-        <f t="shared" ref="B175" si="13">ROUNDUP(I175/G175,0)</f>
+        <f t="shared" ref="B175" si="10">ROUNDUP(I175/G175,0)</f>
         <v>1</v>
       </c>
       <c r="C175" s="32" t="s">
-        <v>754</v>
+        <v>722</v>
       </c>
       <c r="E175" t="s">
-        <v>755</v>
+        <v>723</v>
       </c>
       <c r="F175" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G175">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H175" s="22">
-        <v>2.41</v>
+        <v>3.65</v>
       </c>
       <c r="I175" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C175,B$1:B$161)</f>
-        <v>4</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C175,B$1:B$162)</f>
+        <v>22</v>
       </c>
       <c r="J175" s="33">
-        <f t="shared" ref="J175" si="14">G175*B175-I175</f>
-        <v>6</v>
+        <f t="shared" ref="J175" si="11">G175*B175-I175</f>
+        <v>28</v>
       </c>
       <c r="K175" s="34">
-        <f t="shared" ref="K175" si="15">B175*H175</f>
-        <v>2.41</v>
+        <f t="shared" ref="K175" si="12">B175*H175</f>
+        <v>3.65</v>
       </c>
     </row>
     <row r="176" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="33">
-        <v>4</v>
-      </c>
-      <c r="C176" t="s">
-        <v>814</v>
+        <f t="shared" ref="B176" si="13">ROUNDUP(I176/G176,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C176" s="32" t="s">
+        <v>752</v>
       </c>
       <c r="E176" t="s">
-        <v>714</v>
+        <v>753</v>
+      </c>
+      <c r="F176" t="s">
+        <v>725</v>
       </c>
       <c r="G176">
         <v>10</v>
@@ -14683,58 +14719,57 @@
         <v>2.41</v>
       </c>
       <c r="I176" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C176,B$1:B$161)</f>
-        <v>0</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C176,B$1:B$162)</f>
+        <v>4</v>
       </c>
       <c r="J176" s="33">
-        <f t="shared" ref="J176" si="16">G176*B176-I176</f>
-        <v>40</v>
+        <f t="shared" ref="J176" si="14">G176*B176-I176</f>
+        <v>6</v>
       </c>
       <c r="K176" s="34">
-        <f t="shared" ref="K176" si="17">B176*H176</f>
-        <v>9.64</v>
+        <f t="shared" ref="K176" si="15">B176*H176</f>
+        <v>2.41</v>
       </c>
     </row>
     <row r="177" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C177" s="32" t="s">
-        <v>718</v>
+        <v>4</v>
+      </c>
+      <c r="C177" t="s">
+        <v>810</v>
       </c>
       <c r="E177" t="s">
-        <v>606</v>
+        <v>712</v>
       </c>
       <c r="G177">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H177" s="22">
-        <v>2.09</v>
+        <v>2.41</v>
       </c>
       <c r="I177" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C177,B$1:B$161)</f>
-        <v>16</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C177,B$1:B$162)</f>
+        <v>0</v>
       </c>
       <c r="J177" s="33">
-        <f t="shared" ref="J177:J226" si="18">G177*B177-I177</f>
-        <v>84</v>
+        <f t="shared" ref="J177" si="16">G177*B177-I177</f>
+        <v>40</v>
       </c>
       <c r="K177" s="34">
-        <f t="shared" si="6"/>
-        <v>2.09</v>
+        <f t="shared" ref="K177" si="17">B177*H177</f>
+        <v>9.64</v>
       </c>
     </row>
     <row r="178" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="33">
-        <f t="shared" ref="B178" si="19">ROUNDUP(I178/G178,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C178" s="32" t="s">
-        <v>717</v>
-      </c>
-      <c r="E178" s="29" t="s">
-        <v>618</v>
+        <v>716</v>
+      </c>
+      <c r="E178" t="s">
+        <v>606</v>
       </c>
       <c r="G178">
         <v>100</v>
@@ -14743,12 +14778,12 @@
         <v>2.09</v>
       </c>
       <c r="I178" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C178,B$1:B$161)</f>
-        <v>24</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C178,B$1:B$162)</f>
+        <v>16</v>
       </c>
       <c r="J178" s="33">
-        <f t="shared" ref="J178" si="20">G178*B178-I178</f>
-        <v>76</v>
+        <f t="shared" ref="J178:J226" si="18">G178*B178-I178</f>
+        <v>84</v>
       </c>
       <c r="K178" s="34">
         <f t="shared" si="6"/>
@@ -14757,11 +14792,14 @@
     </row>
     <row r="179" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="33">
-        <f t="shared" ref="B179:B181" si="21">ROUNDUP(I179/G179,0)</f>
+        <f t="shared" ref="B179" si="19">ROUNDUP(I179/G179,0)</f>
         <v>1</v>
       </c>
       <c r="C179" s="32" t="s">
-        <v>719</v>
+        <v>715</v>
+      </c>
+      <c r="E179" s="29" t="s">
+        <v>618</v>
       </c>
       <c r="G179">
         <v>100</v>
@@ -14770,114 +14808,111 @@
         <v>2.09</v>
       </c>
       <c r="I179" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C179,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C179,B$1:B$162)</f>
+        <v>24</v>
+      </c>
+      <c r="J179" s="33">
+        <f t="shared" ref="J179" si="20">G179*B179-I179</f>
+        <v>76</v>
+      </c>
+      <c r="K179" s="34">
+        <f t="shared" si="6"/>
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="180" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="33">
+        <f t="shared" ref="B180:B182" si="21">ROUNDUP(I180/G180,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C180" s="32" t="s">
+        <v>717</v>
+      </c>
+      <c r="G180">
+        <v>100</v>
+      </c>
+      <c r="H180" s="22">
+        <v>2.09</v>
+      </c>
+      <c r="I180" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C180,B$1:B$162)</f>
         <v>16</v>
       </c>
-      <c r="J179" s="33">
-        <f t="shared" ref="J179:J181" si="22">G179*B179-I179</f>
+      <c r="J180" s="33">
+        <f t="shared" ref="J180:J182" si="22">G180*B180-I180</f>
         <v>84</v>
       </c>
-      <c r="K179" s="34">
-        <f t="shared" ref="K179:K181" si="23">B179*H179</f>
+      <c r="K180" s="34">
+        <f t="shared" ref="K180:K182" si="23">B180*H180</f>
         <v>2.09</v>
       </c>
     </row>
-    <row r="180" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="33"/>
-      <c r="C180" s="32"/>
-      <c r="H180" s="22"/>
-      <c r="I180" s="18"/>
-      <c r="J180" s="33"/>
-      <c r="K180" s="34"/>
-    </row>
     <row r="181" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="33">
+      <c r="B181" s="33"/>
+      <c r="C181" s="32"/>
+      <c r="H181" s="22"/>
+      <c r="I181" s="18"/>
+      <c r="J181" s="33"/>
+      <c r="K181" s="34"/>
+    </row>
+    <row r="182" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="33">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="C181" s="32" t="s">
-        <v>750</v>
-      </c>
-      <c r="E181" s="29" t="s">
+      <c r="C182" s="32" t="s">
+        <v>748</v>
+      </c>
+      <c r="E182" s="29" t="s">
         <v>626</v>
       </c>
-      <c r="G181">
+      <c r="G182">
         <v>50</v>
       </c>
-      <c r="H181" s="22">
+      <c r="H182" s="22">
         <v>4.8899999999999997</v>
       </c>
-      <c r="I181" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C181,B$1:B$161)</f>
-        <v>1</v>
-      </c>
-      <c r="J181" s="33">
+      <c r="I182" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C182,B$1:B$162)</f>
+        <v>1</v>
+      </c>
+      <c r="J182" s="33">
         <f t="shared" si="22"/>
         <v>49</v>
       </c>
-      <c r="K181" s="34">
+      <c r="K182" s="34">
         <f t="shared" si="23"/>
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="182" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B182" s="33">
-        <f t="shared" ref="B182" si="24">ROUNDUP(I182/G182,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C182" s="32" t="s">
-        <v>748</v>
-      </c>
-      <c r="E182" s="29" t="s">
-        <v>749</v>
-      </c>
-      <c r="G182">
-        <v>20</v>
-      </c>
-      <c r="H182" s="22">
-        <v>3.89</v>
-      </c>
-      <c r="I182" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C182,B$1:B$161)</f>
-        <v>2</v>
-      </c>
-      <c r="J182" s="33">
-        <f t="shared" ref="J182" si="25">G182*B182-I182</f>
-        <v>18</v>
-      </c>
-      <c r="K182" s="34">
-        <f t="shared" ref="K182" si="26">B182*H182</f>
-        <v>3.89</v>
-      </c>
-    </row>
     <row r="183" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B183" si="24">ROUNDUP(I183/G183,0)</f>
         <v>1</v>
       </c>
       <c r="C183" s="32" t="s">
-        <v>783</v>
+        <v>746</v>
       </c>
       <c r="E183" s="29" t="s">
-        <v>651</v>
+        <v>747</v>
       </c>
       <c r="G183">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H183" s="22">
-        <v>1.79</v>
+        <v>3.89</v>
       </c>
       <c r="I183" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C183,B$1:B$161)</f>
-        <v>71</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C183,B$1:B$162)</f>
+        <v>2</v>
       </c>
       <c r="J183" s="33">
-        <f t="shared" si="18"/>
-        <v>29</v>
+        <f t="shared" ref="J183" si="25">G183*B183-I183</f>
+        <v>18</v>
       </c>
       <c r="K183" s="34">
-        <f t="shared" si="6"/>
-        <v>1.79</v>
+        <f t="shared" ref="K183" si="26">B183*H183</f>
+        <v>3.89</v>
       </c>
     </row>
     <row r="184" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14886,10 +14921,10 @@
         <v>1</v>
       </c>
       <c r="C184" s="32" t="s">
-        <v>663</v>
-      </c>
-      <c r="E184" s="9" t="s">
-        <v>664</v>
+        <v>781</v>
+      </c>
+      <c r="E184" s="29" t="s">
+        <v>651</v>
       </c>
       <c r="G184">
         <v>100</v>
@@ -14898,12 +14933,12 @@
         <v>1.79</v>
       </c>
       <c r="I184" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C184,B$1:B$161)</f>
-        <v>6</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C184,B$1:B$162)</f>
+        <v>71</v>
       </c>
       <c r="J184" s="33">
-        <f>G184*B184-I184</f>
-        <v>94</v>
+        <f t="shared" si="18"/>
+        <v>29</v>
       </c>
       <c r="K184" s="34">
         <f t="shared" si="6"/>
@@ -14912,92 +14947,92 @@
     </row>
     <row r="185" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="33">
-        <f t="shared" ref="B185:B186" si="27">ROUNDUP(I185/G185,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C185" s="32" t="s">
-        <v>751</v>
+        <v>663</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>778</v>
+        <v>664</v>
       </c>
       <c r="G185">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H185" s="22">
-        <v>4.33</v>
+        <v>1.79</v>
       </c>
       <c r="I185" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C185,B$1:B$161)</f>
-        <v>4</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C185,B$1:B$162)</f>
+        <v>6</v>
       </c>
       <c r="J185" s="33">
         <f>G185*B185-I185</f>
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="K185" s="34">
-        <f t="shared" ref="K185:K186" si="28">B185*H185</f>
-        <v>4.33</v>
+        <f t="shared" si="6"/>
+        <v>1.79</v>
       </c>
     </row>
     <row r="186" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B186" s="33">
+        <f t="shared" ref="B186:B187" si="27">ROUNDUP(I186/G186,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C186" s="32" t="s">
+        <v>749</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="G186">
+        <v>50</v>
+      </c>
+      <c r="H186" s="22">
+        <v>4.33</v>
+      </c>
+      <c r="I186" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C186,B$1:B$162)</f>
+        <v>4</v>
+      </c>
+      <c r="J186" s="33">
+        <f>G186*B186-I186</f>
+        <v>46</v>
+      </c>
+      <c r="K186" s="34">
+        <f t="shared" ref="K186:K187" si="28">B186*H186</f>
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="187" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="33">
         <f t="shared" si="27"/>
         <v>2</v>
       </c>
-      <c r="C186" s="32" t="s">
-        <v>782</v>
-      </c>
-      <c r="E186" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="G186">
+      <c r="C187" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="G187">
         <v>10</v>
       </c>
-      <c r="H186" s="22">
+      <c r="H187" s="22">
         <v>1.98</v>
       </c>
-      <c r="I186" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C186,B$1:B$161)</f>
+      <c r="I187" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C187,B$1:B$162)</f>
         <v>16</v>
       </c>
-      <c r="J186" s="33">
-        <f>G186*B186-I186</f>
+      <c r="J187" s="33">
+        <f>G187*B187-I187</f>
         <v>4</v>
       </c>
-      <c r="K186" s="34">
+      <c r="K187" s="34">
         <f t="shared" si="28"/>
         <v>3.96</v>
-      </c>
-    </row>
-    <row r="187" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="33">
-        <f>ROUNDUP(I187/G187,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C187" t="s">
-        <v>675</v>
-      </c>
-      <c r="E187" s="26" t="s">
-        <v>646</v>
-      </c>
-      <c r="G187">
-        <v>500</v>
-      </c>
-      <c r="H187" s="22">
-        <v>4.49</v>
-      </c>
-      <c r="I187" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C187,B$1:B$161)</f>
-        <v>136</v>
-      </c>
-      <c r="J187" s="33">
-        <f t="shared" ref="J187" si="29">G187*B187-I187</f>
-        <v>364</v>
-      </c>
-      <c r="K187" s="34">
-        <f t="shared" si="6"/>
-        <v>4.49</v>
       </c>
     </row>
     <row r="188" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15006,28 +15041,28 @@
         <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>698</v>
+        <v>674</v>
       </c>
       <c r="E188" s="26" t="s">
-        <v>604</v>
+        <v>646</v>
       </c>
       <c r="G188">
         <v>500</v>
       </c>
       <c r="H188" s="22">
-        <v>2.4900000000000002</v>
+        <v>4.49</v>
       </c>
       <c r="I188" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C188,B$1:B$161)</f>
-        <v>50</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C188,B$1:B$162)</f>
+        <v>136</v>
       </c>
       <c r="J188" s="33">
-        <f t="shared" ref="J188:J189" si="30">G188*B188-I188</f>
-        <v>450</v>
+        <f t="shared" ref="J188" si="29">G188*B188-I188</f>
+        <v>364</v>
       </c>
       <c r="K188" s="34">
         <f t="shared" si="6"/>
-        <v>2.4900000000000002</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="189" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15036,28 +15071,28 @@
         <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>737</v>
+        <v>696</v>
       </c>
       <c r="E189" s="26" t="s">
-        <v>738</v>
+        <v>604</v>
       </c>
       <c r="G189">
         <v>500</v>
       </c>
       <c r="H189" s="22">
-        <v>4.49</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="I189" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C189,B$1:B$161)</f>
-        <v>182</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C189,B$1:B$162)</f>
+        <v>50</v>
       </c>
       <c r="J189" s="33">
-        <f t="shared" si="30"/>
-        <v>318</v>
+        <f t="shared" ref="J189:J190" si="30">G189*B189-I189</f>
+        <v>450</v>
       </c>
       <c r="K189" s="34">
-        <f t="shared" ref="K189" si="31">B189*H189</f>
-        <v>4.49</v>
+        <f t="shared" si="6"/>
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="190" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15065,59 +15100,59 @@
         <f>ROUNDUP(I190/G190,0)</f>
         <v>1</v>
       </c>
-      <c r="C190" s="32" t="s">
-        <v>811</v>
+      <c r="C190" t="s">
+        <v>735</v>
       </c>
       <c r="E190" s="26" t="s">
-        <v>810</v>
+        <v>736</v>
       </c>
       <c r="G190">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="H190" s="22">
-        <v>1.59</v>
+        <v>4.49</v>
       </c>
       <c r="I190" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C190,B$1:B$161)</f>
-        <v>12</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C190,B$1:B$162)</f>
+        <v>182</v>
       </c>
       <c r="J190" s="33">
-        <f t="shared" ref="J190" si="32">G190*B190-I190</f>
-        <v>88</v>
+        <f t="shared" si="30"/>
+        <v>318</v>
       </c>
       <c r="K190" s="34">
-        <f t="shared" ref="K190" si="33">B190*H190</f>
-        <v>1.59</v>
+        <f t="shared" ref="K190" si="31">B190*H190</f>
+        <v>4.49</v>
       </c>
     </row>
     <row r="191" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUNDUP(I191/G191,0)</f>
+        <v>1</v>
       </c>
       <c r="C191" s="32" t="s">
-        <v>813</v>
-      </c>
-      <c r="E191" s="9" t="s">
-        <v>668</v>
+        <v>808</v>
+      </c>
+      <c r="E191" s="26" t="s">
+        <v>807</v>
       </c>
       <c r="G191">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H191" s="22">
-        <v>0.15</v>
+        <v>1.59</v>
       </c>
       <c r="I191" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C191,B$1:B$161)</f>
-        <v>0</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C191,B$1:B$162)</f>
+        <v>12</v>
       </c>
       <c r="J191" s="33">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" ref="J191" si="32">G191*B191-I191</f>
+        <v>88</v>
       </c>
       <c r="K191" s="34">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="K191" si="33">B191*H191</f>
+        <v>1.59</v>
       </c>
     </row>
     <row r="192" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15126,10 +15161,10 @@
         <v>33</v>
       </c>
       <c r="C192" s="32" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="E192" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="G192">
         <v>1</v>
@@ -15138,7 +15173,7 @@
         <v>0.3</v>
       </c>
       <c r="I192" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C192,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C192,B$1:B$162)</f>
         <v>33</v>
       </c>
       <c r="J192" s="33">
@@ -15152,32 +15187,32 @@
     </row>
     <row r="193" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="33">
-        <f t="shared" ref="B193" si="36">ROUNDUP(I193/G193,0)</f>
-        <v>0</v>
+        <f>ROUNDUP(I193/G193,0)</f>
+        <v>1</v>
       </c>
       <c r="C193" t="s">
-        <v>784</v>
-      </c>
-      <c r="E193" s="29" t="s">
-        <v>679</v>
+        <v>690</v>
+      </c>
+      <c r="E193" s="26" t="s">
+        <v>691</v>
       </c>
       <c r="G193">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H193" s="22">
-        <v>0.08</v>
+        <v>2.59</v>
       </c>
       <c r="I193" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C193,B$1:B$161)</f>
-        <v>0</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C193,B$1:B$162)</f>
+        <v>2</v>
       </c>
       <c r="J193" s="33">
-        <f t="shared" ref="J193" si="37">G193*B193-I193</f>
-        <v>0</v>
+        <f t="shared" ref="J193" si="36">G193*B193-I193</f>
+        <v>8</v>
       </c>
       <c r="K193" s="34">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>B193*H193</f>
+        <v>2.59</v>
       </c>
     </row>
     <row r="194" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15185,78 +15220,78 @@
         <f>ROUNDUP(I194/G194,0)</f>
         <v>1</v>
       </c>
-      <c r="C194" t="s">
-        <v>692</v>
-      </c>
-      <c r="E194" s="26" t="s">
-        <v>693</v>
+      <c r="C194" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="E194" t="s">
+        <v>805</v>
       </c>
       <c r="G194">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="H194" s="22">
-        <v>2.59</v>
+        <v>1.69</v>
       </c>
       <c r="I194" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C194,B$1:B$161)</f>
-        <v>2</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C194,B$1:B$162)</f>
+        <v>300</v>
       </c>
       <c r="J194" s="33">
-        <f t="shared" ref="J194" si="38">G194*B194-I194</f>
-        <v>8</v>
+        <f t="shared" ref="J194" si="37">G194*B194-I194</f>
+        <v>200</v>
       </c>
       <c r="K194" s="34">
         <f>B194*H194</f>
-        <v>2.59</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="195" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="33">
-        <f>ROUNDUP(I195/G195,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C195" s="32" t="s">
-        <v>809</v>
-      </c>
-      <c r="E195" t="s">
-        <v>808</v>
-      </c>
-      <c r="G195">
-        <v>500</v>
-      </c>
-      <c r="H195" s="22">
-        <v>1.69</v>
-      </c>
-      <c r="I195" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C195,B$1:B$161)</f>
-        <v>300</v>
-      </c>
-      <c r="J195" s="33">
-        <f t="shared" ref="J195" si="39">G195*B195-I195</f>
-        <v>200</v>
-      </c>
-      <c r="K195" s="34">
-        <f>B195*H195</f>
-        <v>1.69</v>
-      </c>
+      <c r="B195" s="33"/>
+      <c r="H195" s="22"/>
+      <c r="I195" s="18"/>
+      <c r="J195" s="33"/>
+      <c r="K195" s="34"/>
     </row>
     <row r="196" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="33"/>
-      <c r="H196" s="22"/>
-      <c r="I196" s="18"/>
-      <c r="J196" s="33"/>
-      <c r="K196" s="34"/>
+      <c r="B196" s="33">
+        <f t="shared" ref="B196:B201" si="38">ROUNDUP(I196/G196,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C196" t="s">
+        <v>632</v>
+      </c>
+      <c r="E196" s="29" t="s">
+        <v>637</v>
+      </c>
+      <c r="G196">
+        <v>1</v>
+      </c>
+      <c r="H196" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I196" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C196,B$1:B$162)</f>
+        <v>4</v>
+      </c>
+      <c r="J196" s="33">
+        <f t="shared" ref="J196" si="39">G196*B196-I196</f>
+        <v>0</v>
+      </c>
+      <c r="K196" s="34">
+        <f t="shared" si="6"/>
+        <v>20.399999999999999</v>
+      </c>
     </row>
     <row r="197" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="33">
-        <f t="shared" ref="B197:B202" si="40">ROUNDUP(I197/G197,0)</f>
-        <v>4</v>
+        <f t="shared" ref="B197" si="40">ROUNDUP(I197/G197,0)</f>
+        <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>632</v>
+        <v>824</v>
       </c>
       <c r="E197" s="29" t="s">
-        <v>637</v>
+        <v>825</v>
       </c>
       <c r="G197">
         <v>1</v>
@@ -15265,101 +15300,101 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I197" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C197,B$1:B$161)</f>
-        <v>4</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C197,B$1:B$162)</f>
+        <v>1</v>
       </c>
       <c r="J197" s="33">
         <f t="shared" ref="J197" si="41">G197*B197-I197</f>
         <v>0</v>
       </c>
       <c r="K197" s="34">
-        <f t="shared" si="6"/>
-        <v>20.399999999999999</v>
+        <f t="shared" ref="K197" si="42">B197*H197</f>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="198" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B198" s="33">
-        <f t="shared" ref="B198" si="42">ROUNDUP(I198/G198,0)</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>829</v>
+        <v>639</v>
       </c>
       <c r="E198" s="29" t="s">
-        <v>830</v>
+        <v>638</v>
       </c>
       <c r="G198">
         <v>1</v>
       </c>
       <c r="H198" s="22">
-        <v>5.0999999999999996</v>
+        <v>5.44</v>
       </c>
       <c r="I198" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C198,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C198,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J198" s="33">
-        <f t="shared" ref="J198" si="43">G198*B198-I198</f>
+        <f t="shared" ref="J198:J200" si="43">G198*B198-I198</f>
         <v>0</v>
       </c>
       <c r="K198" s="34">
-        <f t="shared" ref="K198" si="44">B198*H198</f>
-        <v>5.0999999999999996</v>
+        <f t="shared" si="6"/>
+        <v>5.44</v>
       </c>
     </row>
     <row r="199" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B199" s="33">
-        <f t="shared" si="40"/>
-        <v>1</v>
+        <f t="shared" si="38"/>
+        <v>0</v>
       </c>
       <c r="C199" t="s">
-        <v>639</v>
+        <v>675</v>
       </c>
       <c r="E199" s="29" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="G199">
         <v>1</v>
       </c>
       <c r="H199" s="22">
-        <v>5.44</v>
+        <v>4.46</v>
       </c>
       <c r="I199" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C199,B$1:B$161)</f>
-        <v>1</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C199,B$1:B$162)</f>
+        <v>0</v>
       </c>
       <c r="J199" s="33">
-        <f t="shared" ref="J199:J201" si="45">G199*B199-I199</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="K199" s="34">
         <f t="shared" si="6"/>
-        <v>5.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B200" s="33">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="C200" t="s">
         <v>676</v>
       </c>
       <c r="E200" s="29" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G200">
         <v>1</v>
       </c>
       <c r="H200" s="22">
-        <v>4.46</v>
+        <v>5.01</v>
       </c>
       <c r="I200" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C200,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C200,B$1:B$162)</f>
         <v>0</v>
       </c>
       <c r="J200" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="K200" s="34">
@@ -15369,62 +15404,62 @@
     </row>
     <row r="201" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="33">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>711</v>
+      </c>
+      <c r="E201" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="G201">
+        <v>1</v>
+      </c>
+      <c r="H201" s="22">
+        <v>6.34</v>
+      </c>
+      <c r="I201" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C201,B$1:B$162)</f>
+        <v>1</v>
+      </c>
+      <c r="J201" s="33">
+        <f t="shared" ref="J201" si="44">G201*B201-I201</f>
         <v>0</v>
       </c>
-      <c r="C201" t="s">
-        <v>677</v>
-      </c>
-      <c r="E201" s="29" t="s">
-        <v>640</v>
-      </c>
-      <c r="G201">
-        <v>1</v>
-      </c>
-      <c r="H201" s="22">
-        <v>5.01</v>
-      </c>
-      <c r="I201" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C201,B$1:B$161)</f>
-        <v>0</v>
-      </c>
-      <c r="J201" s="33">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
       <c r="K201" s="34">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="K201" si="45">B201*H201</f>
+        <v>6.34</v>
       </c>
     </row>
     <row r="202" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="33">
-        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>713</v>
-      </c>
+        <v>739</v>
+      </c>
+      <c r="D202" s="32"/>
       <c r="E202" s="26" t="s">
-        <v>712</v>
+        <v>738</v>
       </c>
       <c r="G202">
         <v>1</v>
       </c>
       <c r="H202" s="22">
-        <v>6.34</v>
+        <v>11.6</v>
       </c>
       <c r="I202" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C202,B$1:B$161)</f>
-        <v>1</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C202,B$1:B$162)</f>
+        <v>2</v>
       </c>
       <c r="J202" s="33">
-        <f t="shared" ref="J202" si="46">G202*B202-I202</f>
-        <v>0</v>
+        <f t="shared" ref="J202:J203" si="46">G202*B202-I202</f>
+        <v>-1</v>
       </c>
       <c r="K202" s="34">
-        <f t="shared" ref="K202" si="47">B202*H202</f>
-        <v>6.34</v>
+        <f t="shared" ref="K202:K203" si="47">B202*H202</f>
+        <v>11.6</v>
       </c>
     </row>
     <row r="203" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15432,29 +15467,29 @@
         <v>1</v>
       </c>
       <c r="C203" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="D203" s="32"/>
-      <c r="E203" s="26" t="s">
-        <v>740</v>
+      <c r="E203" s="29" t="s">
+        <v>760</v>
       </c>
       <c r="G203">
         <v>1</v>
       </c>
       <c r="H203" s="22">
-        <v>11.6</v>
+        <v>5.66</v>
       </c>
       <c r="I203" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C203,B$1:B$161)</f>
-        <v>2</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C203,B$1:B$162)</f>
+        <v>4</v>
       </c>
       <c r="J203" s="33">
-        <f t="shared" ref="J203:J204" si="48">G203*B203-I203</f>
-        <v>-1</v>
+        <f t="shared" si="46"/>
+        <v>-3</v>
       </c>
       <c r="K203" s="34">
-        <f t="shared" ref="K203:K204" si="49">B203*H203</f>
-        <v>11.6</v>
+        <f t="shared" si="47"/>
+        <v>5.66</v>
       </c>
     </row>
     <row r="204" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15462,200 +15497,200 @@
         <v>1</v>
       </c>
       <c r="C204" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="D204" s="32"/>
       <c r="E204" s="29" t="s">
-        <v>762</v>
+        <v>740</v>
       </c>
       <c r="G204">
         <v>1</v>
       </c>
       <c r="H204" s="22">
-        <v>5.66</v>
+        <v>5.23</v>
       </c>
       <c r="I204" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C204,B$1:B$161)</f>
-        <v>4</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C204,B$1:B$162)</f>
+        <v>0</v>
       </c>
       <c r="J204" s="33">
-        <f t="shared" si="48"/>
-        <v>-3</v>
+        <f t="shared" ref="J204" si="48">G204*B204-I204</f>
+        <v>1</v>
       </c>
       <c r="K204" s="34">
-        <f t="shared" si="49"/>
-        <v>5.66</v>
+        <f t="shared" ref="K204" si="49">B204*H204</f>
+        <v>5.23</v>
       </c>
     </row>
     <row r="205" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="33">
         <v>1</v>
       </c>
-      <c r="C205" t="s">
-        <v>743</v>
+      <c r="C205" s="32" t="s">
+        <v>764</v>
       </c>
       <c r="D205" s="32"/>
       <c r="E205" s="29" t="s">
-        <v>742</v>
+        <v>654</v>
       </c>
       <c r="G205">
         <v>1</v>
       </c>
       <c r="H205" s="22">
-        <v>5.23</v>
+        <v>4.96</v>
       </c>
       <c r="I205" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C205,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C205,B$1:B$162)</f>
+        <v>1</v>
+      </c>
+      <c r="J205" s="33">
+        <f>G205*B205-I205</f>
         <v>0</v>
       </c>
-      <c r="J205" s="33">
-        <f t="shared" ref="J205" si="50">G205*B205-I205</f>
-        <v>1</v>
-      </c>
       <c r="K205" s="34">
-        <f t="shared" ref="K205" si="51">B205*H205</f>
-        <v>5.23</v>
+        <f>B205*H205</f>
+        <v>4.96</v>
       </c>
     </row>
     <row r="206" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="33">
         <v>1</v>
       </c>
-      <c r="C206" s="32" t="s">
-        <v>766</v>
+      <c r="C206" t="s">
+        <v>765</v>
       </c>
       <c r="D206" s="32"/>
       <c r="E206" s="29" t="s">
-        <v>654</v>
+        <v>677</v>
       </c>
       <c r="G206">
         <v>1</v>
       </c>
       <c r="H206" s="22">
-        <v>4.96</v>
+        <v>4.24</v>
       </c>
       <c r="I206" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C206,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C206,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J206" s="33">
-        <f>G206*B206-I206</f>
+        <f t="shared" ref="J206" si="50">G206*B206-I206</f>
         <v>0</v>
       </c>
       <c r="K206" s="34">
         <f>B206*H206</f>
-        <v>4.96</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="207" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B207" s="33">
-        <v>1</v>
+        <f>ROUNDUP(I207/G207,0)</f>
+        <v>2</v>
       </c>
       <c r="C207" t="s">
-        <v>767</v>
-      </c>
-      <c r="D207" s="32"/>
-      <c r="E207" s="29" t="s">
-        <v>678</v>
+        <v>768</v>
+      </c>
+      <c r="E207" s="26" t="s">
+        <v>698</v>
       </c>
       <c r="G207">
         <v>1</v>
       </c>
       <c r="H207" s="22">
-        <v>4.24</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="I207" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C207,B$1:B$161)</f>
-        <v>1</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C207,B$1:B$162)</f>
+        <v>2</v>
       </c>
       <c r="J207" s="33">
-        <f t="shared" ref="J207" si="52">G207*B207-I207</f>
+        <f t="shared" ref="J207" si="51">G207*B207-I207</f>
         <v>0</v>
       </c>
       <c r="K207" s="34">
         <f>B207*H207</f>
-        <v>4.24</v>
+        <v>8.8800000000000008</v>
       </c>
     </row>
     <row r="208" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B208" s="33">
-        <f>ROUNDUP(I208/G208,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C208" t="s">
+        <v>766</v>
+      </c>
+      <c r="D208" s="32"/>
+      <c r="E208" s="29" t="s">
+        <v>757</v>
+      </c>
+      <c r="G208">
+        <v>1</v>
+      </c>
+      <c r="H208" s="22">
+        <v>7.44</v>
+      </c>
+      <c r="I208" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C208,B$1:B$162)</f>
         <v>2</v>
       </c>
-      <c r="C208" t="s">
-        <v>770</v>
-      </c>
-      <c r="E208" s="26" t="s">
-        <v>700</v>
-      </c>
-      <c r="G208">
-        <v>1</v>
-      </c>
-      <c r="H208" s="22">
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="I208" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C208,B$1:B$161)</f>
-        <v>2</v>
-      </c>
       <c r="J208" s="33">
-        <f t="shared" ref="J208" si="53">G208*B208-I208</f>
-        <v>0</v>
+        <f t="shared" ref="J208" si="52">G208*B208-I208</f>
+        <v>-1</v>
       </c>
       <c r="K208" s="34">
-        <f>B208*H208</f>
-        <v>8.8800000000000008</v>
-      </c>
-    </row>
-    <row r="209" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K208" si="53">B208*H208</f>
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="209" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B209" s="33">
         <v>1</v>
       </c>
       <c r="C209" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D209" s="32"/>
       <c r="E209" s="29" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="G209">
         <v>1</v>
       </c>
       <c r="H209" s="22">
-        <v>7.44</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="I209" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C209,B$1:B$161)</f>
-        <v>2</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C209,B$1:B$162)</f>
+        <v>1</v>
       </c>
       <c r="J209" s="33">
         <f t="shared" ref="J209" si="54">G209*B209-I209</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K209" s="34">
         <f t="shared" ref="K209" si="55">B209*H209</f>
-        <v>7.44</v>
-      </c>
-    </row>
-    <row r="210" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="210" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B210" s="33">
         <v>1</v>
       </c>
       <c r="C210" t="s">
-        <v>769</v>
+        <v>788</v>
       </c>
       <c r="D210" s="32"/>
       <c r="E210" s="29" t="s">
-        <v>759</v>
+        <v>787</v>
       </c>
       <c r="G210">
         <v>1</v>
       </c>
       <c r="H210" s="22">
-        <v>8.8699999999999992</v>
+        <v>7.88</v>
       </c>
       <c r="I210" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C210,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C210,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J210" s="33">
@@ -15664,7 +15699,7 @@
       </c>
       <c r="K210" s="34">
         <f t="shared" ref="K210" si="57">B210*H210</f>
-        <v>8.8699999999999992</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="211" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15672,7 +15707,7 @@
         <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D211" s="32"/>
       <c r="E211" s="29" t="s">
@@ -15685,7 +15720,7 @@
         <v>7.88</v>
       </c>
       <c r="I211" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C211,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C211,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J211" s="33">
@@ -15702,29 +15737,29 @@
         <v>1</v>
       </c>
       <c r="C212" t="s">
-        <v>792</v>
+        <v>766</v>
       </c>
       <c r="D212" s="32"/>
       <c r="E212" s="29" t="s">
-        <v>793</v>
+        <v>757</v>
       </c>
       <c r="G212">
         <v>1</v>
       </c>
       <c r="H212" s="22">
-        <v>7.88</v>
+        <v>7.13</v>
       </c>
       <c r="I212" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C212,B$1:B$161)</f>
-        <v>1</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C212,B$1:B$162)</f>
+        <v>2</v>
       </c>
       <c r="J212" s="33">
         <f t="shared" ref="J212" si="60">G212*B212-I212</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K212" s="34">
         <f t="shared" ref="K212" si="61">B212*H212</f>
-        <v>7.88</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="213" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15732,11 +15767,11 @@
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>768</v>
+        <v>832</v>
       </c>
       <c r="D213" s="32"/>
       <c r="E213" s="29" t="s">
-        <v>759</v>
+        <v>831</v>
       </c>
       <c r="G213">
         <v>1</v>
@@ -15745,12 +15780,12 @@
         <v>7.13</v>
       </c>
       <c r="I213" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C213,B$1:B$161)</f>
-        <v>2</v>
+        <f>SUMIF(C$1:C$162,"="&amp;C213,B$1:B$162)</f>
+        <v>1</v>
       </c>
       <c r="J213" s="33">
         <f t="shared" ref="J213" si="62">G213*B213-I213</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K213" s="34">
         <f t="shared" ref="K213" si="63">B213*H213</f>
@@ -15770,7 +15805,7 @@
         <v>1</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="E215" s="26" t="s">
         <v>648</v>
@@ -15782,7 +15817,7 @@
         <v>14.5</v>
       </c>
       <c r="I215" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C215,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C215,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J215" s="33">
@@ -15799,10 +15834,10 @@
         <v>1</v>
       </c>
       <c r="C216" s="32" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="E216" s="26" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G216">
         <v>1</v>
@@ -15811,7 +15846,7 @@
         <v>8.5</v>
       </c>
       <c r="I216" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C216,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C216,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J216" s="33">
@@ -15828,10 +15863,10 @@
         <v>1</v>
       </c>
       <c r="C217" s="32" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="E217" s="26" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="G217">
         <v>1</v>
@@ -15840,7 +15875,7 @@
         <v>54.2</v>
       </c>
       <c r="I217" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C217,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C217,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J217" s="33">
@@ -15857,10 +15892,10 @@
         <v>1</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="E218" s="26" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="G218">
         <v>1</v>
@@ -15869,7 +15904,7 @@
         <v>37</v>
       </c>
       <c r="I218" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C218,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C218,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J218" s="33">
@@ -15886,10 +15921,10 @@
         <v>1</v>
       </c>
       <c r="C219" s="32" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="E219" s="26" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="G219">
         <v>1</v>
@@ -15898,7 +15933,7 @@
         <v>18</v>
       </c>
       <c r="I219" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C219,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C219,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J219" s="33">
@@ -15928,7 +15963,7 @@
         <v>14.53</v>
       </c>
       <c r="I220" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C220,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C220,B$1:B$162)</f>
         <v>5</v>
       </c>
       <c r="J220" s="33">
@@ -15940,7 +15975,7 @@
         <v>72.649999999999991</v>
       </c>
       <c r="L220" t="s">
-        <v>819</v>
+        <v>835</v>
       </c>
     </row>
     <row r="221" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15949,10 +15984,10 @@
         <v>1</v>
       </c>
       <c r="C221" s="32" t="s">
+        <v>769</v>
+      </c>
+      <c r="E221" s="9" t="s">
         <v>771</v>
-      </c>
-      <c r="E221" s="9" t="s">
-        <v>773</v>
       </c>
       <c r="G221">
         <v>1</v>
@@ -15961,7 +15996,7 @@
         <v>36.42</v>
       </c>
       <c r="I221" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C221,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C221,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J221" s="33">
@@ -15973,7 +16008,7 @@
         <v>36.42</v>
       </c>
       <c r="L221" t="s">
-        <v>819</v>
+        <v>835</v>
       </c>
     </row>
     <row r="222" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16004,7 +16039,7 @@
         <v>1.54</v>
       </c>
       <c r="I223" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C223,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C223,B$1:B$162)</f>
         <v>2</v>
       </c>
       <c r="J223" s="33">
@@ -16022,11 +16057,11 @@
         <v>8</v>
       </c>
       <c r="C224" s="32" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D224" s="32"/>
       <c r="E224" s="29" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="G224">
         <v>1</v>
@@ -16035,7 +16070,7 @@
         <v>1.54</v>
       </c>
       <c r="I224" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C224,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C224,B$1:B$162)</f>
         <v>8</v>
       </c>
       <c r="J224" s="33">
@@ -16053,11 +16088,11 @@
         <v>14</v>
       </c>
       <c r="C225" s="32" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D225" s="32"/>
       <c r="E225" s="29" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G225">
         <v>1</v>
@@ -16066,7 +16101,7 @@
         <v>1.54</v>
       </c>
       <c r="I225" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C225,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C225,B$1:B$162)</f>
         <v>14</v>
       </c>
       <c r="J225" s="33">
@@ -16096,7 +16131,7 @@
         <v>1.95</v>
       </c>
       <c r="I226" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C226,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C226,B$1:B$162)</f>
         <v>6</v>
       </c>
       <c r="J226" s="33">
@@ -16126,7 +16161,7 @@
         <v>1.39</v>
       </c>
       <c r="I227" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C227,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C227,B$1:B$162)</f>
         <v>2</v>
       </c>
       <c r="J227" s="33">
@@ -16156,7 +16191,7 @@
         <v>3.29</v>
       </c>
       <c r="I228" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C228,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C228,B$1:B$162)</f>
         <v>5</v>
       </c>
       <c r="J228" s="33">
@@ -16174,10 +16209,10 @@
         <v>2</v>
       </c>
       <c r="C229" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E229" s="26" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G229">
         <v>1</v>
@@ -16186,7 +16221,7 @@
         <v>1</v>
       </c>
       <c r="I229" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C229,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C229,B$1:B$162)</f>
         <v>2</v>
       </c>
       <c r="J229" s="33">
@@ -16204,10 +16239,10 @@
         <v>4</v>
       </c>
       <c r="C230" s="32" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E230" s="26" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G230">
         <v>1</v>
@@ -16216,7 +16251,7 @@
         <v>1.05</v>
       </c>
       <c r="I230" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C230,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C230,B$1:B$162)</f>
         <v>4</v>
       </c>
       <c r="J230" s="33">
@@ -16234,10 +16269,10 @@
         <v>4</v>
       </c>
       <c r="C231" s="32" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="E231" s="26" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="G231">
         <v>1</v>
@@ -16246,7 +16281,7 @@
         <v>1</v>
       </c>
       <c r="I231" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C231,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C231,B$1:B$162)</f>
         <v>4</v>
       </c>
       <c r="J231" s="33">
@@ -16267,7 +16302,7 @@
         <v>599</v>
       </c>
       <c r="E232" s="29" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="G232">
         <v>1</v>
@@ -16276,7 +16311,7 @@
         <v>26.88</v>
       </c>
       <c r="I232" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C232,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C232,B$1:B$162)</f>
         <v>2</v>
       </c>
       <c r="J232" s="33">
@@ -16294,10 +16329,10 @@
         <v>1</v>
       </c>
       <c r="C233" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="E233" s="29" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="G233">
         <v>1</v>
@@ -16306,7 +16341,7 @@
         <v>24.22</v>
       </c>
       <c r="I233" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C233,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C233,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J233" s="33">
@@ -16330,7 +16365,7 @@
     </row>
     <row r="235" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B235" s="33"/>
       <c r="E235"/>
@@ -16344,10 +16379,10 @@
         <v>1</v>
       </c>
       <c r="C236" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E236" s="29" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G236">
         <v>1</v>
@@ -16356,7 +16391,7 @@
         <v>4.09</v>
       </c>
       <c r="I236" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C236,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C236,B$1:B$162)</f>
         <v>3</v>
       </c>
       <c r="J236" s="33">
@@ -16373,10 +16408,10 @@
         <v>1</v>
       </c>
       <c r="C237" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E237" s="29" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G237">
         <v>1</v>
@@ -16385,7 +16420,7 @@
         <v>2.8</v>
       </c>
       <c r="I237" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C237,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C237,B$1:B$162)</f>
         <v>1</v>
       </c>
       <c r="J237" s="33">
@@ -16402,10 +16437,10 @@
         <v>1</v>
       </c>
       <c r="C238" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E238" s="29" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G238">
         <v>1</v>
@@ -16414,7 +16449,7 @@
         <v>2.8</v>
       </c>
       <c r="I238" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C238,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C238,B$1:B$162)</f>
         <v>2</v>
       </c>
       <c r="J238" s="33">
@@ -16431,10 +16466,10 @@
         <v>1</v>
       </c>
       <c r="C239" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E239" s="29" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G239">
         <v>1</v>
@@ -16443,7 +16478,7 @@
         <v>2.8</v>
       </c>
       <c r="I239" s="18">
-        <f>SUMIF(C$1:C$161,"="&amp;C239,B$1:B$161)</f>
+        <f>SUMIF(C$1:C$162,"="&amp;C239,B$1:B$162)</f>
         <v>3</v>
       </c>
       <c r="J239" s="33">
@@ -16456,93 +16491,124 @@
       </c>
     </row>
     <row r="240" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B240" s="33"/>
-      <c r="H240" s="22"/>
-      <c r="I240" s="18"/>
-      <c r="J240" s="33"/>
-      <c r="K240" s="34"/>
-    </row>
-    <row r="241" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B240" s="33">
+        <v>1</v>
+      </c>
+      <c r="C240" t="s">
+        <v>550</v>
+      </c>
+      <c r="E240" s="29" t="s">
+        <v>839</v>
+      </c>
+      <c r="G240">
+        <v>1</v>
+      </c>
+      <c r="H240" s="22">
+        <v>1869</v>
+      </c>
+      <c r="I240" s="18">
+        <f>SUMIF(C$1:C$162,"="&amp;C240,B$1:B$162)</f>
+        <v>0</v>
+      </c>
+      <c r="J240" s="33">
+        <f t="shared" ref="J240" si="98">G240*B240-I240</f>
+        <v>1</v>
+      </c>
+      <c r="K240" s="34">
+        <f t="shared" ref="K240" si="99">B240*H240</f>
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="241" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B241" s="33"/>
       <c r="H241" s="22"/>
       <c r="I241" s="18"/>
       <c r="J241" s="33"/>
       <c r="K241" s="34"/>
     </row>
-    <row r="242" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="33"/>
       <c r="H242" s="22"/>
       <c r="I242" s="18"/>
       <c r="J242" s="33"/>
-      <c r="K242" s="34"/>
-    </row>
-    <row r="243" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K242" s="38" t="s">
+        <v>837</v>
+      </c>
+      <c r="L242" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="243" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B243" s="33"/>
       <c r="E243" s="26"/>
       <c r="H243" s="22"/>
       <c r="I243" s="18"/>
       <c r="J243" s="33"/>
-      <c r="K243" s="35">
-        <f>SUM(K163:K239)</f>
-        <v>620.05999999999983</v>
-      </c>
-    </row>
-    <row r="244" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K243" s="37">
+        <f>SUM(K164:K241)</f>
+        <v>2496.1899999999996</v>
+      </c>
+      <c r="L243" s="35">
+        <f>SUMIF(L1:L241,"&lt;&gt;Got it",K1:K241)</f>
+        <v>2387.12</v>
+      </c>
+    </row>
+    <row r="244" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="33"/>
       <c r="E244" s="26"/>
       <c r="H244" s="22"/>
       <c r="I244" s="18"/>
       <c r="J244" s="33"/>
     </row>
-    <row r="245" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B245" s="33"/>
       <c r="E245" s="26"/>
       <c r="H245" s="22"/>
       <c r="I245" s="18"/>
       <c r="J245" s="33"/>
     </row>
-    <row r="246" spans="2:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B246" s="33"/>
       <c r="E246" s="26"/>
       <c r="H246" s="22"/>
       <c r="I246" s="18"/>
       <c r="J246" s="33"/>
     </row>
-    <row r="247" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D247" s="6"/>
       <c r="H247" s="22"/>
       <c r="I247" s="22"/>
     </row>
-    <row r="248" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E248" s="30"/>
       <c r="I248" s="22"/>
     </row>
-    <row r="250" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E250" s="26"/>
       <c r="I250" s="22"/>
     </row>
-    <row r="251" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E251" s="26"/>
       <c r="I251" s="22"/>
     </row>
-    <row r="252" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D252" s="6"/>
       <c r="E252" s="26"/>
       <c r="I252" s="22"/>
     </row>
-    <row r="253" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D253" s="8"/>
       <c r="I253" s="22"/>
     </row>
-    <row r="254" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E254" s="26"/>
       <c r="I254" s="22"/>
     </row>
-    <row r="255" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E255" s="30"/>
       <c r="I255" s="22"/>
     </row>
-    <row r="256" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E256" s="26"/>
       <c r="I256" s="22"/>
     </row>
@@ -16599,6 +16665,11 @@
       <c r="I269" s="22"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L220:L221">
+      <formula1>$M$1:$M$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="E226" r:id="rId1"/>
     <hyperlink ref="E220" r:id="rId2"/>

</xml_diff>

<commit_message>
Lagerklemme bei Handgelenk probiert
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2464,9 +2464,6 @@
     <t>http://kugellagershop-duesseldorf.de/61818-2RS-/-6818-2RS</t>
   </si>
   <si>
-    <t>https://www.kugellager-express.de/rillenkugellager-6817-61817-85x110x13-mm.html</t>
-  </si>
-  <si>
     <t>Rillenkugellager DIN 625 SKF - SKF 61818 - 85x110x13</t>
   </si>
   <si>
@@ -2549,6 +2546,9 @@
   </si>
   <si>
     <t>returned</t>
+  </si>
+  <si>
+    <t>http://kugellagershop-duesseldorf.de/epages/1e704d71-b8d3-4e48-be33-4758de826e89.sf/de_DE/?ObjectPath=/Shops/1e704d71-b8d3-4e48-be33-4758de826e89/Products/618172RS</t>
   </si>
 </sst>
 </file>
@@ -11971,8 +11971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K233" sqref="K232:K233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12003,10 +12003,10 @@
         <v>596</v>
       </c>
       <c r="L1" t="s">
+        <v>832</v>
+      </c>
+      <c r="M1" t="s">
         <v>833</v>
-      </c>
-      <c r="M1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -12014,7 +12014,7 @@
         <v>609</v>
       </c>
       <c r="M2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -12032,7 +12032,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -12049,7 +12049,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -12439,7 +12439,7 @@
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E33" s="9"/>
       <c r="H33" s="22"/>
@@ -12454,7 +12454,7 @@
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E34" s="9"/>
       <c r="H34" s="22"/>
@@ -12556,7 +12556,7 @@
         <v>Vierkant Mutter M3 Breite 5.5mm</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="22"/>
@@ -12570,7 +12570,7 @@
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
@@ -12842,7 +12842,7 @@
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E61" s="9"/>
       <c r="H61" s="22"/>
@@ -12857,7 +12857,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E62" s="9"/>
       <c r="H62" s="22"/>
@@ -14116,7 +14116,7 @@
         <v>Senkkopfschraube Innensechskant M3 10mm</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E147" s="9"/>
       <c r="H147" s="22"/>
@@ -14131,7 +14131,7 @@
         <v>Distanzbolzen 2x Innen M3 20mm, Schlüsselweite 5,5mm</v>
       </c>
       <c r="D148" s="32" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E148" s="9"/>
       <c r="H148" s="22"/>
@@ -14146,7 +14146,7 @@
         <v>Zylinderkopfschraube Innensechskant M3 30mm</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E149" s="9"/>
       <c r="H149" s="22"/>
@@ -14206,7 +14206,7 @@
         <v>Muttern M3, Schlüsselweite 5.5 mm</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E153" s="9"/>
       <c r="H153" s="22"/>
@@ -14221,7 +14221,7 @@
         <v>Zylinderkopfschraube Innensechskant M3 20mm</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E154" s="9"/>
       <c r="H154" s="22"/>
@@ -14236,7 +14236,7 @@
         <v>Unterlegscheiben M3 Dicke 0,5mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E155" s="9"/>
       <c r="H155" s="22"/>
@@ -14251,7 +14251,7 @@
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E156" s="9"/>
       <c r="H156" s="22"/>
@@ -14266,7 +14266,7 @@
         <v>Unterlegscheiben M3 Kunststoff 0,8mm, Außendurchmesser 7mm</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E157" s="9"/>
       <c r="H157" s="22"/>
@@ -14281,7 +14281,7 @@
         <v>Zahnriemenscheibe T2,5, 12 Zähne</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E158" s="9"/>
       <c r="H158" s="22"/>
@@ -14296,7 +14296,7 @@
         <v>NEMA 24 - 57x57x56 - 1,26Nm - 6,35mm Achse</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E159" s="9"/>
       <c r="H159" s="22"/>
@@ -14311,7 +14311,7 @@
         <v>Zahnriemen T5 560mm 10mm Breite</v>
       </c>
       <c r="D160" s="32" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E160" s="9"/>
       <c r="H160" s="22"/>
@@ -14512,7 +14512,7 @@
         <v>1</v>
       </c>
       <c r="C169" s="32" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E169" s="9" t="s">
         <v>670</v>
@@ -15288,10 +15288,10 @@
         <v>1</v>
       </c>
       <c r="C197" t="s">
+        <v>823</v>
+      </c>
+      <c r="E197" s="29" t="s">
         <v>824</v>
-      </c>
-      <c r="E197" s="29" t="s">
-        <v>825</v>
       </c>
       <c r="G197">
         <v>1</v>
@@ -15767,11 +15767,11 @@
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D213" s="32"/>
       <c r="E213" s="29" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="G213">
         <v>1</v>
@@ -15805,7 +15805,7 @@
         <v>1</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E215" s="26" t="s">
         <v>648</v>
@@ -15834,7 +15834,7 @@
         <v>1</v>
       </c>
       <c r="C216" s="32" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E216" s="26" t="s">
         <v>707</v>
@@ -15863,7 +15863,7 @@
         <v>1</v>
       </c>
       <c r="C217" s="32" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E217" s="26" t="s">
         <v>763</v>
@@ -15892,7 +15892,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E218" s="26" t="s">
         <v>796</v>
@@ -15921,10 +15921,10 @@
         <v>1</v>
       </c>
       <c r="C219" s="32" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E219" s="26" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G219">
         <v>1</v>
@@ -15975,7 +15975,7 @@
         <v>72.649999999999991</v>
       </c>
       <c r="L220" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="221" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16008,7 +16008,7 @@
         <v>36.42</v>
       </c>
       <c r="L221" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="222" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16308,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="H232" s="22">
-        <v>26.88</v>
+        <v>20</v>
       </c>
       <c r="I232" s="18">
         <f>SUMIF(C$1:C$162,"="&amp;C232,B$1:B$162)</f>
@@ -16320,7 +16320,7 @@
       </c>
       <c r="K232" s="34">
         <f t="shared" ref="K232" si="89">B232*H232</f>
-        <v>53.76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="233" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16329,16 +16329,16 @@
         <v>1</v>
       </c>
       <c r="C233" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E233" s="29" t="s">
-        <v>812</v>
+        <v>840</v>
       </c>
       <c r="G233">
         <v>1</v>
       </c>
       <c r="H233" s="22">
-        <v>24.22</v>
+        <v>18.079999999999998</v>
       </c>
       <c r="I233" s="18">
         <f>SUMIF(C$1:C$162,"="&amp;C233,B$1:B$162)</f>
@@ -16350,7 +16350,7 @@
       </c>
       <c r="K233" s="34">
         <f t="shared" ref="K233" si="91">B233*H233</f>
-        <v>24.22</v>
+        <v>18.079999999999998</v>
       </c>
     </row>
     <row r="234" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16498,7 +16498,7 @@
         <v>550</v>
       </c>
       <c r="E240" s="29" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G240">
         <v>1</v>
@@ -16532,10 +16532,10 @@
       <c r="I242" s="18"/>
       <c r="J242" s="33"/>
       <c r="K242" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="L242" s="1" t="s">
         <v>837</v>
-      </c>
-      <c r="L242" s="1" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="243" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
@@ -16546,11 +16546,11 @@
       <c r="J243" s="33"/>
       <c r="K243" s="37">
         <f>SUM(K164:K241)</f>
-        <v>2496.1899999999996</v>
+        <v>2476.29</v>
       </c>
       <c r="L243" s="35">
         <f>SUMIF(L1:L241,"&lt;&gt;Got it",K1:K241)</f>
-        <v>2387.12</v>
+        <v>2367.2199999999998</v>
       </c>
     </row>
     <row r="244" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Null stellung von Encoders gemacht Plausi Check
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="3"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -2108,9 +2108,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2129,6 +2126,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2778,15 +2778,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>154208</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>39908</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2810,7 +2810,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="15240" y="365760"/>
+          <a:off x="91440" y="579120"/>
           <a:ext cx="4716780" cy="3446048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5190,7 +5190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -5401,8 +5401,8 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -5418,10 +5418,10 @@
       <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="81"/>
+      <c r="E4" s="90"/>
       <c r="F4" s="10" t="s">
         <v>47</v>
       </c>
@@ -8811,14 +8811,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="99" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D99" s="90" t="s">
+      <c r="D99" s="89" t="s">
         <v>578</v>
       </c>
     </row>
@@ -8896,7 +8896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8935,7 +8935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9324,8 +9324,8 @@
   </sheetPr>
   <dimension ref="A1:O321"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9458,7 +9458,7 @@
       <c r="J6" s="38"/>
       <c r="K6" s="35"/>
       <c r="L6" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C6,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L6:L11" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C6,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -9479,7 +9479,7 @@
       <c r="J7" s="38"/>
       <c r="K7" s="35"/>
       <c r="L7" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C7,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9500,7 +9500,7 @@
       <c r="J8" s="38"/>
       <c r="K8" s="35"/>
       <c r="L8" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C8,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9521,7 +9521,7 @@
       <c r="J9" s="38"/>
       <c r="K9" s="35"/>
       <c r="L9" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C9,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9542,7 +9542,7 @@
       <c r="J10" s="38"/>
       <c r="K10" s="35"/>
       <c r="L10" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C10,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9563,7 +9563,7 @@
       <c r="J11" s="38"/>
       <c r="K11" s="35"/>
       <c r="L11" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C11,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9596,7 +9596,7 @@
       <c r="J13" s="69"/>
       <c r="K13" s="70"/>
       <c r="L13" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C13,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L13:L43" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C13,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -9617,7 +9617,7 @@
       <c r="J14" s="69"/>
       <c r="K14" s="70"/>
       <c r="L14" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C14,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9638,7 +9638,7 @@
       <c r="J15" s="61"/>
       <c r="K15" s="62"/>
       <c r="L15" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C15,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9659,7 +9659,7 @@
       <c r="J16" s="69"/>
       <c r="K16" s="70"/>
       <c r="L16" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C16,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9680,7 +9680,7 @@
       <c r="J17" s="69"/>
       <c r="K17" s="70"/>
       <c r="L17" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C17,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9703,7 +9703,7 @@
       <c r="J18" s="69"/>
       <c r="K18" s="70"/>
       <c r="L18" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C18,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9726,7 +9726,7 @@
       <c r="J19" s="77"/>
       <c r="K19" s="78"/>
       <c r="L19" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C19,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -9747,7 +9747,7 @@
       <c r="J20" s="38"/>
       <c r="K20" s="35"/>
       <c r="L20" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C20,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9768,7 +9768,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="35"/>
       <c r="L21" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C21,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9789,7 +9789,7 @@
       <c r="J22" s="38"/>
       <c r="K22" s="35"/>
       <c r="L22" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C22,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9810,7 +9810,7 @@
       <c r="J23" s="38"/>
       <c r="K23" s="35"/>
       <c r="L23" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C23,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9831,7 +9831,7 @@
       <c r="J24" s="38"/>
       <c r="K24" s="35"/>
       <c r="L24" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C24,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9852,7 +9852,7 @@
       <c r="J25" s="38"/>
       <c r="K25" s="35"/>
       <c r="L25" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C25,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9873,7 +9873,7 @@
       <c r="J26" s="38"/>
       <c r="K26" s="35"/>
       <c r="L26" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C26,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9894,7 +9894,7 @@
       <c r="J27" s="38"/>
       <c r="K27" s="35"/>
       <c r="L27" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C27,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9915,7 +9915,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="35"/>
       <c r="L28" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C28,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9936,7 +9936,7 @@
       <c r="J29" s="38"/>
       <c r="K29" s="35"/>
       <c r="L29" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C29,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9957,7 +9957,7 @@
       <c r="J30" s="38"/>
       <c r="K30" s="35"/>
       <c r="L30" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C30,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9978,7 +9978,7 @@
       <c r="J31" s="38"/>
       <c r="K31" s="35"/>
       <c r="L31" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C31,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -9999,7 +9999,7 @@
       <c r="J32" s="38"/>
       <c r="K32" s="35"/>
       <c r="L32" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C32,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10020,7 +10020,7 @@
       <c r="J33" s="38"/>
       <c r="K33" s="35"/>
       <c r="L33" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C33,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10041,7 +10041,7 @@
       <c r="J34" s="38"/>
       <c r="K34" s="35"/>
       <c r="L34" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C34,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10062,7 +10062,7 @@
       <c r="J35" s="38"/>
       <c r="K35" s="35"/>
       <c r="L35" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C35,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10083,7 +10083,7 @@
       <c r="J36" s="38"/>
       <c r="K36" s="35"/>
       <c r="L36" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C36,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10104,7 +10104,7 @@
       <c r="J37" s="38"/>
       <c r="K37" s="35"/>
       <c r="L37" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C37,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10125,7 +10125,7 @@
       <c r="J38" s="38"/>
       <c r="K38" s="35"/>
       <c r="L38" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C38,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10146,7 +10146,7 @@
       <c r="J39" s="38"/>
       <c r="K39" s="35"/>
       <c r="L39" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C39,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10167,7 +10167,7 @@
       <c r="J40" s="38"/>
       <c r="K40" s="35"/>
       <c r="L40" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C40,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10188,7 +10188,7 @@
       <c r="J41" s="38"/>
       <c r="K41" s="35"/>
       <c r="L41" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C41,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10209,7 +10209,7 @@
       <c r="J42" s="38"/>
       <c r="K42" s="35"/>
       <c r="L42" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C42,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
       <c r="J43" s="38"/>
       <c r="K43" s="35"/>
       <c r="L43" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C43,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10281,7 +10281,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="35"/>
       <c r="L47" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C47,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L47:L67" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C47,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -10302,7 +10302,7 @@
       <c r="J48" s="38"/>
       <c r="K48" s="35"/>
       <c r="L48" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C48,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10323,7 +10323,7 @@
       <c r="J49" s="38"/>
       <c r="K49" s="35"/>
       <c r="L49" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C49,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10344,7 +10344,7 @@
       <c r="J50" s="38"/>
       <c r="K50" s="35"/>
       <c r="L50" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C50,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10366,7 +10366,7 @@
       <c r="J51" s="38"/>
       <c r="K51" s="35"/>
       <c r="L51" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C51,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10387,7 +10387,7 @@
       <c r="J52" s="38"/>
       <c r="K52" s="35"/>
       <c r="L52" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C52,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10408,7 +10408,7 @@
       <c r="J53" s="38"/>
       <c r="K53" s="35"/>
       <c r="L53" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C53,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10429,7 +10429,7 @@
       <c r="J54" s="38"/>
       <c r="K54" s="35"/>
       <c r="L54" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C54,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10450,7 +10450,7 @@
       <c r="J55" s="38"/>
       <c r="K55" s="35"/>
       <c r="L55" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C55,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10471,7 +10471,7 @@
       <c r="J56" s="38"/>
       <c r="K56" s="35"/>
       <c r="L56" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C56,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10492,7 +10492,7 @@
       <c r="J57" s="38"/>
       <c r="K57" s="35"/>
       <c r="L57" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C57,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10513,7 +10513,7 @@
       <c r="J58" s="38"/>
       <c r="K58" s="35"/>
       <c r="L58" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C58,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10534,7 +10534,7 @@
       <c r="J59" s="38"/>
       <c r="K59" s="35"/>
       <c r="L59" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C59,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10555,7 +10555,7 @@
       <c r="J60" s="38"/>
       <c r="K60" s="35"/>
       <c r="L60" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C60,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10578,7 +10578,7 @@
       <c r="J61" s="77"/>
       <c r="K61" s="78"/>
       <c r="L61" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C61,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -10599,7 +10599,7 @@
       <c r="J62" s="38"/>
       <c r="K62" s="35"/>
       <c r="L62" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C62,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10620,7 +10620,7 @@
       <c r="J63" s="69"/>
       <c r="K63" s="70"/>
       <c r="L63" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C63,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10641,7 +10641,7 @@
       <c r="J64" s="61"/>
       <c r="K64" s="62"/>
       <c r="L64" s="55" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C64,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10662,7 +10662,7 @@
       <c r="J65" s="61"/>
       <c r="K65" s="62"/>
       <c r="L65" s="55" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C65,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10683,7 +10683,7 @@
       <c r="J66" s="69"/>
       <c r="K66" s="70"/>
       <c r="L66" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C66,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10706,7 +10706,7 @@
       <c r="J67" s="77"/>
       <c r="K67" s="78"/>
       <c r="L67" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C67,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -10739,7 +10739,7 @@
       <c r="J69" s="38"/>
       <c r="K69" s="35"/>
       <c r="L69" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C69,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L69:L116" ca="1" si="3">INDIRECT(ADDRESS(MATCH(C69,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -10760,7 +10760,7 @@
       <c r="J70" s="38"/>
       <c r="K70" s="35"/>
       <c r="L70" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C70,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10781,7 +10781,7 @@
       <c r="J71" s="38"/>
       <c r="K71" s="35"/>
       <c r="L71" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C71,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10802,7 +10802,7 @@
       <c r="J72" s="38"/>
       <c r="K72" s="35"/>
       <c r="L72" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C72,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10823,7 +10823,7 @@
       <c r="J73" s="38"/>
       <c r="K73" s="35"/>
       <c r="L73" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C73,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10844,7 +10844,7 @@
       <c r="J74" s="38"/>
       <c r="K74" s="35"/>
       <c r="L74" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C74,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10865,7 +10865,7 @@
       <c r="J75" s="38"/>
       <c r="K75" s="35"/>
       <c r="L75" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C75,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10886,7 +10886,7 @@
       <c r="J76" s="38"/>
       <c r="K76" s="35"/>
       <c r="L76" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C76,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10907,7 +10907,7 @@
       <c r="J77" s="38"/>
       <c r="K77" s="35"/>
       <c r="L77" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C77,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10928,7 +10928,7 @@
       <c r="J78" s="38"/>
       <c r="K78" s="35"/>
       <c r="L78" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C78,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10949,7 +10949,7 @@
       <c r="J79" s="38"/>
       <c r="K79" s="35"/>
       <c r="L79" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C79,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10970,7 +10970,7 @@
       <c r="J80" s="38"/>
       <c r="K80" s="35"/>
       <c r="L80" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C80,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -10991,7 +10991,7 @@
       <c r="J81" s="38"/>
       <c r="K81" s="35"/>
       <c r="L81" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C81,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11012,7 +11012,7 @@
       <c r="J82" s="38"/>
       <c r="K82" s="35"/>
       <c r="L82" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C82,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11033,7 +11033,7 @@
       <c r="J83" s="38"/>
       <c r="K83" s="35"/>
       <c r="L83" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C83,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11054,7 +11054,7 @@
       <c r="J84" s="38"/>
       <c r="K84" s="35"/>
       <c r="L84" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C84,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11075,7 +11075,7 @@
       <c r="J85" s="38"/>
       <c r="K85" s="35"/>
       <c r="L85" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C85,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11096,7 +11096,7 @@
       <c r="J86" s="38"/>
       <c r="K86" s="35"/>
       <c r="L86" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C86,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11117,7 +11117,7 @@
       <c r="J87" s="38"/>
       <c r="K87" s="35"/>
       <c r="L87" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C87,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11138,7 +11138,7 @@
       <c r="J88" s="38"/>
       <c r="K88" s="35"/>
       <c r="L88" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C88,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11159,7 +11159,7 @@
       <c r="J89" s="38"/>
       <c r="K89" s="35"/>
       <c r="L89" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C89,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11180,7 +11180,7 @@
       <c r="J90" s="38"/>
       <c r="K90" s="35"/>
       <c r="L90" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C90,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11201,7 +11201,7 @@
       <c r="J91" s="38"/>
       <c r="K91" s="35"/>
       <c r="L91" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C91,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11222,7 +11222,7 @@
       <c r="J92" s="38"/>
       <c r="K92" s="35"/>
       <c r="L92" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C92,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11243,7 +11243,7 @@
       <c r="J93" s="38"/>
       <c r="K93" s="35"/>
       <c r="L93" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C93,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -11264,7 +11264,7 @@
       <c r="J94" s="38"/>
       <c r="K94" s="35"/>
       <c r="L94" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C94,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11285,7 +11285,7 @@
       <c r="J95" s="38"/>
       <c r="K95" s="35"/>
       <c r="L95" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C95,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11306,7 +11306,7 @@
       <c r="J96" s="38"/>
       <c r="K96" s="35"/>
       <c r="L96" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C96,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11327,7 +11327,7 @@
       <c r="J97" s="38"/>
       <c r="K97" s="35"/>
       <c r="L97" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C97,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11348,7 +11348,7 @@
       <c r="J98" s="38"/>
       <c r="K98" s="35"/>
       <c r="L98" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C98,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11369,7 +11369,7 @@
       <c r="J99" s="38"/>
       <c r="K99" s="35"/>
       <c r="L99" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C99,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11390,7 +11390,7 @@
       <c r="J100" s="38"/>
       <c r="K100" s="35"/>
       <c r="L100" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C100,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11411,7 +11411,7 @@
       <c r="J101" s="38"/>
       <c r="K101" s="35"/>
       <c r="L101" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C101,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11432,7 +11432,7 @@
       <c r="J102" s="38"/>
       <c r="K102" s="35"/>
       <c r="L102" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C102,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11453,7 +11453,7 @@
       <c r="J103" s="38"/>
       <c r="K103" s="35"/>
       <c r="L103" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C103,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11474,7 +11474,7 @@
       <c r="J104" s="38"/>
       <c r="K104" s="35"/>
       <c r="L104" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C104,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11495,7 +11495,7 @@
       <c r="J105" s="38"/>
       <c r="K105" s="35"/>
       <c r="L105" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C105,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11516,7 +11516,7 @@
       <c r="J106" s="38"/>
       <c r="K106" s="35"/>
       <c r="L106" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C106,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11537,7 +11537,7 @@
       <c r="J107" s="38"/>
       <c r="K107" s="35"/>
       <c r="L107" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C107,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11558,7 +11558,7 @@
       <c r="J108" s="38"/>
       <c r="K108" s="35"/>
       <c r="L108" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C108,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11579,7 +11579,7 @@
       <c r="J109" s="38"/>
       <c r="K109" s="35"/>
       <c r="L109" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C109,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11602,7 +11602,7 @@
       <c r="J110" s="77"/>
       <c r="K110" s="78"/>
       <c r="L110" s="71" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C110,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -11623,7 +11623,7 @@
       <c r="J111" s="38"/>
       <c r="K111" s="35"/>
       <c r="L111" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C111,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11644,7 +11644,7 @@
       <c r="J112" s="38"/>
       <c r="K112" s="35"/>
       <c r="L112" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C112,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11665,7 +11665,7 @@
       <c r="J113" s="38"/>
       <c r="K113" s="35"/>
       <c r="L113" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C113,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11686,7 +11686,7 @@
       <c r="J114" s="38"/>
       <c r="K114" s="35"/>
       <c r="L114" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C114,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       <c r="J115" s="38"/>
       <c r="K115" s="35"/>
       <c r="L115" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C115,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11730,7 +11730,7 @@
       <c r="J116" s="77"/>
       <c r="K116" s="78"/>
       <c r="L116" s="71" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C116,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -11743,48 +11743,48 @@
       <c r="J117" s="61"/>
       <c r="K117" s="62"/>
     </row>
-    <row r="118" spans="1:12" s="82" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="83">
-        <v>1</v>
-      </c>
-      <c r="C118" s="84" t="str">
+    <row r="118" spans="1:12" s="81" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="82">
+        <v>1</v>
+      </c>
+      <c r="C118" s="83" t="str">
         <f>C245</f>
         <v>Zahnriemen T5 295mm 10mm Breite</v>
       </c>
-      <c r="D118" s="82" t="s">
+      <c r="D118" s="81" t="s">
         <v>561</v>
       </c>
-      <c r="E118" s="85" t="s">
+      <c r="E118" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="H118" s="86"/>
-      <c r="I118" s="87"/>
-      <c r="J118" s="88"/>
-      <c r="K118" s="89"/>
-      <c r="L118" s="82" t="str">
+      <c r="H118" s="85"/>
+      <c r="I118" s="86"/>
+      <c r="J118" s="87"/>
+      <c r="K118" s="88"/>
+      <c r="L118" s="81" t="str">
         <f ca="1">INDIRECT(ADDRESS(MATCH(C118,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="82" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="83">
-        <v>1</v>
-      </c>
-      <c r="C119" s="84" t="str">
+    <row r="119" spans="1:12" s="81" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="82">
+        <v>1</v>
+      </c>
+      <c r="C119" s="83" t="str">
         <f>C224</f>
         <v>Zahnriemenscheibe T2,5, 36 Zähne (d=57,30)</v>
       </c>
-      <c r="D119" s="82" t="s">
+      <c r="D119" s="81" t="s">
         <v>517</v>
       </c>
-      <c r="E119" s="85" t="s">
+      <c r="E119" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="H119" s="86"/>
-      <c r="I119" s="87"/>
-      <c r="J119" s="88"/>
-      <c r="K119" s="89"/>
-      <c r="L119" s="82" t="str">
+      <c r="H119" s="85"/>
+      <c r="I119" s="86"/>
+      <c r="J119" s="87"/>
+      <c r="K119" s="88"/>
+      <c r="L119" s="81" t="str">
         <f ca="1">INDIRECT(ADDRESS(MATCH(C119,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>-</v>
       </c>
@@ -11848,7 +11848,7 @@
       <c r="J123" s="38"/>
       <c r="K123" s="35"/>
       <c r="L123" t="str">
-        <f t="shared" ref="L123:L135" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C123,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L123:L135" ca="1" si="4">INDIRECT(ADDRESS(MATCH(C123,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -11869,7 +11869,7 @@
       <c r="J124" s="38"/>
       <c r="K124" s="35"/>
       <c r="L124" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11890,7 +11890,7 @@
       <c r="J125" s="38"/>
       <c r="K125" s="35"/>
       <c r="L125" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11911,7 +11911,7 @@
       <c r="J126" s="38"/>
       <c r="K126" s="35"/>
       <c r="L126" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11932,7 +11932,7 @@
       <c r="J127" s="38"/>
       <c r="K127" s="35"/>
       <c r="L127" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11953,7 +11953,7 @@
       <c r="J128" s="38"/>
       <c r="K128" s="35"/>
       <c r="L128" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11974,7 +11974,7 @@
       <c r="J129" s="38"/>
       <c r="K129" s="35"/>
       <c r="L129" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -11995,7 +11995,7 @@
       <c r="J130" s="38"/>
       <c r="K130" s="35"/>
       <c r="L130" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12016,7 +12016,7 @@
       <c r="J131" s="38"/>
       <c r="K131" s="35"/>
       <c r="L131" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12037,7 +12037,7 @@
       <c r="J132" s="38"/>
       <c r="K132" s="35"/>
       <c r="L132" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12058,7 +12058,7 @@
       <c r="J133" s="38"/>
       <c r="K133" s="35"/>
       <c r="L133" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12079,7 +12079,7 @@
       <c r="J134" s="38"/>
       <c r="K134" s="35"/>
       <c r="L134" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12100,7 +12100,7 @@
       <c r="J135" s="38"/>
       <c r="K135" s="35"/>
       <c r="L135" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12121,7 +12121,7 @@
       <c r="J136" s="38"/>
       <c r="K136" s="35"/>
       <c r="L136" t="str">
-        <f t="shared" ref="L136:L175" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C136,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L136:L175" ca="1" si="5">INDIRECT(ADDRESS(MATCH(C136,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12142,7 +12142,7 @@
       <c r="J137" s="38"/>
       <c r="K137" s="35"/>
       <c r="L137" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12163,7 +12163,7 @@
       <c r="J138" s="38"/>
       <c r="K138" s="35"/>
       <c r="L138" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12184,7 +12184,7 @@
       <c r="J139" s="38"/>
       <c r="K139" s="35"/>
       <c r="L139" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12207,7 +12207,7 @@
       <c r="J140" s="77"/>
       <c r="K140" s="78"/>
       <c r="L140" s="71" t="str">
-        <f t="shared" ref="L140" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C140,C$183:C$292,0)+ROW($B$183)-1,12))</f>
+        <f t="shared" ref="L140" ca="1" si="6">INDIRECT(ADDRESS(MATCH(C140,C$183:C$292,0)+ROW($B$183)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -12228,7 +12228,7 @@
       <c r="J141" s="38"/>
       <c r="K141" s="35"/>
       <c r="L141" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12249,7 +12249,7 @@
       <c r="J142" s="38"/>
       <c r="K142" s="35"/>
       <c r="L142" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12270,7 +12270,7 @@
       <c r="J143" s="38"/>
       <c r="K143" s="35"/>
       <c r="L143" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12291,7 +12291,7 @@
       <c r="J144" s="38"/>
       <c r="K144" s="35"/>
       <c r="L144" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12312,7 +12312,7 @@
       <c r="J145" s="38"/>
       <c r="K145" s="35"/>
       <c r="L145" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12333,7 +12333,7 @@
       <c r="J146" s="38"/>
       <c r="K146" s="35"/>
       <c r="L146" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12354,7 +12354,7 @@
       <c r="J147" s="38"/>
       <c r="K147" s="35"/>
       <c r="L147" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12375,7 +12375,7 @@
       <c r="J148" s="38"/>
       <c r="K148" s="35"/>
       <c r="L148" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12396,7 +12396,7 @@
       <c r="J149" s="38"/>
       <c r="K149" s="35"/>
       <c r="L149" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12417,7 +12417,7 @@
       <c r="J150" s="38"/>
       <c r="K150" s="35"/>
       <c r="L150" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12438,7 +12438,7 @@
       <c r="J151" s="38"/>
       <c r="K151" s="35"/>
       <c r="L151" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12460,7 +12460,7 @@
       <c r="J152" s="38"/>
       <c r="K152" s="35"/>
       <c r="L152" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12481,7 +12481,7 @@
       <c r="J153" s="38"/>
       <c r="K153" s="35"/>
       <c r="L153" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12502,7 +12502,7 @@
       <c r="J154" s="38"/>
       <c r="K154" s="35"/>
       <c r="L154" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12523,7 +12523,7 @@
       <c r="J155" s="38"/>
       <c r="K155" s="35"/>
       <c r="L155" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12544,7 +12544,7 @@
       <c r="J156" s="38"/>
       <c r="K156" s="35"/>
       <c r="L156" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12557,7 +12557,7 @@
       <c r="J157" s="38"/>
       <c r="K157" s="35"/>
       <c r="L157" t="e">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -12581,7 +12581,7 @@
       <c r="J158" s="38"/>
       <c r="K158" s="35"/>
       <c r="L158" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12602,7 +12602,7 @@
       <c r="J159" s="38"/>
       <c r="K159" s="35"/>
       <c r="L159" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12623,7 +12623,7 @@
       <c r="J160" s="38"/>
       <c r="K160" s="35"/>
       <c r="L160" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12644,7 +12644,7 @@
       <c r="J161" s="38"/>
       <c r="K161" s="35"/>
       <c r="L161" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12665,7 +12665,7 @@
       <c r="J162" s="38"/>
       <c r="K162" s="35"/>
       <c r="L162" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12686,7 +12686,7 @@
       <c r="J163" s="38"/>
       <c r="K163" s="35"/>
       <c r="L163" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12707,7 +12707,7 @@
       <c r="J164" s="38"/>
       <c r="K164" s="35"/>
       <c r="L164" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12728,7 +12728,7 @@
       <c r="J165" s="38"/>
       <c r="K165" s="35"/>
       <c r="L165" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12749,7 +12749,7 @@
       <c r="J166" s="38"/>
       <c r="K166" s="35"/>
       <c r="L166" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12770,7 +12770,7 @@
       <c r="J167" s="38"/>
       <c r="K167" s="35"/>
       <c r="L167" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12791,7 +12791,7 @@
       <c r="J168" s="38"/>
       <c r="K168" s="35"/>
       <c r="L168" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12812,7 +12812,7 @@
       <c r="J169" s="38"/>
       <c r="K169" s="35"/>
       <c r="L169" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12833,7 +12833,7 @@
       <c r="J170" s="38"/>
       <c r="K170" s="35"/>
       <c r="L170" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12854,7 +12854,7 @@
       <c r="J171" s="38"/>
       <c r="K171" s="35"/>
       <c r="L171" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12875,7 +12875,7 @@
       <c r="J172" s="38"/>
       <c r="K172" s="35"/>
       <c r="L172" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12896,7 +12896,7 @@
       <c r="J173" s="38"/>
       <c r="K173" s="35"/>
       <c r="L173" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12917,7 +12917,7 @@
       <c r="J174" s="38"/>
       <c r="K174" s="35"/>
       <c r="L174" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -12938,7 +12938,7 @@
       <c r="J175" s="38"/>
       <c r="K175" s="35"/>
       <c r="L175" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -13022,7 +13022,7 @@
     </row>
     <row r="183" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="33">
-        <f t="shared" ref="B183:B213" si="3">ROUNDUP(I183/G183,0)</f>
+        <f t="shared" ref="B183:B213" si="7">ROUNDUP(I183/G183,0)</f>
         <v>1</v>
       </c>
       <c r="C183" s="32" t="s">
@@ -13038,11 +13038,11 @@
         <v>2.5</v>
       </c>
       <c r="I183" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C183,B$1:B$181)</f>
+        <f t="shared" ref="I183:I191" si="8">SUMIF(C$1:C$181,"="&amp;C183,B$1:B$181)</f>
         <v>14</v>
       </c>
       <c r="J183" s="38">
-        <f t="shared" ref="J183:J187" si="4">G183*B183-I183</f>
+        <f t="shared" ref="J183:J187" si="9">G183*B183-I183</f>
         <v>36</v>
       </c>
       <c r="K183" s="35">
@@ -13055,7 +13055,7 @@
     </row>
     <row r="184" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C184" s="32" t="s">
@@ -13071,11 +13071,11 @@
         <v>2.5</v>
       </c>
       <c r="I184" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C184,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="J184" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="K184" s="35">
@@ -13088,7 +13088,7 @@
     </row>
     <row r="185" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="33">
-        <f t="shared" ref="B185" si="5">ROUNDUP(I185/G185,0)</f>
+        <f t="shared" ref="B185" si="10">ROUNDUP(I185/G185,0)</f>
         <v>1</v>
       </c>
       <c r="C185" s="32" t="s">
@@ -13104,11 +13104,11 @@
         <v>2.5</v>
       </c>
       <c r="I185" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C185,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="J185" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="K185" s="35">
@@ -13121,7 +13121,7 @@
     </row>
     <row r="186" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B186" s="33">
-        <f t="shared" ref="B186" si="6">ROUNDUP(I186/G186,0)</f>
+        <f t="shared" ref="B186" si="11">ROUNDUP(I186/G186,0)</f>
         <v>1</v>
       </c>
       <c r="C186" s="32" t="s">
@@ -13137,7 +13137,7 @@
         <v>2.5</v>
       </c>
       <c r="I186" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C186,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="J186" s="38">
@@ -13145,7 +13145,7 @@
         <v>43</v>
       </c>
       <c r="K186" s="35">
-        <f t="shared" ref="K186" si="7">B186*H186</f>
+        <f t="shared" ref="K186" si="12">B186*H186</f>
         <v>2.5</v>
       </c>
       <c r="L186" t="s">
@@ -13154,7 +13154,7 @@
     </row>
     <row r="187" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C187" s="32" t="s">
@@ -13170,11 +13170,11 @@
         <v>2.5</v>
       </c>
       <c r="I187" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C187,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="J187" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="K187" s="35">
@@ -13187,7 +13187,7 @@
     </row>
     <row r="188" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B188" s="33">
-        <f t="shared" ref="B188" si="8">ROUNDUP(I188/G188,0)</f>
+        <f t="shared" ref="B188" si="13">ROUNDUP(I188/G188,0)</f>
         <v>1</v>
       </c>
       <c r="C188" s="32" t="s">
@@ -13203,15 +13203,15 @@
         <v>2.5</v>
       </c>
       <c r="I188" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C188,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J188" s="38">
-        <f t="shared" ref="J188" si="9">G188*B188-I188</f>
+        <f t="shared" ref="J188" si="14">G188*B188-I188</f>
         <v>46</v>
       </c>
       <c r="K188" s="35">
-        <f t="shared" ref="K188:K267" si="10">B188*H188</f>
+        <f t="shared" ref="K188:K267" si="15">B188*H188</f>
         <v>2.5</v>
       </c>
       <c r="L188" t="s">
@@ -13220,7 +13220,7 @@
     </row>
     <row r="189" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="33">
-        <f t="shared" ref="B189" si="11">ROUNDUP(I189/G189,0)</f>
+        <f t="shared" ref="B189" si="16">ROUNDUP(I189/G189,0)</f>
         <v>0</v>
       </c>
       <c r="C189" s="32" t="s">
@@ -13236,15 +13236,15 @@
         <v>2.5</v>
       </c>
       <c r="I189" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C189,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J189" s="38">
-        <f t="shared" ref="J189" si="12">G189*B189-I189</f>
+        <f t="shared" ref="J189" si="17">G189*B189-I189</f>
         <v>0</v>
       </c>
       <c r="K189" s="35">
-        <f t="shared" ref="K189" si="13">B189*H189</f>
+        <f t="shared" ref="K189" si="18">B189*H189</f>
         <v>0</v>
       </c>
       <c r="L189" t="s">
@@ -13269,7 +13269,7 @@
         <v>1.8</v>
       </c>
       <c r="I190" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C190,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="J190" s="38">
@@ -13302,7 +13302,7 @@
         <v>1.8</v>
       </c>
       <c r="I191" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C191,B$1:B$181)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J191" s="38">
@@ -13328,7 +13328,7 @@
     </row>
     <row r="193" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="33">
-        <f t="shared" ref="B193" si="14">ROUNDUP(I193/G193,0)</f>
+        <f t="shared" ref="B193" si="19">ROUNDUP(I193/G193,0)</f>
         <v>1</v>
       </c>
       <c r="C193" s="32" t="s">
@@ -13348,11 +13348,11 @@
         <v>20</v>
       </c>
       <c r="J193" s="38">
-        <f t="shared" ref="J193" si="15">G193*B193-I193</f>
+        <f t="shared" ref="J193" si="20">G193*B193-I193</f>
         <v>30</v>
       </c>
       <c r="K193" s="35">
-        <f t="shared" ref="K193" si="16">B193*H193</f>
+        <f t="shared" ref="K193" si="21">B193*H193</f>
         <v>2.99</v>
       </c>
       <c r="L193" t="s">
@@ -13361,7 +13361,7 @@
     </row>
     <row r="194" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B194" s="33">
-        <f t="shared" ref="B194" si="17">ROUNDUP(I194/G194,0)</f>
+        <f t="shared" ref="B194" si="22">ROUNDUP(I194/G194,0)</f>
         <v>0</v>
       </c>
       <c r="C194" s="32" t="s">
@@ -13384,11 +13384,11 @@
         <v>0</v>
       </c>
       <c r="J194" s="38">
-        <f t="shared" ref="J194" si="18">G194*B194-I194</f>
+        <f t="shared" ref="J194" si="23">G194*B194-I194</f>
         <v>0</v>
       </c>
       <c r="K194" s="35">
-        <f t="shared" ref="K194" si="19">B194*H194</f>
+        <f t="shared" ref="K194" si="24">B194*H194</f>
         <v>0</v>
       </c>
       <c r="L194" t="s">
@@ -13397,7 +13397,7 @@
     </row>
     <row r="195" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C195" s="32" t="s">
@@ -13417,11 +13417,11 @@
         <v>9</v>
       </c>
       <c r="J195" s="38">
-        <f t="shared" ref="J195:J264" si="20">G195*B195-I195</f>
+        <f t="shared" ref="J195:J264" si="25">G195*B195-I195</f>
         <v>91</v>
       </c>
       <c r="K195" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.09</v>
       </c>
       <c r="L195" t="s">
@@ -13430,7 +13430,7 @@
     </row>
     <row r="196" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="33">
-        <f t="shared" ref="B196" si="21">ROUNDUP(I196/G196,0)</f>
+        <f t="shared" ref="B196" si="26">ROUNDUP(I196/G196,0)</f>
         <v>1</v>
       </c>
       <c r="C196" s="32" t="s">
@@ -13450,11 +13450,11 @@
         <v>23</v>
       </c>
       <c r="J196" s="38">
-        <f t="shared" ref="J196" si="22">G196*B196-I196</f>
+        <f t="shared" ref="J196" si="27">G196*B196-I196</f>
         <v>77</v>
       </c>
       <c r="K196" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.09</v>
       </c>
       <c r="L196" t="s">
@@ -13463,7 +13463,7 @@
     </row>
     <row r="197" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="33">
-        <f t="shared" ref="B197:B199" si="23">ROUNDUP(I197/G197,0)</f>
+        <f t="shared" ref="B197:B199" si="28">ROUNDUP(I197/G197,0)</f>
         <v>1</v>
       </c>
       <c r="C197" s="32" t="s">
@@ -13483,11 +13483,11 @@
         <v>16</v>
       </c>
       <c r="J197" s="38">
-        <f t="shared" ref="J197:J199" si="24">G197*B197-I197</f>
+        <f t="shared" ref="J197:J199" si="29">G197*B197-I197</f>
         <v>84</v>
       </c>
       <c r="K197" s="35">
-        <f t="shared" ref="K197:K199" si="25">B197*H197</f>
+        <f t="shared" ref="K197:K199" si="30">B197*H197</f>
         <v>2.09</v>
       </c>
       <c r="L197" t="s">
@@ -13505,7 +13505,7 @@
     </row>
     <row r="199" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B199" s="33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="C199" s="32" t="s">
@@ -13521,15 +13521,15 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="I199" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C199,B$1:B$181)</f>
+        <f t="shared" ref="I199:I214" si="31">SUMIF(C$1:C$181,"="&amp;C199,B$1:B$181)</f>
         <v>1</v>
       </c>
       <c r="J199" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>49</v>
       </c>
       <c r="K199" s="35">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>4.8899999999999997</v>
       </c>
       <c r="L199" t="s">
@@ -13538,7 +13538,7 @@
     </row>
     <row r="200" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B200" s="33">
-        <f t="shared" ref="B200" si="26">ROUNDUP(I200/G200,0)</f>
+        <f t="shared" ref="B200" si="32">ROUNDUP(I200/G200,0)</f>
         <v>1</v>
       </c>
       <c r="C200" s="32" t="s">
@@ -13554,15 +13554,15 @@
         <v>2.29</v>
       </c>
       <c r="I200" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C200,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="J200" s="38">
-        <f t="shared" ref="J200" si="27">G200*B200-I200</f>
+        <f t="shared" ref="J200" si="33">G200*B200-I200</f>
         <v>48</v>
       </c>
       <c r="K200" s="35">
-        <f t="shared" ref="K200" si="28">B200*H200</f>
+        <f t="shared" ref="K200" si="34">B200*H200</f>
         <v>2.29</v>
       </c>
       <c r="L200" t="s">
@@ -13571,7 +13571,7 @@
     </row>
     <row r="201" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C201" s="32" t="s">
@@ -13587,15 +13587,15 @@
         <v>1.79</v>
       </c>
       <c r="I201" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C201,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>73</v>
       </c>
       <c r="J201" s="38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>27</v>
       </c>
       <c r="K201" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.79</v>
       </c>
       <c r="L201" t="s">
@@ -13604,7 +13604,7 @@
     </row>
     <row r="202" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C202" s="32" t="s">
@@ -13620,7 +13620,7 @@
         <v>1.79</v>
       </c>
       <c r="I202" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C202,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="J202" s="38">
@@ -13628,7 +13628,7 @@
         <v>94</v>
       </c>
       <c r="K202" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.79</v>
       </c>
       <c r="L202" t="s">
@@ -13637,7 +13637,7 @@
     </row>
     <row r="203" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B203" s="33">
-        <f t="shared" ref="B203:B204" si="29">ROUNDUP(I203/G203,0)</f>
+        <f t="shared" ref="B203:B204" si="35">ROUNDUP(I203/G203,0)</f>
         <v>1</v>
       </c>
       <c r="C203" s="32" t="s">
@@ -13653,7 +13653,7 @@
         <v>4.33</v>
       </c>
       <c r="I203" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C203,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="J203" s="38">
@@ -13661,7 +13661,7 @@
         <v>46</v>
       </c>
       <c r="K203" s="35">
-        <f t="shared" ref="K203:K204" si="30">B203*H203</f>
+        <f t="shared" ref="K203:K204" si="36">B203*H203</f>
         <v>4.33</v>
       </c>
       <c r="L203" t="s">
@@ -13670,7 +13670,7 @@
     </row>
     <row r="204" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="C204" s="32" t="s">
@@ -13686,7 +13686,7 @@
         <v>1.98</v>
       </c>
       <c r="I204" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C204,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>16</v>
       </c>
       <c r="J204" s="38">
@@ -13694,7 +13694,7 @@
         <v>4</v>
       </c>
       <c r="K204" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>3.96</v>
       </c>
       <c r="L204" t="s">
@@ -13703,7 +13703,7 @@
     </row>
     <row r="205" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="33">
-        <f t="shared" ref="B205:B206" si="31">ROUNDUP(I205/G205,0)</f>
+        <f t="shared" ref="B205:B206" si="37">ROUNDUP(I205/G205,0)</f>
         <v>0</v>
       </c>
       <c r="C205" s="32" t="s">
@@ -13719,7 +13719,7 @@
         <v>1.98</v>
       </c>
       <c r="I205" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C205,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J205" s="38">
@@ -13727,7 +13727,7 @@
         <v>0</v>
       </c>
       <c r="K205" s="35">
-        <f t="shared" ref="K205:K206" si="32">B205*H205</f>
+        <f t="shared" ref="K205:K206" si="38">B205*H205</f>
         <v>0</v>
       </c>
       <c r="L205" t="s">
@@ -13736,7 +13736,7 @@
     </row>
     <row r="206" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="C206" s="32" t="s">
@@ -13752,7 +13752,7 @@
         <v>1.98</v>
       </c>
       <c r="I206" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C206,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J206" s="38">
@@ -13760,7 +13760,7 @@
         <v>0</v>
       </c>
       <c r="K206" s="35">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L206" t="s">
@@ -13785,15 +13785,15 @@
         <v>4.49</v>
       </c>
       <c r="I207" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C207,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>86</v>
       </c>
       <c r="J207" s="38">
-        <f t="shared" ref="J207" si="33">G207*B207-I207</f>
+        <f t="shared" ref="J207" si="39">G207*B207-I207</f>
         <v>414</v>
       </c>
       <c r="K207" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4.49</v>
       </c>
       <c r="L207" t="s">
@@ -13818,15 +13818,15 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="I208" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C208,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>42</v>
       </c>
       <c r="J208" s="38">
-        <f t="shared" ref="J208:J209" si="34">G208*B208-I208</f>
+        <f t="shared" ref="J208:J209" si="40">G208*B208-I208</f>
         <v>458</v>
       </c>
       <c r="K208" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="L208" t="s">
@@ -13851,15 +13851,15 @@
         <v>4.49</v>
       </c>
       <c r="I209" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C209,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>182</v>
       </c>
       <c r="J209" s="38">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>318</v>
       </c>
       <c r="K209" s="35">
-        <f t="shared" ref="K209" si="35">B209*H209</f>
+        <f t="shared" ref="K209" si="41">B209*H209</f>
         <v>4.49</v>
       </c>
       <c r="L209" t="s">
@@ -13884,15 +13884,15 @@
         <v>4.49</v>
       </c>
       <c r="I210" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C210,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>160</v>
       </c>
       <c r="J210" s="38">
-        <f t="shared" ref="J210" si="36">G210*B210-I210</f>
+        <f t="shared" ref="J210" si="42">G210*B210-I210</f>
         <v>340</v>
       </c>
       <c r="K210" s="35">
-        <f t="shared" ref="K210" si="37">B210*H210</f>
+        <f t="shared" ref="K210" si="43">B210*H210</f>
         <v>4.49</v>
       </c>
       <c r="L210" t="s">
@@ -13917,15 +13917,15 @@
         <v>1.59</v>
       </c>
       <c r="I211" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C211,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>12</v>
       </c>
       <c r="J211" s="38">
-        <f t="shared" ref="J211" si="38">G211*B211-I211</f>
+        <f t="shared" ref="J211" si="44">G211*B211-I211</f>
         <v>88</v>
       </c>
       <c r="K211" s="35">
-        <f t="shared" ref="K211" si="39">B211*H211</f>
+        <f t="shared" ref="K211" si="45">B211*H211</f>
         <v>1.59</v>
       </c>
       <c r="L211" t="s">
@@ -13934,7 +13934,7 @@
     </row>
     <row r="212" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B212" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="C212" s="32" t="s">
@@ -13950,15 +13950,15 @@
         <v>0.3</v>
       </c>
       <c r="I212" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C212,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>34</v>
       </c>
       <c r="J212" s="38">
-        <f t="shared" ref="J212" si="40">G212*B212-I212</f>
+        <f t="shared" ref="J212" si="46">G212*B212-I212</f>
         <v>0</v>
       </c>
       <c r="K212" s="35">
-        <f t="shared" ref="K212" si="41">B212*H212</f>
+        <f t="shared" ref="K212" si="47">B212*H212</f>
         <v>10.199999999999999</v>
       </c>
       <c r="L212" t="s">
@@ -13967,7 +13967,7 @@
     </row>
     <row r="213" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B213" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C213" s="32" t="s">
@@ -13983,15 +13983,15 @@
         <v>2.09</v>
       </c>
       <c r="I213" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C213,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="J213" s="38">
-        <f t="shared" ref="J213" si="42">G213*B213-I213</f>
+        <f t="shared" ref="J213" si="48">G213*B213-I213</f>
         <v>7</v>
       </c>
       <c r="K213" s="35">
-        <f t="shared" ref="K213" si="43">B213*H213</f>
+        <f t="shared" ref="K213" si="49">B213*H213</f>
         <v>2.09</v>
       </c>
       <c r="L213" t="s">
@@ -14016,11 +14016,11 @@
         <v>1.69</v>
       </c>
       <c r="I214" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C214,B$1:B$181)</f>
+        <f t="shared" si="31"/>
         <v>300</v>
       </c>
       <c r="J214" s="38">
-        <f t="shared" ref="J214" si="44">G214*B214-I214</f>
+        <f t="shared" ref="J214" si="50">G214*B214-I214</f>
         <v>200</v>
       </c>
       <c r="K214" s="35">
@@ -14040,7 +14040,7 @@
     </row>
     <row r="216" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B216" s="33">
-        <f t="shared" ref="B216" si="45">ROUNDUP(I216/G216,0)</f>
+        <f t="shared" ref="B216" si="51">ROUNDUP(I216/G216,0)</f>
         <v>2</v>
       </c>
       <c r="C216" s="32" t="s">
@@ -14056,15 +14056,15 @@
         <v>4.54</v>
       </c>
       <c r="I216" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C216,B$1:B$181)</f>
+        <f t="shared" ref="I216:I230" si="52">SUMIF(C$1:C$181,"="&amp;C216,B$1:B$181)</f>
         <v>2</v>
       </c>
       <c r="J216" s="38">
-        <f t="shared" ref="J216" si="46">G216*B216-I216</f>
+        <f t="shared" ref="J216" si="53">G216*B216-I216</f>
         <v>0</v>
       </c>
       <c r="K216" s="35">
-        <f t="shared" ref="K216" si="47">B216*H216</f>
+        <f t="shared" ref="K216" si="54">B216*H216</f>
         <v>9.08</v>
       </c>
       <c r="L216" t="s">
@@ -14073,7 +14073,7 @@
     </row>
     <row r="217" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B217" s="33">
-        <f t="shared" ref="B217" si="48">ROUNDUP(I217/G217,0)</f>
+        <f t="shared" ref="B217" si="55">ROUNDUP(I217/G217,0)</f>
         <v>2</v>
       </c>
       <c r="C217" s="32" t="s">
@@ -14089,15 +14089,15 @@
         <v>4.54</v>
       </c>
       <c r="I217" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C217,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="J217" s="38">
-        <f t="shared" ref="J217" si="49">G217*B217-I217</f>
+        <f t="shared" ref="J217" si="56">G217*B217-I217</f>
         <v>0</v>
       </c>
       <c r="K217" s="35">
-        <f t="shared" ref="K217" si="50">B217*H217</f>
+        <f t="shared" ref="K217" si="57">B217*H217</f>
         <v>9.08</v>
       </c>
       <c r="L217" t="s">
@@ -14106,7 +14106,7 @@
     </row>
     <row r="218" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B218" s="33">
-        <f t="shared" ref="B218:B220" si="51">ROUNDUP(I218/G218,0)</f>
+        <f t="shared" ref="B218:B220" si="58">ROUNDUP(I218/G218,0)</f>
         <v>1</v>
       </c>
       <c r="C218" s="32" t="s">
@@ -14122,15 +14122,15 @@
         <v>4.54</v>
       </c>
       <c r="I218" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C218,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="J218" s="38">
-        <f t="shared" ref="J218:J220" si="52">G218*B218-I218</f>
+        <f t="shared" ref="J218:J220" si="59">G218*B218-I218</f>
         <v>0</v>
       </c>
       <c r="K218" s="35">
-        <f t="shared" ref="K218:K220" si="53">B218*H218</f>
+        <f t="shared" ref="K218:K220" si="60">B218*H218</f>
         <v>4.54</v>
       </c>
       <c r="L218" t="s">
@@ -14139,7 +14139,7 @@
     </row>
     <row r="219" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B219" s="33">
-        <f t="shared" si="51"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="C219" s="32" t="s">
@@ -14155,15 +14155,15 @@
         <v>4.96</v>
       </c>
       <c r="I219" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C219,B$1:B$181)</f>
-        <v>0</v>
-      </c>
-      <c r="J219" s="38">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
+      <c r="J219" s="38">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
       <c r="K219" s="35">
-        <f t="shared" si="53"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="L219" t="s">
@@ -14172,7 +14172,7 @@
     </row>
     <row r="220" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B220" s="33">
-        <f t="shared" si="51"/>
+        <f t="shared" si="58"/>
         <v>3</v>
       </c>
       <c r="C220" s="32" t="s">
@@ -14188,81 +14188,81 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I220" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C220,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>3</v>
       </c>
       <c r="J220" s="38">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+      <c r="K220" s="35">
+        <f t="shared" si="60"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="L220" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="221" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B221" s="33">
+        <f t="shared" ref="B221:B270" si="61">ROUNDUP(I221/G221,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C221" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="E221" t="s">
+        <v>543</v>
+      </c>
+      <c r="G221">
+        <v>1</v>
+      </c>
+      <c r="H221" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I221" s="37">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="J221" s="38">
+        <f t="shared" ref="J221" si="62">G221*B221-I221</f>
+        <v>0</v>
+      </c>
+      <c r="K221" s="35">
+        <f t="shared" si="15"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L221" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="222" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B222" s="33">
+        <f t="shared" ref="B222:B225" si="63">ROUNDUP(I222/G222,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C222" s="32" t="s">
+        <v>535</v>
+      </c>
+      <c r="E222" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="G222">
+        <v>1</v>
+      </c>
+      <c r="H222" s="22">
+        <v>4.96</v>
+      </c>
+      <c r="I222" s="37">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="K220" s="35">
-        <f t="shared" si="53"/>
-        <v>15.299999999999999</v>
-      </c>
-      <c r="L220" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="221" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="33">
-        <f t="shared" ref="B221:B270" si="54">ROUNDUP(I221/G221,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C221" s="32" t="s">
-        <v>544</v>
-      </c>
-      <c r="E221" t="s">
-        <v>543</v>
-      </c>
-      <c r="G221">
-        <v>1</v>
-      </c>
-      <c r="H221" s="22">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="I221" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C221,B$1:B$181)</f>
-        <v>1</v>
-      </c>
-      <c r="J221" s="38">
-        <f t="shared" ref="J221" si="55">G221*B221-I221</f>
+      <c r="J222" s="38">
+        <f t="shared" ref="J222:J225" si="64">G222*B222-I222</f>
         <v>0</v>
       </c>
-      <c r="K221" s="35">
-        <f t="shared" si="10"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="L221" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="222" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B222" s="33">
-        <f t="shared" ref="B222:B225" si="56">ROUNDUP(I222/G222,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C222" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="E222" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="G222">
-        <v>1</v>
-      </c>
-      <c r="H222" s="22">
-        <v>4.96</v>
-      </c>
-      <c r="I222" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C222,B$1:B$181)</f>
-        <v>0</v>
-      </c>
-      <c r="J222" s="38">
-        <f t="shared" ref="J222:J225" si="57">G222*B222-I222</f>
-        <v>0</v>
-      </c>
       <c r="K222" s="35">
-        <f t="shared" ref="K222:K225" si="58">B222*H222</f>
+        <f t="shared" ref="K222:K225" si="65">B222*H222</f>
         <v>0</v>
       </c>
       <c r="L222" t="s">
@@ -14271,7 +14271,7 @@
     </row>
     <row r="223" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B223" s="33">
-        <f t="shared" ref="B223:B224" si="59">ROUNDUP(I223/G223,0)</f>
+        <f t="shared" ref="B223:B224" si="66">ROUNDUP(I223/G223,0)</f>
         <v>1</v>
       </c>
       <c r="C223" s="32" t="s">
@@ -14287,15 +14287,15 @@
         <v>5.44</v>
       </c>
       <c r="I223" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C223,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="J223" s="38">
-        <f t="shared" ref="J223:J224" si="60">G223*B223-I223</f>
+        <f t="shared" ref="J223:J224" si="67">G223*B223-I223</f>
         <v>0</v>
       </c>
       <c r="K223" s="35">
-        <f t="shared" ref="K223:K224" si="61">B223*H223</f>
+        <f t="shared" ref="K223:K224" si="68">B223*H223</f>
         <v>5.44</v>
       </c>
       <c r="L223" t="s">
@@ -14304,7 +14304,7 @@
     </row>
     <row r="224" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B224" s="33">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C224" s="32" t="s">
@@ -14320,15 +14320,15 @@
         <v>5.44</v>
       </c>
       <c r="I224" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C224,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="J224" s="38">
-        <f t="shared" si="60"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="K224" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v>5.44</v>
       </c>
       <c r="L224" t="s">
@@ -14337,7 +14337,7 @@
     </row>
     <row r="225" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B225" s="33">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="C225" s="32" t="s">
@@ -14353,15 +14353,15 @@
         <v>5.44</v>
       </c>
       <c r="I225" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C225,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J225" s="38">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K225" s="35">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="L225" t="s">
@@ -14370,7 +14370,7 @@
     </row>
     <row r="226" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B226" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="C226" s="32" t="s">
@@ -14386,15 +14386,15 @@
         <v>5.44</v>
       </c>
       <c r="I226" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C226,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J226" s="38">
-        <f t="shared" ref="J226" si="62">G226*B226-I226</f>
+        <f t="shared" ref="J226" si="69">G226*B226-I226</f>
         <v>0</v>
       </c>
       <c r="K226" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L226" t="s">
@@ -14403,7 +14403,7 @@
     </row>
     <row r="227" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B227" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="C227" s="32" t="s">
@@ -14419,15 +14419,15 @@
         <v>6.34</v>
       </c>
       <c r="I227" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C227,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J227" s="38">
-        <f t="shared" ref="J227:J228" si="63">G227*B227-I227</f>
+        <f t="shared" ref="J227:J228" si="70">G227*B227-I227</f>
         <v>0</v>
       </c>
       <c r="K227" s="35">
-        <f t="shared" ref="K227:K228" si="64">B227*H227</f>
+        <f t="shared" ref="K227:K228" si="71">B227*H227</f>
         <v>0</v>
       </c>
       <c r="L227" t="s">
@@ -14436,7 +14436,7 @@
     </row>
     <row r="228" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B228" s="33">
-        <f t="shared" ref="B228" si="65">ROUNDUP(I228/G228,0)</f>
+        <f t="shared" ref="B228" si="72">ROUNDUP(I228/G228,0)</f>
         <v>0</v>
       </c>
       <c r="C228" s="32" t="s">
@@ -14452,15 +14452,15 @@
         <v>6.67</v>
       </c>
       <c r="I228" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C228,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J228" s="38">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="K228" s="35">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="L228" t="s">
@@ -14469,7 +14469,7 @@
     </row>
     <row r="229" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B229" s="33">
-        <f t="shared" ref="B229" si="66">ROUNDUP(I229/G229,0)</f>
+        <f t="shared" ref="B229" si="73">ROUNDUP(I229/G229,0)</f>
         <v>0</v>
       </c>
       <c r="C229" s="32" t="s">
@@ -14485,15 +14485,15 @@
         <v>6.67</v>
       </c>
       <c r="I229" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C229,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J229" s="38">
-        <f t="shared" ref="J229" si="67">G229*B229-I229</f>
+        <f t="shared" ref="J229" si="74">G229*B229-I229</f>
         <v>0</v>
       </c>
       <c r="K229" s="35">
-        <f t="shared" ref="K229" si="68">B229*H229</f>
+        <f t="shared" ref="K229" si="75">B229*H229</f>
         <v>0</v>
       </c>
       <c r="L229" t="s">
@@ -14502,7 +14502,7 @@
     </row>
     <row r="230" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B230" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="C230" s="32" t="s">
@@ -14518,15 +14518,15 @@
         <v>11.6</v>
       </c>
       <c r="I230" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C230,B$1:B$181)</f>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="J230" s="38">
-        <f t="shared" ref="J230:J232" si="69">G230*B230-I230</f>
+        <f t="shared" ref="J230:J232" si="76">G230*B230-I230</f>
         <v>0</v>
       </c>
       <c r="K230" s="35">
-        <f t="shared" ref="K230:K232" si="70">B230*H230</f>
+        <f t="shared" ref="K230:K232" si="77">B230*H230</f>
         <v>23.2</v>
       </c>
       <c r="L230" t="s">
@@ -14544,7 +14544,7 @@
     </row>
     <row r="232" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B232" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="C232" s="32" t="s">
@@ -14560,15 +14560,15 @@
         <v>5.23</v>
       </c>
       <c r="I232" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C232,B$1:B$181)</f>
+        <f t="shared" ref="I232:I251" si="78">SUMIF(C$1:C$181,"="&amp;C232,B$1:B$181)</f>
         <v>2</v>
       </c>
       <c r="J232" s="38">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K232" s="35">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>10.46</v>
       </c>
       <c r="L232" t="s">
@@ -14577,7 +14577,7 @@
     </row>
     <row r="233" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B233" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>5</v>
       </c>
       <c r="C233" s="32" t="s">
@@ -14593,15 +14593,15 @@
         <v>5.23</v>
       </c>
       <c r="I233" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C233,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>5</v>
       </c>
       <c r="J233" s="38">
-        <f t="shared" ref="J233" si="71">G233*B233-I233</f>
+        <f t="shared" ref="J233" si="79">G233*B233-I233</f>
         <v>0</v>
       </c>
       <c r="K233" s="35">
-        <f t="shared" ref="K233" si="72">B233*H233</f>
+        <f t="shared" ref="K233" si="80">B233*H233</f>
         <v>26.150000000000002</v>
       </c>
       <c r="L233" t="s">
@@ -14610,7 +14610,7 @@
     </row>
     <row r="234" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B234" s="33">
-        <f t="shared" ref="B234" si="73">ROUNDUP(I234/G234,0)</f>
+        <f t="shared" ref="B234" si="81">ROUNDUP(I234/G234,0)</f>
         <v>2</v>
       </c>
       <c r="C234" s="32" t="s">
@@ -14626,15 +14626,15 @@
         <v>5.23</v>
       </c>
       <c r="I234" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C234,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>2</v>
       </c>
       <c r="J234" s="38">
-        <f t="shared" ref="J234" si="74">G234*B234-I234</f>
+        <f t="shared" ref="J234" si="82">G234*B234-I234</f>
         <v>0</v>
       </c>
       <c r="K234" s="35">
-        <f t="shared" ref="K234" si="75">B234*H234</f>
+        <f t="shared" ref="K234" si="83">B234*H234</f>
         <v>10.46</v>
       </c>
       <c r="L234" t="s">
@@ -14643,7 +14643,7 @@
     </row>
     <row r="235" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C235" s="32" t="s">
@@ -14659,15 +14659,15 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="I235" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C235,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J235" s="38">
-        <f t="shared" ref="J235" si="76">G235*B235-I235</f>
+        <f t="shared" ref="J235" si="84">G235*B235-I235</f>
         <v>0</v>
       </c>
       <c r="K235" s="35">
-        <f t="shared" ref="K235" si="77">B235*H235</f>
+        <f t="shared" ref="K235" si="85">B235*H235</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="L235" t="s">
@@ -14676,7 +14676,7 @@
     </row>
     <row r="236" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="33">
-        <f t="shared" ref="B236" si="78">ROUNDUP(I236/G236,0)</f>
+        <f t="shared" ref="B236" si="86">ROUNDUP(I236/G236,0)</f>
         <v>1</v>
       </c>
       <c r="C236" s="32" t="s">
@@ -14692,15 +14692,15 @@
         <v>5.07</v>
       </c>
       <c r="I236" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C236,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J236" s="38">
-        <f t="shared" ref="J236" si="79">G236*B236-I236</f>
+        <f t="shared" ref="J236" si="87">G236*B236-I236</f>
         <v>0</v>
       </c>
       <c r="K236" s="35">
-        <f t="shared" ref="K236" si="80">B236*H236</f>
+        <f t="shared" ref="K236" si="88">B236*H236</f>
         <v>5.07</v>
       </c>
       <c r="L236" t="s">
@@ -14709,7 +14709,7 @@
     </row>
     <row r="237" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B237" s="33">
-        <f t="shared" ref="B237" si="81">ROUNDUP(I237/G237,0)</f>
+        <f t="shared" ref="B237" si="89">ROUNDUP(I237/G237,0)</f>
         <v>1</v>
       </c>
       <c r="C237" s="32" t="s">
@@ -14725,7 +14725,7 @@
         <v>4</v>
       </c>
       <c r="I237" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C237,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J237" s="38">
@@ -14733,7 +14733,7 @@
         <v>0</v>
       </c>
       <c r="K237" s="35">
-        <f t="shared" ref="K237:K242" si="82">B237*H237</f>
+        <f t="shared" ref="K237:K242" si="90">B237*H237</f>
         <v>4</v>
       </c>
       <c r="L237" t="s">
@@ -14742,7 +14742,7 @@
     </row>
     <row r="238" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B238" s="33">
-        <f t="shared" ref="B238" si="83">ROUNDUP(I238/G238,0)</f>
+        <f t="shared" ref="B238" si="91">ROUNDUP(I238/G238,0)</f>
         <v>1</v>
       </c>
       <c r="C238" s="32" t="s">
@@ -14758,15 +14758,15 @@
         <v>4.24</v>
       </c>
       <c r="I238" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C238,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J238" s="38">
-        <f t="shared" ref="J238" si="84">G238*B238-I238</f>
+        <f t="shared" ref="J238" si="92">G238*B238-I238</f>
         <v>0</v>
       </c>
       <c r="K238" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>4.24</v>
       </c>
       <c r="L238" t="s">
@@ -14791,15 +14791,15 @@
         <v>4.24</v>
       </c>
       <c r="I239" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C239,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="J239" s="38">
-        <f t="shared" ref="J239" si="85">G239*B239-I239</f>
+        <f t="shared" ref="J239" si="93">G239*B239-I239</f>
         <v>0</v>
       </c>
       <c r="K239" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="L239" t="s">
@@ -14808,7 +14808,7 @@
     </row>
     <row r="240" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B240" s="33">
-        <f t="shared" ref="B240" si="86">ROUNDUP(I240/G240,0)</f>
+        <f t="shared" ref="B240" si="94">ROUNDUP(I240/G240,0)</f>
         <v>1</v>
       </c>
       <c r="C240" s="32" t="s">
@@ -14824,7 +14824,7 @@
         <v>4</v>
       </c>
       <c r="I240" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C240,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J240" s="38">
@@ -14832,7 +14832,7 @@
         <v>0</v>
       </c>
       <c r="K240" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>4</v>
       </c>
       <c r="L240" t="s">
@@ -14857,15 +14857,15 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="I241" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C241,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="J241" s="38">
-        <f t="shared" ref="J241" si="87">G241*B241-I241</f>
+        <f t="shared" ref="J241" si="95">G241*B241-I241</f>
         <v>0</v>
       </c>
       <c r="K241" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="L241" t="s">
@@ -14874,7 +14874,7 @@
     </row>
     <row r="242" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C242" s="32" t="s">
@@ -14890,7 +14890,7 @@
         <v>4.96</v>
       </c>
       <c r="I242" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C242,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J242" s="38">
@@ -14898,7 +14898,7 @@
         <v>0</v>
       </c>
       <c r="K242" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>4.96</v>
       </c>
       <c r="L242" t="s">
@@ -14907,7 +14907,7 @@
     </row>
     <row r="243" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B243" s="33">
-        <f t="shared" ref="B243:B246" si="88">ROUNDUP(I243/G243,0)</f>
+        <f t="shared" ref="B243:B246" si="96">ROUNDUP(I243/G243,0)</f>
         <v>1</v>
       </c>
       <c r="C243" s="32" t="s">
@@ -14923,7 +14923,7 @@
         <v>4.96</v>
       </c>
       <c r="I243" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C243,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J243" s="38">
@@ -14931,7 +14931,7 @@
         <v>0</v>
       </c>
       <c r="K243" s="35">
-        <f t="shared" ref="K243:K245" si="89">B243*H243</f>
+        <f t="shared" ref="K243:K245" si="97">B243*H243</f>
         <v>4.96</v>
       </c>
       <c r="L243" t="s">
@@ -14940,7 +14940,7 @@
     </row>
     <row r="244" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="33">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="C244" s="32" t="s">
@@ -14956,7 +14956,7 @@
         <v>4</v>
       </c>
       <c r="I244" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C244,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="J244" s="38">
@@ -14964,7 +14964,7 @@
         <v>0</v>
       </c>
       <c r="K244" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="L244" t="s">
@@ -14973,7 +14973,7 @@
     </row>
     <row r="245" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B245" s="33">
-        <f t="shared" ref="B245" si="90">ROUNDUP(I245/G245,0)</f>
+        <f t="shared" ref="B245" si="98">ROUNDUP(I245/G245,0)</f>
         <v>1</v>
       </c>
       <c r="C245" s="32" t="s">
@@ -14989,7 +14989,7 @@
         <v>4.96</v>
       </c>
       <c r="I245" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C245,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J245" s="38">
@@ -14997,7 +14997,7 @@
         <v>0</v>
       </c>
       <c r="K245" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>4.96</v>
       </c>
       <c r="L245" t="s">
@@ -15006,7 +15006,7 @@
     </row>
     <row r="246" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B246" s="33">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>1</v>
       </c>
       <c r="C246" s="32" t="s">
@@ -15022,7 +15022,7 @@
         <v>4.96</v>
       </c>
       <c r="I246" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C246,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J246" s="38">
@@ -15030,7 +15030,7 @@
         <v>0</v>
       </c>
       <c r="K246" s="35">
-        <f t="shared" ref="K246" si="91">B246*H246</f>
+        <f t="shared" ref="K246" si="99">B246*H246</f>
         <v>4.96</v>
       </c>
       <c r="L246" t="s">
@@ -15055,15 +15055,15 @@
         <v>7.13</v>
       </c>
       <c r="I247" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C247,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>3</v>
       </c>
       <c r="J247" s="38">
-        <f t="shared" ref="J247" si="92">G247*B247-I247</f>
+        <f t="shared" ref="J247" si="100">G247*B247-I247</f>
         <v>0</v>
       </c>
       <c r="K247" s="35">
-        <f t="shared" ref="K247" si="93">B247*H247</f>
+        <f t="shared" ref="K247" si="101">B247*H247</f>
         <v>21.39</v>
       </c>
       <c r="L247" t="s">
@@ -15088,15 +15088,15 @@
         <v>7.88</v>
       </c>
       <c r="I248" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C248,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="J248" s="38">
-        <f t="shared" ref="J248" si="94">G248*B248-I248</f>
+        <f t="shared" ref="J248" si="102">G248*B248-I248</f>
         <v>0</v>
       </c>
       <c r="K248" s="35">
-        <f t="shared" ref="K248" si="95">B248*H248</f>
+        <f t="shared" ref="K248" si="103">B248*H248</f>
         <v>0</v>
       </c>
       <c r="L248" t="s">
@@ -15121,15 +15121,15 @@
         <v>7.88</v>
       </c>
       <c r="I249" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C249,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J249" s="38">
-        <f t="shared" ref="J249" si="96">G249*B249-I249</f>
+        <f t="shared" ref="J249" si="104">G249*B249-I249</f>
         <v>0</v>
       </c>
       <c r="K249" s="35">
-        <f t="shared" ref="K249" si="97">B249*H249</f>
+        <f t="shared" ref="K249" si="105">B249*H249</f>
         <v>7.88</v>
       </c>
       <c r="L249" t="s">
@@ -15138,7 +15138,7 @@
     </row>
     <row r="250" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B250" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C250" s="32" t="s">
@@ -15154,15 +15154,15 @@
         <v>8.8699999999999992</v>
       </c>
       <c r="I250" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C250,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J250" s="38">
-        <f t="shared" ref="J250" si="98">G250*B250-I250</f>
+        <f t="shared" ref="J250" si="106">G250*B250-I250</f>
         <v>0</v>
       </c>
       <c r="K250" s="35">
-        <f t="shared" ref="K250" si="99">B250*H250</f>
+        <f t="shared" ref="K250" si="107">B250*H250</f>
         <v>8.8699999999999992</v>
       </c>
       <c r="L250" t="s">
@@ -15171,7 +15171,7 @@
     </row>
     <row r="251" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B251" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C251" s="32" t="s">
@@ -15187,15 +15187,15 @@
         <v>7.13</v>
       </c>
       <c r="I251" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C251,B$1:B$181)</f>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="J251" s="38">
-        <f t="shared" ref="J251" si="100">G251*B251-I251</f>
+        <f t="shared" ref="J251" si="108">G251*B251-I251</f>
         <v>0</v>
       </c>
       <c r="K251" s="35">
-        <f t="shared" ref="K251" si="101">B251*H251</f>
+        <f t="shared" ref="K251" si="109">B251*H251</f>
         <v>7.13</v>
       </c>
       <c r="L251" t="s">
@@ -15212,7 +15212,7 @@
     </row>
     <row r="253" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B253" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C253" s="32" t="s">
@@ -15228,15 +15228,15 @@
         <v>14.5</v>
       </c>
       <c r="I253" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C253,B$1:B$181)</f>
+        <f t="shared" ref="I253:I259" si="110">SUMIF(C$1:C$181,"="&amp;C253,B$1:B$181)</f>
         <v>1</v>
       </c>
       <c r="J253" s="38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K253" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>14.5</v>
       </c>
       <c r="L253" t="s">
@@ -15245,7 +15245,7 @@
     </row>
     <row r="254" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B254" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C254" s="32" t="s">
@@ -15261,15 +15261,15 @@
         <v>8.5</v>
       </c>
       <c r="I254" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C254,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
       <c r="J254" s="38">
-        <f t="shared" ref="J254" si="102">G254*B254-I254</f>
+        <f t="shared" ref="J254" si="111">G254*B254-I254</f>
         <v>0</v>
       </c>
       <c r="K254" s="35">
-        <f t="shared" ref="K254" si="103">B254*H254</f>
+        <f t="shared" ref="K254" si="112">B254*H254</f>
         <v>8.5</v>
       </c>
       <c r="L254" t="s">
@@ -15278,7 +15278,7 @@
     </row>
     <row r="255" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B255" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C255" s="32" t="s">
@@ -15294,15 +15294,15 @@
         <v>54.2</v>
       </c>
       <c r="I255" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C255,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
       <c r="J255" s="38">
-        <f t="shared" ref="J255" si="104">G255*B255-I255</f>
+        <f t="shared" ref="J255" si="113">G255*B255-I255</f>
         <v>0</v>
       </c>
       <c r="K255" s="35">
-        <f t="shared" ref="K255" si="105">B255*H255</f>
+        <f t="shared" ref="K255" si="114">B255*H255</f>
         <v>54.2</v>
       </c>
       <c r="L255" t="s">
@@ -15311,7 +15311,7 @@
     </row>
     <row r="256" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B256" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C256" s="32" t="s">
@@ -15327,15 +15327,15 @@
         <v>37</v>
       </c>
       <c r="I256" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C256,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
       <c r="J256" s="38">
-        <f t="shared" ref="J256" si="106">G256*B256-I256</f>
+        <f t="shared" ref="J256" si="115">G256*B256-I256</f>
         <v>0</v>
       </c>
       <c r="K256" s="35">
-        <f t="shared" ref="K256" si="107">B256*H256</f>
+        <f t="shared" ref="K256" si="116">B256*H256</f>
         <v>37</v>
       </c>
       <c r="L256" t="s">
@@ -15344,7 +15344,7 @@
     </row>
     <row r="257" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B257" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C257" s="32" t="s">
@@ -15360,15 +15360,15 @@
         <v>18</v>
       </c>
       <c r="I257" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C257,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
       <c r="J257" s="38">
-        <f t="shared" ref="J257" si="108">G257*B257-I257</f>
+        <f t="shared" ref="J257" si="117">G257*B257-I257</f>
         <v>0</v>
       </c>
       <c r="K257" s="35">
-        <f t="shared" ref="K257" si="109">B257*H257</f>
+        <f t="shared" ref="K257" si="118">B257*H257</f>
         <v>18</v>
       </c>
       <c r="L257" t="s">
@@ -15377,7 +15377,7 @@
     </row>
     <row r="258" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B258" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>5</v>
       </c>
       <c r="C258" s="32" t="s">
@@ -15393,15 +15393,15 @@
         <v>14.53</v>
       </c>
       <c r="I258" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C258,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>5</v>
       </c>
       <c r="J258" s="38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K258" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>72.649999999999991</v>
       </c>
       <c r="L258" t="s">
@@ -15410,7 +15410,7 @@
     </row>
     <row r="259" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B259" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C259" s="32" t="s">
@@ -15426,15 +15426,15 @@
         <v>36.42</v>
       </c>
       <c r="I259" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C259,B$1:B$181)</f>
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
       <c r="J259" s="38">
-        <f t="shared" ref="J259" si="110">G259*B259-I259</f>
+        <f t="shared" ref="J259" si="119">G259*B259-I259</f>
         <v>0</v>
       </c>
       <c r="K259" s="35">
-        <f t="shared" ref="K259" si="111">B259*H259</f>
+        <f t="shared" ref="K259" si="120">B259*H259</f>
         <v>36.42</v>
       </c>
       <c r="L259" t="s">
@@ -15468,11 +15468,11 @@
         <v>1.05</v>
       </c>
       <c r="I261" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C261,B$1:B$181)</f>
+        <f t="shared" ref="I261:I270" si="121">SUMIF(C$1:C$181,"="&amp;C261,B$1:B$181)</f>
         <v>6</v>
       </c>
       <c r="J261" s="38">
-        <f t="shared" ref="J261" si="112">G261*B261-I261</f>
+        <f t="shared" ref="J261" si="122">G261*B261-I261</f>
         <v>0</v>
       </c>
       <c r="K261" s="35">
@@ -15485,7 +15485,7 @@
     </row>
     <row r="262" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B262" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>8</v>
       </c>
       <c r="C262" s="32" t="s">
@@ -15501,15 +15501,15 @@
         <v>1.54</v>
       </c>
       <c r="I262" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C262,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>8</v>
       </c>
       <c r="J262" s="38">
-        <f t="shared" ref="J262" si="113">G262*B262-I262</f>
+        <f t="shared" ref="J262" si="123">G262*B262-I262</f>
         <v>0</v>
       </c>
       <c r="K262" s="35">
-        <f t="shared" ref="K262" si="114">B262*H262</f>
+        <f t="shared" ref="K262" si="124">B262*H262</f>
         <v>12.32</v>
       </c>
       <c r="L262" t="s">
@@ -15518,7 +15518,7 @@
     </row>
     <row r="263" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B263" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>14</v>
       </c>
       <c r="C263" s="32" t="s">
@@ -15534,15 +15534,15 @@
         <v>1.54</v>
       </c>
       <c r="I263" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C263,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>14</v>
       </c>
       <c r="J263" s="38">
-        <f t="shared" ref="J263" si="115">G263*B263-I263</f>
+        <f t="shared" ref="J263" si="125">G263*B263-I263</f>
         <v>0</v>
       </c>
       <c r="K263" s="35">
-        <f t="shared" ref="K263" si="116">B263*H263</f>
+        <f t="shared" ref="K263" si="126">B263*H263</f>
         <v>21.560000000000002</v>
       </c>
       <c r="L263" t="s">
@@ -15551,7 +15551,7 @@
     </row>
     <row r="264" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B264" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="C264" s="32" t="s">
@@ -15567,15 +15567,15 @@
         <v>1.95</v>
       </c>
       <c r="I264" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C264,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>2</v>
       </c>
       <c r="J264" s="38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K264" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3.9</v>
       </c>
       <c r="L264" t="s">
@@ -15600,11 +15600,11 @@
         <v>1</v>
       </c>
       <c r="I265" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C265,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>2</v>
       </c>
       <c r="J265" s="38">
-        <f t="shared" ref="J265" si="117">G265*B265-I265</f>
+        <f t="shared" ref="J265" si="127">G265*B265-I265</f>
         <v>0</v>
       </c>
       <c r="K265" s="35">
@@ -15617,7 +15617,7 @@
     </row>
     <row r="266" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B266" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="C266" s="32" t="s">
@@ -15633,15 +15633,15 @@
         <v>1.39</v>
       </c>
       <c r="I266" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C266,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>2</v>
       </c>
       <c r="J266" s="38">
-        <f t="shared" ref="J266" si="118">G266*B266-I266</f>
+        <f t="shared" ref="J266" si="128">G266*B266-I266</f>
         <v>0</v>
       </c>
       <c r="K266" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2.78</v>
       </c>
       <c r="L266" t="s">
@@ -15650,7 +15650,7 @@
     </row>
     <row r="267" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B267" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>5</v>
       </c>
       <c r="C267" s="32" t="s">
@@ -15666,15 +15666,15 @@
         <v>3.29</v>
       </c>
       <c r="I267" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C267,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>5</v>
       </c>
       <c r="J267" s="38">
-        <f t="shared" ref="J267" si="119">G267*B267-I267</f>
+        <f t="shared" ref="J267" si="129">G267*B267-I267</f>
         <v>0</v>
       </c>
       <c r="K267" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>16.45</v>
       </c>
       <c r="L267" t="s">
@@ -15683,7 +15683,7 @@
     </row>
     <row r="268" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B268" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>4</v>
       </c>
       <c r="C268" s="32" t="s">
@@ -15699,15 +15699,15 @@
         <v>1</v>
       </c>
       <c r="I268" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C268,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>4</v>
       </c>
       <c r="J268" s="38">
-        <f t="shared" ref="J268" si="120">G268*B268-I268</f>
+        <f t="shared" ref="J268" si="130">G268*B268-I268</f>
         <v>0</v>
       </c>
       <c r="K268" s="35">
-        <f t="shared" ref="K268" si="121">B268*H268</f>
+        <f t="shared" ref="K268" si="131">B268*H268</f>
         <v>4</v>
       </c>
       <c r="L268" t="s">
@@ -15716,7 +15716,7 @@
     </row>
     <row r="269" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B269" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="C269" s="32" t="s">
@@ -15732,15 +15732,15 @@
         <v>20</v>
       </c>
       <c r="I269" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C269,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>2</v>
       </c>
       <c r="J269" s="38">
-        <f t="shared" ref="J269" si="122">G269*B269-I269</f>
+        <f t="shared" ref="J269" si="132">G269*B269-I269</f>
         <v>0</v>
       </c>
       <c r="K269" s="35">
-        <f t="shared" ref="K269" si="123">B269*H269</f>
+        <f t="shared" ref="K269" si="133">B269*H269</f>
         <v>40</v>
       </c>
       <c r="L269" t="s">
@@ -15749,7 +15749,7 @@
     </row>
     <row r="270" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B270" s="33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="C270" s="32" t="s">
@@ -15765,15 +15765,15 @@
         <v>18.079999999999998</v>
       </c>
       <c r="I270" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C270,B$1:B$181)</f>
+        <f t="shared" si="121"/>
         <v>1</v>
       </c>
       <c r="J270" s="38">
-        <f t="shared" ref="J270" si="124">G270*B270-I270</f>
+        <f t="shared" ref="J270" si="134">G270*B270-I270</f>
         <v>0</v>
       </c>
       <c r="K270" s="35">
-        <f t="shared" ref="K270" si="125">B270*H270</f>
+        <f t="shared" ref="K270" si="135">B270*H270</f>
         <v>18.079999999999998</v>
       </c>
       <c r="L270" t="s">
@@ -15818,15 +15818,15 @@
         <v>10.99</v>
       </c>
       <c r="I273" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C273,B$1:B$181)</f>
+        <f t="shared" ref="I273:I282" si="136">SUMIF(C$1:C$181,"="&amp;C273,B$1:B$181)</f>
         <v>0</v>
       </c>
       <c r="J273" s="38">
-        <f t="shared" ref="J273" si="126">G273*B273-I273</f>
+        <f t="shared" ref="J273" si="137">G273*B273-I273</f>
         <v>1</v>
       </c>
       <c r="K273" s="35">
-        <f t="shared" ref="K273" si="127">B273*H273</f>
+        <f t="shared" ref="K273" si="138">B273*H273</f>
         <v>10.99</v>
       </c>
       <c r="L273" t="s">
@@ -15850,15 +15850,15 @@
         <v>10.99</v>
       </c>
       <c r="I274" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C274,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>3</v>
       </c>
       <c r="J274" s="38">
-        <f t="shared" ref="J274:J275" si="128">G274*B274-I274</f>
+        <f t="shared" ref="J274:J275" si="139">G274*B274-I274</f>
         <v>-2</v>
       </c>
       <c r="K274" s="35">
-        <f t="shared" ref="K274:K275" si="129">B274*H274</f>
+        <f t="shared" ref="K274:K275" si="140">B274*H274</f>
         <v>10.99</v>
       </c>
       <c r="L274" t="s">
@@ -15882,15 +15882,15 @@
         <v>2.8</v>
       </c>
       <c r="I275" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C275,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>1</v>
       </c>
       <c r="J275" s="38">
-        <f t="shared" si="128"/>
+        <f t="shared" si="139"/>
         <v>0</v>
       </c>
       <c r="K275" s="35">
-        <f t="shared" si="129"/>
+        <f t="shared" si="140"/>
         <v>2.8</v>
       </c>
       <c r="L275" t="s">
@@ -15914,15 +15914,15 @@
         <v>2.8</v>
       </c>
       <c r="I276" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C276,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>2</v>
       </c>
       <c r="J276" s="38">
-        <f t="shared" ref="J276" si="130">G276*B276-I276</f>
+        <f t="shared" ref="J276" si="141">G276*B276-I276</f>
         <v>-1</v>
       </c>
       <c r="K276" s="35">
-        <f t="shared" ref="K276" si="131">B276*H276</f>
+        <f t="shared" ref="K276" si="142">B276*H276</f>
         <v>2.8</v>
       </c>
       <c r="L276" t="s">
@@ -15946,7 +15946,7 @@
         <v>2.8</v>
       </c>
       <c r="I277" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C277,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="J277" s="38">
@@ -15978,15 +15978,15 @@
         <v>2.8</v>
       </c>
       <c r="I278" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C278,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>3</v>
       </c>
       <c r="J278" s="38">
-        <f t="shared" ref="J278" si="132">G278*B278-I278</f>
+        <f t="shared" ref="J278" si="143">G278*B278-I278</f>
         <v>-2</v>
       </c>
       <c r="K278" s="35">
-        <f t="shared" ref="K278" si="133">B278*H278</f>
+        <f t="shared" ref="K278" si="144">B278*H278</f>
         <v>2.8</v>
       </c>
       <c r="L278" t="s">
@@ -16010,15 +16010,15 @@
         <v>1839</v>
       </c>
       <c r="I279" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C279,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="J279" s="38">
-        <f t="shared" ref="J279" si="134">G279*B279-I279</f>
+        <f t="shared" ref="J279" si="145">G279*B279-I279</f>
         <v>1</v>
       </c>
       <c r="K279" s="35">
-        <f t="shared" ref="K279" si="135">B279*H279</f>
+        <f t="shared" ref="K279" si="146">B279*H279</f>
         <v>1839</v>
       </c>
       <c r="L279" t="s">
@@ -16042,15 +16042,15 @@
         <v>31.5</v>
       </c>
       <c r="I280" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C280,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="J280" s="38">
-        <f t="shared" ref="J280" si="136">G280*B280-I280</f>
+        <f t="shared" ref="J280" si="147">G280*B280-I280</f>
         <v>1</v>
       </c>
       <c r="K280" s="35">
-        <f t="shared" ref="K280" si="137">B280*H280</f>
+        <f t="shared" ref="K280" si="148">B280*H280</f>
         <v>31.5</v>
       </c>
       <c r="L280" t="s">
@@ -16074,15 +16074,15 @@
         <v>49</v>
       </c>
       <c r="I281" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C281,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="J281" s="38">
-        <f t="shared" ref="J281" si="138">G281*B281-I281</f>
+        <f t="shared" ref="J281" si="149">G281*B281-I281</f>
         <v>1</v>
       </c>
       <c r="K281" s="35">
-        <f t="shared" ref="K281" si="139">B281*H281</f>
+        <f t="shared" ref="K281" si="150">B281*H281</f>
         <v>49</v>
       </c>
       <c r="L281" t="s">
@@ -16101,7 +16101,7 @@
       </c>
       <c r="H282" s="22"/>
       <c r="I282" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C282,B$1:B$181)</f>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="J282" s="38"/>
@@ -16143,15 +16143,15 @@
         <v>0.87</v>
       </c>
       <c r="I285" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C285,B$1:B$181)</f>
+        <f t="shared" ref="I285:I290" si="151">SUMIF(C$1:C$181,"="&amp;C285,B$1:B$181)</f>
         <v>0</v>
       </c>
       <c r="J285" s="38">
-        <f t="shared" ref="J285:J286" si="140">G285*B285-I285</f>
+        <f t="shared" ref="J285:J286" si="152">G285*B285-I285</f>
         <v>1</v>
       </c>
       <c r="K285" s="35">
-        <f t="shared" ref="K285:K286" si="141">B285*H285</f>
+        <f t="shared" ref="K285:K286" si="153">B285*H285</f>
         <v>0.87</v>
       </c>
       <c r="L285" t="s">
@@ -16175,15 +16175,15 @@
         <v>0.8</v>
       </c>
       <c r="I286" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C286,B$1:B$181)</f>
+        <f t="shared" si="151"/>
         <v>0</v>
       </c>
       <c r="J286" s="38">
-        <f t="shared" si="140"/>
+        <f t="shared" si="152"/>
         <v>1</v>
       </c>
       <c r="K286" s="35">
-        <f t="shared" si="141"/>
+        <f t="shared" si="153"/>
         <v>0.8</v>
       </c>
       <c r="L286" t="s">
@@ -16207,15 +16207,15 @@
         <v>19.989999999999998</v>
       </c>
       <c r="I287" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C287,B$1:B$181)</f>
+        <f t="shared" si="151"/>
         <v>0</v>
       </c>
       <c r="J287" s="38">
-        <f t="shared" ref="J287:J288" si="142">G287*B287-I287</f>
+        <f t="shared" ref="J287:J288" si="154">G287*B287-I287</f>
         <v>5</v>
       </c>
       <c r="K287" s="35">
-        <f t="shared" ref="K287:K288" si="143">B287*H287</f>
+        <f t="shared" ref="K287:K288" si="155">B287*H287</f>
         <v>99.949999999999989</v>
       </c>
       <c r="L287" t="s">
@@ -16239,15 +16239,15 @@
         <v>44</v>
       </c>
       <c r="I288" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C288,B$1:B$181)</f>
+        <f t="shared" si="151"/>
         <v>0</v>
       </c>
       <c r="J288" s="38">
-        <f t="shared" si="142"/>
+        <f t="shared" si="154"/>
         <v>1</v>
       </c>
       <c r="K288" s="35">
-        <f t="shared" si="143"/>
+        <f t="shared" si="155"/>
         <v>44</v>
       </c>
       <c r="L288" t="s">
@@ -16271,15 +16271,15 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="I289" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C289,B$1:B$181)</f>
+        <f t="shared" si="151"/>
         <v>0</v>
       </c>
       <c r="J289" s="38">
-        <f t="shared" ref="J289:J290" si="144">G289*B289-I289</f>
+        <f t="shared" ref="J289:J290" si="156">G289*B289-I289</f>
         <v>5</v>
       </c>
       <c r="K289" s="35">
-        <f t="shared" ref="K289:K290" si="145">B289*H289</f>
+        <f t="shared" ref="K289:K290" si="157">B289*H289</f>
         <v>10.25</v>
       </c>
       <c r="L289" t="s">
@@ -16303,15 +16303,15 @@
         <v>1.95</v>
       </c>
       <c r="I290" s="37">
-        <f>SUMIF(C$1:C$181,"="&amp;C290,B$1:B$181)</f>
+        <f t="shared" si="151"/>
         <v>0</v>
       </c>
       <c r="J290" s="38">
-        <f t="shared" si="144"/>
+        <f t="shared" si="156"/>
         <v>5</v>
       </c>
       <c r="K290" s="35">
-        <f t="shared" si="145"/>
+        <f t="shared" si="157"/>
         <v>9.75</v>
       </c>
       <c r="L290" t="s">

</xml_diff>

<commit_message>
Unterarm links neu gedruckt mit verbesserter Kabelführung
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2137,7 +2137,157 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="3"/>
@@ -2196,16 +2346,6 @@
     <dxf>
       <font>
         <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -3232,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD109"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -8935,7 +9075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9324,8 +9464,8 @@
   </sheetPr>
   <dimension ref="A1:O321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="B217" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L229" sqref="L229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9727,7 +9867,7 @@
       <c r="K19" s="78"/>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -10579,7 +10719,7 @@
       <c r="K61" s="78"/>
       <c r="L61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="62" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -11603,7 +11743,7 @@
       <c r="K110" s="78"/>
       <c r="L110" s="71" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="111" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -11763,7 +11903,7 @@
       <c r="K118" s="88"/>
       <c r="L118" s="81" t="str">
         <f ca="1">INDIRECT(ADDRESS(MATCH(C118,C$183:C$292,0)+ROW($B$183)-1,12))</f>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="119" spans="1:12" s="81" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -11786,7 +11926,7 @@
       <c r="K119" s="88"/>
       <c r="L119" s="81" t="str">
         <f ca="1">INDIRECT(ADDRESS(MATCH(C119,C$183:C$292,0)+ROW($B$183)-1,12))</f>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -12556,10 +12696,6 @@
       <c r="I157" s="37"/>
       <c r="J157" s="38"/>
       <c r="K157" s="35"/>
-      <c r="L157" t="e">
-        <f t="shared" ca="1" si="5"/>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="158" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
@@ -14332,7 +14468,7 @@
         <v>5.44</v>
       </c>
       <c r="L224" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="225" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14365,7 +14501,7 @@
         <v>0</v>
       </c>
       <c r="L225" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
     </row>
     <row r="226" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14398,7 +14534,7 @@
         <v>0</v>
       </c>
       <c r="L226" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
     </row>
     <row r="227" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14431,7 +14567,7 @@
         <v>0</v>
       </c>
       <c r="L227" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
     </row>
     <row r="228" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14836,7 +14972,7 @@
         <v>4</v>
       </c>
       <c r="L240" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="241" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14935,7 +15071,7 @@
         <v>4.96</v>
       </c>
       <c r="L243" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="244" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -14968,7 +15104,7 @@
         <v>0</v>
       </c>
       <c r="L244" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="245" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15001,7 +15137,7 @@
         <v>4.96</v>
       </c>
       <c r="L245" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="246" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -15034,7 +15170,7 @@
         <v>4.96</v>
       </c>
       <c r="L246" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
     </row>
     <row r="247" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16365,7 +16501,7 @@
       </c>
       <c r="L295" s="34">
         <f ca="1">SUMIF(L1:L293,"=-",K1:K293)</f>
-        <v>88.210000000000008</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="296" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -16481,71 +16617,79 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K17 B18:D19 F18:K19 B20:K60 B61:D61 F61:K61 B62:K109 B110:D110 F110:K110 B111:K115 B116:D119 F116:K119 L186 B183:K214 D215:K215 B216:D218 F216:K218 B274:K282 D292:K292 B292 B285:K291 C273 G273:K273 B247:K251 B253:K271 D252:K252 B252 B221:D221 F221:K221 B219:K220 F243:K244 B243:D244 B222:K242 B119:K180 B246:D246 F246:K246">
-    <cfRule type="expression" dxfId="14" priority="110">
+    <cfRule type="expression" dxfId="42" priority="112">
       <formula>$L2=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:XFD4 B18:K18 A2:L2 A3:K17 A19:K109 M5:XFD109 L3:L109 A215 D215:XFD215 A183:XFD214 A216:D218 A292:B292 D292:XFD292 C273 G273:L273 A274:XFD282 A285:XFD291 A253:XFD271 A252:B252 D252:XFD252 F216:XFD218 A247:XFD251 A221:D221 F221:XFD221 A219:XFD220 F243:XFD244 A243:D244 A222:XFD242 A110:XFD180 A246:D246 F246:XFD246">
-    <cfRule type="expression" dxfId="13" priority="111">
+  <conditionalFormatting sqref="N2:XFD4 B18:K18 A2:L2 A3:K17 A19:K109 M5:XFD109 L3:L109 A215 D215:XFD215 A183:XFD214 A216:D218 A292:B292 D292:XFD292 C273 G273:L273 A274:XFD282 A285:XFD291 A253:XFD271 A252:B252 D252:XFD252 F216:XFD218 A247:XFD251 A221:D221 F221:XFD221 A219:XFD220 A243:D244 A110:XFD180 A246:D246 F243:XFD244 F246:XFD246 A222:XFD242">
+    <cfRule type="expression" dxfId="11" priority="113">
       <formula>$L2=$O$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="112">
+    <cfRule type="expression" dxfId="10" priority="114">
       <formula>$L2=$O$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E218">
-    <cfRule type="expression" dxfId="11" priority="114">
+    <cfRule type="expression" dxfId="41" priority="116">
       <formula>$L215=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E218">
-    <cfRule type="expression" dxfId="10" priority="117">
+    <cfRule type="expression" dxfId="40" priority="119">
       <formula>$L215=$O$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="118">
+    <cfRule type="expression" dxfId="39" priority="120">
       <formula>$L215=$O$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E216:E217">
-    <cfRule type="expression" dxfId="8" priority="120">
+    <cfRule type="expression" dxfId="38" priority="122">
       <formula>$L214=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E216:E217">
-    <cfRule type="expression" dxfId="7" priority="123">
+    <cfRule type="expression" dxfId="37" priority="125">
       <formula>$L214=$O$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="124">
+    <cfRule type="expression" dxfId="36" priority="126">
       <formula>$L214=$O$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E243">
-    <cfRule type="expression" dxfId="5" priority="126">
+    <cfRule type="expression" dxfId="35" priority="128">
       <formula>$L252=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E243">
-    <cfRule type="expression" dxfId="4" priority="130">
+    <cfRule type="expression" dxfId="34" priority="132">
       <formula>$L252=$O$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="131">
+    <cfRule type="expression" dxfId="33" priority="133">
       <formula>$L252=$O$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B245:D245 F245:K245">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="32" priority="3">
       <formula>$L245=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A245:D245 F245:XFD245">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A245:D245 F245:K245 M245:XFD245">
+    <cfRule type="expression" dxfId="31" priority="4">
       <formula>$L245=$O$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>$L245=$O$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <conditionalFormatting sqref="L245">
+    <cfRule type="expression" dxfId="23" priority="1">
+      <formula>$L245=$O$3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="2">
+      <formula>$L245=$O$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L183:L214 L285:L290 L261:L270 L273:L282 L253:L259 L216:L251">
       <formula1>$O$1:$O$4</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Handgreifer etwas fetter und runder gemacht
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="7"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -9178,7 +9178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
@@ -9691,7 +9691,7 @@
   </sheetPr>
   <dimension ref="A1:O334"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ellbogen jetzt ohne Motorloch, weil 26Ncm Motor reicht und nach innen verschoben werden konnte
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2231,37 +2231,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
+  <dxfs count="69">
     <dxf>
       <font>
         <color theme="3"/>
@@ -2500,6 +2470,21 @@
     <dxf>
       <font>
         <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -3671,8 +3656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,7 +4057,7 @@
       </c>
       <c r="C36" s="4">
         <f>C40/C38*(C44/C42)</f>
-        <v>5.6000000000000005</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
@@ -4094,7 +4079,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
@@ -4106,7 +4091,7 @@
       </c>
       <c r="C39" s="4">
         <f>C38*C37/PI()</f>
-        <v>11.93662073189215</v>
+        <v>11.140846016432674</v>
       </c>
       <c r="D39" t="s">
         <v>31</v>
@@ -5629,15 +5614,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="68" priority="1">
       <formula>$L74=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="67" priority="2">
       <formula>$L74=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="66" priority="3">
       <formula>$L74=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5674,7 +5659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -17405,284 +17390,284 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B32:D33 F32:K33 B34:K38 B76:D76 F76:K76 B77:K124 B125:D125 F125:K125 B126:K130 B131:D134 F131:K134 L201 B198:K229 D230:K230 B231:D233 F231:K233 B294:K302 D312:K312 B312 B305:K311 C293 G293:K293 B262:K266 B236:D236 F236:K236 B234:K235 B237:K257 B134:K195 F258:K261 B258:D261 B4:K14 B26:K31 B269:K291 B267:D267 F267:K267 B40:K75">
-    <cfRule type="expression" dxfId="71" priority="167">
+    <cfRule type="expression" dxfId="65" priority="167">
       <formula>$L4=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:XFD6 B32:K32 A33:K38 M7:XFD13 A4:L13 A230 D230:XFD230 A198:XFD229 A231:D233 A312:B312 D312:XFD312 C293 G293:L293 A294:XFD302 A305:XFD311 F231:XFD233 A262:XFD266 A236:D236 F236:XFD236 A234:XFD235 A237:XFD257 A14:XFD14 A258:D261 F258:XFD261 A26:K31 L26:XFD38 A269:XFD291 A267:D267 F267:XFD267 A40:XFD195">
-    <cfRule type="expression" dxfId="70" priority="168">
+    <cfRule type="expression" dxfId="64" priority="168">
       <formula>$L4=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="169">
+    <cfRule type="expression" dxfId="63" priority="169">
       <formula>$L4=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E233">
-    <cfRule type="expression" dxfId="68" priority="171">
+    <cfRule type="expression" dxfId="62" priority="171">
       <formula>$L230=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E233">
-    <cfRule type="expression" dxfId="67" priority="174">
+    <cfRule type="expression" dxfId="61" priority="174">
       <formula>$L230=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="175">
+    <cfRule type="expression" dxfId="60" priority="175">
       <formula>$L230=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E231:E232">
-    <cfRule type="expression" dxfId="65" priority="177">
+    <cfRule type="expression" dxfId="59" priority="177">
       <formula>$L229=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E231:E232">
-    <cfRule type="expression" dxfId="64" priority="180">
+    <cfRule type="expression" dxfId="58" priority="180">
       <formula>$L229=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="181">
+    <cfRule type="expression" dxfId="57" priority="181">
       <formula>$L229=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E258">
-    <cfRule type="expression" dxfId="62" priority="183">
+    <cfRule type="expression" dxfId="56" priority="183">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E258">
-    <cfRule type="expression" dxfId="61" priority="187">
+    <cfRule type="expression" dxfId="55" priority="187">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="188">
+    <cfRule type="expression" dxfId="54" priority="188">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:K25">
-    <cfRule type="expression" dxfId="59" priority="50">
+    <cfRule type="expression" dxfId="53" priority="50">
       <formula>$L25=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:XFD25">
-    <cfRule type="expression" dxfId="58" priority="51">
+    <cfRule type="expression" dxfId="52" priority="51">
       <formula>$L25=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="52">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>$L25=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:K16">
-    <cfRule type="expression" dxfId="56" priority="47">
+    <cfRule type="expression" dxfId="50" priority="47">
       <formula>$L15=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule type="expression" dxfId="55" priority="48">
+    <cfRule type="expression" dxfId="49" priority="48">
       <formula>$L15=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="49">
+    <cfRule type="expression" dxfId="48" priority="49">
       <formula>$L15=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17 M17:XFD17">
-    <cfRule type="expression" dxfId="53" priority="45">
+    <cfRule type="expression" dxfId="47" priority="45">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="46">
+    <cfRule type="expression" dxfId="46" priority="46">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="expression" dxfId="51" priority="41">
+    <cfRule type="expression" dxfId="45" priority="41">
       <formula>$L17=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:L17">
-    <cfRule type="expression" dxfId="50" priority="42">
+    <cfRule type="expression" dxfId="44" priority="42">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="43">
+    <cfRule type="expression" dxfId="43" priority="43">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 M18:XFD18">
-    <cfRule type="expression" dxfId="48" priority="39">
+    <cfRule type="expression" dxfId="42" priority="39">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="40">
+    <cfRule type="expression" dxfId="41" priority="40">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18">
-    <cfRule type="expression" dxfId="46" priority="36">
+    <cfRule type="expression" dxfId="40" priority="36">
       <formula>$L18=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L18">
-    <cfRule type="expression" dxfId="45" priority="37">
+    <cfRule type="expression" dxfId="39" priority="37">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="38">
+    <cfRule type="expression" dxfId="38" priority="38">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21 M21:XFD21">
-    <cfRule type="expression" dxfId="43" priority="34">
+    <cfRule type="expression" dxfId="37" priority="34">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="35">
+    <cfRule type="expression" dxfId="36" priority="35">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21 E21:K21">
-    <cfRule type="expression" dxfId="41" priority="31">
+    <cfRule type="expression" dxfId="35" priority="31">
       <formula>$L21=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21 E21:L21">
-    <cfRule type="expression" dxfId="40" priority="32">
+    <cfRule type="expression" dxfId="34" priority="32">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="33" priority="33">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:K23">
-    <cfRule type="expression" dxfId="38" priority="28">
+    <cfRule type="expression" dxfId="32" priority="28">
       <formula>$L23=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:XFD23">
-    <cfRule type="expression" dxfId="37" priority="29">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>$L23=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="30">
+    <cfRule type="expression" dxfId="30" priority="30">
       <formula>$L23=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:K24">
-    <cfRule type="expression" dxfId="35" priority="25">
+    <cfRule type="expression" dxfId="29" priority="25">
       <formula>$L24=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:XFD24">
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>$L24=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="27" priority="27">
       <formula>$L24=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22 M22:XFD22">
-    <cfRule type="expression" dxfId="32" priority="23">
+    <cfRule type="expression" dxfId="26" priority="23">
       <formula>$L22=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="24">
+    <cfRule type="expression" dxfId="25" priority="24">
       <formula>$L22=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:K22">
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="24" priority="20">
       <formula>$L22=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:L22">
-    <cfRule type="expression" dxfId="29" priority="21">
+    <cfRule type="expression" dxfId="23" priority="21">
       <formula>$L22=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="22">
+    <cfRule type="expression" dxfId="22" priority="22">
       <formula>$L22=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="27" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>$L21=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="26" priority="18">
+    <cfRule type="expression" dxfId="20" priority="18">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="19" priority="19">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19 M19:XFD19">
-    <cfRule type="expression" dxfId="24" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>$L19=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>$L19=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:K19">
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>$L19=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:L19">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$L19=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>$L19=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 M20:XFD20">
-    <cfRule type="expression" dxfId="19" priority="10">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>$L20=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>$L20=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:K20">
-    <cfRule type="expression" dxfId="17" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>$L20=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:L20">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>$L20=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>$L20=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="expression" dxfId="14" priority="190">
+    <cfRule type="expression" dxfId="8" priority="190">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="expression" dxfId="13" priority="194">
+    <cfRule type="expression" dxfId="7" priority="194">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="195">
+    <cfRule type="expression" dxfId="6" priority="195">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B268:D268 F268:K268">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A268:D268 F268:XFD268">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:K39">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$L39=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:XFD39">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$L39=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$L39=$O$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
PCB bekommt die letzten 4 PINs als enhancement Stecker Handgelenk vom Rest des entfernbaren Motordecksl bereinigt
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -3656,8 +3656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="C36" s="4">
         <f>C40/C38*(C44/C42)</f>
-        <v>6</v>
+        <v>6.4166666666666661</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
@@ -4079,7 +4079,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="C39" s="4">
         <f>C38*C37/PI()</f>
-        <v>11.140846016432674</v>
+        <v>9.5492965855137211</v>
       </c>
       <c r="D39" t="s">
         <v>31</v>
@@ -4102,7 +4102,7 @@
         <v>33</v>
       </c>
       <c r="C40" s="7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
         <v>29</v>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="C41" s="4">
         <f>C40*C37/PI()</f>
-        <v>19.098593171027442</v>
+        <v>17.507043740108486</v>
       </c>
       <c r="D41" t="s">
         <v>31</v>
@@ -9417,7 +9417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9806,8 +9806,8 @@
   </sheetPr>
   <dimension ref="A1:O341"/>
   <sheetViews>
-    <sheetView topLeftCell="A255" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E268" sqref="E268"/>
+    <sheetView topLeftCell="A264" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17682,8 +17682,9 @@
     <hyperlink ref="E271" r:id="rId3"/>
     <hyperlink ref="E233" r:id="rId4"/>
     <hyperlink ref="E259" r:id="rId5"/>
+    <hyperlink ref="E269" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="34" orientation="landscape" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="34" orientation="landscape" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stepper geht jetzt wieder
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="7"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="BOM" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">BOM!$A$196:$K$315</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">BOM!$A$196:$K$316</definedName>
     <definedName name="Kaufstatus">BOM!$L:$L</definedName>
     <definedName name="ShoppingStatus">BOM!$L:$L</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="599">
   <si>
     <t>Material</t>
   </si>
@@ -1815,6 +1815,15 @@
   </si>
   <si>
     <t>NEMA 17 - 42x42x34 - 0,26Nm - 5mm Achse - 0.4A 12V</t>
+  </si>
+  <si>
+    <t>http://www.omc-stepperonline.com/nema-17-bipolar-stepper-12v-04a-40ncm567ozin-17hs150404s-p-14.html</t>
+  </si>
+  <si>
+    <t>NEMA 17 - 42x42x39 - 0,40Nm - 5mm Achse - 0,40A 12V</t>
+  </si>
+  <si>
+    <t>Ref Voltage PiBot [V]</t>
   </si>
 </sst>
 </file>
@@ -2006,7 +2015,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2224,6 +2233,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2231,7 +2243,27 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="89">
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="3"/>
@@ -2560,6 +2592,86 @@
     <dxf>
       <font>
         <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -3654,10 +3766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AD110"/>
+  <dimension ref="A3:AD111"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q70" sqref="Q70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3734,7 +3846,7 @@
       </c>
       <c r="C8">
         <f>N73+N74 +0.4</f>
-        <v>0.77</v>
+        <v>0.9</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -3746,7 +3858,7 @@
       </c>
       <c r="C9">
         <f>N74+0.1</f>
-        <v>0.25</v>
+        <v>0.38</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -4284,7 +4396,7 @@
       </c>
       <c r="C58" s="4">
         <f>((C3+C4+C5)*(C7+C8+C9)*(C55))/1000</f>
-        <v>8.7848550000000003</v>
+        <v>9.9326249999999998</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -4296,7 +4408,7 @@
       </c>
       <c r="C59" s="4">
         <f>((C3+C4+C5)*(C7+C8+C9)*(C54+C55))/1000</f>
-        <v>26.354564999999997</v>
+        <v>29.797875000000001</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -4308,7 +4420,7 @@
       </c>
       <c r="C60" s="2">
         <f>((C4+C5)*(C8+C9)*(C54+C55))/1000</f>
-        <v>7.5046499999999998</v>
+        <v>9.4176000000000002</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
@@ -4320,7 +4432,7 @@
       </c>
       <c r="C61" s="2">
         <f>((C5)*(C9+C6)*(C55))/1000</f>
-        <v>0.36787500000000001</v>
+        <v>0.43164000000000002</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -4332,7 +4444,7 @@
       </c>
       <c r="C62" s="2">
         <f>((C5)*(C9+C6)*(C55))/1000</f>
-        <v>0.36787500000000001</v>
+        <v>0.43164000000000002</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -4344,7 +4456,7 @@
       </c>
       <c r="C63" s="2">
         <f>C58/C10</f>
-        <v>1.171314</v>
+        <v>1.3243499999999999</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -4356,7 +4468,7 @@
       </c>
       <c r="C64" s="2">
         <f>C59/C16</f>
-        <v>2.7178145156249998</v>
+        <v>3.072905859375</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -4368,7 +4480,7 @@
       </c>
       <c r="C65" s="2">
         <f>C60/C26</f>
-        <v>0.75046499999999994</v>
+        <v>0.94176000000000004</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -4380,7 +4492,7 @@
       </c>
       <c r="C66" s="2">
         <f>C62/C46</f>
-        <v>7.8830357142857133E-2</v>
+        <v>9.2494285714285709E-2</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -4392,13 +4504,13 @@
       </c>
       <c r="C67" s="2">
         <f>C61/C46</f>
-        <v>7.8830357142857133E-2</v>
+        <v>9.2494285714285709E-2</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="E68" s="10" t="s">
         <v>43</v>
@@ -4430,6 +4542,9 @@
       </c>
       <c r="O68" s="10" t="s">
         <v>51</v>
+      </c>
+      <c r="Q68" s="104" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="69" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
@@ -4469,7 +4584,7 @@
       </c>
       <c r="C70" s="2">
         <f>C63*(1+C53)</f>
-        <v>1.5227082000000001</v>
+        <v>1.7216549999999999</v>
       </c>
       <c r="D70" t="s">
         <v>13</v>
@@ -4508,6 +4623,10 @@
         <f>K70/N70</f>
         <v>180</v>
       </c>
+      <c r="Q70" s="104">
+        <f t="shared" ref="Q70:Q73" si="0">0.6801*L70</f>
+        <v>1.90428</v>
+      </c>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -4515,7 +4634,7 @@
       </c>
       <c r="C71" s="2">
         <f>C64*(1+C53)</f>
-        <v>3.5331588703124996</v>
+        <v>3.9947776171875002</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -4551,8 +4670,12 @@
         <v>1.34</v>
       </c>
       <c r="O71" s="17">
-        <f t="shared" ref="O71:O74" si="0">K71/N71</f>
+        <f t="shared" ref="O71:O74" si="1">K71/N71</f>
         <v>231.34328358208953</v>
+      </c>
+      <c r="Q71" s="104">
+        <f t="shared" si="0"/>
+        <v>2.38035</v>
       </c>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.3">
@@ -4561,7 +4684,7 @@
       </c>
       <c r="C72" s="2">
         <f>C65*(1+C53)</f>
-        <v>0.97560449999999999</v>
+        <v>1.224288</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -4597,10 +4720,13 @@
         <v>0.77</v>
       </c>
       <c r="O72" s="18">
+        <f t="shared" si="1"/>
+        <v>155.84415584415584</v>
+      </c>
+      <c r="Q72" s="104">
         <f t="shared" si="0"/>
-        <v>155.84415584415584</v>
-      </c>
-      <c r="Q72" s="10"/>
+        <v>1.3602000000000001</v>
+      </c>
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
       <c r="X72" s="10"/>
@@ -4617,7 +4743,7 @@
       </c>
       <c r="C73" s="2">
         <f>C66*(1+C53)</f>
-        <v>0.10247946428571428</v>
+        <v>0.12024257142857142</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -4657,7 +4783,10 @@
         <v>118.18181818181819</v>
       </c>
       <c r="P73" s="11"/>
-      <c r="Q73" s="10"/>
+      <c r="Q73" s="104">
+        <f t="shared" si="0"/>
+        <v>0.27204</v>
+      </c>
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
       <c r="T73" s="10"/>
@@ -4678,47 +4807,50 @@
       </c>
       <c r="C74" s="2">
         <f>C67*(1+C53)</f>
-        <v>0.10247946428571428</v>
+        <v>0.12024257142857142</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="F74" s="28">
+      <c r="E74" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="104">
         <v>1.8</v>
       </c>
-      <c r="G74" s="28" t="s">
+      <c r="G74" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="H74" s="28" t="s">
+      <c r="H74" s="104" t="s">
         <v>109</v>
       </c>
-      <c r="I74" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="J74" s="28">
+      <c r="I74" s="104" t="s">
+        <v>116</v>
+      </c>
+      <c r="J74" s="104">
         <v>5</v>
       </c>
-      <c r="K74" s="28">
-        <v>20</v>
-      </c>
-      <c r="L74" s="28">
-        <v>1.2</v>
-      </c>
-      <c r="M74" s="28" t="s">
+      <c r="K74" s="104">
+        <v>40</v>
+      </c>
+      <c r="L74" s="104">
+        <v>0.4</v>
+      </c>
+      <c r="M74" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="N74" s="28">
-        <v>0.15</v>
+      <c r="N74" s="104">
+        <v>0.28000000000000003</v>
       </c>
       <c r="O74" s="18">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
+        <f t="shared" ref="O74" si="2">K74/N74</f>
+        <v>142.85714285714283</v>
       </c>
       <c r="P74" s="11"/>
-      <c r="Q74" s="14"/>
+      <c r="Q74" s="14">
+        <f>0.6801*L74</f>
+        <v>0.27204</v>
+      </c>
       <c r="R74" s="14"/>
       <c r="S74" s="14"/>
       <c r="T74" s="14"/>
@@ -4794,7 +4926,7 @@
         <v>1.34</v>
       </c>
       <c r="O76" s="17">
-        <f t="shared" ref="O76:O84" si="1">K76/N76</f>
+        <f t="shared" ref="O76:O84" si="3">K76/N76</f>
         <v>231.34328358208953</v>
       </c>
     </row>
@@ -4830,7 +4962,7 @@
         <v>0.77</v>
       </c>
       <c r="O77" s="18">
-        <f t="shared" ref="O77" si="2">K77/N77</f>
+        <f t="shared" ref="O77" si="4">K77/N77</f>
         <v>155.84415584415584</v>
       </c>
       <c r="P77" s="11"/>
@@ -4881,7 +5013,7 @@
         <v>0.77</v>
       </c>
       <c r="O78" s="18">
-        <f t="shared" ref="O78" si="3">K78/N78</f>
+        <f t="shared" ref="O78" si="5">K78/N78</f>
         <v>155.84415584415584</v>
       </c>
       <c r="P78" s="11"/>
@@ -4932,7 +5064,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="O79" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>176.9911504424779</v>
       </c>
       <c r="P79" s="10"/>
@@ -4973,7 +5105,7 @@
         <v>1</v>
       </c>
       <c r="O80" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>189</v>
       </c>
       <c r="P80" s="14"/>
@@ -5096,7 +5228,7 @@
         <v>0.45</v>
       </c>
       <c r="O83" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>144.44444444444443</v>
       </c>
     </row>
@@ -5132,7 +5264,7 @@
         <v>0.31</v>
       </c>
       <c r="O84" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>145.16129032258064</v>
       </c>
     </row>
@@ -5174,458 +5306,481 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E86" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" s="104">
+        <v>1.8</v>
+      </c>
+      <c r="G86" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="H86" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="I86" s="104" t="s">
+        <v>116</v>
+      </c>
+      <c r="J86" s="104">
+        <v>5</v>
+      </c>
+      <c r="K86" s="104">
+        <v>40</v>
+      </c>
+      <c r="L86" s="104">
+        <v>0.4</v>
+      </c>
+      <c r="M86" s="104" t="s">
+        <v>63</v>
+      </c>
+      <c r="N86" s="104">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O86" s="18">
+        <f t="shared" ref="O86" si="6">K86/N86</f>
+        <v>142.85714285714283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E87" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="F86" s="31">
+      <c r="F87" s="31">
         <v>1.8</v>
       </c>
-      <c r="G86" s="31" t="s">
+      <c r="G87" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H86" s="31" t="s">
+      <c r="H87" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="I86" s="31" t="s">
+      <c r="I87" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="J86" s="31">
+      <c r="J87" s="31">
         <v>5</v>
       </c>
-      <c r="K86" s="31">
+      <c r="K87" s="31">
         <v>26</v>
       </c>
-      <c r="L86" s="31">
+      <c r="L87" s="31">
         <v>0.4</v>
       </c>
-      <c r="M86" s="31" t="s">
+      <c r="M87" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="N86" s="31">
+      <c r="N87" s="31">
         <v>0.22</v>
       </c>
-      <c r="O86" s="18">
-        <f>K86/N86</f>
+      <c r="O87" s="18">
+        <f>K87/N87</f>
         <v>118.18181818181819</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E87" s="11" t="s">
+    <row r="88" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E88" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F87" s="27">
+      <c r="F88" s="27">
         <v>0.9</v>
       </c>
-      <c r="G87" s="27" t="s">
+      <c r="G88" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="H87" s="27" t="s">
+      <c r="H88" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="I87" s="27" t="s">
+      <c r="I88" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="K87" s="27">
+      <c r="K88" s="27">
         <v>23</v>
       </c>
-      <c r="L87" s="27">
+      <c r="L88" s="27">
         <v>0.31</v>
-      </c>
-      <c r="M87" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="N87" s="27">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="O87" s="18">
-        <f t="shared" ref="O87" si="4">K87/N87</f>
-        <v>82.142857142857139</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E88" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F88" s="27">
-        <v>1.8</v>
-      </c>
-      <c r="G88" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H88" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I88" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="J88" s="27">
-        <v>5</v>
-      </c>
-      <c r="K88" s="27">
-        <v>18</v>
-      </c>
-      <c r="L88" s="27">
-        <v>0.8</v>
       </c>
       <c r="M88" s="27" t="s">
         <v>63</v>
       </c>
       <c r="N88" s="27">
-        <v>0.17</v>
-      </c>
-      <c r="O88" s="17">
-        <f>K88/N88</f>
-        <v>105.88235294117646</v>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O88" s="18">
+        <f t="shared" ref="O88" si="7">K88/N88</f>
+        <v>82.142857142857139</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E89" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F89" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="G89" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F89" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="G89" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H89" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="I89" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="J89" s="16">
+      <c r="H89" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I89" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J89" s="27">
         <v>5</v>
       </c>
-      <c r="K89" s="16">
-        <v>16</v>
-      </c>
-      <c r="L89" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="M89" s="16" t="s">
+      <c r="K89" s="27">
+        <v>18</v>
+      </c>
+      <c r="L89" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="M89" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="N89" s="16">
-        <v>0.12</v>
+      <c r="N89" s="27">
+        <v>0.17</v>
       </c>
       <c r="O89" s="17">
         <f>K89/N89</f>
-        <v>133.33333333333334</v>
+        <v>105.88235294117646</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E90" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F90" s="27">
-        <v>1.8</v>
-      </c>
-      <c r="G90" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F90" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="G90" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H90" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I90" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="J90" s="27">
+      <c r="H90" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I90" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="J90" s="16">
         <v>5</v>
       </c>
-      <c r="K90" s="27">
-        <v>14</v>
-      </c>
-      <c r="L90" s="27">
-        <v>0.4</v>
-      </c>
-      <c r="M90" s="27" t="s">
+      <c r="K90" s="16">
+        <v>16</v>
+      </c>
+      <c r="L90" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="M90" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N90" s="27">
+      <c r="N90" s="16">
         <v>0.12</v>
       </c>
-      <c r="O90" s="18">
-        <f t="shared" ref="O90" si="5">K90/N90</f>
-        <v>116.66666666666667</v>
+      <c r="O90" s="17">
+        <f>K90/N90</f>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E91" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F91" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="G91" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F91" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="G91" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H91" s="16" t="s">
+      <c r="H91" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I91" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="J91" s="16">
+      <c r="I91" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="J91" s="27">
         <v>5</v>
       </c>
-      <c r="K91" s="16">
-        <v>5</v>
-      </c>
-      <c r="L91" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="M91" s="16" t="s">
+      <c r="K91" s="27">
+        <v>14</v>
+      </c>
+      <c r="L91" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="M91" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="N91" s="16">
-        <v>0.09</v>
-      </c>
-      <c r="O91" s="17">
-        <f>K91/N91</f>
-        <v>55.555555555555557</v>
+      <c r="N91" s="27">
+        <v>0.12</v>
+      </c>
+      <c r="O91" s="18">
+        <f t="shared" ref="O91" si="8">K91/N91</f>
+        <v>116.66666666666667</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E92" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F92" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="G92" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H92" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J92" s="16">
+        <v>5</v>
+      </c>
+      <c r="K92" s="16">
+        <v>5</v>
+      </c>
+      <c r="L92" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="M92" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="N92" s="16">
+        <v>0.09</v>
+      </c>
+      <c r="O92" s="17">
+        <f>K92/N92</f>
+        <v>55.555555555555557</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E93" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F92" s="28">
+      <c r="F93" s="28">
         <v>0.9</v>
       </c>
-      <c r="G92" s="28" t="s">
+      <c r="G93" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H92" s="28" t="s">
+      <c r="H93" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="I92" s="28" t="s">
+      <c r="I93" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="J92" s="28">
+      <c r="J93" s="28">
         <v>5</v>
       </c>
-      <c r="K92" s="28">
+      <c r="K93" s="28">
         <v>11</v>
       </c>
-      <c r="L92" s="28">
+      <c r="L93" s="28">
         <v>1.2</v>
       </c>
-      <c r="M92" s="28" t="s">
+      <c r="M93" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="N92" s="28">
+      <c r="N93" s="28">
         <v>0.15</v>
       </c>
-      <c r="O92" s="18">
-        <f t="shared" ref="O92" si="6">K92/N92</f>
+      <c r="O93" s="18">
+        <f t="shared" ref="O93" si="9">K93/N93</f>
         <v>73.333333333333343</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D93" s="11"/>
-      <c r="E93" s="11" t="s">
+    <row r="94" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D94" s="11"/>
+      <c r="E94" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="F93" s="90">
+      <c r="F94" s="90">
         <v>1.8</v>
       </c>
-      <c r="G93" s="90" t="s">
+      <c r="G94" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="H93" s="90" t="s">
+      <c r="H94" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="I93" s="90" t="s">
+      <c r="I94" s="90" t="s">
         <v>593</v>
       </c>
-      <c r="J93" s="90">
+      <c r="J94" s="90">
         <v>5</v>
       </c>
-      <c r="K93" s="90">
+      <c r="K94" s="90">
         <v>20</v>
       </c>
-      <c r="L93" s="90">
+      <c r="L94" s="90">
         <v>0.35</v>
       </c>
-      <c r="M93" s="90" t="s">
+      <c r="M94" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="N93" s="90"/>
-      <c r="O93" s="18"/>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>249</v>
-      </c>
+      <c r="N94" s="90"/>
+      <c r="O94" s="18"/>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>252</v>
-      </c>
-      <c r="C95" s="19">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>252</v>
+      </c>
+      <c r="C96" s="19">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>257</v>
       </c>
-      <c r="C96" s="19">
+      <c r="C97" s="19">
         <f>(C15/1000/2)</f>
         <v>7.1619724391352904E-2</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>253</v>
-      </c>
-      <c r="C97" s="19">
-        <f>C58/C96</f>
-        <v>122.65971524822916</v>
-      </c>
-      <c r="D97" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>253</v>
+      </c>
+      <c r="C98" s="19">
+        <f>C58/C97</f>
+        <v>138.68560769272142</v>
+      </c>
+      <c r="D98" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>254</v>
       </c>
-      <c r="C98" s="19">
-        <f>(C95)*C97*2*PI()</f>
-        <v>770.69372063050537</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C99" s="19">
+        <f>(C96)*C98*2*PI()</f>
+        <v>871.3873725721794</v>
+      </c>
+      <c r="D99" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>252</v>
-      </c>
-      <c r="C101" s="20">
-        <v>1</v>
-      </c>
-      <c r="D101" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>252</v>
+      </c>
+      <c r="C102" s="20">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>257</v>
       </c>
-      <c r="C102" s="20">
+      <c r="C103" s="20">
         <f>(C21/1000/2)</f>
         <v>3.8197186342054885E-2</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>253</v>
-      </c>
-      <c r="C103" s="20">
-        <f>C59/C102</f>
-        <v>689.9608982712889</v>
-      </c>
-      <c r="D103" t="s">
-        <v>250</v>
-      </c>
-      <c r="E103" s="20"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>253</v>
+      </c>
+      <c r="C104" s="20">
+        <f>C59/C103</f>
+        <v>780.10654327155794</v>
+      </c>
+      <c r="D104" t="s">
+        <v>250</v>
+      </c>
+      <c r="E104" s="20"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>254</v>
       </c>
-      <c r="C104" s="20">
-        <f>(C101)*C103*2*PI()</f>
-        <v>4335.1521785465911</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C105" s="20">
+        <f>(C102)*C104*2*PI()</f>
+        <v>4901.5539707185089</v>
+      </c>
+      <c r="D105" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>252</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C108" s="20">
         <f>60*C18/C20</f>
         <v>27.5</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>257</v>
       </c>
-      <c r="C108" s="20">
+      <c r="C109" s="20">
         <f>(C25/1000/2)</f>
         <v>6.3661977236758135E-2</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>253</v>
-      </c>
-      <c r="C109" s="20">
-        <f>C59/(C20/C18)/C108</f>
-        <v>189.73924702460448</v>
-      </c>
-      <c r="D109" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="20">
+        <f>C59/(C20/C18)/C109</f>
+        <v>214.52929939967848</v>
+      </c>
+      <c r="D110" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>254</v>
       </c>
-      <c r="C110" s="20">
-        <f>(C107/60)*C109*2*PI()</f>
-        <v>546.40980583764338</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C111" s="20">
+        <f>(C108/60)*C110*2*PI()</f>
+        <v>617.80003172597878</v>
+      </c>
+      <c r="D111" t="s">
         <v>251</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="68" priority="1">
-      <formula>$L74=$O$6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="67" priority="2">
-      <formula>$L74=$O$5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="3">
-      <formula>$L74=$O$4</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E83" r:id="rId1" display="http://www.omc-stepperonline.com/nema-17-bipolar-stepper-motor-65ncm92ozin-21a-17hs242104s-p-21.html"/>
     <hyperlink ref="E84" r:id="rId2" display="http://www.omc-stepperonline.com/3d-printer-nema-17-stepper-motor-2a-45ncm64ozin-17hs162004s-p-16.html"/>
@@ -5633,25 +5788,27 @@
     <hyperlink ref="E70" r:id="rId4"/>
     <hyperlink ref="E76" r:id="rId5"/>
     <hyperlink ref="E80" r:id="rId6" display="http://www.omc-stepperonline.com/nema-23-cnc-stepper-motor-28a-19nm269ozin-23hs302804s-p-25.html"/>
-    <hyperlink ref="E89" r:id="rId7" display="http://www.omc-stepperonline.com/09-nema-16-bipolar-stepper-06a-16ncm227ozin-16hm100604s-p-97.html"/>
-    <hyperlink ref="E91" r:id="rId8" display="http://www.omc-stepperonline.com/09-nema-14-bipolar-stepper-motor-5ncm7ozin-14hm080504s-p-85.html"/>
+    <hyperlink ref="E90" r:id="rId7" display="http://www.omc-stepperonline.com/09-nema-16-bipolar-stepper-06a-16ncm227ozin-16hm100604s-p-97.html"/>
+    <hyperlink ref="E92" r:id="rId8" display="http://www.omc-stepperonline.com/09-nema-14-bipolar-stepper-motor-5ncm7ozin-14hm080504s-p-85.html"/>
     <hyperlink ref="E71" r:id="rId9"/>
     <hyperlink ref="E82" r:id="rId10"/>
     <hyperlink ref="E81" r:id="rId11"/>
     <hyperlink ref="E85" r:id="rId12"/>
-    <hyperlink ref="E88" r:id="rId13" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-54v-08a-18ncm255ozin-14hs130804s-p-93.html"/>
-    <hyperlink ref="E90" r:id="rId14" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-12v-04a-14ncm20ozin-14hs100404s-p-90.html"/>
-    <hyperlink ref="E87" r:id="rId15" display="http://www.omc-stepperonline.com/9deg-nema-17-unipolar-stepper-motor-12v-031a-16ncm227ozin-17hm130316s-p-262.html"/>
-    <hyperlink ref="E86" r:id="rId16"/>
+    <hyperlink ref="E89" r:id="rId13" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-54v-08a-18ncm255ozin-14hs130804s-p-93.html"/>
+    <hyperlink ref="E91" r:id="rId14" display="http://www.omc-stepperonline.com/nema-14-bipolar-stepper-12v-04a-14ncm20ozin-14hs100404s-p-90.html"/>
+    <hyperlink ref="E88" r:id="rId15" display="http://www.omc-stepperonline.com/9deg-nema-17-unipolar-stepper-motor-12v-031a-16ncm227ozin-17hm130316s-p-262.html"/>
+    <hyperlink ref="E87" r:id="rId16"/>
     <hyperlink ref="E73" r:id="rId17"/>
     <hyperlink ref="E78" r:id="rId18" display="http://www.omc-stepperonline.com/nema-24-cnc-stepper-motor-12nm170ozin-24hs222006s-p-26.html"/>
     <hyperlink ref="E77" r:id="rId19" display="http://www.omc-stepperonline.com/nema-24-cnc-stepper-motor-12nm170ozin-24hs222006s-p-26.html"/>
     <hyperlink ref="E72" r:id="rId20" display="http://www.omc-stepperonline.com/nema-24-cnc-stepper-motor-12nm170ozin-24hs222006s-p-26.html"/>
-    <hyperlink ref="E92" r:id="rId21" display="http://www.omc-stepperonline.com/09-nema-17-bipolar-stepper-12a-11ncm156ozin-17hm081204s-p-99.html"/>
-    <hyperlink ref="E93" r:id="rId22"/>
+    <hyperlink ref="E93" r:id="rId21" display="http://www.omc-stepperonline.com/09-nema-17-bipolar-stepper-12a-11ncm156ozin-17hm081204s-p-99.html"/>
+    <hyperlink ref="E94" r:id="rId22"/>
+    <hyperlink ref="E86" r:id="rId23" display="http://www.omc-stepperonline.com/nema-17-bipolar-stepper-12v-04a-40ncm567ozin-17hs150404s-p-14.html"/>
+    <hyperlink ref="E74" r:id="rId24" display="http://www.omc-stepperonline.com/nema-17-bipolar-stepper-12v-04a-40ncm567ozin-17hs150404s-p-14.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -5849,8 +6006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="J57" sqref="A57:J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5870,8 +6027,8 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -5887,10 +6044,10 @@
       <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="104" t="s">
+      <c r="D4" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="104"/>
+      <c r="E4" s="105"/>
       <c r="F4" s="10" t="s">
         <v>47</v>
       </c>
@@ -9417,7 +9574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9804,10 +9961,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O341"/>
+  <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView topLeftCell="A264" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C273" sqref="C273"/>
+    <sheetView topLeftCell="A258" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E269" sqref="E269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9906,7 +10063,7 @@
       <c r="J5" s="38"/>
       <c r="K5" s="35"/>
       <c r="L5" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C5,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C5,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
       <c r="O5" t="s">
@@ -9930,7 +10087,7 @@
       <c r="J6" s="38"/>
       <c r="K6" s="35"/>
       <c r="L6" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C6,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C6,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
       <c r="O6" t="s">
@@ -9954,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="32" t="str">
-        <f>C287</f>
+        <f>C288</f>
         <v>Rillenkugellager DIN 625 SKF - 61807 35x47x7mm</v>
       </c>
       <c r="D8" t="s">
@@ -9966,7 +10123,7 @@
       <c r="J8" s="38"/>
       <c r="K8" s="35"/>
       <c r="L8" t="str">
-        <f t="shared" ref="L8:L14" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C8,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L8:L14" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C8,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -10038,7 +10195,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="32" t="str">
-        <f>C286</f>
+        <f>C287</f>
         <v>Rillenkugellager DIN 625 SKF - 61902 15x28x7mm</v>
       </c>
       <c r="D12" t="s">
@@ -10059,7 +10216,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="32" t="str">
-        <f>C275</f>
+        <f>C276</f>
         <v xml:space="preserve">Herkulex Servo DRS - 0101 </v>
       </c>
       <c r="D13" t="s">
@@ -10080,7 +10237,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="32" t="str">
-        <f>C279</f>
+        <f>C280</f>
         <v>Rillenkugellager 3x10x4</v>
       </c>
       <c r="D14" t="s">
@@ -10122,7 +10279,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="100" t="str">
-        <f>C277</f>
+        <f>C278</f>
         <v>Rillenkugellager 3x7x3</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -10134,7 +10291,7 @@
       <c r="J17" s="103"/>
       <c r="K17" s="35"/>
       <c r="L17" s="8" t="str">
-        <f t="shared" ref="L17:L24" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C17,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L17:L24" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C17,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Bestellt</v>
       </c>
     </row>
@@ -10143,7 +10300,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="100" t="str">
-        <f>C277</f>
+        <f>C278</f>
         <v>Rillenkugellager 3x7x3</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -10164,7 +10321,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="65" t="str">
-        <f>C280</f>
+        <f>C281</f>
         <v>Rillenkugellager 3x6x2,5</v>
       </c>
       <c r="D19" s="63" t="s">
@@ -10185,7 +10342,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="65" t="str">
-        <f>C280</f>
+        <f>C281</f>
         <v>Rillenkugellager 3x6x2,5</v>
       </c>
       <c r="D20" s="63" t="s">
@@ -10269,7 +10426,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="32" t="str">
-        <f>C275</f>
+        <f>C276</f>
         <v xml:space="preserve">Herkulex Servo DRS - 0101 </v>
       </c>
       <c r="D24" t="s">
@@ -10323,7 +10480,7 @@
       <c r="J27" s="69"/>
       <c r="K27" s="70"/>
       <c r="L27" t="str">
-        <f t="shared" ref="L27:L28" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C27,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L27:L28" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C27,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -10365,7 +10522,7 @@
       <c r="J29" s="61"/>
       <c r="K29" s="62"/>
       <c r="L29" t="str">
-        <f t="shared" ref="L29:L58" ca="1" si="3">INDIRECT(ADDRESS(MATCH(C29,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L29:L58" ca="1" si="3">INDIRECT(ADDRESS(MATCH(C29,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -10483,7 +10640,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="32" t="str">
-        <f>C296</f>
+        <f>C297</f>
         <v>Metallbohrer 6mm</v>
       </c>
       <c r="D35" t="s">
@@ -10504,7 +10661,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="32" t="str">
-        <f>C298</f>
+        <f>C299</f>
         <v>Metallbohrer 2.5mm (als M3 Kernlochborer)</v>
       </c>
       <c r="D36" t="s">
@@ -10525,7 +10682,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="32" t="str">
-        <f>C294</f>
+        <f>C295</f>
         <v>Gewindeschneider M3</v>
       </c>
       <c r="D37" t="s">
@@ -10546,7 +10703,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="32" t="str">
-        <f>C284</f>
+        <f>C285</f>
         <v>Rillenkugellager 6x10x3</v>
       </c>
       <c r="D38" t="s">
@@ -10580,7 +10737,7 @@
       <c r="K39" s="78"/>
       <c r="L39" s="71" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>-</v>
+        <v>Habs</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -10588,7 +10745,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="32" t="str">
-        <f>C269</f>
+        <f>C270</f>
         <v>NEMA 17 - 42x42x21 - 0,13Nm - 5mm Achse - 1.2A</v>
       </c>
       <c r="D40" t="s">
@@ -10714,7 +10871,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="32" t="str">
-        <f>C279</f>
+        <f>C280</f>
         <v>Rillenkugellager 3x10x4</v>
       </c>
       <c r="D46" t="s">
@@ -10777,7 +10934,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="32" t="str">
-        <f>C274</f>
+        <f>C275</f>
         <v>Rotary Sensor</v>
       </c>
       <c r="D49" t="s">
@@ -11017,7 +11174,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="32" t="str">
-        <f>C287</f>
+        <f>C288</f>
         <v>Rillenkugellager DIN 625 SKF - 61807 35x47x7mm</v>
       </c>
       <c r="D62" t="s">
@@ -11029,7 +11186,7 @@
       <c r="J62" s="38"/>
       <c r="K62" s="35"/>
       <c r="L62" t="str">
-        <f t="shared" ref="L62:L82" ca="1" si="4">INDIRECT(ADDRESS(MATCH(C62,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L62:L82" ca="1" si="4">INDIRECT(ADDRESS(MATCH(C62,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -11038,7 +11195,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="32" t="str">
-        <f>C285</f>
+        <f>C286</f>
         <v>RillenKugellager 6x19x6</v>
       </c>
       <c r="D63" t="s">
@@ -11059,7 +11216,7 @@
         <v>4</v>
       </c>
       <c r="C64" s="32" t="str">
-        <f>C279</f>
+        <f>C280</f>
         <v>Rillenkugellager 3x10x4</v>
       </c>
       <c r="D64" t="s">
@@ -11123,7 +11280,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="32" t="str">
-        <f>C296</f>
+        <f>C297</f>
         <v>Metallbohrer 6mm</v>
       </c>
       <c r="D67" t="s">
@@ -11144,7 +11301,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="32" t="str">
-        <f>C294</f>
+        <f>C295</f>
         <v>Gewindeschneider M3</v>
       </c>
       <c r="D68" t="s">
@@ -11165,7 +11322,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="32" t="str">
-        <f>C298</f>
+        <f>C299</f>
         <v>Metallbohrer 2.5mm (als M3 Kernlochborer)</v>
       </c>
       <c r="D69" t="s">
@@ -11270,7 +11427,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="32" t="str">
-        <f>C270</f>
+        <f>C271</f>
         <v>NEMA 17 - 42x42x34 - 0,26Nm - 5mm Achse - 0.4A 12V</v>
       </c>
       <c r="D74" t="s">
@@ -11291,7 +11448,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="32" t="str">
-        <f>C274</f>
+        <f>C275</f>
         <v>Rotary Sensor</v>
       </c>
       <c r="D75" t="s">
@@ -11487,7 +11644,7 @@
       <c r="J84" s="38"/>
       <c r="K84" s="35"/>
       <c r="L84" t="str">
-        <f t="shared" ref="L84:L131" ca="1" si="5">INDIRECT(ADDRESS(MATCH(C84,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L84:L131" ca="1" si="5">INDIRECT(ADDRESS(MATCH(C84,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -11517,7 +11674,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="32" t="str">
-        <f>C274</f>
+        <f>C275</f>
         <v>Rotary Sensor</v>
       </c>
       <c r="D86" t="s">
@@ -11559,7 +11716,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="32" t="str">
-        <f>C287</f>
+        <f>C288</f>
         <v>Rillenkugellager DIN 625 SKF - 61807 35x47x7mm</v>
       </c>
       <c r="D88" t="s">
@@ -11727,7 +11884,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="32" t="str">
-        <f>C282</f>
+        <f>C283</f>
         <v>Rillenkugellager  4 x13 x 5 mm mit Flansch</v>
       </c>
       <c r="D96" t="s">
@@ -11874,7 +12031,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="32" t="str">
-        <f>C295</f>
+        <f>C296</f>
         <v>Metallbohrer 8mm</v>
       </c>
       <c r="D103" t="s">
@@ -11895,7 +12052,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="32" t="str">
-        <f>C294</f>
+        <f>C295</f>
         <v>Gewindeschneider M3</v>
       </c>
       <c r="D104" t="s">
@@ -11916,7 +12073,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="32" t="str">
-        <f>C298</f>
+        <f>C299</f>
         <v>Metallbohrer 2.5mm (als M3 Kernlochborer)</v>
       </c>
       <c r="D105" t="s">
@@ -11958,7 +12115,7 @@
         <v>2</v>
       </c>
       <c r="C107" s="32" t="str">
-        <f>C288</f>
+        <f>C289</f>
         <v>Rillenkugellager 8x22x7</v>
       </c>
       <c r="D107" t="s">
@@ -12126,7 +12283,7 @@
         <v>2</v>
       </c>
       <c r="C115" s="32" t="str">
-        <f>C283</f>
+        <f>C284</f>
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D115" t="s">
@@ -12510,7 +12667,7 @@
       <c r="J133" s="87"/>
       <c r="K133" s="88"/>
       <c r="L133" s="81" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C133,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C133,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12533,7 +12690,7 @@
       <c r="J134" s="87"/>
       <c r="K134" s="88"/>
       <c r="L134" s="81" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C134,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C134,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12542,7 +12699,7 @@
         <v>1</v>
       </c>
       <c r="C135" s="32" t="str">
-        <f>C271</f>
+        <f>C272</f>
         <v xml:space="preserve">NEMA 24 - 60x60x57 - 1.9Nm - 6,35mm Achse - 2.8A - 2.ST6018M2008 </v>
       </c>
       <c r="D135" t="s">
@@ -12554,7 +12711,7 @@
       <c r="J135" s="38"/>
       <c r="K135" s="35"/>
       <c r="L135" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C135,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C135,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12596,7 +12753,7 @@
       <c r="J138" s="38"/>
       <c r="K138" s="35"/>
       <c r="L138" t="str">
-        <f t="shared" ref="L138:L150" ca="1" si="6">INDIRECT(ADDRESS(MATCH(C138,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L138:L150" ca="1" si="6">INDIRECT(ADDRESS(MATCH(C138,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12626,7 +12783,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="32" t="str">
-        <f>C274</f>
+        <f>C275</f>
         <v>Rotary Sensor</v>
       </c>
       <c r="D140" t="s">
@@ -12668,7 +12825,7 @@
         <v>6</v>
       </c>
       <c r="C142" s="32" t="str">
-        <f>C283</f>
+        <f>C284</f>
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D142" t="s">
@@ -12857,7 +13014,7 @@
         <v>2</v>
       </c>
       <c r="C151" s="32" t="str">
-        <f>C288</f>
+        <f>C289</f>
         <v>Rillenkugellager 8x22x7</v>
       </c>
       <c r="D151" t="s">
@@ -12869,7 +13026,7 @@
       <c r="J151" s="38"/>
       <c r="K151" s="35"/>
       <c r="L151" t="str">
-        <f t="shared" ref="L151:L190" ca="1" si="7">INDIRECT(ADDRESS(MATCH(C151,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L151:L190" ca="1" si="7">INDIRECT(ADDRESS(MATCH(C151,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -12955,7 +13112,7 @@
       <c r="J155" s="77"/>
       <c r="K155" s="78"/>
       <c r="L155" s="71" t="str">
-        <f t="shared" ref="L155" ca="1" si="8">INDIRECT(ADDRESS(MATCH(C155,C$198:C$312,0)+ROW($B$198)-1,12))</f>
+        <f t="shared" ref="L155" ca="1" si="8">INDIRECT(ADDRESS(MATCH(C155,C$198:C$313,0)+ROW($B$198)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -13259,7 +13416,7 @@
         <v>1</v>
       </c>
       <c r="C170" s="32" t="str">
-        <f>C272</f>
+        <f>C273</f>
         <v>NEMA 24 - 60x60x87 - 3.1Nm - 8mm Achse - 4.2A</v>
       </c>
       <c r="D170" t="s">
@@ -13280,7 +13437,7 @@
         <v>2</v>
       </c>
       <c r="C171" s="32" t="str">
-        <f>C289</f>
+        <f>C290</f>
         <v>Rillenkugellager DIN 625 SKF - SKF 61818 - 90x115x13</v>
       </c>
       <c r="D171" t="s">
@@ -13313,7 +13470,7 @@
         <v>1</v>
       </c>
       <c r="C173" s="32" t="str">
-        <f>C290</f>
+        <f>C291</f>
         <v>Rillenkugellager DIN 625 SKF - SKF 61818 - 85x110x13</v>
       </c>
       <c r="D173" t="s">
@@ -13439,7 +13596,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="32" t="str">
-        <f>C274</f>
+        <f>C275</f>
         <v>Rotary Sensor</v>
       </c>
       <c r="D179" t="s">
@@ -13565,7 +13722,7 @@
         <v>6</v>
       </c>
       <c r="C185" s="32" t="str">
-        <f>C283</f>
+        <f>C284</f>
         <v xml:space="preserve">Rillenkugellager  4 x13 x 5 mm </v>
       </c>
       <c r="D185" t="s">
@@ -13649,7 +13806,7 @@
         <v>1</v>
       </c>
       <c r="C189" s="32" t="str">
-        <f>C273</f>
+        <f>C274</f>
         <v>NEMA 23 - 57x57x56 - 1,26Nm - 6,35mm Achse - 2.8A</v>
       </c>
       <c r="D189" t="s">
@@ -13955,7 +14112,7 @@
         <v>46</v>
       </c>
       <c r="K203" s="35">
-        <f t="shared" ref="K203:K287" si="17">B203*H203</f>
+        <f t="shared" ref="K203:K288" si="17">B203*H203</f>
         <v>2.5</v>
       </c>
       <c r="L203" t="s">
@@ -14161,7 +14318,7 @@
         <v>9</v>
       </c>
       <c r="J210" s="38">
-        <f t="shared" ref="J210:J284" si="27">G210*B210-I210</f>
+        <f t="shared" ref="J210:J285" si="27">G210*B210-I210</f>
         <v>91</v>
       </c>
       <c r="K210" s="35">
@@ -14949,7 +15106,7 @@
     </row>
     <row r="236" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="33">
-        <f t="shared" ref="B236:B290" si="63">ROUNDUP(I236/G236,0)</f>
+        <f t="shared" ref="B236:B291" si="63">ROUNDUP(I236/G236,0)</f>
         <v>1</v>
       </c>
       <c r="C236" s="32" t="s">
@@ -15972,7 +16129,7 @@
         <v>14.5</v>
       </c>
       <c r="I268" s="37">
-        <f t="shared" ref="I268:I275" si="113">SUMIF(C$1:C$196,"="&amp;C268,B$1:B$196)</f>
+        <f t="shared" ref="I268:I276" si="113">SUMIF(C$1:C$196,"="&amp;C268,B$1:B$196)</f>
         <v>1</v>
       </c>
       <c r="J268" s="38">
@@ -15984,19 +16141,19 @@
         <v>14.5</v>
       </c>
       <c r="L268" t="s">
-        <v>424</v>
+        <v>483</v>
       </c>
     </row>
     <row r="269" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B269" s="33">
-        <f t="shared" si="63"/>
-        <v>1</v>
+        <f t="shared" ref="B269" si="116">ROUNDUP(I269/G269,0)</f>
+        <v>0</v>
       </c>
       <c r="C269" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="E269" s="9" t="s">
-        <v>575</v>
+        <v>597</v>
+      </c>
+      <c r="E269" t="s">
+        <v>596</v>
       </c>
       <c r="G269">
         <v>1</v>
@@ -16005,16 +16162,16 @@
         <v>14.5</v>
       </c>
       <c r="I269" s="37">
-        <f t="shared" si="113"/>
-        <v>1</v>
+        <f t="shared" ref="I269" si="117">SUMIF(C$1:C$196,"="&amp;C269,B$1:B$196)</f>
+        <v>0</v>
       </c>
       <c r="J269" s="38">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="J269" si="118">G269*B269-I269</f>
         <v>0</v>
       </c>
       <c r="K269" s="35">
-        <f t="shared" si="17"/>
-        <v>14.5</v>
+        <f t="shared" ref="K269" si="119">B269*H269</f>
+        <v>0</v>
       </c>
       <c r="L269" t="s">
         <v>483</v>
@@ -16026,28 +16183,28 @@
         <v>1</v>
       </c>
       <c r="C270" s="32" t="s">
-        <v>595</v>
+        <v>576</v>
       </c>
       <c r="E270" s="9" t="s">
-        <v>466</v>
+        <v>575</v>
       </c>
       <c r="G270">
         <v>1</v>
       </c>
       <c r="H270" s="22">
-        <v>8.5</v>
+        <v>14.5</v>
       </c>
       <c r="I270" s="37">
         <f t="shared" si="113"/>
         <v>1</v>
       </c>
       <c r="J270" s="38">
-        <f t="shared" ref="J270" si="116">G270*B270-I270</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K270" s="35">
-        <f t="shared" ref="K270" si="117">B270*H270</f>
-        <v>8.5</v>
+        <f t="shared" si="17"/>
+        <v>14.5</v>
       </c>
       <c r="L270" t="s">
         <v>483</v>
@@ -16059,28 +16216,28 @@
         <v>1</v>
       </c>
       <c r="C271" s="32" t="s">
-        <v>442</v>
+        <v>595</v>
       </c>
       <c r="E271" s="9" t="s">
-        <v>364</v>
+        <v>466</v>
       </c>
       <c r="G271">
         <v>1</v>
       </c>
       <c r="H271" s="22">
-        <v>54.2</v>
+        <v>8.5</v>
       </c>
       <c r="I271" s="37">
         <f t="shared" si="113"/>
         <v>1</v>
       </c>
       <c r="J271" s="38">
-        <f t="shared" ref="J271" si="118">G271*B271-I271</f>
+        <f t="shared" ref="J271" si="120">G271*B271-I271</f>
         <v>0</v>
       </c>
       <c r="K271" s="35">
-        <f t="shared" ref="K271" si="119">B271*H271</f>
-        <v>54.2</v>
+        <f t="shared" ref="K271" si="121">B271*H271</f>
+        <v>8.5</v>
       </c>
       <c r="L271" t="s">
         <v>483</v>
@@ -16092,28 +16249,28 @@
         <v>1</v>
       </c>
       <c r="C272" s="32" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E272" s="9" t="s">
-        <v>467</v>
+        <v>364</v>
       </c>
       <c r="G272">
         <v>1</v>
       </c>
       <c r="H272" s="22">
-        <v>37</v>
+        <v>54.2</v>
       </c>
       <c r="I272" s="37">
         <f t="shared" si="113"/>
         <v>1</v>
       </c>
       <c r="J272" s="38">
-        <f t="shared" ref="J272" si="120">G272*B272-I272</f>
+        <f t="shared" ref="J272" si="122">G272*B272-I272</f>
         <v>0</v>
       </c>
       <c r="K272" s="35">
-        <f t="shared" ref="K272" si="121">B272*H272</f>
-        <v>37</v>
+        <f t="shared" ref="K272" si="123">B272*H272</f>
+        <v>54.2</v>
       </c>
       <c r="L272" t="s">
         <v>483</v>
@@ -16125,28 +16282,28 @@
         <v>1</v>
       </c>
       <c r="C273" s="32" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="E273" s="9" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="G273">
         <v>1</v>
       </c>
       <c r="H273" s="22">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="I273" s="37">
         <f t="shared" si="113"/>
         <v>1</v>
       </c>
       <c r="J273" s="38">
-        <f t="shared" ref="J273" si="122">G273*B273-I273</f>
+        <f t="shared" ref="J273" si="124">G273*B273-I273</f>
         <v>0</v>
       </c>
       <c r="K273" s="35">
-        <f t="shared" ref="K273" si="123">B273*H273</f>
-        <v>18</v>
+        <f t="shared" ref="K273" si="125">B273*H273</f>
+        <v>37</v>
       </c>
       <c r="L273" t="s">
         <v>483</v>
@@ -16155,31 +16312,31 @@
     <row r="274" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B274" s="33">
         <f t="shared" si="63"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C274" s="32" t="s">
-        <v>298</v>
+        <v>462</v>
       </c>
       <c r="E274" s="9" t="s">
-        <v>235</v>
+        <v>465</v>
       </c>
       <c r="G274">
         <v>1</v>
       </c>
       <c r="H274" s="22">
-        <v>14.53</v>
+        <v>18</v>
       </c>
       <c r="I274" s="37">
         <f t="shared" si="113"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J274" s="38">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="J274" si="126">G274*B274-I274</f>
         <v>0</v>
       </c>
       <c r="K274" s="35">
-        <f t="shared" si="17"/>
-        <v>72.649999999999991</v>
+        <f t="shared" ref="K274" si="127">B274*H274</f>
+        <v>18</v>
       </c>
       <c r="L274" t="s">
         <v>483</v>
@@ -16188,88 +16345,88 @@
     <row r="275" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B275" s="33">
         <f t="shared" si="63"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C275" s="32" t="s">
-        <v>587</v>
+        <v>298</v>
       </c>
       <c r="E275" s="9" t="s">
-        <v>371</v>
+        <v>235</v>
       </c>
       <c r="G275">
         <v>1</v>
       </c>
       <c r="H275" s="22">
-        <v>36.42</v>
+        <v>14.53</v>
       </c>
       <c r="I275" s="37">
         <f t="shared" si="113"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J275" s="38">
-        <f t="shared" ref="J275" si="124">G275*B275-I275</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K275" s="35">
-        <f t="shared" ref="K275" si="125">B275*H275</f>
-        <v>72.84</v>
+        <f t="shared" si="17"/>
+        <v>72.649999999999991</v>
       </c>
       <c r="L275" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="276" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B276" s="33"/>
-      <c r="C276" s="32"/>
-      <c r="E276" s="9"/>
-      <c r="H276" s="22"/>
-      <c r="I276" s="37"/>
-      <c r="J276" s="38"/>
-      <c r="K276" s="35"/>
+      <c r="B276" s="33">
+        <f t="shared" si="63"/>
+        <v>2</v>
+      </c>
+      <c r="C276" s="32" t="s">
+        <v>587</v>
+      </c>
+      <c r="E276" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="G276">
+        <v>1</v>
+      </c>
+      <c r="H276" s="22">
+        <v>36.42</v>
+      </c>
+      <c r="I276" s="37">
+        <f t="shared" si="113"/>
+        <v>2</v>
+      </c>
+      <c r="J276" s="38">
+        <f t="shared" ref="J276" si="128">G276*B276-I276</f>
+        <v>0</v>
+      </c>
+      <c r="K276" s="35">
+        <f t="shared" ref="K276" si="129">B276*H276</f>
+        <v>72.84</v>
+      </c>
+      <c r="L276" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="277" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B277" s="33">
-        <f>ROUNDUP(I277/G277,0)</f>
-        <v>16</v>
-      </c>
-      <c r="C277" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="E277" s="9" t="s">
-        <v>586</v>
-      </c>
-      <c r="G277">
-        <v>1</v>
-      </c>
-      <c r="H277" s="22">
-        <v>1.35</v>
-      </c>
-      <c r="I277" s="37">
-        <f t="shared" ref="I277:I290" si="126">SUMIF(C$1:C$196,"="&amp;C277,B$1:B$196)</f>
-        <v>16</v>
-      </c>
-      <c r="J277" s="38">
-        <f t="shared" ref="J277" si="127">G277*B277-I277</f>
-        <v>0</v>
-      </c>
-      <c r="K277" s="35">
-        <f>B277*H277</f>
-        <v>21.6</v>
-      </c>
-      <c r="L277" t="s">
-        <v>484</v>
-      </c>
+      <c r="B277" s="33"/>
+      <c r="C277" s="32"/>
+      <c r="E277" s="9"/>
+      <c r="H277" s="22"/>
+      <c r="I277" s="37"/>
+      <c r="J277" s="38"/>
+      <c r="K277" s="35"/>
     </row>
     <row r="278" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B278" s="33">
         <f>ROUNDUP(I278/G278,0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C278" s="32" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E278" s="9" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="G278">
         <v>1</v>
@@ -16278,16 +16435,16 @@
         <v>1.35</v>
       </c>
       <c r="I278" s="37">
-        <f t="shared" si="126"/>
-        <v>0</v>
+        <f t="shared" ref="I278:I291" si="130">SUMIF(C$1:C$196,"="&amp;C278,B$1:B$196)</f>
+        <v>16</v>
       </c>
       <c r="J278" s="38">
-        <f t="shared" ref="J278" si="128">G278*B278-I278</f>
+        <f t="shared" ref="J278" si="131">G278*B278-I278</f>
         <v>0</v>
       </c>
       <c r="K278" s="35">
         <f>B278*H278</f>
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="L278" t="s">
         <v>484</v>
@@ -16296,64 +16453,64 @@
     <row r="279" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B279" s="33">
         <f>ROUNDUP(I279/G279,0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C279" s="32" t="s">
-        <v>319</v>
+        <v>590</v>
       </c>
       <c r="E279" s="9" t="s">
-        <v>318</v>
+        <v>589</v>
       </c>
       <c r="G279">
         <v>1</v>
       </c>
       <c r="H279" s="22">
-        <v>1.05</v>
+        <v>1.35</v>
       </c>
       <c r="I279" s="37">
-        <f t="shared" si="126"/>
-        <v>7</v>
+        <f t="shared" si="130"/>
+        <v>0</v>
       </c>
       <c r="J279" s="38">
-        <f t="shared" ref="J279" si="129">G279*B279-I279</f>
+        <f t="shared" ref="J279" si="132">G279*B279-I279</f>
         <v>0</v>
       </c>
       <c r="K279" s="35">
         <f>B279*H279</f>
-        <v>7.3500000000000005</v>
+        <v>0</v>
       </c>
       <c r="L279" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="280" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B280" s="33">
         <f>ROUNDUP(I280/G280,0)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C280" s="32" t="s">
-        <v>582</v>
+        <v>319</v>
       </c>
       <c r="E280" s="9" t="s">
-        <v>581</v>
+        <v>318</v>
       </c>
       <c r="G280">
         <v>1</v>
       </c>
       <c r="H280" s="22">
-        <v>1.35</v>
+        <v>1.05</v>
       </c>
       <c r="I280" s="37">
-        <f t="shared" si="126"/>
-        <v>16</v>
+        <f t="shared" si="130"/>
+        <v>7</v>
       </c>
       <c r="J280" s="38">
-        <f t="shared" ref="J280" si="130">G280*B280-I280</f>
+        <f t="shared" ref="J280" si="133">G280*B280-I280</f>
         <v>0</v>
       </c>
       <c r="K280" s="35">
         <f>B280*H280</f>
-        <v>21.6</v>
+        <v>7.3500000000000005</v>
       </c>
       <c r="L280" t="s">
         <v>483</v>
@@ -16362,79 +16519,79 @@
     <row r="281" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B281" s="33">
         <f>ROUNDUP(I281/G281,0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C281" s="32" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="E281" s="9" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="G281">
         <v>1</v>
       </c>
       <c r="H281" s="22">
-        <v>2.19</v>
+        <v>1.35</v>
       </c>
       <c r="I281" s="37">
-        <f t="shared" si="126"/>
-        <v>0</v>
+        <f t="shared" si="130"/>
+        <v>16</v>
       </c>
       <c r="J281" s="38">
-        <f t="shared" ref="J281" si="131">G281*B281-I281</f>
+        <f t="shared" ref="J281" si="134">G281*B281-I281</f>
         <v>0</v>
       </c>
       <c r="K281" s="35">
         <f>B281*H281</f>
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="L281" t="s">
-        <v>424</v>
+        <v>483</v>
       </c>
     </row>
     <row r="282" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B282" s="33">
-        <f t="shared" si="63"/>
-        <v>8</v>
+        <f>ROUNDUP(I282/G282,0)</f>
+        <v>0</v>
       </c>
       <c r="C282" s="32" t="s">
-        <v>361</v>
+        <v>578</v>
       </c>
       <c r="E282" s="9" t="s">
-        <v>372</v>
+        <v>577</v>
       </c>
       <c r="G282">
         <v>1</v>
       </c>
       <c r="H282" s="22">
-        <v>1.54</v>
+        <v>2.19</v>
       </c>
       <c r="I282" s="37">
-        <f t="shared" si="126"/>
-        <v>8</v>
+        <f t="shared" si="130"/>
+        <v>0</v>
       </c>
       <c r="J282" s="38">
-        <f t="shared" ref="J282" si="132">G282*B282-I282</f>
+        <f t="shared" ref="J282" si="135">G282*B282-I282</f>
         <v>0</v>
       </c>
       <c r="K282" s="35">
-        <f t="shared" ref="K282" si="133">B282*H282</f>
-        <v>12.32</v>
+        <f>B282*H282</f>
+        <v>0</v>
       </c>
       <c r="L282" t="s">
-        <v>483</v>
+        <v>424</v>
       </c>
     </row>
     <row r="283" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B283" s="33">
         <f t="shared" si="63"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C283" s="32" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="E283" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G283">
         <v>1</v>
@@ -16443,16 +16600,16 @@
         <v>1.54</v>
       </c>
       <c r="I283" s="37">
-        <f t="shared" si="126"/>
-        <v>14</v>
+        <f t="shared" si="130"/>
+        <v>8</v>
       </c>
       <c r="J283" s="38">
-        <f t="shared" ref="J283" si="134">G283*B283-I283</f>
+        <f t="shared" ref="J283" si="136">G283*B283-I283</f>
         <v>0</v>
       </c>
       <c r="K283" s="35">
-        <f t="shared" ref="K283" si="135">B283*H283</f>
-        <v>21.560000000000002</v>
+        <f t="shared" ref="K283" si="137">B283*H283</f>
+        <v>12.32</v>
       </c>
       <c r="L283" t="s">
         <v>483</v>
@@ -16461,97 +16618,97 @@
     <row r="284" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B284" s="33">
         <f t="shared" si="63"/>
+        <v>14</v>
+      </c>
+      <c r="C284" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="E284" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G284">
+        <v>1</v>
+      </c>
+      <c r="H284" s="22">
+        <v>1.54</v>
+      </c>
+      <c r="I284" s="37">
+        <f t="shared" si="130"/>
+        <v>14</v>
+      </c>
+      <c r="J284" s="38">
+        <f t="shared" ref="J284" si="138">G284*B284-I284</f>
+        <v>0</v>
+      </c>
+      <c r="K284" s="35">
+        <f t="shared" ref="K284" si="139">B284*H284</f>
+        <v>21.560000000000002</v>
+      </c>
+      <c r="L284" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="285" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B285" s="33">
+        <f t="shared" si="63"/>
         <v>2</v>
       </c>
-      <c r="C284" s="32" t="s">
+      <c r="C285" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="E284" s="9" t="s">
+      <c r="E285" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G284">
-        <v>1</v>
-      </c>
-      <c r="H284" s="22">
+      <c r="G285">
+        <v>1</v>
+      </c>
+      <c r="H285" s="22">
         <v>1.95</v>
       </c>
-      <c r="I284" s="37">
-        <f t="shared" si="126"/>
+      <c r="I285" s="37">
+        <f t="shared" si="130"/>
         <v>2</v>
       </c>
-      <c r="J284" s="38">
+      <c r="J285" s="38">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="K284" s="35">
+      <c r="K285" s="35">
         <f t="shared" si="17"/>
         <v>3.9</v>
       </c>
-      <c r="L284" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="285" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B285" s="33">
-        <f>ROUNDUP(I285/G285,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C285" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="E285" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="G285">
-        <v>1</v>
-      </c>
-      <c r="H285" s="22">
-        <v>1</v>
-      </c>
-      <c r="I285" s="37">
-        <f t="shared" si="126"/>
-        <v>2</v>
-      </c>
-      <c r="J285" s="38">
-        <f t="shared" ref="J285" si="136">G285*B285-I285</f>
-        <v>0</v>
-      </c>
-      <c r="K285" s="35">
-        <f>B285*H285</f>
-        <v>2</v>
-      </c>
       <c r="L285" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="286" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B286" s="33">
-        <f t="shared" si="63"/>
+        <f>ROUNDUP(I286/G286,0)</f>
         <v>2</v>
       </c>
       <c r="C286" s="32" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="E286" s="9" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="G286">
         <v>1</v>
       </c>
       <c r="H286" s="22">
-        <v>1.39</v>
+        <v>1</v>
       </c>
       <c r="I286" s="37">
-        <f t="shared" si="126"/>
+        <f t="shared" si="130"/>
         <v>2</v>
       </c>
       <c r="J286" s="38">
-        <f t="shared" ref="J286" si="137">G286*B286-I286</f>
+        <f t="shared" ref="J286" si="140">G286*B286-I286</f>
         <v>0</v>
       </c>
       <c r="K286" s="35">
-        <f t="shared" si="17"/>
-        <v>2.78</v>
+        <f>B286*H286</f>
+        <v>2</v>
       </c>
       <c r="L286" t="s">
         <v>483</v>
@@ -16560,31 +16717,31 @@
     <row r="287" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B287" s="33">
         <f t="shared" si="63"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C287" s="32" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="E287" s="9" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
       <c r="G287">
         <v>1</v>
       </c>
       <c r="H287" s="22">
-        <v>3.29</v>
+        <v>1.39</v>
       </c>
       <c r="I287" s="37">
-        <f t="shared" si="126"/>
-        <v>5</v>
+        <f t="shared" si="130"/>
+        <v>2</v>
       </c>
       <c r="J287" s="38">
-        <f t="shared" ref="J287" si="138">G287*B287-I287</f>
+        <f t="shared" ref="J287" si="141">G287*B287-I287</f>
         <v>0</v>
       </c>
       <c r="K287" s="35">
         <f t="shared" si="17"/>
-        <v>16.45</v>
+        <v>2.78</v>
       </c>
       <c r="L287" t="s">
         <v>483</v>
@@ -16593,31 +16750,31 @@
     <row r="288" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B288" s="33">
         <f t="shared" si="63"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C288" s="32" t="s">
-        <v>390</v>
+        <v>272</v>
       </c>
       <c r="E288" s="9" t="s">
-        <v>391</v>
+        <v>233</v>
       </c>
       <c r="G288">
         <v>1</v>
       </c>
       <c r="H288" s="22">
-        <v>1</v>
+        <v>3.29</v>
       </c>
       <c r="I288" s="37">
-        <f t="shared" si="126"/>
-        <v>4</v>
+        <f t="shared" si="130"/>
+        <v>5</v>
       </c>
       <c r="J288" s="38">
-        <f t="shared" ref="J288" si="139">G288*B288-I288</f>
+        <f t="shared" ref="J288" si="142">G288*B288-I288</f>
         <v>0</v>
       </c>
       <c r="K288" s="35">
-        <f t="shared" ref="K288" si="140">B288*H288</f>
-        <v>4</v>
+        <f t="shared" si="17"/>
+        <v>16.45</v>
       </c>
       <c r="L288" t="s">
         <v>483</v>
@@ -16626,31 +16783,31 @@
     <row r="289" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B289" s="33">
         <f t="shared" si="63"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C289" s="32" t="s">
-        <v>266</v>
+        <v>390</v>
       </c>
       <c r="E289" s="9" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="G289">
         <v>1</v>
       </c>
       <c r="H289" s="22">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I289" s="37">
-        <f t="shared" si="126"/>
-        <v>2</v>
+        <f t="shared" si="130"/>
+        <v>4</v>
       </c>
       <c r="J289" s="38">
-        <f t="shared" ref="J289" si="141">G289*B289-I289</f>
+        <f t="shared" ref="J289" si="143">G289*B289-I289</f>
         <v>0</v>
       </c>
       <c r="K289" s="35">
-        <f t="shared" ref="K289" si="142">B289*H289</f>
-        <v>40</v>
+        <f t="shared" ref="K289" si="144">B289*H289</f>
+        <v>4</v>
       </c>
       <c r="L289" t="s">
         <v>483</v>
@@ -16659,98 +16816,99 @@
     <row r="290" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B290" s="33">
         <f t="shared" si="63"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C290" s="32" t="s">
-        <v>401</v>
+        <v>266</v>
       </c>
       <c r="E290" s="9" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="G290">
         <v>1</v>
       </c>
       <c r="H290" s="22">
-        <v>18.079999999999998</v>
+        <v>20</v>
       </c>
       <c r="I290" s="37">
-        <f t="shared" si="126"/>
-        <v>1</v>
+        <f t="shared" si="130"/>
+        <v>2</v>
       </c>
       <c r="J290" s="38">
-        <f t="shared" ref="J290" si="143">G290*B290-I290</f>
+        <f t="shared" ref="J290" si="145">G290*B290-I290</f>
         <v>0</v>
       </c>
       <c r="K290" s="35">
-        <f t="shared" ref="K290" si="144">B290*H290</f>
-        <v>18.079999999999998</v>
+        <f t="shared" ref="K290" si="146">B290*H290</f>
+        <v>40</v>
       </c>
       <c r="L290" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="291" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B291" s="33"/>
-      <c r="C291" s="32"/>
-      <c r="E291" s="9"/>
-      <c r="H291" s="22"/>
-      <c r="I291" s="37"/>
-      <c r="J291" s="38"/>
-      <c r="K291" s="35"/>
+      <c r="B291" s="33">
+        <f t="shared" si="63"/>
+        <v>1</v>
+      </c>
+      <c r="C291" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="E291" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="G291">
+        <v>1</v>
+      </c>
+      <c r="H291" s="22">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="I291" s="37">
+        <f t="shared" si="130"/>
+        <v>1</v>
+      </c>
+      <c r="J291" s="38">
+        <f t="shared" ref="J291" si="147">G291*B291-I291</f>
+        <v>0</v>
+      </c>
+      <c r="K291" s="35">
+        <f t="shared" ref="K291" si="148">B291*H291</f>
+        <v>18.079999999999998</v>
+      </c>
+      <c r="L291" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="292" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="6" t="s">
-        <v>352</v>
-      </c>
       <c r="B292" s="33"/>
-      <c r="E292"/>
+      <c r="C292" s="32"/>
+      <c r="E292" s="9"/>
       <c r="H292" s="22"/>
       <c r="I292" s="37"/>
       <c r="J292" s="38"/>
       <c r="K292" s="35"/>
     </row>
     <row r="293" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A293" s="6"/>
-      <c r="B293" s="33">
-        <v>1</v>
-      </c>
-      <c r="C293" s="32" t="s">
+      <c r="A293" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B293" s="33"/>
+      <c r="E293"/>
+      <c r="H293" s="22"/>
+      <c r="I293" s="37"/>
+      <c r="J293" s="38"/>
+      <c r="K293" s="35"/>
+    </row>
+    <row r="294" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="6"/>
+      <c r="B294" s="33">
+        <v>1</v>
+      </c>
+      <c r="C294" s="32" t="s">
         <v>469</v>
       </c>
-      <c r="E293" t="s">
+      <c r="E294" t="s">
         <v>468</v>
-      </c>
-      <c r="G293">
-        <v>1</v>
-      </c>
-      <c r="H293" s="22">
-        <v>10.99</v>
-      </c>
-      <c r="I293" s="37">
-        <f t="shared" ref="I293:I302" si="145">SUMIF(C$1:C$196,"="&amp;C293,B$1:B$196)</f>
-        <v>0</v>
-      </c>
-      <c r="J293" s="38">
-        <f t="shared" ref="J293" si="146">G293*B293-I293</f>
-        <v>1</v>
-      </c>
-      <c r="K293" s="35">
-        <f t="shared" ref="K293" si="147">B293*H293</f>
-        <v>10.99</v>
-      </c>
-      <c r="L293" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="294" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B294" s="33">
-        <v>1</v>
-      </c>
-      <c r="C294" s="32" t="s">
-        <v>344</v>
-      </c>
-      <c r="E294" s="9" t="s">
-        <v>450</v>
       </c>
       <c r="G294">
         <v>1</v>
@@ -16759,15 +16917,15 @@
         <v>10.99</v>
       </c>
       <c r="I294" s="37">
-        <f t="shared" si="145"/>
-        <v>3</v>
+        <f t="shared" ref="I294:I303" si="149">SUMIF(C$1:C$196,"="&amp;C294,B$1:B$196)</f>
+        <v>0</v>
       </c>
       <c r="J294" s="38">
-        <f t="shared" ref="J294:J295" si="148">G294*B294-I294</f>
-        <v>-2</v>
+        <f t="shared" ref="J294" si="150">G294*B294-I294</f>
+        <v>1</v>
       </c>
       <c r="K294" s="35">
-        <f t="shared" ref="K294:K295" si="149">B294*H294</f>
+        <f t="shared" ref="K294" si="151">B294*H294</f>
         <v>10.99</v>
       </c>
       <c r="L294" t="s">
@@ -16779,28 +16937,28 @@
         <v>1</v>
       </c>
       <c r="C295" s="32" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E295" s="9" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G295">
         <v>1</v>
       </c>
       <c r="H295" s="22">
-        <v>2.8</v>
+        <v>10.99</v>
       </c>
       <c r="I295" s="37">
-        <f t="shared" si="145"/>
-        <v>1</v>
+        <f t="shared" si="149"/>
+        <v>3</v>
       </c>
       <c r="J295" s="38">
-        <f t="shared" si="148"/>
-        <v>0</v>
+        <f t="shared" ref="J295:J296" si="152">G295*B295-I295</f>
+        <v>-2</v>
       </c>
       <c r="K295" s="35">
-        <f t="shared" si="149"/>
-        <v>2.8</v>
+        <f t="shared" ref="K295:K296" si="153">B295*H295</f>
+        <v>10.99</v>
       </c>
       <c r="L295" t="s">
         <v>483</v>
@@ -16811,10 +16969,10 @@
         <v>1</v>
       </c>
       <c r="C296" s="32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E296" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G296">
         <v>1</v>
@@ -16823,15 +16981,15 @@
         <v>2.8</v>
       </c>
       <c r="I296" s="37">
-        <f t="shared" si="145"/>
-        <v>2</v>
+        <f t="shared" si="149"/>
+        <v>1</v>
       </c>
       <c r="J296" s="38">
-        <f t="shared" ref="J296" si="150">G296*B296-I296</f>
-        <v>-1</v>
+        <f t="shared" si="152"/>
+        <v>0</v>
       </c>
       <c r="K296" s="35">
-        <f t="shared" ref="K296" si="151">B296*H296</f>
+        <f t="shared" si="153"/>
         <v>2.8</v>
       </c>
       <c r="L296" t="s">
@@ -16843,10 +17001,10 @@
         <v>1</v>
       </c>
       <c r="C297" s="32" t="s">
-        <v>452</v>
+        <v>351</v>
       </c>
       <c r="E297" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G297">
         <v>1</v>
@@ -16855,15 +17013,15 @@
         <v>2.8</v>
       </c>
       <c r="I297" s="37">
-        <f t="shared" si="145"/>
-        <v>0</v>
+        <f t="shared" si="149"/>
+        <v>2</v>
       </c>
       <c r="J297" s="38">
-        <f>G297*B297-I297</f>
-        <v>1</v>
+        <f t="shared" ref="J297" si="154">G297*B297-I297</f>
+        <v>-1</v>
       </c>
       <c r="K297" s="35">
-        <f>B297*H297</f>
+        <f t="shared" ref="K297" si="155">B297*H297</f>
         <v>2.8</v>
       </c>
       <c r="L297" t="s">
@@ -16875,10 +17033,10 @@
         <v>1</v>
       </c>
       <c r="C298" s="32" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E298" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G298">
         <v>1</v>
@@ -16887,15 +17045,15 @@
         <v>2.8</v>
       </c>
       <c r="I298" s="37">
-        <f t="shared" si="145"/>
-        <v>3</v>
+        <f t="shared" si="149"/>
+        <v>0</v>
       </c>
       <c r="J298" s="38">
-        <f t="shared" ref="J298" si="152">G298*B298-I298</f>
-        <v>-2</v>
+        <f>G298*B298-I298</f>
+        <v>1</v>
       </c>
       <c r="K298" s="35">
-        <f t="shared" ref="K298" si="153">B298*H298</f>
+        <f>B298*H298</f>
         <v>2.8</v>
       </c>
       <c r="L298" t="s">
@@ -16907,28 +17065,28 @@
         <v>1</v>
       </c>
       <c r="C299" s="32" t="s">
-        <v>231</v>
+        <v>451</v>
       </c>
       <c r="E299" s="9" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
       <c r="G299">
         <v>1</v>
       </c>
       <c r="H299" s="22">
-        <v>1839</v>
+        <v>2.8</v>
       </c>
       <c r="I299" s="37">
-        <f t="shared" si="145"/>
-        <v>0</v>
+        <f t="shared" si="149"/>
+        <v>3</v>
       </c>
       <c r="J299" s="38">
-        <f t="shared" ref="J299" si="154">G299*B299-I299</f>
-        <v>1</v>
+        <f t="shared" ref="J299" si="156">G299*B299-I299</f>
+        <v>-2</v>
       </c>
       <c r="K299" s="35">
-        <f t="shared" ref="K299" si="155">B299*H299</f>
-        <v>1839</v>
+        <f t="shared" ref="K299" si="157">B299*H299</f>
+        <v>2.8</v>
       </c>
       <c r="L299" t="s">
         <v>483</v>
@@ -16939,28 +17097,28 @@
         <v>1</v>
       </c>
       <c r="C300" s="32" t="s">
-        <v>422</v>
+        <v>231</v>
       </c>
       <c r="E300" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G300">
         <v>1</v>
       </c>
       <c r="H300" s="22">
-        <v>31.5</v>
+        <v>1839</v>
       </c>
       <c r="I300" s="37">
-        <f t="shared" si="145"/>
+        <f t="shared" si="149"/>
         <v>0</v>
       </c>
       <c r="J300" s="38">
-        <f t="shared" ref="J300" si="156">G300*B300-I300</f>
+        <f t="shared" ref="J300" si="158">G300*B300-I300</f>
         <v>1</v>
       </c>
       <c r="K300" s="35">
-        <f t="shared" ref="K300" si="157">B300*H300</f>
-        <v>31.5</v>
+        <f t="shared" ref="K300" si="159">B300*H300</f>
+        <v>1839</v>
       </c>
       <c r="L300" t="s">
         <v>483</v>
@@ -16971,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="C301" s="32" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E301" s="9" t="s">
         <v>423</v>
@@ -16980,19 +17138,19 @@
         <v>1</v>
       </c>
       <c r="H301" s="22">
-        <v>49</v>
+        <v>31.5</v>
       </c>
       <c r="I301" s="37">
-        <f t="shared" si="145"/>
+        <f t="shared" si="149"/>
         <v>0</v>
       </c>
       <c r="J301" s="38">
-        <f t="shared" ref="J301" si="158">G301*B301-I301</f>
+        <f t="shared" ref="J301" si="160">G301*B301-I301</f>
         <v>1</v>
       </c>
       <c r="K301" s="35">
-        <f t="shared" ref="K301" si="159">B301*H301</f>
-        <v>49</v>
+        <f t="shared" ref="K301" si="161">B301*H301</f>
+        <v>31.5</v>
       </c>
       <c r="L301" t="s">
         <v>483</v>
@@ -17003,372 +17161,400 @@
         <v>1</v>
       </c>
       <c r="C302" s="32" t="s">
-        <v>457</v>
+        <v>430</v>
       </c>
       <c r="E302" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="H302" s="22"/>
+        <v>423</v>
+      </c>
+      <c r="G302">
+        <v>1</v>
+      </c>
+      <c r="H302" s="22">
+        <v>49</v>
+      </c>
       <c r="I302" s="37">
-        <f t="shared" si="145"/>
+        <f t="shared" si="149"/>
         <v>0</v>
       </c>
-      <c r="J302" s="38"/>
-      <c r="K302" s="35"/>
+      <c r="J302" s="38">
+        <f t="shared" ref="J302" si="162">G302*B302-I302</f>
+        <v>1</v>
+      </c>
+      <c r="K302" s="35">
+        <f t="shared" ref="K302" si="163">B302*H302</f>
+        <v>49</v>
+      </c>
       <c r="L302" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="303" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B303" s="33"/>
+      <c r="B303" s="33">
+        <v>1</v>
+      </c>
+      <c r="C303" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="E303" s="9" t="s">
+        <v>458</v>
+      </c>
       <c r="H303" s="22"/>
-      <c r="I303" s="37"/>
+      <c r="I303" s="37">
+        <f t="shared" si="149"/>
+        <v>0</v>
+      </c>
       <c r="J303" s="38"/>
       <c r="K303" s="35"/>
+      <c r="L303" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="304" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="6" t="s">
-        <v>419</v>
-      </c>
+      <c r="B304" s="33"/>
       <c r="H304" s="22"/>
       <c r="I304" s="37"/>
       <c r="J304" s="38"/>
       <c r="K304" s="35"/>
     </row>
-    <row r="305" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B305" s="33">
-        <v>1</v>
-      </c>
-      <c r="C305" s="32" t="s">
+    <row r="305" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="H305" s="22"/>
+      <c r="I305" s="37"/>
+      <c r="J305" s="38"/>
+      <c r="K305" s="35"/>
+    </row>
+    <row r="306" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B306" s="33">
+        <v>1</v>
+      </c>
+      <c r="C306" s="32" t="s">
         <v>420</v>
       </c>
-      <c r="E305" s="9" t="s">
+      <c r="E306" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="G305">
-        <v>1</v>
-      </c>
-      <c r="H305" s="22">
+      <c r="G306">
+        <v>1</v>
+      </c>
+      <c r="H306" s="22">
         <v>0.87</v>
       </c>
-      <c r="I305" s="37">
-        <f t="shared" ref="I305:I310" si="160">SUMIF(C$1:C$196,"="&amp;C305,B$1:B$196)</f>
+      <c r="I306" s="37">
+        <f t="shared" ref="I306:I311" si="164">SUMIF(C$1:C$196,"="&amp;C306,B$1:B$196)</f>
         <v>0</v>
       </c>
-      <c r="J305" s="38">
-        <f t="shared" ref="J305:J306" si="161">G305*B305-I305</f>
-        <v>1</v>
-      </c>
-      <c r="K305" s="35">
-        <f t="shared" ref="K305:K306" si="162">B305*H305</f>
+      <c r="J306" s="38">
+        <f t="shared" ref="J306:J307" si="165">G306*B306-I306</f>
+        <v>1</v>
+      </c>
+      <c r="K306" s="35">
+        <f t="shared" ref="K306:K307" si="166">B306*H306</f>
         <v>0.87</v>
-      </c>
-      <c r="L305" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="306" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B306" s="33">
-        <v>1</v>
-      </c>
-      <c r="C306" s="32" t="s">
-        <v>425</v>
-      </c>
-      <c r="E306" s="9" t="s">
-        <v>459</v>
-      </c>
-      <c r="G306">
-        <v>1</v>
-      </c>
-      <c r="H306" s="22">
-        <v>0.8</v>
-      </c>
-      <c r="I306" s="37">
-        <f t="shared" si="160"/>
-        <v>0</v>
-      </c>
-      <c r="J306" s="38">
-        <f t="shared" si="161"/>
-        <v>1</v>
-      </c>
-      <c r="K306" s="35">
-        <f t="shared" si="162"/>
-        <v>0.8</v>
       </c>
       <c r="L306" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="307" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B307" s="33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C307" s="32" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="E307" s="9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G307">
         <v>1</v>
       </c>
       <c r="H307" s="22">
-        <v>19.989999999999998</v>
+        <v>0.8</v>
       </c>
       <c r="I307" s="37">
-        <f t="shared" si="160"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="J307" s="38">
-        <f t="shared" ref="J307:J308" si="163">G307*B307-I307</f>
-        <v>5</v>
+        <f t="shared" si="165"/>
+        <v>1</v>
       </c>
       <c r="K307" s="35">
-        <f t="shared" ref="K307:K308" si="164">B307*H307</f>
-        <v>99.949999999999989</v>
+        <f t="shared" si="166"/>
+        <v>0.8</v>
       </c>
       <c r="L307" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="308" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B308" s="33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C308" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="E308" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="G308">
+        <v>1</v>
+      </c>
+      <c r="H308" s="22">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I308" s="37">
+        <f t="shared" si="164"/>
+        <v>0</v>
+      </c>
+      <c r="J308" s="38">
+        <f t="shared" ref="J308:J309" si="167">G308*B308-I308</f>
+        <v>5</v>
+      </c>
+      <c r="K308" s="35">
+        <f t="shared" ref="K308:K309" si="168">B308*H308</f>
+        <v>99.949999999999989</v>
+      </c>
+      <c r="L308" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B309" s="33">
+        <v>1</v>
+      </c>
+      <c r="C309" s="32" t="s">
         <v>449</v>
       </c>
-      <c r="E308" s="9" t="s">
+      <c r="E309" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="G308">
-        <v>1</v>
-      </c>
-      <c r="H308" s="22">
+      <c r="G309">
+        <v>1</v>
+      </c>
+      <c r="H309" s="22">
         <v>44</v>
       </c>
-      <c r="I308" s="37">
-        <f t="shared" si="160"/>
+      <c r="I309" s="37">
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
-      <c r="J308" s="38">
-        <f t="shared" si="163"/>
-        <v>1</v>
-      </c>
-      <c r="K308" s="35">
-        <f t="shared" si="164"/>
+      <c r="J309" s="38">
+        <f t="shared" si="167"/>
+        <v>1</v>
+      </c>
+      <c r="K309" s="35">
+        <f t="shared" si="168"/>
         <v>44</v>
       </c>
-      <c r="L308" t="s">
+      <c r="L309" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="309" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B309" s="33">
-        <v>5</v>
-      </c>
-      <c r="C309" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="E309" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="G309">
-        <v>1</v>
-      </c>
-      <c r="H309" s="22">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="I309" s="37">
-        <f t="shared" si="160"/>
-        <v>0</v>
-      </c>
-      <c r="J309" s="38">
-        <f t="shared" ref="J309:J310" si="165">G309*B309-I309</f>
-        <v>5</v>
-      </c>
-      <c r="K309" s="35">
-        <f t="shared" ref="K309:K310" si="166">B309*H309</f>
-        <v>10.25</v>
-      </c>
-      <c r="L309" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="310" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B310" s="33">
         <v>5</v>
       </c>
       <c r="C310" s="32" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E310" s="9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G310">
         <v>1</v>
       </c>
       <c r="H310" s="22">
-        <v>1.95</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="I310" s="37">
-        <f t="shared" si="160"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="J310" s="38">
-        <f t="shared" si="165"/>
+        <f t="shared" ref="J310:J311" si="169">G310*B310-I310</f>
         <v>5</v>
       </c>
       <c r="K310" s="35">
-        <f t="shared" si="166"/>
-        <v>9.75</v>
+        <f t="shared" ref="K310:K311" si="170">B310*H310</f>
+        <v>10.25</v>
       </c>
       <c r="L310" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="311" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B311" s="33"/>
-      <c r="C311" s="32"/>
-      <c r="E311" s="9"/>
-      <c r="H311" s="22"/>
-      <c r="I311" s="37"/>
-      <c r="J311" s="38"/>
-      <c r="K311" s="35"/>
-    </row>
-    <row r="312" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B311" s="33">
+        <v>5</v>
+      </c>
+      <c r="C311" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="E311" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="G311">
+        <v>1</v>
+      </c>
+      <c r="H311" s="22">
+        <v>1.95</v>
+      </c>
+      <c r="I311" s="37">
+        <f t="shared" si="164"/>
+        <v>0</v>
+      </c>
+      <c r="J311" s="38">
+        <f t="shared" si="169"/>
+        <v>5</v>
+      </c>
+      <c r="K311" s="35">
+        <f t="shared" si="170"/>
+        <v>9.75</v>
+      </c>
+      <c r="L311" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B312" s="33"/>
+      <c r="C312" s="32"/>
       <c r="E312" s="9"/>
       <c r="H312" s="22"/>
       <c r="I312" s="37"/>
       <c r="J312" s="38"/>
       <c r="K312" s="35"/>
     </row>
-    <row r="313" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B313" s="33"/>
+      <c r="E313" s="9"/>
       <c r="H313" s="22"/>
       <c r="I313" s="37"/>
       <c r="J313" s="38"/>
       <c r="K313" s="35"/>
     </row>
-    <row r="314" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B314" s="33"/>
       <c r="H314" s="22"/>
       <c r="I314" s="37"/>
       <c r="J314" s="38"/>
-      <c r="K314" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="L314" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="315" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B315" s="33"/>
-      <c r="E315" s="26"/>
+      <c r="K314" s="35"/>
+    </row>
+    <row r="315" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H315" s="22"/>
       <c r="I315" s="37"/>
       <c r="J315" s="38"/>
-      <c r="K315" s="39">
-        <f>SUM(K198:K313)</f>
-        <v>2872.5299999999997</v>
-      </c>
-      <c r="L315" s="34">
-        <f ca="1">SUMIF(L1:L313,"=-",K1:K313)</f>
-        <v>78.39</v>
-      </c>
-    </row>
-    <row r="316" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K315" s="35" t="s">
+        <v>410</v>
+      </c>
+      <c r="L315" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B316" s="33"/>
       <c r="E316" s="26"/>
       <c r="H316" s="22"/>
       <c r="I316" s="37"/>
       <c r="J316" s="38"/>
-    </row>
-    <row r="317" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K316" s="39">
+        <f>SUM(K198:K314)</f>
+        <v>2872.5299999999997</v>
+      </c>
+      <c r="L316" s="34">
+        <f ca="1">SUMIF(L1:L314,"=-",K1:K314)</f>
+        <v>63.89</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B317" s="33"/>
       <c r="E317" s="26"/>
       <c r="H317" s="22"/>
       <c r="I317" s="37"/>
       <c r="J317" s="38"/>
     </row>
-    <row r="318" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B318" s="33"/>
       <c r="E318" s="26"/>
       <c r="H318" s="22"/>
       <c r="I318" s="37"/>
       <c r="J318" s="38"/>
     </row>
-    <row r="319" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D319" s="6"/>
+    <row r="319" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B319" s="33"/>
+      <c r="E319" s="26"/>
       <c r="H319" s="22"/>
-      <c r="I319" s="36"/>
-    </row>
-    <row r="320" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E320" s="30"/>
+      <c r="I319" s="37"/>
+      <c r="J319" s="38"/>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D320" s="6"/>
+      <c r="H320" s="22"/>
       <c r="I320" s="36"/>
     </row>
-    <row r="322" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E322" s="26"/>
-      <c r="I322" s="36"/>
+    <row r="321" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E321" s="30"/>
+      <c r="I321" s="36"/>
     </row>
     <row r="323" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E323" s="26"/>
       <c r="I323" s="36"/>
     </row>
     <row r="324" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D324" s="6"/>
       <c r="E324" s="26"/>
       <c r="I324" s="36"/>
     </row>
     <row r="325" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D325" s="8"/>
+      <c r="D325" s="6"/>
+      <c r="E325" s="26"/>
       <c r="I325" s="36"/>
     </row>
     <row r="326" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E326" s="26"/>
+      <c r="D326" s="8"/>
       <c r="I326" s="36"/>
     </row>
     <row r="327" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E327" s="30"/>
+      <c r="E327" s="26"/>
       <c r="I327" s="36"/>
     </row>
     <row r="328" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E328" s="26"/>
+      <c r="E328" s="30"/>
       <c r="I328" s="36"/>
     </row>
     <row r="329" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E329" s="26"/>
       <c r="I329" s="36"/>
     </row>
     <row r="330" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E330" s="26"/>
       <c r="I330" s="36"/>
     </row>
     <row r="331" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D331" s="6"/>
       <c r="E331" s="26"/>
       <c r="I331" s="36"/>
     </row>
     <row r="332" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E332" s="25"/>
+      <c r="D332" s="6"/>
+      <c r="E332" s="26"/>
       <c r="I332" s="36"/>
     </row>
-    <row r="333" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E333" s="26"/>
+    <row r="333" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E333" s="25"/>
       <c r="I333" s="36"/>
     </row>
-    <row r="334" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E334" s="25"/>
+    <row r="334" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E334" s="26"/>
       <c r="I334" s="36"/>
     </row>
     <row r="335" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E335" s="26"/>
+      <c r="E335" s="25"/>
       <c r="I335" s="36"/>
     </row>
     <row r="336" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E336" s="25"/>
+      <c r="E336" s="26"/>
       <c r="I336" s="36"/>
     </row>
-    <row r="337" spans="5:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E337" s="25"/>
       <c r="I337" s="36"/>
     </row>
@@ -17376,313 +17562,333 @@
       <c r="E338" s="25"/>
       <c r="I338" s="36"/>
     </row>
-    <row r="339" spans="5:9" x14ac:dyDescent="0.3">
+    <row r="339" spans="5:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E339" s="25"/>
       <c r="I339" s="36"/>
     </row>
     <row r="340" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="H340" s="22"/>
+      <c r="E340" s="25"/>
       <c r="I340" s="36"/>
     </row>
     <row r="341" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="H341" s="23"/>
+      <c r="H341" s="22"/>
       <c r="I341" s="36"/>
     </row>
+    <row r="342" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="H342" s="23"/>
+      <c r="I342" s="36"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B32:D33 F32:K33 B34:K38 B76:D76 F76:K76 B77:K124 B125:D125 F125:K125 B126:K130 B131:D134 F131:K134 L201 B198:K229 D230:K230 B231:D233 F231:K233 B294:K302 D312:K312 B312 B305:K311 C293 G293:K293 B262:K266 B236:D236 F236:K236 B234:K235 B237:K257 B134:K195 F258:K261 B258:D261 B4:K14 B26:K31 B269:K291 B267:D267 F267:K267 B40:K75">
-    <cfRule type="expression" dxfId="65" priority="167">
+  <conditionalFormatting sqref="B32:D33 F32:K33 B34:K38 B76:D76 F76:K76 B77:K124 B125:D125 F125:K125 B126:K130 B131:D134 F131:K134 L201 B198:K229 D230:K230 B231:D233 F231:K233 B295:K303 D313:K313 B313 B306:K312 C294 G294:K294 B262:K266 B236:D236 F236:K236 B234:K235 B237:K257 B134:K195 F258:K261 B258:D261 B4:K14 B26:K31 B270:K292 F267:K267 B40:K75 B267:C267">
+    <cfRule type="expression" dxfId="69" priority="171">
       <formula>$L4=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:XFD6 B32:K32 A33:K38 M7:XFD13 A4:L13 A230 D230:XFD230 A198:XFD229 A231:D233 A312:B312 D312:XFD312 C293 G293:L293 A294:XFD302 A305:XFD311 F231:XFD233 A262:XFD266 A236:D236 F236:XFD236 A234:XFD235 A237:XFD257 A14:XFD14 A258:D261 F258:XFD261 A26:K31 L26:XFD38 A269:XFD291 A267:D267 F267:XFD267 A40:XFD195">
-    <cfRule type="expression" dxfId="64" priority="168">
+  <conditionalFormatting sqref="N4:XFD6 B32:K32 A33:K38 M7:XFD13 A4:L13 A230 D230:XFD230 A198:XFD229 A231:D233 A313:B313 D313:XFD313 C294 G294:L294 A295:XFD303 A306:XFD312 F231:XFD233 A262:XFD266 A236:D236 F236:XFD236 A234:XFD235 A237:XFD257 A14:XFD14 A258:D261 F258:XFD261 A26:K31 L26:XFD38 A270:XFD292 F267:XFD267 A40:XFD195 A267:C267">
+    <cfRule type="expression" dxfId="68" priority="172">
       <formula>$L4=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="169">
+    <cfRule type="expression" dxfId="67" priority="173">
       <formula>$L4=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E233">
-    <cfRule type="expression" dxfId="62" priority="171">
+    <cfRule type="expression" dxfId="66" priority="175">
       <formula>$L230=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E233">
-    <cfRule type="expression" dxfId="61" priority="174">
+    <cfRule type="expression" dxfId="65" priority="178">
       <formula>$L230=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="175">
+    <cfRule type="expression" dxfId="64" priority="179">
       <formula>$L230=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E231:E232">
-    <cfRule type="expression" dxfId="59" priority="177">
+  <conditionalFormatting sqref="E231:E232 E269">
+    <cfRule type="expression" dxfId="63" priority="181">
       <formula>$L229=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E231:E232">
-    <cfRule type="expression" dxfId="58" priority="180">
+  <conditionalFormatting sqref="E231:E232 E269">
+    <cfRule type="expression" dxfId="62" priority="184">
       <formula>$L229=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="181">
+    <cfRule type="expression" dxfId="61" priority="185">
       <formula>$L229=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E258">
-    <cfRule type="expression" dxfId="56" priority="183">
+    <cfRule type="expression" dxfId="60" priority="187">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E258">
-    <cfRule type="expression" dxfId="55" priority="187">
+    <cfRule type="expression" dxfId="59" priority="191">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="188">
+    <cfRule type="expression" dxfId="58" priority="192">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:K25">
-    <cfRule type="expression" dxfId="53" priority="50">
+    <cfRule type="expression" dxfId="57" priority="54">
       <formula>$L25=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:XFD25">
-    <cfRule type="expression" dxfId="52" priority="51">
+    <cfRule type="expression" dxfId="56" priority="55">
       <formula>$L25=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="55" priority="56">
       <formula>$L25=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:K16">
-    <cfRule type="expression" dxfId="50" priority="47">
+    <cfRule type="expression" dxfId="54" priority="51">
       <formula>$L15=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule type="expression" dxfId="49" priority="48">
+    <cfRule type="expression" dxfId="53" priority="52">
       <formula>$L15=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>$L15=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17 M17:XFD17">
-    <cfRule type="expression" dxfId="47" priority="45">
+    <cfRule type="expression" dxfId="51" priority="49">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="46">
+    <cfRule type="expression" dxfId="50" priority="50">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="expression" dxfId="45" priority="41">
+    <cfRule type="expression" dxfId="49" priority="45">
       <formula>$L17=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:L17">
-    <cfRule type="expression" dxfId="44" priority="42">
+    <cfRule type="expression" dxfId="48" priority="46">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="43">
+    <cfRule type="expression" dxfId="47" priority="47">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 M18:XFD18">
-    <cfRule type="expression" dxfId="42" priority="39">
+    <cfRule type="expression" dxfId="46" priority="43">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="40">
+    <cfRule type="expression" dxfId="45" priority="44">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18">
-    <cfRule type="expression" dxfId="40" priority="36">
+    <cfRule type="expression" dxfId="44" priority="40">
       <formula>$L18=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L18">
-    <cfRule type="expression" dxfId="39" priority="37">
+    <cfRule type="expression" dxfId="43" priority="41">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="42" priority="42">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21 M21:XFD21">
-    <cfRule type="expression" dxfId="37" priority="34">
+    <cfRule type="expression" dxfId="41" priority="38">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="35">
+    <cfRule type="expression" dxfId="40" priority="39">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21 E21:K21">
-    <cfRule type="expression" dxfId="35" priority="31">
+    <cfRule type="expression" dxfId="39" priority="35">
       <formula>$L21=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21 E21:L21">
-    <cfRule type="expression" dxfId="34" priority="32">
+    <cfRule type="expression" dxfId="38" priority="36">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="33">
+    <cfRule type="expression" dxfId="37" priority="37">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:K23">
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="36" priority="32">
       <formula>$L23=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:XFD23">
-    <cfRule type="expression" dxfId="31" priority="29">
+    <cfRule type="expression" dxfId="35" priority="33">
       <formula>$L23=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="34" priority="34">
       <formula>$L23=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:K24">
-    <cfRule type="expression" dxfId="29" priority="25">
+    <cfRule type="expression" dxfId="33" priority="29">
       <formula>$L24=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:XFD24">
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="32" priority="30">
       <formula>$L24=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27">
+    <cfRule type="expression" dxfId="31" priority="31">
       <formula>$L24=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22 M22:XFD22">
-    <cfRule type="expression" dxfId="26" priority="23">
+    <cfRule type="expression" dxfId="30" priority="27">
       <formula>$L22=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="24">
+    <cfRule type="expression" dxfId="29" priority="28">
       <formula>$L22=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:K22">
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="28" priority="24">
       <formula>$L22=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:L22">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>$L22=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="26" priority="26">
       <formula>$L22=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="21" priority="17">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>$L21=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="24" priority="22">
       <formula>$L21=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="23" priority="23">
       <formula>$L21=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19 M19:XFD19">
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="22" priority="19">
       <formula>$L19=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="21" priority="20">
       <formula>$L19=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:K19">
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="20" priority="16">
       <formula>$L19=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:L19">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>$L19=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>$L19=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 M20:XFD20">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>$L20=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="16" priority="15">
       <formula>$L20=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:K20">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>$L20=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:L20">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>$L20=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>$L20=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="expression" dxfId="8" priority="190">
+    <cfRule type="expression" dxfId="12" priority="194">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="expression" dxfId="7" priority="194">
+    <cfRule type="expression" dxfId="11" priority="198">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="195">
+    <cfRule type="expression" dxfId="10" priority="199">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B268:D268 F268:K268">
-    <cfRule type="expression" dxfId="5" priority="4">
+  <conditionalFormatting sqref="F268:K269 B268:D269">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>$L268=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A268:D268 F268:XFD268">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="F268:K269 M268:XFD269 A268:D269">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$L268=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>$L268=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:K39">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$L39=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:XFD39">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$L39=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$L39=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L198:L229 L305:L310 L293:L302 L231:L275 L277:L290">
+  <conditionalFormatting sqref="L269">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$L269=$O$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$L269=$O$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L268">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$L268=$O$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$L268=$O$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L198:L229 L306:L311 L294:L303 L278:L291 L231:L276">
       <formula1>$O$1:$O$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E284" r:id="rId1"/>
-    <hyperlink ref="E274" r:id="rId2"/>
-    <hyperlink ref="E271" r:id="rId3"/>
+    <hyperlink ref="E285" r:id="rId1"/>
+    <hyperlink ref="E275" r:id="rId2"/>
+    <hyperlink ref="E272" r:id="rId3"/>
     <hyperlink ref="E233" r:id="rId4"/>
     <hyperlink ref="E259" r:id="rId5"/>
-    <hyperlink ref="E269" r:id="rId6"/>
+    <hyperlink ref="E270" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="34" orientation="landscape" r:id="rId7"/>

</xml_diff>

<commit_message>
Kabelstütze mit mehr findament
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" activeTab="8"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -2178,27 +2178,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color theme="3"/>
@@ -3393,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD111"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3564,7 +3544,7 @@
       </c>
       <c r="C16" s="5">
         <f>C20/C18*(C24/C22)</f>
-        <v>11.851851851851851</v>
+        <v>15.238095238095237</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -3632,7 +3612,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="6">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
@@ -3644,7 +3624,7 @@
       </c>
       <c r="C23" s="4">
         <f>C22*C17/PI()</f>
-        <v>28.647889756541161</v>
+        <v>22.281692032865347</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -4093,7 +4073,7 @@
       </c>
       <c r="C64" s="2">
         <f>C59/C16</f>
-        <v>2.1510341015624999</v>
+        <v>1.6730265234374999</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -4259,7 +4239,7 @@
       </c>
       <c r="C71" s="2">
         <f>C64*(1+C53)</f>
-        <v>2.79634433203125</v>
+        <v>2.17493448046875</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -9062,7 +9042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
@@ -9588,8 +9568,8 @@
   </sheetPr>
   <dimension ref="A1:O330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L267" sqref="L267"/>
+    <sheetView topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16943,101 +16923,101 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:K14 B26:D26 F26:K26 B19:K25 B121:D122 F121:K122 L189 B186:K217 D218:K218 B219:D221 F219:K221 B283:K291 D301:K301 B301 B294:K300 C282 G282:K282 B250:K254 B224:D224 F224:K224 B222:K223 B225:K245 B123:K183 F246:K249 B246:D249 B258:K280 B255:C255 E256 F255:K257 B256:D257 B27:K121">
-    <cfRule type="expression" dxfId="26" priority="174">
+    <cfRule type="expression" dxfId="22" priority="174">
       <formula>$L4=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:XFD6 M7:XFD13 A4:L13 A14:XFD14 A218 D218:XFD218 A186:XFD217 A219:D221 A301:B301 D301:XFD301 C282 G282:L282 A283:XFD291 A294:XFD300 F219:XFD221 A250:XFD254 A224:D224 F224:XFD224 A222:XFD223 A225:XFD245 A246:D249 F246:XFD249 A255:C255 E256 A256:D257 F255:XFD257 A19:XFD183 A258:XFD280">
-    <cfRule type="expression" dxfId="25" priority="175">
+    <cfRule type="expression" dxfId="21" priority="175">
       <formula>$L4=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="176">
+    <cfRule type="expression" dxfId="20" priority="176">
       <formula>$L4=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E221">
-    <cfRule type="expression" dxfId="23" priority="178">
+    <cfRule type="expression" dxfId="19" priority="178">
       <formula>$L218=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E221">
-    <cfRule type="expression" dxfId="22" priority="181">
+    <cfRule type="expression" dxfId="18" priority="181">
       <formula>$L218=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="182">
+    <cfRule type="expression" dxfId="17" priority="182">
       <formula>$L218=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E219:E220 E257">
-    <cfRule type="expression" dxfId="20" priority="184">
+    <cfRule type="expression" dxfId="16" priority="184">
       <formula>$L217=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E219:E220 E257">
-    <cfRule type="expression" dxfId="19" priority="187">
+    <cfRule type="expression" dxfId="15" priority="187">
       <formula>$L217=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="188">
+    <cfRule type="expression" dxfId="14" priority="188">
       <formula>$L217=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E246">
-    <cfRule type="expression" dxfId="17" priority="190">
+    <cfRule type="expression" dxfId="13" priority="190">
       <formula>$L256=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E246">
-    <cfRule type="expression" dxfId="16" priority="194">
+    <cfRule type="expression" dxfId="12" priority="194">
       <formula>$L256=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="195">
+    <cfRule type="expression" dxfId="11" priority="195">
       <formula>$L256=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:K16">
-    <cfRule type="expression" dxfId="14" priority="54">
+    <cfRule type="expression" dxfId="10" priority="54">
       <formula>$L15=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule type="expression" dxfId="13" priority="55">
+    <cfRule type="expression" dxfId="9" priority="55">
       <formula>$L15=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="56">
+    <cfRule type="expression" dxfId="8" priority="56">
       <formula>$L15=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 M18:XFD18">
-    <cfRule type="expression" dxfId="11" priority="46">
+    <cfRule type="expression" dxfId="7" priority="46">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="47">
+    <cfRule type="expression" dxfId="6" priority="47">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18">
-    <cfRule type="expression" dxfId="9" priority="43">
+    <cfRule type="expression" dxfId="5" priority="43">
       <formula>$L18=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L18">
-    <cfRule type="expression" dxfId="8" priority="44">
+    <cfRule type="expression" dxfId="4" priority="44">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="45">
+    <cfRule type="expression" dxfId="3" priority="45">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$L17=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:XFD17">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Neuer Oberarm mit horizontalem Riemenspanner
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2969,13 +2969,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>127870</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3024,13 +3024,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>182879</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>69762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3367,8 +3367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4310,7 +4310,7 @@
         <v>190</v>
       </c>
       <c r="L72" s="31">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="M72" s="31" t="s">
         <v>63</v>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="Q72" s="88">
         <f t="shared" si="0"/>
-        <v>1.3602000000000001</v>
+        <v>0.95213999999999999</v>
       </c>
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
@@ -9171,10 +9171,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9484,11 +9484,20 @@
       <c r="J51" s="51"/>
       <c r="K51" s="51"/>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+    </row>
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A56" s="46"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
@@ -9496,59 +9505,62 @@
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="47"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="47"/>
-    </row>
-    <row r="81" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="42"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="47"/>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="47"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="47"/>
+    </row>
+    <row r="82" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="42"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="47"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="47"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="47"/>
-    </row>
-    <row r="94" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A94" s="42"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="47"/>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="47"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="47"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="47"/>
+    </row>
+    <row r="95" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A95" s="42"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="47"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="47"/>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="47"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="47"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="47"/>
-    </row>
-    <row r="108" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A108" s="42"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="47"/>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="47"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="47"/>
+    </row>
+    <row r="109" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A109" s="42"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="47"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="47"/>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="47"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9564,8 +9576,8 @@
   </sheetPr>
   <dimension ref="A1:O327"/>
   <sheetViews>
-    <sheetView topLeftCell="A245" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+    <sheetView topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11882,8 +11894,8 @@
         <v>1</v>
       </c>
       <c r="C115" s="32" t="str">
-        <f>C233</f>
-        <v>Zahnriemenscheibe T5, 14 Zähne (d=22,48)</v>
+        <f>C236</f>
+        <v>Zahnriemenscheibe T5, 12 Zähne (d=19,10)</v>
       </c>
       <c r="D115" t="s">
         <v>506</v>
@@ -14755,7 +14767,7 @@
     <row r="233" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B233" s="33">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C233" s="32" t="s">
         <v>545</v>
@@ -14771,7 +14783,7 @@
       </c>
       <c r="I233" s="37">
         <f>SUMIF(C$1:C$181,"="&amp;C233,B$1:B$181)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J233" s="38">
         <f t="shared" ref="J233" si="71">G233*B233-I233</f>
@@ -14779,7 +14791,7 @@
       </c>
       <c r="K233" s="35">
         <f t="shared" ref="K233" si="72">B233*H233</f>
-        <v>26.150000000000002</v>
+        <v>20.92</v>
       </c>
       <c r="L233" t="s">
         <v>478</v>
@@ -14854,7 +14866,7 @@
     <row r="236" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="33">
         <f t="shared" ref="B236" si="78">ROUNDUP(I236/G236,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>546</v>
@@ -14870,7 +14882,7 @@
       </c>
       <c r="I236" s="37">
         <f>SUMIF(C$1:C$181,"="&amp;C236,B$1:B$181)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J236" s="38">
         <f t="shared" ref="J236" si="79">G236*B236-I236</f>
@@ -14878,7 +14890,7 @@
       </c>
       <c r="K236" s="35">
         <f t="shared" ref="K236" si="80">B236*H236</f>
-        <v>0</v>
+        <v>5.07</v>
       </c>
       <c r="L236" t="s">
         <v>478</v>
@@ -16736,7 +16748,7 @@
       <c r="J301" s="38"/>
       <c r="K301" s="39">
         <f>SUM(K183:K299)</f>
-        <v>2776.5</v>
+        <v>2776.34</v>
       </c>
       <c r="L301" s="34">
         <f ca="1">SUMIF(L1:L299,"=-",K1:K299)</f>

</xml_diff>

<commit_message>
More torque for the shoulder
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="599">
   <si>
     <t>Material</t>
   </si>
@@ -1805,9 +1805,6 @@
     <t>Noch zu besorgen</t>
   </si>
   <si>
-    <t>Riemen für Schulter T5 480mm</t>
-  </si>
-  <si>
     <t>Gehäuse-Lager, 10 hab ich , 16 brauch ich</t>
   </si>
   <si>
@@ -1818,6 +1815,15 @@
   </si>
   <si>
     <t>http://www.cncshop.at/index.php?a=5289</t>
+  </si>
+  <si>
+    <t>Drehmoment Oberarm Motor</t>
+  </si>
+  <si>
+    <t>Riemenspanner am Motor Schulter 4</t>
+  </si>
+  <si>
+    <t>Riemenspanner am Hüftmotor 4</t>
   </si>
 </sst>
 </file>
@@ -2174,7 +2180,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="67">
     <dxf>
       <font>
         <color theme="3"/>
@@ -2183,21 +2189,6 @@
     <dxf>
       <font>
         <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -2288,6 +2279,51 @@
     <dxf>
       <font>
         <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -3559,8 +3595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD111"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,7 +3766,7 @@
       </c>
       <c r="C16" s="5">
         <f>C20/C18*(C24/C22)</f>
-        <v>15.238095238095237</v>
+        <v>22.857142857142858</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -3752,7 +3788,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="6">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
@@ -3764,7 +3800,7 @@
       </c>
       <c r="C19" s="4">
         <f>C18*C17/PI()</f>
-        <v>28.647889756541161</v>
+        <v>19.098593171027442</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -4201,8 +4237,8 @@
         <v>27</v>
       </c>
       <c r="C59" s="4">
-        <f>((C3+C4+C5)*(C7+C8+C9)*(C54+C55))/1000</f>
-        <v>25.493737499999998</v>
+        <f>((C3+C4+C5)*(C6+C7+C8+C9)*(C54+C55))/1000</f>
+        <v>34.558177499999999</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -4258,11 +4294,11 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>596</v>
       </c>
       <c r="C64" s="2">
         <f>C59/C16</f>
-        <v>1.6730265234374999</v>
+        <v>1.5119202656249999</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -4428,7 +4464,7 @@
       </c>
       <c r="C71" s="2">
         <f>C64*(1+C53)</f>
-        <v>2.17493448046875</v>
+        <v>1.9654963453125001</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -5502,7 +5538,7 @@
       </c>
       <c r="C104" s="20">
         <f>C59/C103</f>
-        <v>667.42448702122169</v>
+        <v>904.73097129543396</v>
       </c>
       <c r="D104" t="s">
         <v>249</v>
@@ -5515,7 +5551,7 @@
       </c>
       <c r="C105" s="20">
         <f>(C102)*C104*2*PI()</f>
-        <v>4193.5517305036128</v>
+        <v>5684.592345793787</v>
       </c>
       <c r="D105" t="s">
         <v>250</v>
@@ -5532,7 +5568,7 @@
       </c>
       <c r="C108" s="20">
         <f>60*C18/C20</f>
-        <v>22.5</v>
+        <v>15</v>
       </c>
       <c r="D108" t="s">
         <v>258</v>
@@ -5556,7 +5592,7 @@
       </c>
       <c r="C110" s="20">
         <f>C59/(C20/C18)/C109</f>
-        <v>150.17050957977492</v>
+        <v>135.7096456943151</v>
       </c>
       <c r="D110" t="s">
         <v>249</v>
@@ -5568,7 +5604,7 @@
       </c>
       <c r="C111" s="20">
         <f>(C108/60)*C110*2*PI()</f>
-        <v>353.83092726124238</v>
+        <v>213.172212967267</v>
       </c>
       <c r="D111" t="s">
         <v>250</v>
@@ -5610,7 +5646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -9771,8 +9807,8 @@
   </sheetPr>
   <dimension ref="A1:O324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E307" sqref="E307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15888,7 +15924,7 @@
         <v>571</v>
       </c>
       <c r="E260" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G260">
         <v>1</v>
@@ -16904,7 +16940,7 @@
         <v>2</v>
       </c>
       <c r="C298" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E298" s="9" t="s">
         <v>365</v>
@@ -16914,21 +16950,28 @@
       <c r="J298" s="38"/>
     </row>
     <row r="299" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B299" s="33"/>
-      <c r="E299" s="9"/>
+      <c r="B299" s="33">
+        <v>4</v>
+      </c>
+      <c r="C299" t="s">
+        <v>597</v>
+      </c>
+      <c r="E299" s="9" t="s">
+        <v>365</v>
+      </c>
       <c r="H299" s="22"/>
       <c r="I299" s="37"/>
       <c r="J299" s="38"/>
     </row>
     <row r="300" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B300" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C300" t="s">
-        <v>592</v>
-      </c>
-      <c r="E300" s="26" t="s">
-        <v>377</v>
+        <v>598</v>
+      </c>
+      <c r="E300" s="9" t="s">
+        <v>365</v>
       </c>
       <c r="H300" s="22"/>
       <c r="I300" s="37"/>
@@ -16939,10 +16982,10 @@
         <v>6</v>
       </c>
       <c r="C301" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E301" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H301" s="22"/>
       <c r="I301" s="37"/>
@@ -16951,7 +16994,7 @@
     <row r="302" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D302" s="6"/>
       <c r="E302" s="29" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H302" s="22"/>
       <c r="I302" s="36"/>
@@ -17042,155 +17085,155 @@
       <c r="I324" s="36"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:K14 B26:D26 F26:K26 B19:K25 B111:D112 F111:K112 L181 D210:K210 B211:D213 F211:K213 B276:K284 D294:K294 B294 B287:K293 C275 G275:K275 B242:K246 B216:D216 F216:K216 B214:K215 B217:K237 F238:K241 B238:D241 B247:C247 E248 F247:K249 B248:D249 B177:K209 B27:K111 B113:K174 B250:K259 B261:K273 B260:D260 F260:K260">
-    <cfRule type="expression" dxfId="37" priority="186">
+  <conditionalFormatting sqref="B4:K14 B26:D26 F26:K26 B19:K25 B111:D112 F111:K112 L181 D210:K210 B211:D213 F211:K213 B276:K284 D294:K294 B294 B287:K293 C275 G275:K275 B242:K246 B216:D216 F216:K216 B214:K215 B217:K237 F238:K241 B238:D241 B247:C247 E248 F247:K249 B248:D249 B177:K209 B27:K111 B113:K174 B250:K259 B261:K273 B260:D260 F260:K260 E301">
+    <cfRule type="expression" dxfId="34" priority="192">
       <formula>$L4=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:XFD6 M7:XFD13 A4:L13 A14:XFD14 A210 D210:XFD210 A211:D213 A294:B294 D294:XFD294 C275 G275:L275 A276:XFD284 A287:XFD293 F211:XFD213 A242:XFD246 A216:D216 F216:XFD216 A214:XFD215 A217:XFD237 A238:D241 F238:XFD241 A247:C247 E248 A248:D249 F247:XFD249 A177:XFD209 A19:XFD174 A250:XFD259 A261:XFD273 A260:D260 F260:XFD260">
-    <cfRule type="expression" dxfId="36" priority="187">
+  <conditionalFormatting sqref="N4:XFD6 M7:XFD13 A4:L13 A14:XFD14 A210 D210:XFD210 A211:D213 A294:B294 D294:XFD294 C275 G275:L275 A276:XFD284 A287:XFD293 F211:XFD213 A242:XFD246 A216:D216 F216:XFD216 A214:XFD215 A217:XFD237 A238:D241 F238:XFD241 A247:C247 E248 A248:D249 F247:XFD249 A177:XFD209 A19:XFD174 A250:XFD259 A261:XFD273 A260:D260 F260:XFD260 E301">
+    <cfRule type="expression" dxfId="33" priority="193">
       <formula>$L4=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="188">
+    <cfRule type="expression" dxfId="32" priority="194">
       <formula>$L4=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E213">
-    <cfRule type="expression" dxfId="34" priority="190">
+    <cfRule type="expression" dxfId="31" priority="196">
       <formula>$L210=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E213">
-    <cfRule type="expression" dxfId="33" priority="193">
+    <cfRule type="expression" dxfId="30" priority="199">
       <formula>$L210=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="194">
+    <cfRule type="expression" dxfId="29" priority="200">
       <formula>$L210=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E249 E211:E212">
-    <cfRule type="expression" dxfId="31" priority="196">
+    <cfRule type="expression" dxfId="28" priority="202">
       <formula>$L209=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E249 E211:E212">
-    <cfRule type="expression" dxfId="30" priority="199">
+    <cfRule type="expression" dxfId="27" priority="205">
       <formula>$L209=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="200">
+    <cfRule type="expression" dxfId="26" priority="206">
       <formula>$L209=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E238">
-    <cfRule type="expression" dxfId="28" priority="202">
+    <cfRule type="expression" dxfId="25" priority="208">
       <formula>$L248=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E238">
-    <cfRule type="expression" dxfId="27" priority="206">
+    <cfRule type="expression" dxfId="24" priority="212">
       <formula>$L248=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="207">
+    <cfRule type="expression" dxfId="23" priority="213">
       <formula>$L248=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:K16">
-    <cfRule type="expression" dxfId="25" priority="66">
+    <cfRule type="expression" dxfId="22" priority="72">
       <formula>$L15=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule type="expression" dxfId="24" priority="67">
+    <cfRule type="expression" dxfId="21" priority="73">
       <formula>$L15=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="68">
+    <cfRule type="expression" dxfId="20" priority="74">
       <formula>$L15=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 M18:XFD18">
-    <cfRule type="expression" dxfId="22" priority="58">
+    <cfRule type="expression" dxfId="19" priority="64">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="59">
+    <cfRule type="expression" dxfId="18" priority="65">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18">
-    <cfRule type="expression" dxfId="20" priority="55">
+    <cfRule type="expression" dxfId="17" priority="61">
       <formula>$L18=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L18">
-    <cfRule type="expression" dxfId="19" priority="56">
+    <cfRule type="expression" dxfId="16" priority="62">
       <formula>$L18=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="57">
+    <cfRule type="expression" dxfId="15" priority="63">
       <formula>$L18=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>$L17=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:XFD17">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>$L17=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="12" priority="21">
       <formula>$L17=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E260">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>$L260=$O$6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E260">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>$L260=$O$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>$L260=$O$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E298">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$L298=$O$6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E298">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$L298=$O$5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>$L298=$O$4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E299">
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$L299=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E299">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$L299=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$L299=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E301">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>$L301=$O$6</formula>
+  <conditionalFormatting sqref="E300">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$L300=$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E301">
-    <cfRule type="expression" dxfId="10" priority="8">
-      <formula>$L301=$O$5</formula>
+  <conditionalFormatting sqref="E300">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$L300=$O$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>$L301=$O$4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E260">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$L260=$O$6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E260">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$L260=$O$5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$L260=$O$4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E298">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>$L298=$O$6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E298">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$L298=$O$5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$L298=$O$4</formula>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$L300=$O$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
Forearm's motor moved 1mm down
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -22,11 +22,12 @@
     <definedName name="ShoppingStatus">BOM!$L:$L</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="474">
   <si>
     <t>Material</t>
   </si>
@@ -1415,6 +1416,39 @@
   </si>
   <si>
     <t>Zahnriemen T2,5 250mm 6mm Breite</t>
+  </si>
+  <si>
+    <t>Kabel</t>
+  </si>
+  <si>
+    <t>RXD</t>
+  </si>
+  <si>
+    <t>TXD</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>schwarz/rot</t>
+  </si>
+  <si>
+    <t>Kabel Phase 1</t>
+  </si>
+  <si>
+    <t>Kabel Phase 2</t>
+  </si>
+  <si>
+    <t>grün/blau</t>
+  </si>
+  <si>
+    <t>Gleichstrom Widerstand</t>
+  </si>
+  <si>
+    <t>30 Ohm</t>
   </si>
 </sst>
 </file>
@@ -1696,22 +1730,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color theme="3"/>
@@ -1795,36 +1814,6 @@
     <dxf>
       <font>
         <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -2911,7 +2900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE93"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -2927,6 +2916,7 @@
     <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3547,7 +3537,7 @@
       </c>
       <c r="D46" s="4">
         <f>D50/D48</f>
-        <v>3.6111111111111112</v>
+        <v>4.0625</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -3575,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="D48" s="6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E48" t="s">
         <v>28</v>
@@ -3591,7 +3581,7 @@
       </c>
       <c r="D49" s="4">
         <f>D48*D47/PI()</f>
-        <v>14.323944878270581</v>
+        <v>12.732395447351628</v>
       </c>
       <c r="E49" t="s">
         <v>30</v>
@@ -3802,7 +3792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="F68" s="10" t="s">
@@ -3838,6 +3828,15 @@
       </c>
       <c r="R68" s="51" t="s">
         <v>384</v>
+      </c>
+      <c r="S68" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="T68" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="U68" s="51" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="69" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
@@ -3919,7 +3918,7 @@
         <v>180</v>
       </c>
       <c r="R70" s="52">
-        <f t="shared" ref="R70:R73" si="0">0.6801*M70</f>
+        <f>0.6801*M70</f>
         <v>1.90428</v>
       </c>
     </row>
@@ -3966,11 +3965,11 @@
         <v>1.34</v>
       </c>
       <c r="P71" s="14">
-        <f t="shared" ref="P71:P72" si="1">L71/O71</f>
+        <f>L71/O71</f>
         <v>223.88059701492537</v>
       </c>
       <c r="R71" s="52">
-        <f t="shared" si="0"/>
+        <f>0.6801*M71</f>
         <v>2.7204000000000002</v>
       </c>
     </row>
@@ -4017,11 +4016,11 @@
         <v>0.77</v>
       </c>
       <c r="P72" s="15">
-        <f t="shared" si="1"/>
+        <f>L72/O72</f>
         <v>246.75324675324674</v>
       </c>
       <c r="R72" s="52">
-        <f t="shared" si="0"/>
+        <f>0.6801*M72</f>
         <v>0.95213999999999999</v>
       </c>
       <c r="S72" s="10"/>
@@ -4082,7 +4081,7 @@
       </c>
       <c r="Q73" s="11"/>
       <c r="R73" s="52">
-        <f t="shared" si="0"/>
+        <f>0.6801*M73</f>
         <v>0.47606999999999999</v>
       </c>
       <c r="S73" s="10"/>
@@ -4147,12 +4146,18 @@
       </c>
       <c r="Q74" s="11"/>
       <c r="R74" s="52">
-        <f t="shared" ref="R74" si="2">0.6801*M74</f>
+        <f>0.6801*M74</f>
         <v>0.27204</v>
       </c>
-      <c r="S74" s="12"/>
-      <c r="T74" s="12"/>
-      <c r="U74" s="12"/>
+      <c r="S74" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="T74" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="U74" s="12" t="s">
+        <v>473</v>
+      </c>
       <c r="V74" s="12"/>
       <c r="W74" s="12"/>
       <c r="X74" s="12"/>
@@ -4397,7 +4402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -4640,7 +4645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -4809,10 +4814,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4840,9 +4845,47 @@
         <v>240</v>
       </c>
     </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>466</v>
+      </c>
+      <c r="F23" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>439</v>
+      </c>
+      <c r="F24" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>443</v>
+      </c>
+      <c r="F25" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>441</v>
+      </c>
+      <c r="F26" t="s">
+        <v>464</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4850,7 +4893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
@@ -5253,8 +5296,8 @@
   </sheetPr>
   <dimension ref="A1:O298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5350,7 +5393,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="29"/>
       <c r="L5" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C5,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L5:L11" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C5,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5371,7 +5414,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="29"/>
       <c r="L6" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C6,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5392,7 +5435,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="29"/>
       <c r="L7" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C7,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5413,7 +5456,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="29"/>
       <c r="L8" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C8,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5434,7 +5477,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="29"/>
       <c r="L9" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C9,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5455,7 +5498,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="29"/>
       <c r="L10" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C10,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5476,7 +5519,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="29"/>
       <c r="L11" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C11,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5556,7 +5599,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="29"/>
       <c r="L17">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C17,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L17:L22" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C17,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -5577,7 +5620,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="29"/>
       <c r="L18" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C18,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5598,7 +5641,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="29"/>
       <c r="L19">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C19,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5619,7 +5662,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="29"/>
       <c r="L20">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C20,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5640,7 +5683,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="29"/>
       <c r="L21" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C21,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5661,7 +5704,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="29"/>
       <c r="L22" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C22,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -5703,7 +5746,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="29"/>
       <c r="L25" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C25,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L25:L38" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C25,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5724,7 +5767,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="29"/>
       <c r="L26" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C26,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5745,7 +5788,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="29"/>
       <c r="L27" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C27,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5766,7 +5809,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="29"/>
       <c r="L28" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C28,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5787,7 +5830,7 @@
       <c r="J29" s="32"/>
       <c r="K29" s="29"/>
       <c r="L29" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C29,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5808,7 +5851,7 @@
       <c r="J30" s="32"/>
       <c r="K30" s="29"/>
       <c r="L30" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C30,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5829,7 +5872,7 @@
       <c r="J31" s="32"/>
       <c r="K31" s="29"/>
       <c r="L31" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C31,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5850,7 +5893,7 @@
       <c r="J32" s="32"/>
       <c r="K32" s="29"/>
       <c r="L32" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C32,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5871,7 +5914,7 @@
       <c r="J33" s="32"/>
       <c r="K33" s="29"/>
       <c r="L33" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C33,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5892,7 +5935,7 @@
       <c r="J34" s="32"/>
       <c r="K34" s="29"/>
       <c r="L34" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C34,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5913,7 +5956,7 @@
       <c r="J35" s="32"/>
       <c r="K35" s="29"/>
       <c r="L35" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C35,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5934,7 +5977,7 @@
       <c r="J36" s="32"/>
       <c r="K36" s="29"/>
       <c r="L36" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C36,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5955,7 +5998,7 @@
       <c r="J37" s="32"/>
       <c r="K37" s="29"/>
       <c r="L37" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C37,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -5976,7 +6019,7 @@
       <c r="J38" s="32"/>
       <c r="K38" s="29"/>
       <c r="L38" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C38,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6009,7 +6052,7 @@
       <c r="J40" s="32"/>
       <c r="K40" s="29"/>
       <c r="L40">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C40,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L40:L55" ca="1" si="3">INDIRECT(ADDRESS(MATCH(C40,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6030,7 +6073,7 @@
       <c r="J41" s="32"/>
       <c r="K41" s="29"/>
       <c r="L41" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C41,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6051,7 +6094,7 @@
       <c r="J42" s="32"/>
       <c r="K42" s="29"/>
       <c r="L42" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C42,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6072,7 +6115,7 @@
       <c r="J43" s="32"/>
       <c r="K43" s="29"/>
       <c r="L43" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C43,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6094,7 +6137,7 @@
       <c r="J44" s="32"/>
       <c r="K44" s="29"/>
       <c r="L44" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C44,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6115,7 +6158,7 @@
       <c r="J45" s="32"/>
       <c r="K45" s="29"/>
       <c r="L45">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C45,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6136,7 +6179,7 @@
       <c r="J46" s="32"/>
       <c r="K46" s="29"/>
       <c r="L46" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C46,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6157,7 +6200,7 @@
       <c r="J47" s="32"/>
       <c r="K47" s="29"/>
       <c r="L47" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C47,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6178,7 +6221,7 @@
       <c r="J48" s="32"/>
       <c r="K48" s="29"/>
       <c r="L48" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C48,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6199,7 +6242,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="29"/>
       <c r="L49">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C49,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6220,7 +6263,7 @@
       <c r="J50" s="32"/>
       <c r="K50" s="29"/>
       <c r="L50" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C50,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6241,7 +6284,7 @@
       <c r="J51" s="32"/>
       <c r="K51" s="29"/>
       <c r="L51">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C51,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6262,7 +6305,7 @@
       <c r="J52" s="32"/>
       <c r="K52" s="29"/>
       <c r="L52" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C52,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6283,7 +6326,7 @@
       <c r="J53" s="32"/>
       <c r="K53" s="29"/>
       <c r="L53" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C53,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6304,7 +6347,7 @@
       <c r="J54" s="32"/>
       <c r="K54" s="29"/>
       <c r="L54" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C54,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6325,7 +6368,7 @@
       <c r="J55" s="32"/>
       <c r="K55" s="29"/>
       <c r="L55" t="str">
-        <f ca="1">INDIRECT(ADDRESS(MATCH(C55,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6358,7 +6401,7 @@
       <c r="J57" s="32"/>
       <c r="K57" s="29"/>
       <c r="L57" t="str">
-        <f t="shared" ref="L57:L89" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C57,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L57:L89" ca="1" si="4">INDIRECT(ADDRESS(MATCH(C57,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6379,7 +6422,7 @@
       <c r="J58" s="32"/>
       <c r="K58" s="29"/>
       <c r="L58" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6400,7 +6443,7 @@
       <c r="J59" s="32"/>
       <c r="K59" s="29"/>
       <c r="L59" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6421,7 +6464,7 @@
       <c r="J60" s="32"/>
       <c r="K60" s="29"/>
       <c r="L60">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -6442,7 +6485,7 @@
       <c r="J61" s="32"/>
       <c r="K61" s="29"/>
       <c r="L61" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6463,7 +6506,7 @@
       <c r="J62" s="32"/>
       <c r="K62" s="29"/>
       <c r="L62" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6484,7 +6527,7 @@
       <c r="J63" s="32"/>
       <c r="K63" s="29"/>
       <c r="L63" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6505,7 +6548,7 @@
       <c r="J64" s="32"/>
       <c r="K64" s="29"/>
       <c r="L64" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6526,7 +6569,7 @@
       <c r="J65" s="32"/>
       <c r="K65" s="29"/>
       <c r="L65" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -6547,7 +6590,7 @@
       <c r="J66" s="32"/>
       <c r="K66" s="29"/>
       <c r="L66" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6568,7 +6611,7 @@
       <c r="J67" s="32"/>
       <c r="K67" s="29"/>
       <c r="L67" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6589,7 +6632,7 @@
       <c r="J68" s="32"/>
       <c r="K68" s="29"/>
       <c r="L68" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6610,7 +6653,7 @@
       <c r="J69" s="32"/>
       <c r="K69" s="29"/>
       <c r="L69" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -6631,7 +6674,7 @@
       <c r="J70" s="32"/>
       <c r="K70" s="29"/>
       <c r="L70" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6652,7 +6695,7 @@
       <c r="J71" s="32"/>
       <c r="K71" s="29"/>
       <c r="L71">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -6673,7 +6716,7 @@
       <c r="J72" s="32"/>
       <c r="K72" s="29"/>
       <c r="L72" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6694,7 +6737,7 @@
       <c r="J73" s="32"/>
       <c r="K73" s="29"/>
       <c r="L73" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6715,7 +6758,7 @@
       <c r="J74" s="32"/>
       <c r="K74" s="29"/>
       <c r="L74" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6736,7 +6779,7 @@
       <c r="J75" s="32"/>
       <c r="K75" s="29"/>
       <c r="L75" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6757,7 +6800,7 @@
       <c r="J76" s="32"/>
       <c r="K76" s="29"/>
       <c r="L76" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6778,7 +6821,7 @@
       <c r="J77" s="32"/>
       <c r="K77" s="29"/>
       <c r="L77" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6799,7 +6842,7 @@
       <c r="J78" s="32"/>
       <c r="K78" s="29"/>
       <c r="L78" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6820,7 +6863,7 @@
       <c r="J79" s="32"/>
       <c r="K79" s="29"/>
       <c r="L79" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -6841,7 +6884,7 @@
       <c r="J80" s="32"/>
       <c r="K80" s="29"/>
       <c r="L80" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6862,7 +6905,7 @@
       <c r="J81" s="32"/>
       <c r="K81" s="29"/>
       <c r="L81" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6883,7 +6926,7 @@
       <c r="J82" s="32"/>
       <c r="K82" s="29"/>
       <c r="L82" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6904,7 +6947,7 @@
       <c r="J83" s="32"/>
       <c r="K83" s="29"/>
       <c r="L83" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6925,7 +6968,7 @@
       <c r="J84" s="32"/>
       <c r="K84" s="29"/>
       <c r="L84">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -6946,7 +6989,7 @@
       <c r="J85" s="32"/>
       <c r="K85" s="29"/>
       <c r="L85" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6967,7 +7010,7 @@
       <c r="J86" s="32"/>
       <c r="K86" s="29"/>
       <c r="L86" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -6988,7 +7031,7 @@
       <c r="J87" s="32"/>
       <c r="K87" s="29"/>
       <c r="L87" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7009,7 +7052,7 @@
       <c r="J88" s="32"/>
       <c r="K88" s="29"/>
       <c r="L88" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7030,7 +7073,7 @@
       <c r="J89" s="32"/>
       <c r="K89" s="29"/>
       <c r="L89" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -7072,7 +7115,7 @@
       <c r="J92" s="32"/>
       <c r="K92" s="29"/>
       <c r="L92" t="str">
-        <f t="shared" ref="L92:L119" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C92,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L92:L119" ca="1" si="5">INDIRECT(ADDRESS(MATCH(C92,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7093,7 +7136,7 @@
       <c r="J93" s="32"/>
       <c r="K93" s="29"/>
       <c r="L93" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7114,7 +7157,7 @@
       <c r="J94" s="32"/>
       <c r="K94" s="29"/>
       <c r="L94" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7135,7 +7178,7 @@
       <c r="J95" s="32"/>
       <c r="K95" s="29"/>
       <c r="L95" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7156,7 +7199,7 @@
       <c r="J96" s="32"/>
       <c r="K96" s="29"/>
       <c r="L96" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7177,7 +7220,7 @@
       <c r="J97" s="32"/>
       <c r="K97" s="29"/>
       <c r="L97" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -7198,7 +7241,7 @@
       <c r="J98" s="32"/>
       <c r="K98" s="29"/>
       <c r="L98" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7219,7 +7262,7 @@
       <c r="J99" s="32"/>
       <c r="K99" s="29"/>
       <c r="L99" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7240,7 +7283,7 @@
       <c r="J100" s="32"/>
       <c r="K100" s="29"/>
       <c r="L100" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7261,7 +7304,7 @@
       <c r="J101" s="32"/>
       <c r="K101" s="29"/>
       <c r="L101" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7282,7 +7325,7 @@
       <c r="J102" s="32"/>
       <c r="K102" s="29"/>
       <c r="L102" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7303,7 +7346,7 @@
       <c r="J103" s="32"/>
       <c r="K103" s="29"/>
       <c r="L103" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7324,7 +7367,7 @@
       <c r="J104" s="32"/>
       <c r="K104" s="29"/>
       <c r="L104">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7345,7 +7388,7 @@
       <c r="J105" s="32"/>
       <c r="K105" s="29"/>
       <c r="L105" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7366,7 +7409,7 @@
       <c r="J106" s="32"/>
       <c r="K106" s="29"/>
       <c r="L106">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7387,7 +7430,7 @@
       <c r="J107" s="32"/>
       <c r="K107" s="29"/>
       <c r="L107" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7408,7 +7451,7 @@
       <c r="J108" s="32"/>
       <c r="K108" s="29"/>
       <c r="L108">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7429,7 +7472,7 @@
       <c r="J109" s="32"/>
       <c r="K109" s="29"/>
       <c r="L109" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7450,7 +7493,7 @@
       <c r="J110" s="32"/>
       <c r="K110" s="29"/>
       <c r="L110">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7471,7 +7514,7 @@
       <c r="J111" s="32"/>
       <c r="K111" s="29"/>
       <c r="L111">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7492,7 +7535,7 @@
       <c r="J112" s="32"/>
       <c r="K112" s="29"/>
       <c r="L112" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7513,7 +7556,7 @@
       <c r="J113" s="32"/>
       <c r="K113" s="29"/>
       <c r="L113" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7534,7 +7577,7 @@
       <c r="J114" s="32"/>
       <c r="K114" s="29"/>
       <c r="L114" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7556,7 +7599,7 @@
       <c r="J115" s="32"/>
       <c r="K115" s="29"/>
       <c r="L115" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7577,7 +7620,7 @@
       <c r="J116" s="32"/>
       <c r="K116" s="29"/>
       <c r="L116" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -7598,7 +7641,7 @@
       <c r="J117" s="32"/>
       <c r="K117" s="29"/>
       <c r="L117" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7619,7 +7662,7 @@
       <c r="J118" s="32"/>
       <c r="K118" s="29"/>
       <c r="L118" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -7640,7 +7683,7 @@
       <c r="J119" s="32"/>
       <c r="K119" s="29"/>
       <c r="L119" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7673,7 +7716,7 @@
       <c r="J121" s="32"/>
       <c r="K121" s="29"/>
       <c r="L121" t="str">
-        <f t="shared" ref="L121:L139" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C121,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f t="shared" ref="L121:L139" ca="1" si="6">INDIRECT(ADDRESS(MATCH(C121,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7694,7 +7737,7 @@
       <c r="J122" s="32"/>
       <c r="K122" s="29"/>
       <c r="L122" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7715,7 +7758,7 @@
       <c r="J123" s="32"/>
       <c r="K123" s="29"/>
       <c r="L123" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -7736,7 +7779,7 @@
       <c r="J124" s="32"/>
       <c r="K124" s="29"/>
       <c r="L124" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7757,7 +7800,7 @@
       <c r="J125" s="32"/>
       <c r="K125" s="29"/>
       <c r="L125" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7778,7 +7821,7 @@
       <c r="J126" s="32"/>
       <c r="K126" s="29"/>
       <c r="L126" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7799,7 +7842,7 @@
       <c r="J127" s="32"/>
       <c r="K127" s="29"/>
       <c r="L127" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7820,7 +7863,7 @@
       <c r="J128" s="32"/>
       <c r="K128" s="29"/>
       <c r="L128" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7841,7 +7884,7 @@
       <c r="J129" s="32"/>
       <c r="K129" s="29"/>
       <c r="L129" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7862,7 +7905,7 @@
       <c r="J130" s="32"/>
       <c r="K130" s="29"/>
       <c r="L130" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7883,7 +7926,7 @@
       <c r="J131" s="32"/>
       <c r="K131" s="29"/>
       <c r="L131" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7904,7 +7947,7 @@
       <c r="J132" s="32"/>
       <c r="K132" s="29"/>
       <c r="L132" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7926,7 +7969,7 @@
       <c r="J133" s="32"/>
       <c r="K133" s="29"/>
       <c r="L133" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -7947,7 +7990,7 @@
       <c r="J134" s="32"/>
       <c r="K134" s="29"/>
       <c r="L134" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7968,7 +8011,7 @@
       <c r="J135" s="32"/>
       <c r="K135" s="29"/>
       <c r="L135" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -7989,7 +8032,7 @@
       <c r="J136" s="32"/>
       <c r="K136" s="29"/>
       <c r="L136" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -8010,7 +8053,7 @@
       <c r="J137" s="32"/>
       <c r="K137" s="29"/>
       <c r="L137" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -8031,7 +8074,7 @@
       <c r="J138" s="32"/>
       <c r="K138" s="29"/>
       <c r="L138" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -8052,7 +8095,7 @@
       <c r="J139" s="32"/>
       <c r="K139" s="29"/>
       <c r="L139" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>Habs</v>
       </c>
     </row>
@@ -8135,7 +8178,7 @@
     </row>
     <row r="146" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="27">
-        <f t="shared" ref="B146" si="3">ROUNDUP(I146/G146,0)</f>
+        <f t="shared" ref="B146:B155" si="7">ROUNDUP(I146/G146,0)</f>
         <v>0</v>
       </c>
       <c r="C146" s="26" t="s">
@@ -8151,15 +8194,15 @@
         <v>2.5</v>
       </c>
       <c r="I146" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C146,B$1:B$144)</f>
+        <f t="shared" ref="I146:I155" si="8">SUMIF(C$1:C$144,"="&amp;C146,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J146" s="32">
-        <f t="shared" ref="J146" si="4">G146*B146-I146</f>
+        <f t="shared" ref="J146:J155" si="9">G146*B146-I146</f>
         <v>0</v>
       </c>
       <c r="K146" s="29">
-        <f t="shared" ref="K146:K245" si="5">B146*H146</f>
+        <f>B146*H146</f>
         <v>0</v>
       </c>
       <c r="L146" t="s">
@@ -8168,7 +8211,7 @@
     </row>
     <row r="147" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="27">
-        <f t="shared" ref="B147" si="6">ROUNDUP(I147/G147,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C147" s="26" t="s">
@@ -8184,15 +8227,15 @@
         <v>2.5</v>
       </c>
       <c r="I147" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C147,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J147" s="32">
-        <f t="shared" ref="J147" si="7">G147*B147-I147</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K147" s="29">
-        <f t="shared" ref="K147" si="8">B147*H147</f>
+        <f>B147*H147</f>
         <v>0</v>
       </c>
       <c r="L147" t="s">
@@ -8201,7 +8244,7 @@
     </row>
     <row r="148" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="27">
-        <f>ROUNDUP(I148/G148,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C148" s="26" t="s">
@@ -8217,11 +8260,11 @@
         <v>2.5</v>
       </c>
       <c r="I148" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C148,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="J148" s="32">
-        <f>G148*B148-I148</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K148" s="29">
@@ -8234,7 +8277,7 @@
     </row>
     <row r="149" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="27">
-        <f t="shared" ref="B149" si="9">ROUNDUP(I149/G149,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C149" s="26" t="s">
@@ -8250,15 +8293,15 @@
         <v>2.5</v>
       </c>
       <c r="I149" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C149,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="J149" s="32">
-        <f>G149*B149-I149</f>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="K149" s="29">
-        <f t="shared" ref="K149" si="10">B149*H149</f>
+        <f>B149*H149</f>
         <v>2.5</v>
       </c>
       <c r="L149" t="s">
@@ -8267,7 +8310,7 @@
     </row>
     <row r="150" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="27">
-        <f t="shared" ref="B150" si="11">ROUNDUP(I150/G150,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C150" s="26" t="s">
@@ -8283,15 +8326,15 @@
         <v>2.5</v>
       </c>
       <c r="I150" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C150,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="J150" s="32">
-        <f>G150*B150-I150</f>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K150" s="29">
-        <f t="shared" ref="K150:K155" si="12">B150*H150</f>
+        <f t="shared" ref="K150:K155" si="10">B150*H150</f>
         <v>2.5</v>
       </c>
       <c r="L150" t="s">
@@ -8300,7 +8343,7 @@
     </row>
     <row r="151" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B151" s="27">
-        <f>ROUNDUP(I151/G151,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C151" s="26" t="s">
@@ -8316,15 +8359,15 @@
         <v>2.5</v>
       </c>
       <c r="I151" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C151,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J151" s="32">
-        <f t="shared" ref="J151" si="13">G151*B151-I151</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K151" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L151" t="s">
@@ -8333,7 +8376,7 @@
     </row>
     <row r="152" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B152" s="27">
-        <f>ROUNDUP(I152/G152,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C152" s="26" t="s">
@@ -8349,15 +8392,15 @@
         <v>2.5</v>
       </c>
       <c r="I152" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C152,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="J152" s="32">
-        <f>G152*B152-I152</f>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="K152" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="L152" t="s">
@@ -8366,7 +8409,7 @@
     </row>
     <row r="153" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="27">
-        <f>ROUNDUP(I153/G153,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C153" s="26" t="s">
@@ -8382,15 +8425,15 @@
         <v>2.5</v>
       </c>
       <c r="I153" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C153,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="J153" s="32">
-        <f t="shared" ref="J153" si="14">G153*B153-I153</f>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="K153" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="L153" t="s">
@@ -8399,7 +8442,7 @@
     </row>
     <row r="154" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="27">
-        <f>ROUNDUP(I154/G154,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C154" s="26" t="s">
@@ -8415,15 +8458,15 @@
         <v>1.8</v>
       </c>
       <c r="I154" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C154,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="J154" s="32">
-        <f>G154*B154-I154</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K154" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.8</v>
       </c>
       <c r="L154" t="s">
@@ -8432,7 +8475,7 @@
     </row>
     <row r="155" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="27">
-        <f>ROUNDUP(I155/G155,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C155" s="26" t="s">
@@ -8448,15 +8491,15 @@
         <v>1.8</v>
       </c>
       <c r="I155" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C155,B$1:B$144)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J155" s="32">
-        <f>G155*B155-I155</f>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="K155" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.8</v>
       </c>
       <c r="L155" t="s">
@@ -8474,7 +8517,7 @@
     </row>
     <row r="157" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="27">
-        <f t="shared" ref="B157" si="15">ROUNDUP(I157/G157,0)</f>
+        <f>ROUNDUP(I157/G157,0)</f>
         <v>1</v>
       </c>
       <c r="C157" s="26" t="s">
@@ -8494,11 +8537,11 @@
         <v>20</v>
       </c>
       <c r="J157" s="32">
-        <f t="shared" ref="J157" si="16">G157*B157-I157</f>
+        <f>G157*B157-I157</f>
         <v>30</v>
       </c>
       <c r="K157" s="29">
-        <f t="shared" ref="K157" si="17">B157*H157</f>
+        <f>B157*H157</f>
         <v>2.99</v>
       </c>
       <c r="L157" t="s">
@@ -8507,7 +8550,7 @@
     </row>
     <row r="158" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B158" s="27">
-        <f t="shared" ref="B158" si="18">ROUNDUP(I158/G158,0)</f>
+        <f>ROUNDUP(I158/G158,0)</f>
         <v>0</v>
       </c>
       <c r="C158" s="26" t="s">
@@ -8530,11 +8573,11 @@
         <v>0</v>
       </c>
       <c r="J158" s="32">
-        <f t="shared" ref="J158" si="19">G158*B158-I158</f>
+        <f>G158*B158-I158</f>
         <v>0</v>
       </c>
       <c r="K158" s="29">
-        <f t="shared" ref="K158" si="20">B158*H158</f>
+        <f>B158*H158</f>
         <v>0</v>
       </c>
       <c r="L158" t="s">
@@ -8543,7 +8586,7 @@
     </row>
     <row r="159" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="27">
-        <f t="shared" ref="B159:B177" si="21">ROUNDUP(I159/G159,0)</f>
+        <f>ROUNDUP(I159/G159,0)</f>
         <v>1</v>
       </c>
       <c r="C159" s="26" t="s">
@@ -8563,11 +8606,11 @@
         <v>10</v>
       </c>
       <c r="J159" s="32">
-        <f t="shared" ref="J159:J242" si="22">G159*B159-I159</f>
+        <f>G159*B159-I159</f>
         <v>90</v>
       </c>
       <c r="K159" s="29">
-        <f t="shared" si="5"/>
+        <f>B159*H159</f>
         <v>2.09</v>
       </c>
       <c r="L159" t="s">
@@ -8576,7 +8619,7 @@
     </row>
     <row r="160" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B160" s="27">
-        <f t="shared" ref="B160" si="23">ROUNDUP(I160/G160,0)</f>
+        <f>ROUNDUP(I160/G160,0)</f>
         <v>1</v>
       </c>
       <c r="C160" s="26" t="s">
@@ -8596,11 +8639,11 @@
         <v>10</v>
       </c>
       <c r="J160" s="32">
-        <f t="shared" ref="J160" si="24">G160*B160-I160</f>
+        <f>G160*B160-I160</f>
         <v>90</v>
       </c>
       <c r="K160" s="29">
-        <f t="shared" si="5"/>
+        <f>B160*H160</f>
         <v>2.09</v>
       </c>
       <c r="L160" t="s">
@@ -8609,7 +8652,7 @@
     </row>
     <row r="161" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B161" s="27">
-        <f t="shared" ref="B161:B163" si="25">ROUNDUP(I161/G161,0)</f>
+        <f>ROUNDUP(I161/G161,0)</f>
         <v>0</v>
       </c>
       <c r="C161" s="26" t="s">
@@ -8629,11 +8672,11 @@
         <v>0</v>
       </c>
       <c r="J161" s="32">
-        <f t="shared" ref="J161:J163" si="26">G161*B161-I161</f>
+        <f>G161*B161-I161</f>
         <v>0</v>
       </c>
       <c r="K161" s="29">
-        <f t="shared" ref="K161:K163" si="27">B161*H161</f>
+        <f>B161*H161</f>
         <v>0</v>
       </c>
       <c r="L161" t="s">
@@ -8651,7 +8694,7 @@
     </row>
     <row r="163" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B163" s="27">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="B163:B179" si="11">ROUNDUP(I163/G163,0)</f>
         <v>1</v>
       </c>
       <c r="C163" s="26" t="s">
@@ -8667,15 +8710,15 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="I163" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C163,B$1:B$144)</f>
+        <f t="shared" ref="I163:I179" si="12">SUMIF(C$1:C$144,"="&amp;C163,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J163" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="J163:J179" si="13">G163*B163-I163</f>
         <v>49</v>
       </c>
       <c r="K163" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="K163:K179" si="14">B163*H163</f>
         <v>4.8899999999999997</v>
       </c>
       <c r="L163" t="s">
@@ -8684,7 +8727,7 @@
     </row>
     <row r="164" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="27">
-        <f t="shared" ref="B164" si="28">ROUNDUP(I164/G164,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C164" s="26" t="s">
@@ -8700,15 +8743,15 @@
         <v>2.29</v>
       </c>
       <c r="I164" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C164,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="J164" s="32">
-        <f t="shared" ref="J164" si="29">G164*B164-I164</f>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="K164" s="29">
-        <f t="shared" ref="K164" si="30">B164*H164</f>
+        <f t="shared" si="14"/>
         <v>2.29</v>
       </c>
       <c r="L164" t="s">
@@ -8717,7 +8760,7 @@
     </row>
     <row r="165" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B165" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C165" s="26" t="s">
@@ -8733,15 +8776,15 @@
         <v>1.79</v>
       </c>
       <c r="I165" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C165,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="J165" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="13"/>
         <v>93</v>
       </c>
       <c r="K165" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1.79</v>
       </c>
       <c r="L165" t="s">
@@ -8750,7 +8793,7 @@
     </row>
     <row r="166" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C166" s="26" t="s">
@@ -8766,15 +8809,15 @@
         <v>1.79</v>
       </c>
       <c r="I166" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C166,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="J166" s="32">
-        <f>G166*B166-I166</f>
+        <f t="shared" si="13"/>
         <v>96</v>
       </c>
       <c r="K166" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1.79</v>
       </c>
       <c r="L166" t="s">
@@ -8783,7 +8826,7 @@
     </row>
     <row r="167" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="27">
-        <f t="shared" ref="B167:B168" si="31">ROUNDUP(I167/G167,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C167" s="26" t="s">
@@ -8799,15 +8842,15 @@
         <v>4.33</v>
       </c>
       <c r="I167" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C167,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J167" s="32">
-        <f>G167*B167-I167</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K167" s="29">
-        <f t="shared" ref="K167:K168" si="32">B167*H167</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L167" t="s">
@@ -8816,7 +8859,7 @@
     </row>
     <row r="168" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="27">
-        <f t="shared" si="31"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="C168" s="26" t="s">
@@ -8832,15 +8875,15 @@
         <v>1.98</v>
       </c>
       <c r="I168" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C168,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="J168" s="32">
-        <f>G168*B168-I168</f>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="K168" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="14"/>
         <v>3.96</v>
       </c>
       <c r="L168" t="s">
@@ -8849,7 +8892,7 @@
     </row>
     <row r="169" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="27">
-        <f t="shared" ref="B169:B170" si="33">ROUNDUP(I169/G169,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C169" s="26" t="s">
@@ -8865,15 +8908,15 @@
         <v>1.98</v>
       </c>
       <c r="I169" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C169,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J169" s="32">
-        <f>G169*B169-I169</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K169" s="29">
-        <f t="shared" ref="K169:K170" si="34">B169*H169</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L169" t="s">
@@ -8882,7 +8925,7 @@
     </row>
     <row r="170" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C170" s="26" t="s">
@@ -8898,15 +8941,15 @@
         <v>1.98</v>
       </c>
       <c r="I170" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C170,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J170" s="32">
-        <f>G170*B170-I170</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K170" s="29">
-        <f t="shared" si="34"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L170" t="s">
@@ -8915,7 +8958,7 @@
     </row>
     <row r="171" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B171" s="27">
-        <f>ROUNDUP(I171/G171,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C171" s="26" t="s">
@@ -8931,15 +8974,15 @@
         <v>4.49</v>
       </c>
       <c r="I171" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C171,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="J171" s="32">
-        <f t="shared" ref="J171" si="35">G171*B171-I171</f>
+        <f t="shared" si="13"/>
         <v>460</v>
       </c>
       <c r="K171" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>4.49</v>
       </c>
       <c r="L171" t="s">
@@ -8948,7 +8991,7 @@
     </row>
     <row r="172" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B172" s="27">
-        <f>ROUNDUP(I172/G172,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C172" s="26" t="s">
@@ -8964,15 +9007,15 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="I172" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C172,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>168</v>
       </c>
       <c r="J172" s="32">
-        <f t="shared" ref="J172:J173" si="36">G172*B172-I172</f>
+        <f t="shared" si="13"/>
         <v>332</v>
       </c>
       <c r="K172" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="L172" t="s">
@@ -8981,7 +9024,7 @@
     </row>
     <row r="173" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B173" s="27">
-        <f>ROUNDUP(I173/G173,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C173" s="26" t="s">
@@ -8997,15 +9040,15 @@
         <v>4.49</v>
       </c>
       <c r="I173" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C173,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>192</v>
       </c>
       <c r="J173" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="13"/>
         <v>308</v>
       </c>
       <c r="K173" s="29">
-        <f t="shared" ref="K173" si="37">B173*H173</f>
+        <f t="shared" si="14"/>
         <v>4.49</v>
       </c>
       <c r="L173" t="s">
@@ -9014,7 +9057,7 @@
     </row>
     <row r="174" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B174" s="27">
-        <f>ROUNDUP(I174/G174,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C174" s="26" t="s">
@@ -9030,15 +9073,15 @@
         <v>4.49</v>
       </c>
       <c r="I174" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C174,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>144</v>
       </c>
       <c r="J174" s="32">
-        <f t="shared" ref="J174" si="38">G174*B174-I174</f>
+        <f t="shared" si="13"/>
         <v>356</v>
       </c>
       <c r="K174" s="29">
-        <f t="shared" ref="K174" si="39">B174*H174</f>
+        <f t="shared" si="14"/>
         <v>4.49</v>
       </c>
       <c r="L174" t="s">
@@ -9047,7 +9090,7 @@
     </row>
     <row r="175" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B175" s="27">
-        <f>ROUNDUP(I175/G175,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C175" s="26" t="s">
@@ -9063,15 +9106,15 @@
         <v>1.59</v>
       </c>
       <c r="I175" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C175,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="J175" s="32">
-        <f t="shared" ref="J175" si="40">G175*B175-I175</f>
+        <f t="shared" si="13"/>
         <v>88</v>
       </c>
       <c r="K175" s="29">
-        <f t="shared" ref="K175" si="41">B175*H175</f>
+        <f t="shared" si="14"/>
         <v>1.59</v>
       </c>
       <c r="L175" t="s">
@@ -9080,7 +9123,7 @@
     </row>
     <row r="176" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="C176" s="26" t="s">
@@ -9096,15 +9139,15 @@
         <v>0.3</v>
       </c>
       <c r="I176" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C176,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
       <c r="J176" s="32">
-        <f t="shared" ref="J176" si="42">G176*B176-I176</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K176" s="29">
-        <f t="shared" ref="K176" si="43">B176*H176</f>
+        <f t="shared" si="14"/>
         <v>10.5</v>
       </c>
       <c r="L176" t="s">
@@ -9113,7 +9156,7 @@
     </row>
     <row r="177" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C177" s="26" t="s">
@@ -9129,15 +9172,15 @@
         <v>2.09</v>
       </c>
       <c r="I177" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C177,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J177" s="32">
-        <f t="shared" ref="J177" si="44">G177*B177-I177</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K177" s="29">
-        <f t="shared" ref="K177" si="45">B177*H177</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L177" t="s">
@@ -9146,7 +9189,7 @@
     </row>
     <row r="178" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="27">
-        <f>ROUNDUP(I178/G178,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C178" s="26" t="s">
@@ -9162,15 +9205,15 @@
         <v>1.69</v>
       </c>
       <c r="I178" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C178,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>300</v>
       </c>
       <c r="J178" s="32">
-        <f t="shared" ref="J178" si="46">G178*B178-I178</f>
+        <f t="shared" si="13"/>
         <v>200</v>
       </c>
       <c r="K178" s="29">
-        <f>B178*H178</f>
+        <f t="shared" si="14"/>
         <v>1.69</v>
       </c>
       <c r="L178" t="s">
@@ -9179,7 +9222,7 @@
     </row>
     <row r="179" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="27">
-        <f>ROUNDUP(I179/G179,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="C179" t="s">
@@ -9195,15 +9238,15 @@
         <v>0.45</v>
       </c>
       <c r="I179" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C179,B$1:B$144)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="J179" s="32">
-        <f t="shared" ref="J179" si="47">G179*B179-I179</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K179" s="29">
-        <f>B179*H179</f>
+        <f t="shared" si="14"/>
         <v>0.45</v>
       </c>
       <c r="L179" t="s">
@@ -9219,7 +9262,7 @@
     </row>
     <row r="181" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B181" s="27">
-        <f>ROUNDUP(I181/G181,0)</f>
+        <f t="shared" ref="B181:B193" si="15">ROUNDUP(I181/G181,0)</f>
         <v>0</v>
       </c>
       <c r="C181" s="26" t="s">
@@ -9235,15 +9278,15 @@
         <v>4.96</v>
       </c>
       <c r="I181" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C181,B$1:B$144)</f>
+        <f t="shared" ref="I181:I193" si="16">SUMIF(C$1:C$144,"="&amp;C181,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J181" s="32">
-        <f>G181*B181-I181</f>
+        <f t="shared" ref="J181:J193" si="17">G181*B181-I181</f>
         <v>0</v>
       </c>
       <c r="K181" s="29">
-        <f>B181*H181</f>
+        <f t="shared" ref="K181:K193" si="18">B181*H181</f>
         <v>0</v>
       </c>
       <c r="L181" t="s">
@@ -9252,7 +9295,7 @@
     </row>
     <row r="182" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B182" s="27">
-        <f>ROUNDUP(I182/G182,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="C182" s="26" t="s">
@@ -9268,15 +9311,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I182" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C182,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="J182" s="32">
-        <f t="shared" ref="J182" si="48">G182*B182-I182</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K182" s="29">
-        <f>B182*H182</f>
+        <f t="shared" si="18"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="L182" t="s">
@@ -9285,7 +9328,7 @@
     </row>
     <row r="183" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="27">
-        <f>ROUNDUP(I183/G183,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="C183" s="26" t="s">
@@ -9301,15 +9344,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I183" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C183,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="J183" s="32">
-        <f>G183*B183-I183</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K183" s="29">
-        <f>B183*H183</f>
+        <f t="shared" si="18"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="L183" t="s">
@@ -9318,7 +9361,7 @@
     </row>
     <row r="184" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="27">
-        <f t="shared" ref="B184" si="49">ROUNDUP(I184/G184,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C184" s="26" t="s">
@@ -9334,15 +9377,15 @@
         <v>4.96</v>
       </c>
       <c r="I184" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C184,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J184" s="32">
-        <f t="shared" ref="J184" si="50">G184*B184-I184</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K184" s="29">
-        <f t="shared" ref="K184" si="51">B184*H184</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L184" t="s">
@@ -9351,7 +9394,7 @@
     </row>
     <row r="185" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="27">
-        <f>ROUNDUP(I185/G185,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C185" s="26" t="s">
@@ -9367,15 +9410,15 @@
         <v>4.54</v>
       </c>
       <c r="I185" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C185,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J185" s="32">
-        <f>G185*B185-I185</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K185" s="29">
-        <f>B185*H185</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L185" t="s">
@@ -9384,7 +9427,7 @@
     </row>
     <row r="186" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B186" s="27">
-        <f t="shared" ref="B186" si="52">ROUNDUP(I186/G186,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C186" s="26" t="s">
@@ -9400,15 +9443,15 @@
         <v>4.54</v>
       </c>
       <c r="I186" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C186,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J186" s="32">
-        <f t="shared" ref="J186" si="53">G186*B186-I186</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K186" s="29">
-        <f t="shared" ref="K186" si="54">B186*H186</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L186" t="s">
@@ -9417,7 +9460,7 @@
     </row>
     <row r="187" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="27">
-        <f t="shared" ref="B187" si="55">ROUNDUP(I187/G187,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C187" s="26" t="s">
@@ -9433,15 +9476,15 @@
         <v>4.54</v>
       </c>
       <c r="I187" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C187,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J187" s="32">
-        <f t="shared" ref="J187" si="56">G187*B187-I187</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K187" s="29">
-        <f t="shared" ref="K187" si="57">B187*H187</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L187" t="s">
@@ -9450,7 +9493,7 @@
     </row>
     <row r="188" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B188" s="27">
-        <f t="shared" ref="B188:B190" si="58">ROUNDUP(I188/G188,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C188" s="26" t="s">
@@ -9466,15 +9509,15 @@
         <v>5.44</v>
       </c>
       <c r="I188" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C188,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J188" s="32">
-        <f t="shared" ref="J188:J190" si="59">G188*B188-I188</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K188" s="29">
-        <f t="shared" ref="K188:K190" si="60">B188*H188</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L188" t="s">
@@ -9483,7 +9526,7 @@
     </row>
     <row r="189" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="27">
-        <f t="shared" ref="B189" si="61">ROUNDUP(I189/G189,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C189" s="26" t="s">
@@ -9499,15 +9542,15 @@
         <v>5.44</v>
       </c>
       <c r="I189" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C189,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J189" s="32">
-        <f t="shared" ref="J189" si="62">G189*B189-I189</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K189" s="29">
-        <f t="shared" ref="K189" si="63">B189*H189</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L189" t="s">
@@ -9516,7 +9559,7 @@
     </row>
     <row r="190" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B190" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C190" s="26" t="s">
@@ -9532,15 +9575,15 @@
         <v>5.44</v>
       </c>
       <c r="I190" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C190,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J190" s="32">
-        <f t="shared" si="59"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K190" s="29">
-        <f t="shared" si="60"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L190" t="s">
@@ -9549,7 +9592,7 @@
     </row>
     <row r="191" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="27">
-        <f t="shared" ref="B191" si="64">ROUNDUP(I191/G191,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C191" s="26" t="s">
@@ -9565,15 +9608,15 @@
         <v>5.44</v>
       </c>
       <c r="I191" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C191,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J191" s="32">
-        <f t="shared" ref="J191" si="65">G191*B191-I191</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K191" s="29">
-        <f t="shared" ref="K191" si="66">B191*H191</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L191" t="s">
@@ -9582,7 +9625,7 @@
     </row>
     <row r="192" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B192" s="27">
-        <f t="shared" ref="B192:B249" si="67">ROUNDUP(I192/G192,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C192" s="26" t="s">
@@ -9598,15 +9641,15 @@
         <v>5.44</v>
       </c>
       <c r="I192" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C192,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J192" s="32">
-        <f t="shared" ref="J192" si="68">G192*B192-I192</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K192" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L192" t="s">
@@ -9615,7 +9658,7 @@
     </row>
     <row r="193" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="C193" s="26" t="s">
@@ -9631,15 +9674,15 @@
         <v>6.34</v>
       </c>
       <c r="I193" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C193,B$1:B$144)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J193" s="32">
-        <f t="shared" ref="J193" si="69">G193*B193-I193</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K193" s="29">
-        <f t="shared" ref="K193" si="70">B193*H193</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L193" t="s">
@@ -9657,7 +9700,7 @@
     </row>
     <row r="195" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="27">
-        <f>ROUNDUP(I195/G195,0)</f>
+        <f t="shared" ref="B195:B202" si="19">ROUNDUP(I195/G195,0)</f>
         <v>1</v>
       </c>
       <c r="C195" s="26" t="s">
@@ -9673,15 +9716,15 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="I195" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C195,B$1:B$144)</f>
+        <f t="shared" ref="I195:I202" si="20">SUMIF(C$1:C$144,"="&amp;C195,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J195" s="32">
-        <f t="shared" ref="J195" si="71">G195*B195-I195</f>
+        <f t="shared" ref="J195:J202" si="21">G195*B195-I195</f>
         <v>0</v>
       </c>
       <c r="K195" s="29">
-        <f t="shared" ref="K195" si="72">B195*H195</f>
+        <f t="shared" ref="K195:K202" si="22">B195*H195</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="L195" t="s">
@@ -9690,7 +9733,7 @@
     </row>
     <row r="196" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="27">
-        <f t="shared" ref="B196" si="73">ROUNDUP(I196/G196,0)</f>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="C196" s="26" t="s">
@@ -9706,15 +9749,15 @@
         <v>5.07</v>
       </c>
       <c r="I196" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C196,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="J196" s="32">
-        <f t="shared" ref="J196" si="74">G196*B196-I196</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K196" s="29">
-        <f t="shared" ref="K196" si="75">B196*H196</f>
+        <f t="shared" si="22"/>
         <v>10.14</v>
       </c>
       <c r="L196" t="s">
@@ -9723,7 +9766,7 @@
     </row>
     <row r="197" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="27">
-        <f>ROUNDUP(I197/G197,0)</f>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="C197" s="26" t="s">
@@ -9739,15 +9782,15 @@
         <v>5.23</v>
       </c>
       <c r="I197" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C197,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="J197" s="32">
-        <f t="shared" ref="J197" si="76">G197*B197-I197</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K197" s="29">
-        <f t="shared" ref="K197" si="77">B197*H197</f>
+        <f t="shared" si="22"/>
         <v>10.46</v>
       </c>
       <c r="L197" t="s">
@@ -9756,7 +9799,7 @@
     </row>
     <row r="198" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B198" s="27">
-        <f t="shared" ref="B198" si="78">ROUNDUP(I198/G198,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C198" s="26" t="s">
@@ -9772,15 +9815,15 @@
         <v>5.23</v>
       </c>
       <c r="I198" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C198,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J198" s="32">
-        <f t="shared" ref="J198" si="79">G198*B198-I198</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K198" s="29">
-        <f t="shared" ref="K198" si="80">B198*H198</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L198" t="s">
@@ -9789,7 +9832,7 @@
     </row>
     <row r="199" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B199" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C199" s="26" t="s">
@@ -9805,15 +9848,15 @@
         <v>5.23</v>
       </c>
       <c r="I199" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C199,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J199" s="32">
-        <f t="shared" ref="J199" si="81">G199*B199-I199</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K199" s="29">
-        <f t="shared" ref="K199" si="82">B199*H199</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L199" t="s">
@@ -9822,7 +9865,7 @@
     </row>
     <row r="200" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B200" s="27">
-        <f t="shared" ref="B200" si="83">ROUNDUP(I200/G200,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C200" s="26" t="s">
@@ -9838,15 +9881,15 @@
         <v>6.67</v>
       </c>
       <c r="I200" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C200,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J200" s="32">
-        <f>G200*B200-I200</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K200" s="29">
-        <f>B200*H200</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L200" t="s">
@@ -9855,7 +9898,7 @@
     </row>
     <row r="201" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="27">
-        <f t="shared" ref="B201" si="84">ROUNDUP(I201/G201,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C201" s="26" t="s">
@@ -9871,15 +9914,15 @@
         <v>6.67</v>
       </c>
       <c r="I201" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C201,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J201" s="32">
-        <f t="shared" ref="J201" si="85">G201*B201-I201</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K201" s="29">
-        <f t="shared" ref="K201" si="86">B201*H201</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L201" t="s">
@@ -9888,7 +9931,7 @@
     </row>
     <row r="202" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="27">
-        <f>ROUNDUP(I202/G202,0)</f>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="C202" s="26" t="s">
@@ -9904,15 +9947,15 @@
         <v>11.6</v>
       </c>
       <c r="I202" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C202,B$1:B$144)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="J202" s="32">
-        <f>G202*B202-I202</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K202" s="29">
-        <f>B202*H202</f>
+        <f t="shared" si="22"/>
         <v>23.2</v>
       </c>
       <c r="L202" t="s">
@@ -9930,7 +9973,7 @@
     </row>
     <row r="204" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" s="27">
-        <f t="shared" ref="B204" si="87">ROUNDUP(I204/G204,0)</f>
+        <f t="shared" ref="B204:B214" si="23">ROUNDUP(I204/G204,0)</f>
         <v>1</v>
       </c>
       <c r="C204" s="26" t="s">
@@ -9946,15 +9989,15 @@
         <v>4</v>
       </c>
       <c r="I204" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C204,B$1:B$144)</f>
+        <f t="shared" ref="I204:I222" si="24">SUMIF(C$1:C$144,"="&amp;C204,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J204" s="32">
-        <f>G204*B204-I204</f>
+        <f t="shared" ref="J204:J222" si="25">G204*B204-I204</f>
         <v>0</v>
       </c>
       <c r="K204" s="29">
-        <f t="shared" ref="K204:K209" si="88">B204*H204</f>
+        <f t="shared" ref="K204:K209" si="26">B204*H204</f>
         <v>4</v>
       </c>
       <c r="L204" t="s">
@@ -9963,7 +10006,7 @@
     </row>
     <row r="205" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="27">
-        <f t="shared" ref="B205" si="89">ROUNDUP(I205/G205,0)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C205" s="26" t="s">
@@ -9979,15 +10022,15 @@
         <v>4.24</v>
       </c>
       <c r="I205" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C205,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="J205" s="32">
-        <f t="shared" ref="J205" si="90">G205*B205-I205</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K205" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="26"/>
         <v>4.24</v>
       </c>
       <c r="L205" t="s">
@@ -9996,7 +10039,7 @@
     </row>
     <row r="206" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="27">
-        <f>ROUNDUP(I206/G206,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C206" s="26" t="s">
@@ -10012,15 +10055,15 @@
         <v>4.24</v>
       </c>
       <c r="I206" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C206,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J206" s="32">
-        <f t="shared" ref="J206" si="91">G206*B206-I206</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K206" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L206" t="s">
@@ -10029,7 +10072,7 @@
     </row>
     <row r="207" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B207" s="27">
-        <f t="shared" ref="B207" si="92">ROUNDUP(I207/G207,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C207" s="26" t="s">
@@ -10045,15 +10088,15 @@
         <v>4</v>
       </c>
       <c r="I207" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C207,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J207" s="32">
-        <f>G207*B207-I207</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K207" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L207" t="s">
@@ -10062,7 +10105,7 @@
     </row>
     <row r="208" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B208" s="27">
-        <f>ROUNDUP(I208/G208,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C208" s="26" t="s">
@@ -10078,15 +10121,15 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="I208" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C208,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J208" s="32">
-        <f t="shared" ref="J208" si="93">G208*B208-I208</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K208" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L208" t="s">
@@ -10095,7 +10138,7 @@
     </row>
     <row r="209" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B209" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C209" s="26" t="s">
@@ -10111,15 +10154,15 @@
         <v>4.96</v>
       </c>
       <c r="I209" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C209,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J209" s="32">
-        <f>G209*B209-I209</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K209" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L209" t="s">
@@ -10128,7 +10171,7 @@
     </row>
     <row r="210" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B210" s="27">
-        <f t="shared" ref="B210" si="94">ROUNDUP(I210/G210,0)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C210" s="26" t="s">
@@ -10144,15 +10187,15 @@
         <v>4.96</v>
       </c>
       <c r="I210" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C210,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="J210" s="32">
-        <f>G210*B210-I210</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K210" s="29">
-        <f t="shared" ref="K210" si="95">B210*H210</f>
+        <f t="shared" ref="K210:K222" si="27">B210*H210</f>
         <v>4.96</v>
       </c>
       <c r="L210" t="s">
@@ -10161,7 +10204,7 @@
     </row>
     <row r="211" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B211" s="27">
-        <f t="shared" ref="B211:B214" si="96">ROUNDUP(I211/G211,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C211" s="26" t="s">
@@ -10177,15 +10220,15 @@
         <v>4.96</v>
       </c>
       <c r="I211" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C211,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J211" s="32">
-        <f>G211*B211-I211</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K211" s="29">
-        <f t="shared" ref="K211:K213" si="97">B211*H211</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L211" t="s">
@@ -10194,7 +10237,7 @@
     </row>
     <row r="212" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B212" s="27">
-        <f t="shared" si="96"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C212" s="26" t="s">
@@ -10210,15 +10253,15 @@
         <v>4</v>
       </c>
       <c r="I212" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C212,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J212" s="32">
-        <f>G212*B212-I212</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K212" s="29">
-        <f t="shared" si="97"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L212" t="s">
@@ -10227,7 +10270,7 @@
     </row>
     <row r="213" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B213" s="27">
-        <f t="shared" ref="B213" si="98">ROUNDUP(I213/G213,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="C213" s="26" t="s">
@@ -10243,15 +10286,15 @@
         <v>4.96</v>
       </c>
       <c r="I213" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C213,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J213" s="32">
-        <f>G213*B213-I213</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K213" s="29">
-        <f t="shared" si="97"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L213" t="s">
@@ -10260,7 +10303,7 @@
     </row>
     <row r="214" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B214" s="27">
-        <f t="shared" si="96"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C214" s="26" t="s">
@@ -10276,15 +10319,15 @@
         <v>4.96</v>
       </c>
       <c r="I214" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C214,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="J214" s="32">
-        <f>G214*B214-I214</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K214" s="29">
-        <f t="shared" ref="K214" si="99">B214*H214</f>
+        <f t="shared" si="27"/>
         <v>4.96</v>
       </c>
       <c r="L214" t="s">
@@ -10293,7 +10336,7 @@
     </row>
     <row r="215" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B215" s="27">
-        <f t="shared" ref="B215:B220" si="100">ROUNDUP(I215/G215,0)</f>
+        <f t="shared" ref="B215:B220" si="28">ROUNDUP(I215/G215,0)</f>
         <v>0</v>
       </c>
       <c r="C215" s="26" t="s">
@@ -10309,15 +10352,15 @@
         <v>7.13</v>
       </c>
       <c r="I215" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C215,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J215" s="32">
-        <f t="shared" ref="J215:J217" si="101">G215*B215-I215</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K215" s="29">
-        <f t="shared" ref="K215:K217" si="102">B215*H215</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L215" t="s">
@@ -10326,7 +10369,7 @@
     </row>
     <row r="216" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B216" s="27">
-        <f t="shared" si="100"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="C216" s="26" t="s">
@@ -10342,15 +10385,15 @@
         <v>7.88</v>
       </c>
       <c r="I216" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C216,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="J216" s="32">
-        <f t="shared" ref="J216" si="103">G216*B216-I216</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K216" s="29">
-        <f t="shared" ref="K216" si="104">B216*H216</f>
+        <f t="shared" si="27"/>
         <v>15.76</v>
       </c>
       <c r="L216" t="s">
@@ -10359,7 +10402,7 @@
     </row>
     <row r="217" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B217" s="27">
-        <f t="shared" si="100"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="C217" s="26" t="s">
@@ -10375,15 +10418,15 @@
         <v>7.88</v>
       </c>
       <c r="I217" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C217,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="J217" s="32">
-        <f t="shared" si="101"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K217" s="29">
-        <f t="shared" si="102"/>
+        <f t="shared" si="27"/>
         <v>15.76</v>
       </c>
       <c r="L217" t="s">
@@ -10392,7 +10435,7 @@
     </row>
     <row r="218" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B218" s="27">
-        <f t="shared" si="100"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="C218" s="26" t="s">
@@ -10408,15 +10451,15 @@
         <v>7.88</v>
       </c>
       <c r="I218" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C218,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="J218" s="32">
-        <f t="shared" ref="J218" si="105">G218*B218-I218</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K218" s="29">
-        <f t="shared" ref="K218" si="106">B218*H218</f>
+        <f t="shared" si="27"/>
         <v>7.88</v>
       </c>
       <c r="L218" t="s">
@@ -10425,7 +10468,7 @@
     </row>
     <row r="219" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B219" s="27">
-        <f t="shared" si="100"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="C219" s="26" t="s">
@@ -10441,15 +10484,15 @@
         <v>7.88</v>
       </c>
       <c r="I219" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C219,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J219" s="32">
-        <f t="shared" ref="J219" si="107">G219*B219-I219</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K219" s="29">
-        <f t="shared" ref="K219" si="108">B219*H219</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L219" t="s">
@@ -10458,7 +10501,7 @@
     </row>
     <row r="220" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B220" s="27">
-        <f t="shared" si="100"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="C220" s="26" t="s">
@@ -10474,15 +10517,15 @@
         <v>7.88</v>
       </c>
       <c r="I220" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C220,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J220" s="32">
-        <f t="shared" ref="J220" si="109">G220*B220-I220</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K220" s="29">
-        <f t="shared" ref="K220" si="110">B220*H220</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L220" t="s">
@@ -10491,7 +10534,7 @@
     </row>
     <row r="221" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B221" s="27">
-        <f t="shared" si="67"/>
+        <f>ROUNDUP(I221/G221,0)</f>
         <v>0</v>
       </c>
       <c r="C221" s="26" t="s">
@@ -10507,15 +10550,15 @@
         <v>8.8699999999999992</v>
       </c>
       <c r="I221" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C221,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J221" s="32">
-        <f t="shared" ref="J221" si="111">G221*B221-I221</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K221" s="29">
-        <f t="shared" ref="K221" si="112">B221*H221</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L221" t="s">
@@ -10524,7 +10567,7 @@
     </row>
     <row r="222" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B222" s="27">
-        <f t="shared" si="67"/>
+        <f>ROUNDUP(I222/G222,0)</f>
         <v>0</v>
       </c>
       <c r="C222" s="26" t="s">
@@ -10540,15 +10583,15 @@
         <v>7.13</v>
       </c>
       <c r="I222" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C222,B$1:B$144)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J222" s="32">
-        <f t="shared" ref="J222" si="113">G222*B222-I222</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K222" s="29">
-        <f t="shared" ref="K222" si="114">B222*H222</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L222" t="s">
@@ -10565,7 +10608,7 @@
     </row>
     <row r="224" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B224" s="27">
-        <f t="shared" ref="B224" si="115">ROUNDUP(I224/G224,0)</f>
+        <f t="shared" ref="B224:B232" si="29">ROUNDUP(I224/G224,0)</f>
         <v>0</v>
       </c>
       <c r="C224" s="26" t="s">
@@ -10581,15 +10624,15 @@
         <v>14.5</v>
       </c>
       <c r="I224" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C224,B$1:B$144)</f>
+        <f t="shared" ref="I224:I232" si="30">SUMIF(C$1:C$144,"="&amp;C224,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J224" s="32">
-        <f t="shared" ref="J224" si="116">G224*B224-I224</f>
+        <f t="shared" ref="J224:J232" si="31">G224*B224-I224</f>
         <v>0</v>
       </c>
       <c r="K224" s="29">
-        <f t="shared" ref="K224" si="117">B224*H224</f>
+        <f t="shared" ref="K224:K232" si="32">B224*H224</f>
         <v>0</v>
       </c>
       <c r="L224" t="s">
@@ -10598,7 +10641,7 @@
     </row>
     <row r="225" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B225" s="27">
-        <f t="shared" ref="B225" si="118">ROUNDUP(I225/G225,0)</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="C225" s="26" t="s">
@@ -10614,15 +10657,15 @@
         <v>14.5</v>
       </c>
       <c r="I225" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C225,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J225" s="32">
-        <f t="shared" ref="J225" si="119">G225*B225-I225</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K225" s="29">
-        <f t="shared" ref="K225" si="120">B225*H225</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L225" t="s">
@@ -10631,7 +10674,7 @@
     </row>
     <row r="226" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B226" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="C226" s="26" t="s">
@@ -10647,15 +10690,15 @@
         <v>14.5</v>
       </c>
       <c r="I226" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C226,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="J226" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K226" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="32"/>
         <v>14.5</v>
       </c>
       <c r="L226" t="s">
@@ -10664,7 +10707,7 @@
     </row>
     <row r="227" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B227" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="C227" s="26" t="s">
@@ -10680,15 +10723,15 @@
         <v>8.5</v>
       </c>
       <c r="I227" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C227,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="J227" s="32">
-        <f t="shared" ref="J227" si="121">G227*B227-I227</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K227" s="29">
-        <f t="shared" ref="K227" si="122">B227*H227</f>
+        <f t="shared" si="32"/>
         <v>8.5</v>
       </c>
       <c r="L227" t="s">
@@ -10697,7 +10740,7 @@
     </row>
     <row r="228" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B228" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="C228" s="26" t="s">
@@ -10713,15 +10756,15 @@
         <v>54.2</v>
       </c>
       <c r="I228" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C228,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="J228" s="32">
-        <f t="shared" ref="J228" si="123">G228*B228-I228</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K228" s="29">
-        <f t="shared" ref="K228" si="124">B228*H228</f>
+        <f t="shared" si="32"/>
         <v>54.2</v>
       </c>
       <c r="L228" t="s">
@@ -10730,7 +10773,7 @@
     </row>
     <row r="229" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B229" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="C229" s="26" t="s">
@@ -10746,15 +10789,15 @@
         <v>37</v>
       </c>
       <c r="I229" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C229,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="J229" s="32">
-        <f t="shared" ref="J229" si="125">G229*B229-I229</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K229" s="29">
-        <f t="shared" ref="K229" si="126">B229*H229</f>
+        <f t="shared" si="32"/>
         <v>37</v>
       </c>
       <c r="L229" t="s">
@@ -10763,7 +10806,7 @@
     </row>
     <row r="230" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B230" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="C230" s="26" t="s">
@@ -10779,15 +10822,15 @@
         <v>18</v>
       </c>
       <c r="I230" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C230,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="J230" s="32">
-        <f t="shared" ref="J230" si="127">G230*B230-I230</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K230" s="29">
-        <f t="shared" ref="K230" si="128">B230*H230</f>
+        <f t="shared" si="32"/>
         <v>18</v>
       </c>
       <c r="L230" t="s">
@@ -10796,7 +10839,7 @@
     </row>
     <row r="231" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B231" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>5</v>
       </c>
       <c r="C231" s="26" t="s">
@@ -10812,15 +10855,15 @@
         <v>14.53</v>
       </c>
       <c r="I231" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C231,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
       <c r="J231" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K231" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="32"/>
         <v>72.649999999999991</v>
       </c>
       <c r="L231" t="s">
@@ -10829,7 +10872,7 @@
     </row>
     <row r="232" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B232" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="C232" s="26" t="s">
@@ -10845,15 +10888,15 @@
         <v>36.42</v>
       </c>
       <c r="I232" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C232,B$1:B$144)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="J232" s="32">
-        <f t="shared" ref="J232" si="129">G232*B232-I232</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K232" s="29">
-        <f t="shared" ref="K232" si="130">B232*H232</f>
+        <f t="shared" si="32"/>
         <v>72.84</v>
       </c>
       <c r="L232" t="s">
@@ -10871,7 +10914,7 @@
     </row>
     <row r="234" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B234" s="27">
-        <f t="shared" ref="B234:B239" si="131">ROUNDUP(I234/G234,0)</f>
+        <f t="shared" ref="B234:B239" si="33">ROUNDUP(I234/G234,0)</f>
         <v>16</v>
       </c>
       <c r="C234" s="26" t="s">
@@ -10887,15 +10930,15 @@
         <v>1.35</v>
       </c>
       <c r="I234" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C234,B$1:B$144)</f>
+        <f t="shared" ref="I234:I250" si="34">SUMIF(C$1:C$144,"="&amp;C234,B$1:B$144)</f>
         <v>16</v>
       </c>
       <c r="J234" s="32">
-        <f t="shared" ref="J234" si="132">G234*B234-I234</f>
+        <f t="shared" ref="J234:J250" si="35">G234*B234-I234</f>
         <v>0</v>
       </c>
       <c r="K234" s="29">
-        <f t="shared" ref="K234:K239" si="133">B234*H234</f>
+        <f t="shared" ref="K234:K239" si="36">B234*H234</f>
         <v>21.6</v>
       </c>
       <c r="L234" t="s">
@@ -10904,7 +10947,7 @@
     </row>
     <row r="235" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="27">
-        <f t="shared" si="131"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="C235" s="26" t="s">
@@ -10920,15 +10963,15 @@
         <v>1.35</v>
       </c>
       <c r="I235" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C235,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J235" s="32">
-        <f t="shared" ref="J235" si="134">G235*B235-I235</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K235" s="29">
-        <f t="shared" si="133"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L235" t="s">
@@ -10937,7 +10980,7 @@
     </row>
     <row r="236" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="27">
-        <f t="shared" si="131"/>
+        <f t="shared" si="33"/>
         <v>16</v>
       </c>
       <c r="C236" s="26" t="s">
@@ -10953,15 +10996,15 @@
         <v>1.35</v>
       </c>
       <c r="I236" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C236,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>16</v>
       </c>
       <c r="J236" s="32">
-        <f t="shared" ref="J236" si="135">G236*B236-I236</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K236" s="29">
-        <f t="shared" si="133"/>
+        <f t="shared" si="36"/>
         <v>21.6</v>
       </c>
       <c r="L236" t="s">
@@ -10970,7 +11013,7 @@
     </row>
     <row r="237" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B237" s="27">
-        <f t="shared" si="131"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="C237" s="26" t="s">
@@ -10986,15 +11029,15 @@
         <v>1.05</v>
       </c>
       <c r="I237" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C237,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="J237" s="32">
-        <f t="shared" ref="J237" si="136">G237*B237-I237</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K237" s="29">
-        <f t="shared" si="133"/>
+        <f t="shared" si="36"/>
         <v>6.3000000000000007</v>
       </c>
       <c r="L237" t="s">
@@ -11003,7 +11046,7 @@
     </row>
     <row r="238" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B238" s="27">
-        <f t="shared" si="131"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="C238" s="26" t="s">
@@ -11019,15 +11062,15 @@
         <v>1.35</v>
       </c>
       <c r="I238" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C238,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J238" s="32">
-        <f t="shared" ref="J238" si="137">G238*B238-I238</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K238" s="29">
-        <f t="shared" si="133"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L238" t="s">
@@ -11036,7 +11079,7 @@
     </row>
     <row r="239" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B239" s="27">
-        <f t="shared" si="131"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="C239" s="26" t="s">
@@ -11052,15 +11095,15 @@
         <v>2.19</v>
       </c>
       <c r="I239" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C239,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J239" s="32">
-        <f t="shared" ref="J239" si="138">G239*B239-I239</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K239" s="29">
-        <f t="shared" si="133"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L239" t="s">
@@ -11069,7 +11112,7 @@
     </row>
     <row r="240" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B240" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" ref="B240:B250" si="37">ROUNDUP(I240/G240,0)</f>
         <v>16</v>
       </c>
       <c r="C240" s="26" t="s">
@@ -11085,15 +11128,15 @@
         <v>1.54</v>
       </c>
       <c r="I240" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C240,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>16</v>
       </c>
       <c r="J240" s="32">
-        <f t="shared" ref="J240" si="139">G240*B240-I240</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K240" s="29">
-        <f t="shared" ref="K240" si="140">B240*H240</f>
+        <f t="shared" ref="K240:K250" si="38">B240*H240</f>
         <v>24.64</v>
       </c>
       <c r="L240" t="s">
@@ -11102,7 +11145,7 @@
     </row>
     <row r="241" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B241" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="C241" s="26" t="s">
@@ -11118,15 +11161,15 @@
         <v>1.54</v>
       </c>
       <c r="I241" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C241,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>10</v>
       </c>
       <c r="J241" s="32">
-        <f t="shared" ref="J241" si="141">G241*B241-I241</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K241" s="29">
-        <f t="shared" ref="K241" si="142">B241*H241</f>
+        <f t="shared" si="38"/>
         <v>15.4</v>
       </c>
       <c r="L241" t="s">
@@ -11135,7 +11178,7 @@
     </row>
     <row r="242" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="C242" s="26" t="s">
@@ -11151,15 +11194,15 @@
         <v>1.95</v>
       </c>
       <c r="I242" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C242,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J242" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K242" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L242" t="s">
@@ -11168,7 +11211,7 @@
     </row>
     <row r="243" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B243" s="27">
-        <f>ROUNDUP(I243/G243,0)</f>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="C243" s="26" t="s">
@@ -11184,15 +11227,15 @@
         <v>1</v>
       </c>
       <c r="I243" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C243,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
       <c r="J243" s="32">
-        <f t="shared" ref="J243" si="143">G243*B243-I243</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K243" s="29">
-        <f>B243*H243</f>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="L243" t="s">
@@ -11201,7 +11244,7 @@
     </row>
     <row r="244" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="C244" s="26" t="s">
@@ -11217,15 +11260,15 @@
         <v>1.39</v>
       </c>
       <c r="I244" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C244,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="J244" s="32">
-        <f t="shared" ref="J244" si="144">G244*B244-I244</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K244" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="38"/>
         <v>1.39</v>
       </c>
       <c r="L244" t="s">
@@ -11234,7 +11277,7 @@
     </row>
     <row r="245" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B245" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="C245" s="26" t="s">
@@ -11250,15 +11293,15 @@
         <v>3.29</v>
       </c>
       <c r="I245" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C245,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J245" s="32">
-        <f t="shared" ref="J245" si="145">G245*B245-I245</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K245" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="38"/>
         <v>16.45</v>
       </c>
       <c r="L245" t="s">
@@ -11267,7 +11310,7 @@
     </row>
     <row r="246" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B246" s="27">
-        <f t="shared" ref="B246" si="146">ROUNDUP(I246/G246,0)</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="C246" s="26" t="s">
@@ -11283,15 +11326,15 @@
         <v>3.29</v>
       </c>
       <c r="I246" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C246,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="J246" s="32">
-        <f t="shared" ref="J246" si="147">G246*B246-I246</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K246" s="29">
-        <f t="shared" ref="K246" si="148">B246*H246</f>
+        <f t="shared" si="38"/>
         <v>3.29</v>
       </c>
       <c r="L246" t="s">
@@ -11300,7 +11343,7 @@
     </row>
     <row r="247" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B247" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="C247" s="26" t="s">
@@ -11316,15 +11359,15 @@
         <v>1</v>
       </c>
       <c r="I247" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C247,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="J247" s="32">
-        <f t="shared" ref="J247" si="149">G247*B247-I247</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K247" s="29">
-        <f t="shared" ref="K247" si="150">B247*H247</f>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="L247" t="s">
@@ -11333,7 +11376,7 @@
     </row>
     <row r="248" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B248" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="C248" s="26" t="s">
@@ -11349,15 +11392,15 @@
         <v>20</v>
       </c>
       <c r="I248" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C248,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="J248" s="32">
-        <f t="shared" ref="J248" si="151">G248*B248-I248</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K248" s="29">
-        <f t="shared" ref="K248" si="152">B248*H248</f>
+        <f t="shared" si="38"/>
         <v>20</v>
       </c>
       <c r="L248" t="s">
@@ -11366,7 +11409,7 @@
     </row>
     <row r="249" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B249" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="C249" s="26" t="s">
@@ -11382,15 +11425,15 @@
         <v>18.079999999999998</v>
       </c>
       <c r="I249" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C249,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J249" s="32">
-        <f t="shared" ref="J249" si="153">G249*B249-I249</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K249" s="29">
-        <f t="shared" ref="K249" si="154">B249*H249</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L249" t="s">
@@ -11399,7 +11442,7 @@
     </row>
     <row r="250" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B250" s="27">
-        <f t="shared" ref="B250" si="155">ROUNDUP(I250/G250,0)</f>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="C250" s="26" t="s">
@@ -11415,15 +11458,15 @@
         <v>18.079999999999998</v>
       </c>
       <c r="I250" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C250,B$1:B$144)</f>
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
       <c r="J250" s="32">
-        <f t="shared" ref="J250" si="156">G250*B250-I250</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="K250" s="29">
-        <f t="shared" ref="K250" si="157">B250*H250</f>
+        <f t="shared" si="38"/>
         <v>36.159999999999997</v>
       </c>
       <c r="L250" t="s">
@@ -11468,15 +11511,15 @@
         <v>10.99</v>
       </c>
       <c r="I253" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C253,B$1:B$144)</f>
+        <f t="shared" ref="I253:I261" si="39">SUMIF(C$1:C$144,"="&amp;C253,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J253" s="32">
-        <f t="shared" ref="J253" si="158">G253*B253-I253</f>
+        <f t="shared" ref="J253:J260" si="40">G253*B253-I253</f>
         <v>1</v>
       </c>
       <c r="K253" s="29">
-        <f t="shared" ref="K253" si="159">B253*H253</f>
+        <f t="shared" ref="K253:K260" si="41">B253*H253</f>
         <v>10.99</v>
       </c>
       <c r="L253" t="s">
@@ -11500,15 +11543,15 @@
         <v>10.99</v>
       </c>
       <c r="I254" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C254,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="J254" s="32">
-        <f t="shared" ref="J254:J255" si="160">G254*B254-I254</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K254" s="29">
-        <f t="shared" ref="K254:K255" si="161">B254*H254</f>
+        <f t="shared" si="41"/>
         <v>10.99</v>
       </c>
       <c r="L254" t="s">
@@ -11532,15 +11575,15 @@
         <v>2.8</v>
       </c>
       <c r="I255" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C255,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J255" s="32">
-        <f t="shared" si="160"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="K255" s="29">
-        <f t="shared" si="161"/>
+        <f t="shared" si="41"/>
         <v>2.8</v>
       </c>
       <c r="L255" t="s">
@@ -11564,15 +11607,15 @@
         <v>2.8</v>
       </c>
       <c r="I256" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C256,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="J256" s="32">
-        <f t="shared" ref="J256" si="162">G256*B256-I256</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K256" s="29">
-        <f t="shared" ref="K256" si="163">B256*H256</f>
+        <f t="shared" si="41"/>
         <v>2.8</v>
       </c>
       <c r="L256" t="s">
@@ -11596,15 +11639,15 @@
         <v>2.8</v>
       </c>
       <c r="I257" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C257,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J257" s="32">
-        <f>G257*B257-I257</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="K257" s="29">
-        <f>B257*H257</f>
+        <f t="shared" si="41"/>
         <v>2.8</v>
       </c>
       <c r="L257" t="s">
@@ -11628,15 +11671,15 @@
         <v>2.8</v>
       </c>
       <c r="I258" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C258,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="J258" s="32">
-        <f t="shared" ref="J258" si="164">G258*B258-I258</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K258" s="29">
-        <f t="shared" ref="K258" si="165">B258*H258</f>
+        <f t="shared" si="41"/>
         <v>2.8</v>
       </c>
       <c r="L258" t="s">
@@ -11660,15 +11703,15 @@
         <v>1839</v>
       </c>
       <c r="I259" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C259,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J259" s="32">
-        <f t="shared" ref="J259" si="166">G259*B259-I259</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="K259" s="29">
-        <f t="shared" ref="K259" si="167">B259*H259</f>
+        <f t="shared" si="41"/>
         <v>1839</v>
       </c>
       <c r="L259" t="s">
@@ -11692,15 +11735,15 @@
         <v>49</v>
       </c>
       <c r="I260" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C260,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J260" s="32">
-        <f t="shared" ref="J260" si="168">G260*B260-I260</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="K260" s="29">
-        <f t="shared" ref="K260" si="169">B260*H260</f>
+        <f t="shared" si="41"/>
         <v>49</v>
       </c>
       <c r="L260" t="s">
@@ -11719,7 +11762,7 @@
       </c>
       <c r="H261" s="19"/>
       <c r="I261" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C261,B$1:B$144)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J261" s="32"/>
@@ -11761,15 +11804,15 @@
         <v>0.87</v>
       </c>
       <c r="I264" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C264,B$1:B$144)</f>
+        <f t="shared" ref="I264:I269" si="42">SUMIF(C$1:C$144,"="&amp;C264,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J264" s="32">
-        <f t="shared" ref="J264:J265" si="170">G264*B264-I264</f>
+        <f t="shared" ref="J264:J269" si="43">G264*B264-I264</f>
         <v>1</v>
       </c>
       <c r="K264" s="29">
-        <f t="shared" ref="K264:K265" si="171">B264*H264</f>
+        <f t="shared" ref="K264:K269" si="44">B264*H264</f>
         <v>0.87</v>
       </c>
       <c r="L264" t="s">
@@ -11793,15 +11836,15 @@
         <v>0.8</v>
       </c>
       <c r="I265" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C265,B$1:B$144)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J265" s="32">
-        <f t="shared" si="170"/>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="K265" s="29">
-        <f t="shared" si="171"/>
+        <f t="shared" si="44"/>
         <v>0.8</v>
       </c>
       <c r="L265" t="s">
@@ -11825,15 +11868,15 @@
         <v>19.989999999999998</v>
       </c>
       <c r="I266" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C266,B$1:B$144)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J266" s="32">
-        <f t="shared" ref="J266:J267" si="172">G266*B266-I266</f>
+        <f t="shared" si="43"/>
         <v>5</v>
       </c>
       <c r="K266" s="29">
-        <f t="shared" ref="K266:K267" si="173">B266*H266</f>
+        <f t="shared" si="44"/>
         <v>99.949999999999989</v>
       </c>
       <c r="L266" t="s">
@@ -11857,15 +11900,15 @@
         <v>44</v>
       </c>
       <c r="I267" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C267,B$1:B$144)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J267" s="32">
-        <f t="shared" si="172"/>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="K267" s="29">
-        <f t="shared" si="173"/>
+        <f t="shared" si="44"/>
         <v>44</v>
       </c>
       <c r="L267" t="s">
@@ -11889,15 +11932,15 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="I268" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C268,B$1:B$144)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J268" s="32">
-        <f t="shared" ref="J268:J269" si="174">G268*B268-I268</f>
+        <f t="shared" si="43"/>
         <v>5</v>
       </c>
       <c r="K268" s="29">
-        <f t="shared" ref="K268:K269" si="175">B268*H268</f>
+        <f t="shared" si="44"/>
         <v>10.25</v>
       </c>
       <c r="L268" t="s">
@@ -11921,15 +11964,15 @@
         <v>1.95</v>
       </c>
       <c r="I269" s="31">
-        <f>SUMIF(C$1:C$144,"="&amp;C269,B$1:B$144)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J269" s="32">
-        <f t="shared" si="174"/>
+        <f t="shared" si="43"/>
         <v>5</v>
       </c>
       <c r="K269" s="29">
-        <f t="shared" si="175"/>
+        <f t="shared" si="44"/>
         <v>9.75</v>
       </c>
       <c r="L269" t="s">
@@ -12130,80 +12173,80 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L149 D180:K180 B181:K181 B182:D182 F182:K182 F185:K187 B185:D187 B183:K184 C253 G253:K253 F211:K214 B211:D214 B223:C223 E224 F223:K225 B224:D225 B179 F179:K179 D179 B215:K222 B254:K261 D271:K271 B271 B264:K270 E275:E276 B146:K178 B4:K14 B226:K251 B16:K143 B188:K210">
-    <cfRule type="expression" dxfId="20" priority="462">
+    <cfRule type="expression" dxfId="17" priority="462">
       <formula>$L4=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E225">
-    <cfRule type="expression" dxfId="19" priority="497">
+    <cfRule type="expression" dxfId="16" priority="497">
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E211">
-    <cfRule type="expression" dxfId="18" priority="498">
+    <cfRule type="expression" dxfId="15" priority="498">
       <formula>$L224=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E187">
-    <cfRule type="expression" dxfId="17" priority="499">
+    <cfRule type="expression" dxfId="14" priority="499">
       <formula>$L180=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="expression" dxfId="16" priority="500">
+    <cfRule type="expression" dxfId="13" priority="500">
       <formula>$L180=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E186">
-    <cfRule type="expression" dxfId="15" priority="501">
+    <cfRule type="expression" dxfId="12" priority="501">
       <formula>$L178=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A180 D180:XFD180 A181:XFD181 A182:D182 F182:XFD182 F185:XFD187 A185:D187 A183:XFD184 C253 G253:L253 A211:D214 F211:XFD214 A223:C223 E224 A224:D225 F223:XFD225 A179:B179 F179:XFD179 D179 A215:XFD222 A271:B271 D271:XFD271 A254:XFD261 A264:XFD270 E275:E276 A146:XFD178 A4:XFD14 A226:XFD251 A16:XFD143 A188:XFD210">
-    <cfRule type="expression" dxfId="14" priority="502">
+    <cfRule type="expression" dxfId="11" priority="502">
       <formula>$L4=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="503">
+    <cfRule type="expression" dxfId="10" priority="503">
       <formula>$L4=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E225">
-    <cfRule type="expression" dxfId="12" priority="566">
+    <cfRule type="expression" dxfId="9" priority="566">
       <formula>$L223=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="567">
+    <cfRule type="expression" dxfId="8" priority="567">
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E211">
-    <cfRule type="expression" dxfId="10" priority="568">
+    <cfRule type="expression" dxfId="7" priority="568">
       <formula>$L224=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="569">
+    <cfRule type="expression" dxfId="6" priority="569">
       <formula>$L224=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E187">
-    <cfRule type="expression" dxfId="8" priority="570">
+    <cfRule type="expression" dxfId="5" priority="570">
       <formula>$L180=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="571">
+    <cfRule type="expression" dxfId="4" priority="571">
       <formula>$L180=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="expression" dxfId="6" priority="572">
+    <cfRule type="expression" dxfId="3" priority="572">
       <formula>$L180=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="573">
+    <cfRule type="expression" dxfId="2" priority="573">
       <formula>$L180=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E186">
-    <cfRule type="expression" dxfId="4" priority="574">
+    <cfRule type="expression" dxfId="1" priority="574">
       <formula>$L178=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="575">
+    <cfRule type="expression" dxfId="0" priority="575">
       <formula>$L178=#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
flansch im ellenbogen 15Z statt 14Z
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="475">
   <si>
     <t>Material</t>
   </si>
@@ -1449,6 +1449,9 @@
   </si>
   <si>
     <t>30 Ohm</t>
+  </si>
+  <si>
+    <t>4,2 Ohm</t>
   </si>
 </sst>
 </file>
@@ -2900,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4086,7 +4089,9 @@
       </c>
       <c r="S73" s="10"/>
       <c r="T73" s="10"/>
-      <c r="U73" s="10"/>
+      <c r="U73" s="10" t="s">
+        <v>474</v>
+      </c>
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
       <c r="X73" s="10"/>
@@ -4129,7 +4134,7 @@
         <v>5</v>
       </c>
       <c r="L74" s="51">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="M74" s="51">
         <v>0.4</v>
@@ -4141,8 +4146,7 @@
         <v>0.22</v>
       </c>
       <c r="P74" s="15">
-        <f>L74/O74</f>
-        <v>118.18181818181819</v>
+        <v>290</v>
       </c>
       <c r="Q74" s="11"/>
       <c r="R74" s="52">
@@ -4893,7 +4897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
forearm with 245 belt (instead of 250mm)
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -2903,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U74" sqref="U74"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D36" s="4">
         <f>D40/D38*(D44/D42)</f>
-        <v>8.5</v>
+        <v>7.9333333333333327</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -3478,7 +3478,7 @@
         <v>16</v>
       </c>
       <c r="D42" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E42" t="s">
         <v>28</v>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="D43" s="4">
         <f>D42*D37/PI()</f>
-        <v>11.140846016432674</v>
+        <v>11.93662073189215</v>
       </c>
       <c r="E43" t="s">
         <v>30</v>
@@ -5300,8 +5300,8 @@
   </sheetPr>
   <dimension ref="A1:O298"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5397,7 +5397,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="29"/>
       <c r="L5" t="str">
-        <f t="shared" ref="L5:L11" ca="1" si="0">INDIRECT(ADDRESS(MATCH(C5,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C5,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5418,7 +5418,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="29"/>
       <c r="L6" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C6,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5439,7 +5439,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="29"/>
       <c r="L7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C7,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5460,7 +5460,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="29"/>
       <c r="L8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C8,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="29"/>
       <c r="L9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C9,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5502,7 +5502,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="29"/>
       <c r="L10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C10,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5523,7 +5523,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="29"/>
       <c r="L11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C11,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5603,7 +5603,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="29"/>
       <c r="L17">
-        <f t="shared" ref="L17:L22" ca="1" si="1">INDIRECT(ADDRESS(MATCH(C17,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C17,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="29"/>
       <c r="L18" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C18,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5645,7 +5645,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="29"/>
       <c r="L19">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C19,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -5666,7 +5666,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="29"/>
       <c r="L20">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C20,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="29"/>
       <c r="L21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C21,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5708,7 +5708,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="29"/>
       <c r="L22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C22,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -5750,7 +5750,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="29"/>
       <c r="L25" t="str">
-        <f t="shared" ref="L25:L38" ca="1" si="2">INDIRECT(ADDRESS(MATCH(C25,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C25,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="C26" s="26" t="str">
         <f>C210</f>
-        <v>Zahnriemen T2,5 250mm 6mm Breite</v>
+        <v>Zahnriemen T2,5 245mm 6mm Breite</v>
       </c>
       <c r="D26" t="s">
         <v>432</v>
@@ -5771,7 +5771,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="29"/>
       <c r="L26" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C26,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5792,7 +5792,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="29"/>
       <c r="L27" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C27,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5813,7 +5813,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="29"/>
       <c r="L28" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C28,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5834,7 +5834,7 @@
       <c r="J29" s="32"/>
       <c r="K29" s="29"/>
       <c r="L29" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C29,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       <c r="J30" s="32"/>
       <c r="K30" s="29"/>
       <c r="L30" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C30,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       <c r="J31" s="32"/>
       <c r="K31" s="29"/>
       <c r="L31" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C31,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5897,7 +5897,7 @@
       <c r="J32" s="32"/>
       <c r="K32" s="29"/>
       <c r="L32" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C32,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5918,7 +5918,7 @@
       <c r="J33" s="32"/>
       <c r="K33" s="29"/>
       <c r="L33" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C33,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5939,7 +5939,7 @@
       <c r="J34" s="32"/>
       <c r="K34" s="29"/>
       <c r="L34" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C34,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5960,7 +5960,7 @@
       <c r="J35" s="32"/>
       <c r="K35" s="29"/>
       <c r="L35" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C35,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -5981,7 +5981,7 @@
       <c r="J36" s="32"/>
       <c r="K36" s="29"/>
       <c r="L36" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C36,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6002,7 +6002,7 @@
       <c r="J37" s="32"/>
       <c r="K37" s="29"/>
       <c r="L37" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C37,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       <c r="J38" s="32"/>
       <c r="K38" s="29"/>
       <c r="L38" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C38,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6056,7 +6056,7 @@
       <c r="J40" s="32"/>
       <c r="K40" s="29"/>
       <c r="L40">
-        <f t="shared" ref="L40:L55" ca="1" si="3">INDIRECT(ADDRESS(MATCH(C40,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C40,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       <c r="J41" s="32"/>
       <c r="K41" s="29"/>
       <c r="L41" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C41,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6098,7 +6098,7 @@
       <c r="J42" s="32"/>
       <c r="K42" s="29"/>
       <c r="L42" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C42,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6119,7 +6119,7 @@
       <c r="J43" s="32"/>
       <c r="K43" s="29"/>
       <c r="L43" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C43,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       <c r="J44" s="32"/>
       <c r="K44" s="29"/>
       <c r="L44" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C44,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6162,7 +6162,7 @@
       <c r="J45" s="32"/>
       <c r="K45" s="29"/>
       <c r="L45">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C45,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6183,7 +6183,7 @@
       <c r="J46" s="32"/>
       <c r="K46" s="29"/>
       <c r="L46" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C46,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6204,7 +6204,7 @@
       <c r="J47" s="32"/>
       <c r="K47" s="29"/>
       <c r="L47" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C47,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       <c r="J48" s="32"/>
       <c r="K48" s="29"/>
       <c r="L48" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C48,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="29"/>
       <c r="L49">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C49,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6267,7 +6267,7 @@
       <c r="J50" s="32"/>
       <c r="K50" s="29"/>
       <c r="L50" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C50,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6288,7 +6288,7 @@
       <c r="J51" s="32"/>
       <c r="K51" s="29"/>
       <c r="L51">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C51,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6309,7 +6309,7 @@
       <c r="J52" s="32"/>
       <c r="K52" s="29"/>
       <c r="L52" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C52,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6330,7 +6330,7 @@
       <c r="J53" s="32"/>
       <c r="K53" s="29"/>
       <c r="L53" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C53,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       <c r="J54" s="32"/>
       <c r="K54" s="29"/>
       <c r="L54" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C54,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6372,7 +6372,7 @@
       <c r="J55" s="32"/>
       <c r="K55" s="29"/>
       <c r="L55" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C55,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6405,7 +6405,7 @@
       <c r="J57" s="32"/>
       <c r="K57" s="29"/>
       <c r="L57" t="str">
-        <f t="shared" ref="L57:L89" ca="1" si="4">INDIRECT(ADDRESS(MATCH(C57,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C57,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6426,7 +6426,7 @@
       <c r="J58" s="32"/>
       <c r="K58" s="29"/>
       <c r="L58" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C58,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6447,7 +6447,7 @@
       <c r="J59" s="32"/>
       <c r="K59" s="29"/>
       <c r="L59" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C59,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6468,7 +6468,7 @@
       <c r="J60" s="32"/>
       <c r="K60" s="29"/>
       <c r="L60">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C60,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6489,7 +6489,7 @@
       <c r="J61" s="32"/>
       <c r="K61" s="29"/>
       <c r="L61" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C61,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6510,7 +6510,7 @@
       <c r="J62" s="32"/>
       <c r="K62" s="29"/>
       <c r="L62" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C62,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6531,7 +6531,7 @@
       <c r="J63" s="32"/>
       <c r="K63" s="29"/>
       <c r="L63" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C63,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6552,7 +6552,7 @@
       <c r="J64" s="32"/>
       <c r="K64" s="29"/>
       <c r="L64" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C64,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6573,7 +6573,7 @@
       <c r="J65" s="32"/>
       <c r="K65" s="29"/>
       <c r="L65" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C65,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -6594,7 +6594,7 @@
       <c r="J66" s="32"/>
       <c r="K66" s="29"/>
       <c r="L66" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C66,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6615,7 +6615,7 @@
       <c r="J67" s="32"/>
       <c r="K67" s="29"/>
       <c r="L67" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C67,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6636,7 +6636,7 @@
       <c r="J68" s="32"/>
       <c r="K68" s="29"/>
       <c r="L68" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C68,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       <c r="J69" s="32"/>
       <c r="K69" s="29"/>
       <c r="L69" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C69,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -6678,7 +6678,7 @@
       <c r="J70" s="32"/>
       <c r="K70" s="29"/>
       <c r="L70" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C70,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
       <c r="J71" s="32"/>
       <c r="K71" s="29"/>
       <c r="L71">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C71,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6720,7 +6720,7 @@
       <c r="J72" s="32"/>
       <c r="K72" s="29"/>
       <c r="L72" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C72,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6741,7 +6741,7 @@
       <c r="J73" s="32"/>
       <c r="K73" s="29"/>
       <c r="L73" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C73,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6762,7 +6762,7 @@
       <c r="J74" s="32"/>
       <c r="K74" s="29"/>
       <c r="L74" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C74,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6783,7 +6783,7 @@
       <c r="J75" s="32"/>
       <c r="K75" s="29"/>
       <c r="L75" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C75,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6804,7 +6804,7 @@
       <c r="J76" s="32"/>
       <c r="K76" s="29"/>
       <c r="L76" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C76,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6825,7 +6825,7 @@
       <c r="J77" s="32"/>
       <c r="K77" s="29"/>
       <c r="L77" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C77,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6846,7 +6846,7 @@
       <c r="J78" s="32"/>
       <c r="K78" s="29"/>
       <c r="L78" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C78,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6867,7 +6867,7 @@
       <c r="J79" s="32"/>
       <c r="K79" s="29"/>
       <c r="L79" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C79,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -6888,7 +6888,7 @@
       <c r="J80" s="32"/>
       <c r="K80" s="29"/>
       <c r="L80" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C80,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6909,7 +6909,7 @@
       <c r="J81" s="32"/>
       <c r="K81" s="29"/>
       <c r="L81" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C81,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       <c r="J82" s="32"/>
       <c r="K82" s="29"/>
       <c r="L82" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C82,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6951,7 +6951,7 @@
       <c r="J83" s="32"/>
       <c r="K83" s="29"/>
       <c r="L83" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C83,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -6972,7 +6972,7 @@
       <c r="J84" s="32"/>
       <c r="K84" s="29"/>
       <c r="L84">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C84,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -6993,7 +6993,7 @@
       <c r="J85" s="32"/>
       <c r="K85" s="29"/>
       <c r="L85" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C85,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7014,7 +7014,7 @@
       <c r="J86" s="32"/>
       <c r="K86" s="29"/>
       <c r="L86" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C86,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7035,7 +7035,7 @@
       <c r="J87" s="32"/>
       <c r="K87" s="29"/>
       <c r="L87" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C87,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7056,7 +7056,7 @@
       <c r="J88" s="32"/>
       <c r="K88" s="29"/>
       <c r="L88" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C88,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7077,7 +7077,7 @@
       <c r="J89" s="32"/>
       <c r="K89" s="29"/>
       <c r="L89" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C89,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7119,7 +7119,7 @@
       <c r="J92" s="32"/>
       <c r="K92" s="29"/>
       <c r="L92" t="str">
-        <f t="shared" ref="L92:L119" ca="1" si="5">INDIRECT(ADDRESS(MATCH(C92,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C92,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7140,7 +7140,7 @@
       <c r="J93" s="32"/>
       <c r="K93" s="29"/>
       <c r="L93" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C93,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       <c r="J94" s="32"/>
       <c r="K94" s="29"/>
       <c r="L94" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C94,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7182,7 +7182,7 @@
       <c r="J95" s="32"/>
       <c r="K95" s="29"/>
       <c r="L95" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C95,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7203,7 +7203,7 @@
       <c r="J96" s="32"/>
       <c r="K96" s="29"/>
       <c r="L96" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C96,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7224,7 +7224,7 @@
       <c r="J97" s="32"/>
       <c r="K97" s="29"/>
       <c r="L97" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C97,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7245,7 +7245,7 @@
       <c r="J98" s="32"/>
       <c r="K98" s="29"/>
       <c r="L98" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C98,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7266,7 +7266,7 @@
       <c r="J99" s="32"/>
       <c r="K99" s="29"/>
       <c r="L99" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C99,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7287,7 +7287,7 @@
       <c r="J100" s="32"/>
       <c r="K100" s="29"/>
       <c r="L100" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C100,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7308,7 +7308,7 @@
       <c r="J101" s="32"/>
       <c r="K101" s="29"/>
       <c r="L101" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C101,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7329,7 +7329,7 @@
       <c r="J102" s="32"/>
       <c r="K102" s="29"/>
       <c r="L102" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C102,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7350,7 +7350,7 @@
       <c r="J103" s="32"/>
       <c r="K103" s="29"/>
       <c r="L103" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C103,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7371,7 +7371,7 @@
       <c r="J104" s="32"/>
       <c r="K104" s="29"/>
       <c r="L104">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C104,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -7392,7 +7392,7 @@
       <c r="J105" s="32"/>
       <c r="K105" s="29"/>
       <c r="L105" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C105,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7413,7 +7413,7 @@
       <c r="J106" s="32"/>
       <c r="K106" s="29"/>
       <c r="L106">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C106,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -7434,7 +7434,7 @@
       <c r="J107" s="32"/>
       <c r="K107" s="29"/>
       <c r="L107" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C107,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7455,7 +7455,7 @@
       <c r="J108" s="32"/>
       <c r="K108" s="29"/>
       <c r="L108">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C108,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -7476,7 +7476,7 @@
       <c r="J109" s="32"/>
       <c r="K109" s="29"/>
       <c r="L109" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C109,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7497,7 +7497,7 @@
       <c r="J110" s="32"/>
       <c r="K110" s="29"/>
       <c r="L110">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C110,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -7518,7 +7518,7 @@
       <c r="J111" s="32"/>
       <c r="K111" s="29"/>
       <c r="L111">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C111,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>0</v>
       </c>
     </row>
@@ -7539,7 +7539,7 @@
       <c r="J112" s="32"/>
       <c r="K112" s="29"/>
       <c r="L112" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C112,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7560,7 +7560,7 @@
       <c r="J113" s="32"/>
       <c r="K113" s="29"/>
       <c r="L113" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C113,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7581,7 +7581,7 @@
       <c r="J114" s="32"/>
       <c r="K114" s="29"/>
       <c r="L114" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C114,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       <c r="J115" s="32"/>
       <c r="K115" s="29"/>
       <c r="L115" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C115,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7624,7 +7624,7 @@
       <c r="J116" s="32"/>
       <c r="K116" s="29"/>
       <c r="L116" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C116,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7645,7 +7645,7 @@
       <c r="J117" s="32"/>
       <c r="K117" s="29"/>
       <c r="L117" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C117,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7666,7 +7666,7 @@
       <c r="J118" s="32"/>
       <c r="K118" s="29"/>
       <c r="L118" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C118,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7687,7 +7687,7 @@
       <c r="J119" s="32"/>
       <c r="K119" s="29"/>
       <c r="L119" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C119,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7720,7 +7720,7 @@
       <c r="J121" s="32"/>
       <c r="K121" s="29"/>
       <c r="L121" t="str">
-        <f t="shared" ref="L121:L139" ca="1" si="6">INDIRECT(ADDRESS(MATCH(C121,C$146:C$271,0)+ROW($B$153)-1,12))</f>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C121,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7741,7 +7741,7 @@
       <c r="J122" s="32"/>
       <c r="K122" s="29"/>
       <c r="L122" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C122,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7762,7 +7762,7 @@
       <c r="J123" s="32"/>
       <c r="K123" s="29"/>
       <c r="L123" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C123,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7783,7 +7783,7 @@
       <c r="J124" s="32"/>
       <c r="K124" s="29"/>
       <c r="L124" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C124,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7804,7 +7804,7 @@
       <c r="J125" s="32"/>
       <c r="K125" s="29"/>
       <c r="L125" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C125,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7825,7 +7825,7 @@
       <c r="J126" s="32"/>
       <c r="K126" s="29"/>
       <c r="L126" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C126,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7846,7 +7846,7 @@
       <c r="J127" s="32"/>
       <c r="K127" s="29"/>
       <c r="L127" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C127,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7867,7 +7867,7 @@
       <c r="J128" s="32"/>
       <c r="K128" s="29"/>
       <c r="L128" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C128,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7888,7 +7888,7 @@
       <c r="J129" s="32"/>
       <c r="K129" s="29"/>
       <c r="L129" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C129,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7909,7 +7909,7 @@
       <c r="J130" s="32"/>
       <c r="K130" s="29"/>
       <c r="L130" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C130,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
       <c r="J131" s="32"/>
       <c r="K131" s="29"/>
       <c r="L131" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C131,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       <c r="J132" s="32"/>
       <c r="K132" s="29"/>
       <c r="L132" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C132,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -7973,7 +7973,7 @@
       <c r="J133" s="32"/>
       <c r="K133" s="29"/>
       <c r="L133" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C133,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>-</v>
       </c>
     </row>
@@ -7994,7 +7994,7 @@
       <c r="J134" s="32"/>
       <c r="K134" s="29"/>
       <c r="L134" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C134,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8015,7 +8015,7 @@
       <c r="J135" s="32"/>
       <c r="K135" s="29"/>
       <c r="L135" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C135,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8036,7 +8036,7 @@
       <c r="J136" s="32"/>
       <c r="K136" s="29"/>
       <c r="L136" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C136,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8057,7 +8057,7 @@
       <c r="J137" s="32"/>
       <c r="K137" s="29"/>
       <c r="L137" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C137,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8078,7 +8078,7 @@
       <c r="J138" s="32"/>
       <c r="K138" s="29"/>
       <c r="L138" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C138,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8099,7 +8099,7 @@
       <c r="J139" s="32"/>
       <c r="K139" s="29"/>
       <c r="L139" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">INDIRECT(ADDRESS(MATCH(C139,C$146:C$271,0)+ROW($B$153)-1,12))</f>
         <v>Habs</v>
       </c>
     </row>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="146" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="27">
-        <f t="shared" ref="B146:B155" si="7">ROUNDUP(I146/G146,0)</f>
+        <f t="shared" ref="B146:B155" si="0">ROUNDUP(I146/G146,0)</f>
         <v>0</v>
       </c>
       <c r="C146" s="26" t="s">
@@ -8198,11 +8198,11 @@
         <v>2.5</v>
       </c>
       <c r="I146" s="31">
-        <f t="shared" ref="I146:I155" si="8">SUMIF(C$1:C$144,"="&amp;C146,B$1:B$144)</f>
+        <f t="shared" ref="I146:I155" si="1">SUMIF(C$1:C$144,"="&amp;C146,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J146" s="32">
-        <f t="shared" ref="J146:J155" si="9">G146*B146-I146</f>
+        <f t="shared" ref="J146:J155" si="2">G146*B146-I146</f>
         <v>0</v>
       </c>
       <c r="K146" s="29">
@@ -8215,7 +8215,7 @@
     </row>
     <row r="147" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C147" s="26" t="s">
@@ -8231,11 +8231,11 @@
         <v>2.5</v>
       </c>
       <c r="I147" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J147" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K147" s="29">
@@ -8248,7 +8248,7 @@
     </row>
     <row r="148" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C148" s="26" t="s">
@@ -8264,11 +8264,11 @@
         <v>2.5</v>
       </c>
       <c r="I148" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="J148" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K148" s="29">
@@ -8281,7 +8281,7 @@
     </row>
     <row r="149" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C149" s="26" t="s">
@@ -8297,11 +8297,11 @@
         <v>2.5</v>
       </c>
       <c r="I149" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J149" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="K149" s="29">
@@ -8314,7 +8314,7 @@
     </row>
     <row r="150" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C150" s="26" t="s">
@@ -8330,15 +8330,15 @@
         <v>2.5</v>
       </c>
       <c r="I150" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J150" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="K150" s="29">
-        <f t="shared" ref="K150:K155" si="10">B150*H150</f>
+        <f t="shared" ref="K150:K155" si="3">B150*H150</f>
         <v>2.5</v>
       </c>
       <c r="L150" t="s">
@@ -8347,7 +8347,7 @@
     </row>
     <row r="151" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B151" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C151" s="26" t="s">
@@ -8363,15 +8363,15 @@
         <v>2.5</v>
       </c>
       <c r="I151" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J151" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K151" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L151" t="s">
@@ -8380,7 +8380,7 @@
     </row>
     <row r="152" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B152" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C152" s="26" t="s">
@@ -8396,15 +8396,15 @@
         <v>2.5</v>
       </c>
       <c r="I152" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J152" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="K152" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
       <c r="L152" t="s">
@@ -8413,7 +8413,7 @@
     </row>
     <row r="153" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C153" s="26" t="s">
@@ -8429,15 +8429,15 @@
         <v>2.5</v>
       </c>
       <c r="I153" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J153" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K153" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
       <c r="L153" t="s">
@@ -8446,7 +8446,7 @@
     </row>
     <row r="154" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C154" s="26" t="s">
@@ -8462,15 +8462,15 @@
         <v>1.8</v>
       </c>
       <c r="I154" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J154" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K154" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
       <c r="L154" t="s">
@@ -8479,7 +8479,7 @@
     </row>
     <row r="155" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C155" s="26" t="s">
@@ -8495,15 +8495,15 @@
         <v>1.8</v>
       </c>
       <c r="I155" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J155" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K155" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
       <c r="L155" t="s">
@@ -8698,7 +8698,7 @@
     </row>
     <row r="163" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B163" s="27">
-        <f t="shared" ref="B163:B179" si="11">ROUNDUP(I163/G163,0)</f>
+        <f t="shared" ref="B163:B179" si="4">ROUNDUP(I163/G163,0)</f>
         <v>1</v>
       </c>
       <c r="C163" s="26" t="s">
@@ -8714,15 +8714,15 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="I163" s="31">
-        <f t="shared" ref="I163:I179" si="12">SUMIF(C$1:C$144,"="&amp;C163,B$1:B$144)</f>
+        <f t="shared" ref="I163:I179" si="5">SUMIF(C$1:C$144,"="&amp;C163,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J163" s="32">
-        <f t="shared" ref="J163:J179" si="13">G163*B163-I163</f>
+        <f t="shared" ref="J163:J179" si="6">G163*B163-I163</f>
         <v>49</v>
       </c>
       <c r="K163" s="29">
-        <f t="shared" ref="K163:K179" si="14">B163*H163</f>
+        <f t="shared" ref="K163:K179" si="7">B163*H163</f>
         <v>4.8899999999999997</v>
       </c>
       <c r="L163" t="s">
@@ -8731,7 +8731,7 @@
     </row>
     <row r="164" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C164" s="26" t="s">
@@ -8747,15 +8747,15 @@
         <v>2.29</v>
       </c>
       <c r="I164" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J164" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="K164" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>2.29</v>
       </c>
       <c r="L164" t="s">
@@ -8764,7 +8764,7 @@
     </row>
     <row r="165" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B165" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C165" s="26" t="s">
@@ -8780,15 +8780,15 @@
         <v>1.79</v>
       </c>
       <c r="I165" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="J165" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
       <c r="K165" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>1.79</v>
       </c>
       <c r="L165" t="s">
@@ -8797,7 +8797,7 @@
     </row>
     <row r="166" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C166" s="26" t="s">
@@ -8813,15 +8813,15 @@
         <v>1.79</v>
       </c>
       <c r="I166" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J166" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="K166" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>1.79</v>
       </c>
       <c r="L166" t="s">
@@ -8830,7 +8830,7 @@
     </row>
     <row r="167" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C167" s="26" t="s">
@@ -8846,15 +8846,15 @@
         <v>4.33</v>
       </c>
       <c r="I167" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J167" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K167" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L167" t="s">
@@ -8863,7 +8863,7 @@
     </row>
     <row r="168" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="C168" s="26" t="s">
@@ -8879,15 +8879,15 @@
         <v>1.98</v>
       </c>
       <c r="I168" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="J168" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="K168" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>3.96</v>
       </c>
       <c r="L168" t="s">
@@ -8896,7 +8896,7 @@
     </row>
     <row r="169" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C169" s="26" t="s">
@@ -8912,15 +8912,15 @@
         <v>1.98</v>
       </c>
       <c r="I169" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J169" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K169" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L169" t="s">
@@ -8929,7 +8929,7 @@
     </row>
     <row r="170" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C170" s="26" t="s">
@@ -8945,15 +8945,15 @@
         <v>1.98</v>
       </c>
       <c r="I170" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J170" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K170" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L170" t="s">
@@ -8962,7 +8962,7 @@
     </row>
     <row r="171" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B171" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C171" s="26" t="s">
@@ -8978,15 +8978,15 @@
         <v>4.49</v>
       </c>
       <c r="I171" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="J171" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>460</v>
       </c>
       <c r="K171" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>4.49</v>
       </c>
       <c r="L171" t="s">
@@ -8995,7 +8995,7 @@
     </row>
     <row r="172" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B172" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C172" s="26" t="s">
@@ -9011,15 +9011,15 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="I172" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="J172" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>332</v>
       </c>
       <c r="K172" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="L172" t="s">
@@ -9028,7 +9028,7 @@
     </row>
     <row r="173" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B173" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C173" s="26" t="s">
@@ -9044,15 +9044,15 @@
         <v>4.49</v>
       </c>
       <c r="I173" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="J173" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>308</v>
       </c>
       <c r="K173" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>4.49</v>
       </c>
       <c r="L173" t="s">
@@ -9061,7 +9061,7 @@
     </row>
     <row r="174" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B174" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C174" s="26" t="s">
@@ -9077,15 +9077,15 @@
         <v>4.49</v>
       </c>
       <c r="I174" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="J174" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>356</v>
       </c>
       <c r="K174" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>4.49</v>
       </c>
       <c r="L174" t="s">
@@ -9094,7 +9094,7 @@
     </row>
     <row r="175" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B175" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C175" s="26" t="s">
@@ -9110,15 +9110,15 @@
         <v>1.59</v>
       </c>
       <c r="I175" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="J175" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>88</v>
       </c>
       <c r="K175" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>1.59</v>
       </c>
       <c r="L175" t="s">
@@ -9127,7 +9127,7 @@
     </row>
     <row r="176" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="C176" s="26" t="s">
@@ -9143,15 +9143,15 @@
         <v>0.3</v>
       </c>
       <c r="I176" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="J176" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K176" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>10.5</v>
       </c>
       <c r="L176" t="s">
@@ -9160,7 +9160,7 @@
     </row>
     <row r="177" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C177" s="26" t="s">
@@ -9176,15 +9176,15 @@
         <v>2.09</v>
       </c>
       <c r="I177" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J177" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K177" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L177" t="s">
@@ -9193,7 +9193,7 @@
     </row>
     <row r="178" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C178" s="26" t="s">
@@ -9209,15 +9209,15 @@
         <v>1.69</v>
       </c>
       <c r="I178" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="J178" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="K178" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>1.69</v>
       </c>
       <c r="L178" t="s">
@@ -9226,7 +9226,7 @@
     </row>
     <row r="179" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C179" t="s">
@@ -9242,15 +9242,15 @@
         <v>0.45</v>
       </c>
       <c r="I179" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J179" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K179" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="7"/>
         <v>0.45</v>
       </c>
       <c r="L179" t="s">
@@ -9266,7 +9266,7 @@
     </row>
     <row r="181" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B181" s="27">
-        <f t="shared" ref="B181:B193" si="15">ROUNDUP(I181/G181,0)</f>
+        <f t="shared" ref="B181:B193" si="8">ROUNDUP(I181/G181,0)</f>
         <v>0</v>
       </c>
       <c r="C181" s="26" t="s">
@@ -9282,15 +9282,15 @@
         <v>4.96</v>
       </c>
       <c r="I181" s="31">
-        <f t="shared" ref="I181:I193" si="16">SUMIF(C$1:C$144,"="&amp;C181,B$1:B$144)</f>
+        <f t="shared" ref="I181:I193" si="9">SUMIF(C$1:C$144,"="&amp;C181,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J181" s="32">
-        <f t="shared" ref="J181:J193" si="17">G181*B181-I181</f>
+        <f t="shared" ref="J181:J193" si="10">G181*B181-I181</f>
         <v>0</v>
       </c>
       <c r="K181" s="29">
-        <f t="shared" ref="K181:K193" si="18">B181*H181</f>
+        <f t="shared" ref="K181:K193" si="11">B181*H181</f>
         <v>0</v>
       </c>
       <c r="L181" t="s">
@@ -9299,7 +9299,7 @@
     </row>
     <row r="182" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B182" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="C182" s="26" t="s">
@@ -9315,15 +9315,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I182" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J182" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K182" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="L182" t="s">
@@ -9332,7 +9332,7 @@
     </row>
     <row r="183" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="C183" s="26" t="s">
@@ -9348,15 +9348,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I183" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J183" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K183" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="L183" t="s">
@@ -9365,7 +9365,7 @@
     </row>
     <row r="184" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C184" s="26" t="s">
@@ -9381,15 +9381,15 @@
         <v>4.96</v>
       </c>
       <c r="I184" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J184" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K184" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L184" t="s">
@@ -9398,7 +9398,7 @@
     </row>
     <row r="185" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C185" s="26" t="s">
@@ -9414,15 +9414,15 @@
         <v>4.54</v>
       </c>
       <c r="I185" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J185" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K185" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L185" t="s">
@@ -9431,7 +9431,7 @@
     </row>
     <row r="186" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B186" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C186" s="26" t="s">
@@ -9447,15 +9447,15 @@
         <v>4.54</v>
       </c>
       <c r="I186" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J186" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K186" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L186" t="s">
@@ -9464,7 +9464,7 @@
     </row>
     <row r="187" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C187" s="26" t="s">
@@ -9480,15 +9480,15 @@
         <v>4.54</v>
       </c>
       <c r="I187" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J187" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K187" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L187" t="s">
@@ -9497,7 +9497,7 @@
     </row>
     <row r="188" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B188" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C188" s="26" t="s">
@@ -9513,15 +9513,15 @@
         <v>5.44</v>
       </c>
       <c r="I188" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J188" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K188" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L188" t="s">
@@ -9530,7 +9530,7 @@
     </row>
     <row r="189" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C189" s="26" t="s">
@@ -9546,15 +9546,15 @@
         <v>5.44</v>
       </c>
       <c r="I189" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J189" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K189" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L189" t="s">
@@ -9563,7 +9563,7 @@
     </row>
     <row r="190" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B190" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C190" s="26" t="s">
@@ -9579,15 +9579,15 @@
         <v>5.44</v>
       </c>
       <c r="I190" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J190" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K190" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L190" t="s">
@@ -9596,7 +9596,7 @@
     </row>
     <row r="191" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C191" s="26" t="s">
@@ -9612,15 +9612,15 @@
         <v>5.44</v>
       </c>
       <c r="I191" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J191" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K191" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L191" t="s">
@@ -9629,7 +9629,7 @@
     </row>
     <row r="192" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B192" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C192" s="26" t="s">
@@ -9645,15 +9645,15 @@
         <v>5.44</v>
       </c>
       <c r="I192" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J192" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K192" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L192" t="s">
@@ -9662,7 +9662,7 @@
     </row>
     <row r="193" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C193" s="26" t="s">
@@ -9678,15 +9678,15 @@
         <v>6.34</v>
       </c>
       <c r="I193" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J193" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K193" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L193" t="s">
@@ -9704,7 +9704,7 @@
     </row>
     <row r="195" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="27">
-        <f t="shared" ref="B195:B202" si="19">ROUNDUP(I195/G195,0)</f>
+        <f t="shared" ref="B195:B202" si="12">ROUNDUP(I195/G195,0)</f>
         <v>1</v>
       </c>
       <c r="C195" s="26" t="s">
@@ -9720,15 +9720,15 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="I195" s="31">
-        <f t="shared" ref="I195:I202" si="20">SUMIF(C$1:C$144,"="&amp;C195,B$1:B$144)</f>
+        <f t="shared" ref="I195:I202" si="13">SUMIF(C$1:C$144,"="&amp;C195,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J195" s="32">
-        <f t="shared" ref="J195:J202" si="21">G195*B195-I195</f>
+        <f t="shared" ref="J195:J202" si="14">G195*B195-I195</f>
         <v>0</v>
       </c>
       <c r="K195" s="29">
-        <f t="shared" ref="K195:K202" si="22">B195*H195</f>
+        <f t="shared" ref="K195:K202" si="15">B195*H195</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="L195" t="s">
@@ -9737,7 +9737,7 @@
     </row>
     <row r="196" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C196" s="26" t="s">
@@ -9753,15 +9753,15 @@
         <v>5.07</v>
       </c>
       <c r="I196" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="J196" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K196" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>10.14</v>
       </c>
       <c r="L196" t="s">
@@ -9770,7 +9770,7 @@
     </row>
     <row r="197" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C197" s="26" t="s">
@@ -9786,15 +9786,15 @@
         <v>5.23</v>
       </c>
       <c r="I197" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="J197" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K197" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>10.46</v>
       </c>
       <c r="L197" t="s">
@@ -9803,7 +9803,7 @@
     </row>
     <row r="198" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B198" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="C198" s="26" t="s">
@@ -9819,15 +9819,15 @@
         <v>5.23</v>
       </c>
       <c r="I198" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J198" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K198" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L198" t="s">
@@ -9836,7 +9836,7 @@
     </row>
     <row r="199" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B199" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="C199" s="26" t="s">
@@ -9852,15 +9852,15 @@
         <v>5.23</v>
       </c>
       <c r="I199" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J199" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K199" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L199" t="s">
@@ -9869,7 +9869,7 @@
     </row>
     <row r="200" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B200" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="C200" s="26" t="s">
@@ -9885,15 +9885,15 @@
         <v>6.67</v>
       </c>
       <c r="I200" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J200" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K200" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L200" t="s">
@@ -9902,7 +9902,7 @@
     </row>
     <row r="201" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="C201" s="26" t="s">
@@ -9918,15 +9918,15 @@
         <v>6.67</v>
       </c>
       <c r="I201" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J201" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K201" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L201" t="s">
@@ -9935,7 +9935,7 @@
     </row>
     <row r="202" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C202" s="26" t="s">
@@ -9951,15 +9951,15 @@
         <v>11.6</v>
       </c>
       <c r="I202" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="J202" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K202" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="15"/>
         <v>23.2</v>
       </c>
       <c r="L202" t="s">
@@ -9977,7 +9977,7 @@
     </row>
     <row r="204" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" s="27">
-        <f t="shared" ref="B204:B214" si="23">ROUNDUP(I204/G204,0)</f>
+        <f t="shared" ref="B204:B214" si="16">ROUNDUP(I204/G204,0)</f>
         <v>1</v>
       </c>
       <c r="C204" s="26" t="s">
@@ -9993,15 +9993,15 @@
         <v>4</v>
       </c>
       <c r="I204" s="31">
-        <f t="shared" ref="I204:I222" si="24">SUMIF(C$1:C$144,"="&amp;C204,B$1:B$144)</f>
+        <f t="shared" ref="I204:I222" si="17">SUMIF(C$1:C$144,"="&amp;C204,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J204" s="32">
-        <f t="shared" ref="J204:J222" si="25">G204*B204-I204</f>
+        <f t="shared" ref="J204:J222" si="18">G204*B204-I204</f>
         <v>0</v>
       </c>
       <c r="K204" s="29">
-        <f t="shared" ref="K204:K209" si="26">B204*H204</f>
+        <f t="shared" ref="K204:K209" si="19">B204*H204</f>
         <v>4</v>
       </c>
       <c r="L204" t="s">
@@ -10010,7 +10010,7 @@
     </row>
     <row r="205" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="C205" s="26" t="s">
@@ -10026,15 +10026,15 @@
         <v>4.24</v>
       </c>
       <c r="I205" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="J205" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K205" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="19"/>
         <v>4.24</v>
       </c>
       <c r="L205" t="s">
@@ -10043,7 +10043,7 @@
     </row>
     <row r="206" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C206" s="26" t="s">
@@ -10059,15 +10059,15 @@
         <v>4.24</v>
       </c>
       <c r="I206" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J206" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K206" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L206" t="s">
@@ -10076,7 +10076,7 @@
     </row>
     <row r="207" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B207" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C207" s="26" t="s">
@@ -10092,15 +10092,15 @@
         <v>4</v>
       </c>
       <c r="I207" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J207" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K207" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L207" t="s">
@@ -10109,7 +10109,7 @@
     </row>
     <row r="208" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B208" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C208" s="26" t="s">
@@ -10125,15 +10125,15 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="I208" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J208" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K208" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L208" t="s">
@@ -10142,7 +10142,7 @@
     </row>
     <row r="209" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B209" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C209" s="26" t="s">
@@ -10158,15 +10158,15 @@
         <v>4.96</v>
       </c>
       <c r="I209" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J209" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K209" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L209" t="s">
@@ -10175,14 +10175,14 @@
     </row>
     <row r="210" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B210" s="27">
-        <f t="shared" si="23"/>
+        <f>ROUNDUP(I210/G210,0)</f>
         <v>1</v>
       </c>
       <c r="C210" s="26" t="s">
-        <v>462</v>
-      </c>
-      <c r="E210" s="9" t="s">
-        <v>126</v>
+        <v>336</v>
+      </c>
+      <c r="E210" s="26" t="s">
+        <v>335</v>
       </c>
       <c r="G210">
         <v>1</v>
@@ -10191,15 +10191,15 @@
         <v>4.96</v>
       </c>
       <c r="I210" s="31">
-        <f t="shared" si="24"/>
+        <f>SUMIF(C$1:C$144,"="&amp;C210,B$1:B$144)</f>
         <v>1</v>
       </c>
       <c r="J210" s="32">
-        <f t="shared" si="25"/>
+        <f>G210*B210-I210</f>
         <v>0</v>
       </c>
       <c r="K210" s="29">
-        <f t="shared" ref="K210:K222" si="27">B210*H210</f>
+        <f>B210*H210</f>
         <v>4.96</v>
       </c>
       <c r="L210" t="s">
@@ -10208,14 +10208,14 @@
     </row>
     <row r="211" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B211" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C211" s="26" t="s">
-        <v>336</v>
-      </c>
-      <c r="E211" s="26" t="s">
-        <v>335</v>
+        <v>462</v>
+      </c>
+      <c r="E211" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="G211">
         <v>1</v>
@@ -10224,15 +10224,15 @@
         <v>4.96</v>
       </c>
       <c r="I211" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J211" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K211" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="K211:K222" si="20">B211*H211</f>
         <v>0</v>
       </c>
       <c r="L211" t="s">
@@ -10241,7 +10241,7 @@
     </row>
     <row r="212" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B212" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C212" s="26" t="s">
@@ -10257,15 +10257,15 @@
         <v>4</v>
       </c>
       <c r="I212" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J212" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K212" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L212" t="s">
@@ -10274,7 +10274,7 @@
     </row>
     <row r="213" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B213" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="C213" s="26" t="s">
@@ -10290,15 +10290,15 @@
         <v>4.96</v>
       </c>
       <c r="I213" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J213" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K213" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L213" t="s">
@@ -10307,7 +10307,7 @@
     </row>
     <row r="214" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B214" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="C214" s="26" t="s">
@@ -10323,15 +10323,15 @@
         <v>4.96</v>
       </c>
       <c r="I214" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="J214" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K214" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>4.96</v>
       </c>
       <c r="L214" t="s">
@@ -10340,7 +10340,7 @@
     </row>
     <row r="215" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B215" s="27">
-        <f t="shared" ref="B215:B220" si="28">ROUNDUP(I215/G215,0)</f>
+        <f t="shared" ref="B215:B220" si="21">ROUNDUP(I215/G215,0)</f>
         <v>0</v>
       </c>
       <c r="C215" s="26" t="s">
@@ -10356,15 +10356,15 @@
         <v>7.13</v>
       </c>
       <c r="I215" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J215" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K215" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L215" t="s">
@@ -10373,7 +10373,7 @@
     </row>
     <row r="216" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B216" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="C216" s="26" t="s">
@@ -10389,15 +10389,15 @@
         <v>7.88</v>
       </c>
       <c r="I216" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="J216" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K216" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>15.76</v>
       </c>
       <c r="L216" t="s">
@@ -10406,7 +10406,7 @@
     </row>
     <row r="217" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B217" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="C217" s="26" t="s">
@@ -10422,15 +10422,15 @@
         <v>7.88</v>
       </c>
       <c r="I217" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="J217" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K217" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>15.76</v>
       </c>
       <c r="L217" t="s">
@@ -10439,7 +10439,7 @@
     </row>
     <row r="218" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B218" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="C218" s="26" t="s">
@@ -10455,15 +10455,15 @@
         <v>7.88</v>
       </c>
       <c r="I218" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="J218" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K218" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>7.88</v>
       </c>
       <c r="L218" t="s">
@@ -10472,7 +10472,7 @@
     </row>
     <row r="219" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B219" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="C219" s="26" t="s">
@@ -10488,15 +10488,15 @@
         <v>7.88</v>
       </c>
       <c r="I219" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J219" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K219" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L219" t="s">
@@ -10505,7 +10505,7 @@
     </row>
     <row r="220" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B220" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="C220" s="26" t="s">
@@ -10521,15 +10521,15 @@
         <v>7.88</v>
       </c>
       <c r="I220" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J220" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K220" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L220" t="s">
@@ -10554,15 +10554,15 @@
         <v>8.8699999999999992</v>
       </c>
       <c r="I221" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J221" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K221" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L221" t="s">
@@ -10587,15 +10587,15 @@
         <v>7.13</v>
       </c>
       <c r="I222" s="31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J222" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K222" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L222" t="s">
@@ -10612,7 +10612,7 @@
     </row>
     <row r="224" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B224" s="27">
-        <f t="shared" ref="B224:B232" si="29">ROUNDUP(I224/G224,0)</f>
+        <f t="shared" ref="B224:B232" si="22">ROUNDUP(I224/G224,0)</f>
         <v>0</v>
       </c>
       <c r="C224" s="26" t="s">
@@ -10628,15 +10628,15 @@
         <v>14.5</v>
       </c>
       <c r="I224" s="31">
-        <f t="shared" ref="I224:I232" si="30">SUMIF(C$1:C$144,"="&amp;C224,B$1:B$144)</f>
+        <f t="shared" ref="I224:I232" si="23">SUMIF(C$1:C$144,"="&amp;C224,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J224" s="32">
-        <f t="shared" ref="J224:J232" si="31">G224*B224-I224</f>
+        <f t="shared" ref="J224:J232" si="24">G224*B224-I224</f>
         <v>0</v>
       </c>
       <c r="K224" s="29">
-        <f t="shared" ref="K224:K232" si="32">B224*H224</f>
+        <f t="shared" ref="K224:K232" si="25">B224*H224</f>
         <v>0</v>
       </c>
       <c r="L224" t="s">
@@ -10645,7 +10645,7 @@
     </row>
     <row r="225" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B225" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="C225" s="26" t="s">
@@ -10661,15 +10661,15 @@
         <v>14.5</v>
       </c>
       <c r="I225" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J225" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K225" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L225" t="s">
@@ -10678,7 +10678,7 @@
     </row>
     <row r="226" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B226" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="C226" s="26" t="s">
@@ -10694,15 +10694,15 @@
         <v>14.5</v>
       </c>
       <c r="I226" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J226" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K226" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>14.5</v>
       </c>
       <c r="L226" t="s">
@@ -10711,7 +10711,7 @@
     </row>
     <row r="227" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B227" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="C227" s="26" t="s">
@@ -10727,15 +10727,15 @@
         <v>8.5</v>
       </c>
       <c r="I227" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J227" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K227" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>8.5</v>
       </c>
       <c r="L227" t="s">
@@ -10744,7 +10744,7 @@
     </row>
     <row r="228" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B228" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="C228" s="26" t="s">
@@ -10760,15 +10760,15 @@
         <v>54.2</v>
       </c>
       <c r="I228" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J228" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K228" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>54.2</v>
       </c>
       <c r="L228" t="s">
@@ -10777,7 +10777,7 @@
     </row>
     <row r="229" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B229" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="C229" s="26" t="s">
@@ -10793,15 +10793,15 @@
         <v>37</v>
       </c>
       <c r="I229" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J229" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K229" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>37</v>
       </c>
       <c r="L229" t="s">
@@ -10810,7 +10810,7 @@
     </row>
     <row r="230" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B230" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="C230" s="26" t="s">
@@ -10826,15 +10826,15 @@
         <v>18</v>
       </c>
       <c r="I230" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J230" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K230" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>18</v>
       </c>
       <c r="L230" t="s">
@@ -10843,7 +10843,7 @@
     </row>
     <row r="231" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B231" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="C231" s="26" t="s">
@@ -10859,15 +10859,15 @@
         <v>14.53</v>
       </c>
       <c r="I231" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J231" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K231" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>72.649999999999991</v>
       </c>
       <c r="L231" t="s">
@@ -10876,7 +10876,7 @@
     </row>
     <row r="232" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B232" s="27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="C232" s="26" t="s">
@@ -10892,15 +10892,15 @@
         <v>36.42</v>
       </c>
       <c r="I232" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="J232" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K232" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>72.84</v>
       </c>
       <c r="L232" t="s">
@@ -10918,7 +10918,7 @@
     </row>
     <row r="234" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B234" s="27">
-        <f t="shared" ref="B234:B239" si="33">ROUNDUP(I234/G234,0)</f>
+        <f t="shared" ref="B234:B239" si="26">ROUNDUP(I234/G234,0)</f>
         <v>16</v>
       </c>
       <c r="C234" s="26" t="s">
@@ -10934,15 +10934,15 @@
         <v>1.35</v>
       </c>
       <c r="I234" s="31">
-        <f t="shared" ref="I234:I250" si="34">SUMIF(C$1:C$144,"="&amp;C234,B$1:B$144)</f>
+        <f t="shared" ref="I234:I250" si="27">SUMIF(C$1:C$144,"="&amp;C234,B$1:B$144)</f>
         <v>16</v>
       </c>
       <c r="J234" s="32">
-        <f t="shared" ref="J234:J250" si="35">G234*B234-I234</f>
+        <f t="shared" ref="J234:J250" si="28">G234*B234-I234</f>
         <v>0</v>
       </c>
       <c r="K234" s="29">
-        <f t="shared" ref="K234:K239" si="36">B234*H234</f>
+        <f t="shared" ref="K234:K239" si="29">B234*H234</f>
         <v>21.6</v>
       </c>
       <c r="L234" t="s">
@@ -10951,7 +10951,7 @@
     </row>
     <row r="235" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="C235" s="26" t="s">
@@ -10967,15 +10967,15 @@
         <v>1.35</v>
       </c>
       <c r="I235" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J235" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K235" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L235" t="s">
@@ -10984,7 +10984,7 @@
     </row>
     <row r="236" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="26"/>
         <v>16</v>
       </c>
       <c r="C236" s="26" t="s">
@@ -11000,15 +11000,15 @@
         <v>1.35</v>
       </c>
       <c r="I236" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>16</v>
       </c>
       <c r="J236" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K236" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="29"/>
         <v>21.6</v>
       </c>
       <c r="L236" t="s">
@@ -11017,7 +11017,7 @@
     </row>
     <row r="237" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B237" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="26"/>
         <v>6</v>
       </c>
       <c r="C237" s="26" t="s">
@@ -11033,15 +11033,15 @@
         <v>1.05</v>
       </c>
       <c r="I237" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>6</v>
       </c>
       <c r="J237" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K237" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="29"/>
         <v>6.3000000000000007</v>
       </c>
       <c r="L237" t="s">
@@ -11050,7 +11050,7 @@
     </row>
     <row r="238" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B238" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="C238" s="26" t="s">
@@ -11066,15 +11066,15 @@
         <v>1.35</v>
       </c>
       <c r="I238" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J238" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K238" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L238" t="s">
@@ -11083,7 +11083,7 @@
     </row>
     <row r="239" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B239" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="C239" s="26" t="s">
@@ -11099,15 +11099,15 @@
         <v>2.19</v>
       </c>
       <c r="I239" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J239" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K239" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L239" t="s">
@@ -11116,7 +11116,7 @@
     </row>
     <row r="240" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B240" s="27">
-        <f t="shared" ref="B240:B250" si="37">ROUNDUP(I240/G240,0)</f>
+        <f t="shared" ref="B240:B250" si="30">ROUNDUP(I240/G240,0)</f>
         <v>16</v>
       </c>
       <c r="C240" s="26" t="s">
@@ -11132,15 +11132,15 @@
         <v>1.54</v>
       </c>
       <c r="I240" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>16</v>
       </c>
       <c r="J240" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K240" s="29">
-        <f t="shared" ref="K240:K250" si="38">B240*H240</f>
+        <f t="shared" ref="K240:K250" si="31">B240*H240</f>
         <v>24.64</v>
       </c>
       <c r="L240" t="s">
@@ -11149,7 +11149,7 @@
     </row>
     <row r="241" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B241" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
       <c r="C241" s="26" t="s">
@@ -11165,15 +11165,15 @@
         <v>1.54</v>
       </c>
       <c r="I241" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>10</v>
       </c>
       <c r="J241" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K241" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>15.4</v>
       </c>
       <c r="L241" t="s">
@@ -11182,7 +11182,7 @@
     </row>
     <row r="242" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="C242" s="26" t="s">
@@ -11198,15 +11198,15 @@
         <v>1.95</v>
       </c>
       <c r="I242" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J242" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K242" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L242" t="s">
@@ -11215,7 +11215,7 @@
     </row>
     <row r="243" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B243" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="C243" s="26" t="s">
@@ -11231,15 +11231,15 @@
         <v>1</v>
       </c>
       <c r="I243" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="J243" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K243" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="L243" t="s">
@@ -11248,7 +11248,7 @@
     </row>
     <row r="244" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C244" s="26" t="s">
@@ -11264,15 +11264,15 @@
         <v>1.39</v>
       </c>
       <c r="I244" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J244" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K244" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>1.39</v>
       </c>
       <c r="L244" t="s">
@@ -11281,7 +11281,7 @@
     </row>
     <row r="245" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B245" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
       <c r="C245" s="26" t="s">
@@ -11297,15 +11297,15 @@
         <v>3.29</v>
       </c>
       <c r="I245" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>5</v>
       </c>
       <c r="J245" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K245" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>16.45</v>
       </c>
       <c r="L245" t="s">
@@ -11314,7 +11314,7 @@
     </row>
     <row r="246" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B246" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C246" s="26" t="s">
@@ -11330,15 +11330,15 @@
         <v>3.29</v>
       </c>
       <c r="I246" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J246" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K246" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>3.29</v>
       </c>
       <c r="L246" t="s">
@@ -11347,7 +11347,7 @@
     </row>
     <row r="247" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B247" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="C247" s="26" t="s">
@@ -11363,15 +11363,15 @@
         <v>1</v>
       </c>
       <c r="I247" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="J247" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K247" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="L247" t="s">
@@ -11380,7 +11380,7 @@
     </row>
     <row r="248" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B248" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C248" s="26" t="s">
@@ -11396,15 +11396,15 @@
         <v>20</v>
       </c>
       <c r="I248" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J248" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K248" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>20</v>
       </c>
       <c r="L248" t="s">
@@ -11413,7 +11413,7 @@
     </row>
     <row r="249" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B249" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="C249" s="26" t="s">
@@ -11429,15 +11429,15 @@
         <v>18.079999999999998</v>
       </c>
       <c r="I249" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J249" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K249" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L249" t="s">
@@ -11446,7 +11446,7 @@
     </row>
     <row r="250" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B250" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="C250" s="26" t="s">
@@ -11462,15 +11462,15 @@
         <v>18.079999999999998</v>
       </c>
       <c r="I250" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="J250" s="32">
-        <f t="shared" si="35"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K250" s="29">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v>36.159999999999997</v>
       </c>
       <c r="L250" t="s">
@@ -11515,15 +11515,15 @@
         <v>10.99</v>
       </c>
       <c r="I253" s="31">
-        <f t="shared" ref="I253:I261" si="39">SUMIF(C$1:C$144,"="&amp;C253,B$1:B$144)</f>
+        <f t="shared" ref="I253:I261" si="32">SUMIF(C$1:C$144,"="&amp;C253,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J253" s="32">
-        <f t="shared" ref="J253:J260" si="40">G253*B253-I253</f>
+        <f t="shared" ref="J253:J260" si="33">G253*B253-I253</f>
         <v>1</v>
       </c>
       <c r="K253" s="29">
-        <f t="shared" ref="K253:K260" si="41">B253*H253</f>
+        <f t="shared" ref="K253:K260" si="34">B253*H253</f>
         <v>10.99</v>
       </c>
       <c r="L253" t="s">
@@ -11547,15 +11547,15 @@
         <v>10.99</v>
       </c>
       <c r="I254" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="J254" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K254" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>10.99</v>
       </c>
       <c r="L254" t="s">
@@ -11579,15 +11579,15 @@
         <v>2.8</v>
       </c>
       <c r="I255" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J255" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="K255" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>2.8</v>
       </c>
       <c r="L255" t="s">
@@ -11611,15 +11611,15 @@
         <v>2.8</v>
       </c>
       <c r="I256" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="J256" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K256" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>2.8</v>
       </c>
       <c r="L256" t="s">
@@ -11643,15 +11643,15 @@
         <v>2.8</v>
       </c>
       <c r="I257" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J257" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="K257" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>2.8</v>
       </c>
       <c r="L257" t="s">
@@ -11675,15 +11675,15 @@
         <v>2.8</v>
       </c>
       <c r="I258" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="J258" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K258" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>2.8</v>
       </c>
       <c r="L258" t="s">
@@ -11707,15 +11707,15 @@
         <v>1839</v>
       </c>
       <c r="I259" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J259" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="K259" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>1839</v>
       </c>
       <c r="L259" t="s">
@@ -11739,15 +11739,15 @@
         <v>49</v>
       </c>
       <c r="I260" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J260" s="32">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="K260" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>49</v>
       </c>
       <c r="L260" t="s">
@@ -11766,7 +11766,7 @@
       </c>
       <c r="H261" s="19"/>
       <c r="I261" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J261" s="32"/>
@@ -11808,15 +11808,15 @@
         <v>0.87</v>
       </c>
       <c r="I264" s="31">
-        <f t="shared" ref="I264:I269" si="42">SUMIF(C$1:C$144,"="&amp;C264,B$1:B$144)</f>
+        <f t="shared" ref="I264:I269" si="35">SUMIF(C$1:C$144,"="&amp;C264,B$1:B$144)</f>
         <v>0</v>
       </c>
       <c r="J264" s="32">
-        <f t="shared" ref="J264:J269" si="43">G264*B264-I264</f>
+        <f t="shared" ref="J264:J269" si="36">G264*B264-I264</f>
         <v>1</v>
       </c>
       <c r="K264" s="29">
-        <f t="shared" ref="K264:K269" si="44">B264*H264</f>
+        <f t="shared" ref="K264:K269" si="37">B264*H264</f>
         <v>0.87</v>
       </c>
       <c r="L264" t="s">
@@ -11840,15 +11840,15 @@
         <v>0.8</v>
       </c>
       <c r="I265" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J265" s="32">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="K265" s="29">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>0.8</v>
       </c>
       <c r="L265" t="s">
@@ -11872,15 +11872,15 @@
         <v>19.989999999999998</v>
       </c>
       <c r="I266" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J266" s="32">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="K266" s="29">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>99.949999999999989</v>
       </c>
       <c r="L266" t="s">
@@ -11904,15 +11904,15 @@
         <v>44</v>
       </c>
       <c r="I267" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J267" s="32">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="K267" s="29">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>44</v>
       </c>
       <c r="L267" t="s">
@@ -11936,15 +11936,15 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="I268" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J268" s="32">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="K268" s="29">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>10.25</v>
       </c>
       <c r="L268" t="s">
@@ -11968,15 +11968,15 @@
         <v>1.95</v>
       </c>
       <c r="I269" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J269" s="32">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="K269" s="29">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>9.75</v>
       </c>
       <c r="L269" t="s">
@@ -12176,7 +12176,7 @@
       <c r="K298"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L149 D180:K180 B181:K181 B182:D182 F182:K182 F185:K187 B185:D187 B183:K184 C253 G253:K253 F211:K214 B211:D214 B223:C223 E224 F223:K225 B224:D225 B179 F179:K179 D179 B215:K222 B254:K261 D271:K271 B271 B264:K270 E275:E276 B146:K178 B4:K14 B226:K251 B16:K143 B188:K210">
+  <conditionalFormatting sqref="L149 D180:K180 B181:K181 B182:D182 F182:K182 F185:K187 B185:D187 B183:K184 C253 G253:K253 B223:C223 E224 F223:K225 B224:D225 B179 F179:K179 D179 B215:K222 B254:K261 D271:K271 B271 B264:K270 E275:E276 B146:K178 B4:K14 B226:K251 B16:K143 B188:K209 B211:K211 F212:K214 F210:K210 B212:D214 B210:D210">
     <cfRule type="expression" dxfId="17" priority="462">
       <formula>$L4=#REF!</formula>
     </cfRule>
@@ -12186,7 +12186,7 @@
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E211">
+  <conditionalFormatting sqref="E210">
     <cfRule type="expression" dxfId="15" priority="498">
       <formula>$L224=#REF!</formula>
     </cfRule>
@@ -12206,7 +12206,7 @@
       <formula>$L178=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A180 D180:XFD180 A181:XFD181 A182:D182 F182:XFD182 F185:XFD187 A185:D187 A183:XFD184 C253 G253:L253 A211:D214 F211:XFD214 A223:C223 E224 A224:D225 F223:XFD225 A179:B179 F179:XFD179 D179 A215:XFD222 A271:B271 D271:XFD271 A254:XFD261 A264:XFD270 E275:E276 A146:XFD178 A4:XFD14 A226:XFD251 A16:XFD143 A188:XFD210">
+  <conditionalFormatting sqref="A180 D180:XFD180 A181:XFD181 A182:D182 F182:XFD182 F185:XFD187 A185:D187 A183:XFD184 C253 G253:L253 A223:C223 E224 A224:D225 F223:XFD225 A179:B179 F179:XFD179 D179 A215:XFD222 A271:B271 D271:XFD271 A254:XFD261 A264:XFD270 E275:E276 A146:XFD178 A4:XFD14 A226:XFD251 A16:XFD143 A188:XFD209 A211:XFD211 A212:D214 A210:D210 F212:XFD214 F210:XFD210">
     <cfRule type="expression" dxfId="11" priority="502">
       <formula>$L4=#REF!</formula>
     </cfRule>
@@ -12222,7 +12222,7 @@
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E211">
+  <conditionalFormatting sqref="E210">
     <cfRule type="expression" dxfId="7" priority="568">
       <formula>$L224=#REF!</formula>
     </cfRule>
@@ -12255,7 +12255,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L146:L179 L234:L250 L253:L261 L264:L269 L181:L232">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L146:L179 L234:L250 L253:L261 L264:L269 L181:L211 L212:L232">
       <formula1>$O$1:$O$22</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Unterarm Kabelkanal etwas größer, Kabeldeckel eingeführt und Zahnriemenraddurchbruch
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="1"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
     <sheet name="Zahnriemenscheiben" sheetId="5" r:id="rId2"/>
     <sheet name="DIN" sheetId="8" r:id="rId3"/>
     <sheet name="Rotary Encoder" sheetId="6" r:id="rId4"/>
-    <sheet name="Linearlager" sheetId="12" r:id="rId5"/>
-    <sheet name="Herkulex Servo" sheetId="10" r:id="rId6"/>
-    <sheet name="PiBot Stepper Driver" sheetId="11" r:id="rId7"/>
-    <sheet name="BOM" sheetId="7" r:id="rId8"/>
+    <sheet name="Herkulex Servo" sheetId="10" r:id="rId5"/>
+    <sheet name="PiBot Stepper Driver" sheetId="11" r:id="rId6"/>
+    <sheet name="BOM" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">BOM!$A$142:$K$272</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">BOM!$A$142:$K$272</definedName>
     <definedName name="Kaufstatus">BOM!$L:$L</definedName>
     <definedName name="ShoppingStatus">BOM!$L:$L</definedName>
   </definedNames>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="482">
   <si>
     <t>Material</t>
   </si>
@@ -1467,6 +1466,12 @@
   </si>
   <si>
     <t>Innendurchmesser</t>
+  </si>
+  <si>
+    <t>Riemenbiegestelle trapezlänge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zahnoberkantelänge </t>
   </si>
 </sst>
 </file>
@@ -2293,66 +2298,6 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>65352</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1" descr="http://g01.a.alicdn.com/kf/HTB1jZSHGFXXXXaiXFXXq6xXFXXXP/221585428/HTB1jZSHGFXXXXaiXFXXq6xXFXXXP.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="5836920" cy="6283272"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2407,7 +2352,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4452,10 +4397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4500,17 +4445,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>100</v>
       </c>
       <c r="C36">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
         <v>476</v>
@@ -4519,13 +4464,13 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>102</v>
       </c>
       <c r="C37" s="2">
         <f>C36*2.5/PI()</f>
-        <v>47.7464829275686</v>
+        <v>11.93662073189215</v>
       </c>
       <c r="D37" t="s">
         <v>30</v>
@@ -4535,20 +4480,20 @@
       </c>
       <c r="G37">
         <f>RADIANS(25-360/C36/2)</f>
-        <v>0.38397243543875248</v>
-      </c>
-      <c r="H37">
+        <v>0.22689280275926285</v>
+      </c>
+      <c r="H37" s="4">
         <f>DEGREES(G37)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>101</v>
       </c>
       <c r="C38" s="2">
         <f>C37-G36</f>
-        <v>47.196482927568603</v>
+        <v>11.386620731892149</v>
       </c>
       <c r="D38" t="s">
         <v>30</v>
@@ -4557,17 +4502,25 @@
         <v>478</v>
       </c>
       <c r="G38">
-        <f>(2.5*C38/C37)-1*C38/C39-2*(C38-C39)/2*SIN(G37)</f>
-        <v>0.67773764965221417</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <f>(2.5-1-2*SIN(RADIANS(20))*0.7)/C37*C38</f>
+        <v>0.97411958060860215</v>
+      </c>
+      <c r="H38">
+        <f>(1*(C38/2-0.7)/(C39/2)*C38/C39)</f>
+        <v>1.2906095401756847</v>
+      </c>
+      <c r="I38">
+        <f>2*SIN(RADIANS(G37))*0.7*C38/C39</f>
+        <v>6.7252831353765584E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>479</v>
       </c>
       <c r="C39" s="2">
         <f>C38-2</f>
-        <v>45.196482927568603</v>
+        <v>9.3866207318921493</v>
       </c>
       <c r="D39" t="s">
         <v>30</v>
@@ -4576,23 +4529,37 @@
         <v>418</v>
       </c>
       <c r="G39">
-        <f>C38+2*((G38/2)/TAN(G37))</f>
-        <v>48.873942474288057</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <f>C38+1.4*((G38/2)/TAN(G37))</f>
+        <v>14.340183555343922</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>418</v>
       </c>
       <c r="C40" s="2">
         <f>G39</f>
-        <v>48.873942474288057</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>14.340183555343922</v>
+      </c>
+      <c r="E40" t="s">
+        <v>480</v>
+      </c>
+      <c r="G40">
+        <f>2.5-1-2*(SIN(RADIANS(20)))*0.7</f>
+        <v>1.0211717993440639</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>481</v>
+      </c>
+      <c r="G41">
+        <f>G40+SIN(RADIANS(H37))*2*(C37-C38)/2</f>
+        <v>1.1448948792331899</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C43" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -4856,22 +4823,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F25" sqref="F25:G26"/>
     </sheetView>
   </sheetViews>
@@ -4944,7 +4898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
@@ -5344,15 +5298,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O296"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A214" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Oberarm lagerring an der Seite hat jetzt keine durchgehenden Schlitz mehr
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5470,10 +5470,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O301"/>
+  <dimension ref="A1:O302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A273" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B284" sqref="B284"/>
+      <selection activeCell="A294" sqref="A294:XFD294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12368,97 +12368,97 @@
         <v>502</v>
       </c>
       <c r="C292" t="s">
-        <v>523</v>
-      </c>
+        <v>519</v>
+      </c>
+      <c r="D292" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="E292" s="22"/>
+      <c r="I292" s="30"/>
+      <c r="J292"/>
+      <c r="K292"/>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B293" t="s">
         <v>502</v>
       </c>
       <c r="C293" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B295" t="s">
+        <v>502</v>
+      </c>
+      <c r="C295" t="s">
         <v>510</v>
       </c>
-      <c r="D293" s="8" t="s">
+      <c r="D295" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="E293" s="21"/>
-      <c r="I293" s="30"/>
-      <c r="J293"/>
-      <c r="K293"/>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B294" t="s">
-        <v>502</v>
-      </c>
-      <c r="C294" t="s">
-        <v>519</v>
-      </c>
-      <c r="D294" s="8" t="s">
-        <v>520</v>
-      </c>
-      <c r="E294" s="22"/>
-      <c r="I294" s="30"/>
-      <c r="J294"/>
-      <c r="K294"/>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D295" s="8"/>
-      <c r="E295" s="22"/>
+      <c r="E295" s="21"/>
       <c r="I295" s="30"/>
       <c r="J295"/>
       <c r="K295"/>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A296" t="s">
+      <c r="D296" s="8"/>
+      <c r="E296" s="22"/>
+      <c r="I296" s="30"/>
+      <c r="J296"/>
+      <c r="K296"/>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B297" t="s">
-        <v>502</v>
-      </c>
-      <c r="C297" t="s">
-        <v>501</v>
-      </c>
-      <c r="D297" t="s">
-        <v>514</v>
-      </c>
-      <c r="I297" s="30"/>
-      <c r="J297"/>
-      <c r="K297"/>
-    </row>
-    <row r="298" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B298" t="s">
         <v>502</v>
       </c>
       <c r="C298" t="s">
-        <v>507</v>
-      </c>
-      <c r="D298" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="E298" s="22"/>
+        <v>501</v>
+      </c>
+      <c r="D298" t="s">
+        <v>514</v>
+      </c>
       <c r="I298" s="30"/>
       <c r="J298"/>
       <c r="K298"/>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E299" s="21"/>
+    <row r="299" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B299" t="s">
+        <v>502</v>
+      </c>
+      <c r="C299" t="s">
+        <v>507</v>
+      </c>
+      <c r="D299" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="E299" s="22"/>
       <c r="I299" s="30"/>
       <c r="J299"/>
       <c r="K299"/>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H300" s="19"/>
+      <c r="E300" s="21"/>
       <c r="I300" s="30"/>
       <c r="J300"/>
       <c r="K300"/>
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H301" s="20"/>
+      <c r="H301" s="19"/>
       <c r="I301" s="30"/>
       <c r="J301"/>
       <c r="K301"/>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H302" s="20"/>
+      <c r="I302" s="30"/>
+      <c r="J302"/>
+      <c r="K302"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L146 D177:K177 B178:K178 B179:D179 F179:K179 F182:K184 B182:D184 B180:K181 C250 G250:K250 B220:C220 E221 F220:K222 B221:D222 B176 F176:K176 D176 B212:K219 B251:K258 D268:K268 B268 B261:K267 E272:E273 B143:K175 B223:K248 B185:K206 B208:K208 F209:K211 F207:K207 B209:D211 B207:D207 B3:K12 B14:K140">

</xml_diff>

<commit_message>
connect To Bot mode
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="1"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -4541,7 +4541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -5472,8 +5472,8 @@
   </sheetPr>
   <dimension ref="A1:O300"/>
   <sheetViews>
-    <sheetView topLeftCell="A278" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A292" sqref="A292:XFD292"/>
+    <sheetView tabSelected="1" topLeftCell="A278" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C295" sqref="C295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
interface to uC converts from radian to degrees
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="522">
   <si>
     <t>Material</t>
   </si>
@@ -1585,6 +1585,12 @@
   </si>
   <si>
     <t>Riss beim zuschrauben  nicht plane Ebene auf dem Podest, da muss ich ncoh was stabiler machen</t>
+  </si>
+  <si>
+    <t>Schulter links (sensorseite)</t>
+  </si>
+  <si>
+    <t>Kabelführung 0,6 an der Wand enger gemacht, Wand ist etwas zu unstabil. Ist aber nicht wirklich nötig</t>
   </si>
 </sst>
 </file>
@@ -5470,10 +5476,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O300"/>
+  <dimension ref="A1:O299"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A278" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+      <selection activeCell="C293" sqref="C293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12273,40 +12279,67 @@
       <c r="K282"/>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D283" s="8"/>
-      <c r="E283" s="21"/>
-      <c r="I283" s="30"/>
-      <c r="J283"/>
-      <c r="K283"/>
+      <c r="C283" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A284" t="s">
-        <v>507</v>
-      </c>
-      <c r="E284" s="24"/>
+      <c r="B284" t="s">
+        <v>500</v>
+      </c>
+      <c r="C284" t="s">
+        <v>509</v>
+      </c>
+      <c r="D284" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="E284" s="21"/>
       <c r="I284" s="30"/>
       <c r="J284"/>
       <c r="K284"/>
     </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D285" s="8"/>
+      <c r="E285" s="21"/>
+      <c r="I285" s="30"/>
+      <c r="J285"/>
+      <c r="K285"/>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>507</v>
+      </c>
+      <c r="E286" s="24"/>
+      <c r="I286" s="30"/>
+      <c r="J286"/>
+      <c r="K286"/>
+    </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
         <v>500</v>
       </c>
       <c r="C287" t="s">
-        <v>510</v>
-      </c>
+        <v>512</v>
+      </c>
+      <c r="D287" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="H287" s="19"/>
+      <c r="I287" s="30"/>
+      <c r="J287"/>
+      <c r="K287"/>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B288" t="s">
         <v>500</v>
       </c>
       <c r="C288" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D288" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="E288" s="21"/>
+        <v>514</v>
+      </c>
+      <c r="H288" s="20"/>
       <c r="I288" s="30"/>
       <c r="J288"/>
       <c r="K288"/>
@@ -12316,86 +12349,67 @@
         <v>500</v>
       </c>
       <c r="C289" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="D289" s="8" t="s">
-        <v>515</v>
-      </c>
-      <c r="H289" s="19"/>
-      <c r="I289" s="30"/>
-      <c r="J289"/>
-      <c r="K289"/>
+        <v>517</v>
+      </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B290" t="s">
         <v>500</v>
       </c>
       <c r="C290" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="D290" s="8" t="s">
-        <v>514</v>
-      </c>
-      <c r="H290" s="20"/>
-      <c r="I290" s="30"/>
-      <c r="J290"/>
-      <c r="K290"/>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B291" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B297" t="s">
         <v>500</v>
       </c>
-      <c r="C291" t="s">
-        <v>516</v>
-      </c>
-      <c r="D291" s="8" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B292" t="s">
+      <c r="C297" t="s">
+        <v>499</v>
+      </c>
+      <c r="D297" t="s">
+        <v>505</v>
+      </c>
+      <c r="I297" s="30"/>
+      <c r="J297"/>
+      <c r="K297"/>
+    </row>
+    <row r="298" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B298" t="s">
         <v>500</v>
       </c>
-      <c r="C292" t="s">
-        <v>518</v>
-      </c>
-      <c r="D292" s="8" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A293" t="s">
-        <v>506</v>
-      </c>
+      <c r="C298" t="s">
+        <v>501</v>
+      </c>
+      <c r="D298" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="E298" s="22"/>
+      <c r="I298" s="30"/>
+      <c r="J298"/>
+      <c r="K298"/>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B299" t="s">
         <v>500</v>
       </c>
       <c r="C299" t="s">
-        <v>499</v>
+        <v>520</v>
       </c>
       <c r="D299" t="s">
-        <v>505</v>
-      </c>
-      <c r="I299" s="30"/>
-      <c r="J299"/>
-      <c r="K299"/>
-    </row>
-    <row r="300" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B300" t="s">
-        <v>500</v>
-      </c>
-      <c r="C300" t="s">
-        <v>501</v>
-      </c>
-      <c r="D300" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="E300" s="22"/>
-      <c r="I300" s="30"/>
-      <c r="J300"/>
-      <c r="K300"/>
+        <v>521</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L146 D177:K177 B178:K178 B179:D179 F179:K179 F182:K184 B182:D184 B180:K181 C250 G250:K250 B220:C220 E221 F220:K222 B221:D222 B176 F176:K176 D176 B212:K219 B251:K258 D268:K268 B268 B261:K267 E272:E273 B143:K175 B223:K248 B185:K206 B208:K208 F209:K211 F207:K207 B209:D211 B207:D207 B3:K12 B14:K140">

</xml_diff>

<commit_message>
einzelne Motoren Regelung eingestellt
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="6"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
-    <sheet name="Zahnriemenscheiben" sheetId="5" r:id="rId2"/>
-    <sheet name="DIN" sheetId="8" r:id="rId3"/>
-    <sheet name="Rotary Encoder" sheetId="6" r:id="rId4"/>
-    <sheet name="Herkulex Servo" sheetId="10" r:id="rId5"/>
-    <sheet name="PiBot Stepper Driver" sheetId="11" r:id="rId6"/>
-    <sheet name="BOM" sheetId="7" r:id="rId7"/>
+    <sheet name="Tabelle1" sheetId="12" r:id="rId2"/>
+    <sheet name="Zahnriemenscheiben" sheetId="5" r:id="rId3"/>
+    <sheet name="DIN" sheetId="8" r:id="rId4"/>
+    <sheet name="Rotary Encoder" sheetId="6" r:id="rId5"/>
+    <sheet name="Herkulex Servo" sheetId="10" r:id="rId6"/>
+    <sheet name="PiBot Stepper Driver" sheetId="11" r:id="rId7"/>
+    <sheet name="BOM" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">BOM!$A$141:$K$271</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">BOM!$A$141:$K$271</definedName>
     <definedName name="Kaufstatus">BOM!$L:$L</definedName>
     <definedName name="ShoppingStatus">BOM!$L:$L</definedName>
   </definedNames>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="526">
   <si>
     <t>Material</t>
   </si>
@@ -1425,9 +1426,6 @@
     <t>4,2 Ohm</t>
   </si>
   <si>
-    <t>Snorre</t>
-  </si>
-  <si>
     <t>Walter</t>
   </si>
   <si>
@@ -1591,6 +1589,21 @@
   </si>
   <si>
     <t>Kabelführung 0,6 an der Wand enger gemacht, Wand ist etwas zu unstabil. Ist aber nicht wirklich nötig</t>
+  </si>
+  <si>
+    <t>Gehäuse</t>
+  </si>
+  <si>
+    <t>http://gkshop.co.uk/de/0-5-a-dc-ammeter-amp-current-panel-meter-round-analogue-analog.html</t>
+  </si>
+  <si>
+    <t>Kippschalter</t>
+  </si>
+  <si>
+    <t>http://www.ebay.de/itm/Kippschalter-aus-Aluminium-Ein-Aus-2polig-Schalter-6V-12V-345-01/322256822791?_trksid=p2047675.c100005.m1851&amp;_trkparms=aid%3D222007%26algo%3DSIC.MBE%26ao%3D2%26asc%3D38052%26meid%3Dccb372c197a04cd49a68967fbfc41da1%26pid%3D100005%26rk%3D3%26rkt%3D6%26sd%3D322247093065</t>
+  </si>
+  <si>
+    <t>gedruckt, nicht montiert</t>
   </si>
 </sst>
 </file>
@@ -1991,6 +2004,176 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1" descr="https://lh6.googleusercontent.com/-A7GTgUQ_rls/VvxZrnxnkOI/AAAAAAAAPR0/3WOZyZapWrEsnV1htVbUmJE0j5XHwRbKw/w649-h865-no/IMG_0013.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5394960" cy="7185660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2" descr="http://gkshop.co.uk/media/products/9da489d1dfc92b8a20701fa4ca07a172/images/thumbnail/big_RC042B.jpg?lm=1472838465"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7132320" y="914400"/>
+          <a:ext cx="7620000" cy="5715000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21985</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>629428</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="viEnlargeImgLayer_img_ctr" descr="http://i.ebayimg.com/images/g/0e0AAOSwU-pXq1em/s-l1600.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5569345" y="7277100"/>
+          <a:ext cx="2192403" cy="2750820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -2151,7 +2334,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2359,7 +2542,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2419,7 +2602,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2479,7 +2662,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2993,8 +3176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AE93"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3014,59 +3197,56 @@
     <col min="24" max="24" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>466</v>
       </c>
-      <c r="D2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>400</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>270</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>0.8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3074,11 +3254,11 @@
         <f>Q72+0.2</f>
         <v>0.97</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3086,11 +3266,11 @@
         <f>Q73+Q74 +0.4</f>
         <v>0.81</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3098,11 +3278,11 @@
         <f>Q74+0.1</f>
         <v>0.33</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>397</v>
       </c>
@@ -3110,43 +3290,33 @@
         <f>C14/C12</f>
         <v>9</v>
       </c>
-      <c r="D10" s="5">
-        <f>D14/D12</f>
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="8">
         <v>5</v>
       </c>
-      <c r="D11" s="8">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="6">
         <v>10</v>
       </c>
-      <c r="D12" s="6">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -3154,29 +3324,22 @@
         <f>C12*C11/PI()</f>
         <v>15.915494309189533</v>
       </c>
-      <c r="D13" s="4">
-        <f>D12*D11/PI()</f>
-        <v>15.915494309189533</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="7">
         <v>90</v>
       </c>
-      <c r="D14" s="7">
-        <v>90</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -3184,89 +3347,68 @@
         <f>C14*C11/PI()</f>
         <v>143.23944878270581</v>
       </c>
-      <c r="D15" s="4">
-        <f>D14*D11/PI()</f>
-        <v>143.23944878270581</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="5">
         <f>C20/C18*(C24/C22)</f>
-        <v>22.857142857142858</v>
-      </c>
-      <c r="D16" s="5">
-        <f>D20/D18*(D24/D22)</f>
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
+        <v>20.571428571428569</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="6">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="4">
         <f>C18*C17/PI()</f>
-        <v>19.098593171027442</v>
-      </c>
-      <c r="D19" s="4">
-        <f>D18*D17/PI()</f>
-        <v>19.098593171027442</v>
-      </c>
-      <c r="E19" t="s">
+        <v>22.281692032865347</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="7">
         <v>48</v>
       </c>
-      <c r="D20" s="7">
-        <v>48</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -3274,149 +3416,114 @@
         <f>C20*C17/PI()</f>
         <v>76.394372684109769</v>
       </c>
-      <c r="D21" s="4">
-        <f>D20*D17/PI()</f>
-        <v>76.394372684109769</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="6">
-        <v>14</v>
-      </c>
-      <c r="D22" s="6">
         <v>12</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="4">
         <f>C22*C17/PI()</f>
-        <v>22.281692032865347</v>
-      </c>
-      <c r="D23" s="4">
-        <f>D22*D17/PI()</f>
         <v>19.098593171027442</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="7">
-        <v>80</v>
-      </c>
-      <c r="D24" s="7">
         <v>72</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="4">
         <f>C24*C17/PI()</f>
-        <v>127.32395447351627</v>
-      </c>
-      <c r="D25" s="4">
-        <f>D24*D17/PI()</f>
         <v>114.59155902616465</v>
       </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5">
         <f>C30/C28*(C34/C32)</f>
-        <v>11.428571428571427</v>
-      </c>
-      <c r="D26" s="5">
-        <f>D30/D28*(D34/D32)</f>
         <v>11.755102040816325</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="6">
-        <v>18</v>
-      </c>
-      <c r="D28" s="6">
         <v>14</v>
       </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="4">
         <f>C28*C27/PI()</f>
-        <v>28.647889756541161</v>
-      </c>
-      <c r="D29" s="4">
-        <f>D28*D27/PI()</f>
         <v>22.281692032865347</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="7">
         <v>48</v>
       </c>
-      <c r="D30" s="7">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -3424,29 +3531,22 @@
         <f>C30*C27/PI()</f>
         <v>76.394372684109769</v>
       </c>
-      <c r="D31" s="4">
-        <f>D30*D27/PI()</f>
-        <v>76.394372684109769</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="6">
         <v>14</v>
       </c>
-      <c r="D32" s="6">
-        <v>14</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>38</v>
       </c>
@@ -3454,45 +3554,34 @@
         <f>C32*C27/PI()</f>
         <v>22.281692032865347</v>
       </c>
-      <c r="D33" s="4">
-        <f>D32*D27/PI()</f>
-        <v>22.281692032865347</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="7">
-        <v>60</v>
-      </c>
-      <c r="D34" s="7">
         <v>48</v>
       </c>
-      <c r="E34" t="s">
+      <c r="D34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="4">
         <f>C34*C27/PI()</f>
-        <v>95.4929658551372</v>
-      </c>
-      <c r="D35" s="4">
-        <f>D34*D27/PI()</f>
         <v>76.394372684109769</v>
       </c>
-      <c r="E35" t="s">
+      <c r="D35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -3501,105 +3590,81 @@
       </c>
       <c r="C36" s="4">
         <f>C40/C38*(C44/C42)</f>
-        <v>5.1333333333333329</v>
-      </c>
-      <c r="D36" s="4">
-        <f>D40/D38*(D44/D42)</f>
         <v>7.4374999999999991</v>
       </c>
-      <c r="E36" t="s">
+      <c r="D36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>29</v>
       </c>
       <c r="C37">
         <v>2.5</v>
       </c>
-      <c r="D37">
-        <v>2.5</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="6">
-        <v>15</v>
-      </c>
-      <c r="D38" s="6">
         <v>14</v>
       </c>
-      <c r="E38" t="s">
+      <c r="D38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="4">
         <f>C38*C37/PI()</f>
-        <v>11.93662073189215</v>
-      </c>
-      <c r="D39" s="4">
-        <f>D38*D37/PI()</f>
         <v>11.140846016432674</v>
       </c>
-      <c r="E39" t="s">
+      <c r="D39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>32</v>
       </c>
       <c r="C40" s="7">
-        <v>22</v>
-      </c>
-      <c r="D40" s="7">
         <v>34</v>
       </c>
-      <c r="E40" t="s">
+      <c r="D40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="4">
         <f>C40*C37/PI()</f>
-        <v>17.507043740108486</v>
-      </c>
-      <c r="D41" s="4">
-        <f>D40*D37/PI()</f>
         <v>27.056340325622209</v>
       </c>
-      <c r="E41" t="s">
+      <c r="D41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="6">
         <v>16</v>
       </c>
-      <c r="D42" s="6">
-        <v>16</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>38</v>
       </c>
@@ -3607,85 +3672,64 @@
         <f>C42*C37/PI()</f>
         <v>12.732395447351628</v>
       </c>
-      <c r="D43" s="4">
-        <f>D42*D37/PI()</f>
-        <v>12.732395447351628</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="7">
-        <v>56</v>
-      </c>
-      <c r="D44" s="7">
         <v>49</v>
       </c>
-      <c r="E44" t="s">
+      <c r="D44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="4">
         <f>C44*C37/PI()</f>
-        <v>44.563384065730695</v>
-      </c>
-      <c r="D45" s="4">
-        <f>D44*D37/PI()</f>
         <v>38.992961057514357</v>
       </c>
-      <c r="E45" t="s">
+      <c r="D45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>136</v>
       </c>
       <c r="C46" s="4">
         <f>C50/C48</f>
-        <v>3.5</v>
-      </c>
-      <c r="D46" s="4">
-        <f>D50/D48</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="E46" t="s">
+      <c r="D46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>29</v>
       </c>
       <c r="C47">
         <v>2.5</v>
       </c>
-      <c r="D47">
-        <v>2.5</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>34</v>
       </c>
       <c r="C48" s="6">
-        <v>16</v>
-      </c>
-      <c r="D48" s="6">
         <v>15</v>
       </c>
-      <c r="E48" t="s">
+      <c r="D48" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3695,13 +3739,9 @@
       </c>
       <c r="C49" s="4">
         <f>C48*C47/PI()</f>
-        <v>12.732395447351628</v>
-      </c>
-      <c r="D49" s="4">
-        <f>D48*D47/PI()</f>
         <v>11.93662073189215</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D49" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3710,12 +3750,9 @@
         <v>35</v>
       </c>
       <c r="C50" s="7">
-        <v>56</v>
-      </c>
-      <c r="D50" s="7">
         <v>65</v>
       </c>
-      <c r="E50" t="s">
+      <c r="D50" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3725,13 +3762,9 @@
       </c>
       <c r="C51" s="4">
         <f>C50*C47/PI()</f>
-        <v>44.563384065730695</v>
-      </c>
-      <c r="D51" s="4">
-        <f>D50*D47/PI()</f>
         <v>51.725356504865985</v>
       </c>
-      <c r="E51" t="s">
+      <c r="D51" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3864,7 +3897,7 @@
       </c>
       <c r="C64" s="2">
         <f>C59/C16</f>
-        <v>1.442520646875</v>
+        <v>1.6028007187500004</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s">
@@ -3877,7 +3910,7 @@
       </c>
       <c r="C65" s="2">
         <f>C60/C26</f>
-        <v>0.92421236250000027</v>
+        <v>0.89853979687500019</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s">
@@ -3889,7 +3922,7 @@
         <v>139</v>
       </c>
       <c r="C66" s="2">
-        <f>C61/D36</f>
+        <f>C61/C36</f>
         <v>7.4523025210084054E-2</v>
       </c>
       <c r="D66" s="2"/>
@@ -3902,7 +3935,7 @@
         <v>137</v>
       </c>
       <c r="C67" s="2">
-        <f>C62/D46</f>
+        <f>C62/C46</f>
         <v>0.12790730769230774</v>
       </c>
       <c r="D67" s="2"/>
@@ -3914,7 +3947,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="F68" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>40</v>
@@ -3960,7 +3993,7 @@
         <v>463</v>
       </c>
       <c r="W68" s="51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="69" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
@@ -3992,7 +4025,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
@@ -4053,7 +4086,7 @@
       </c>
       <c r="C71" s="2">
         <f>C64*(1+C53)</f>
-        <v>1.8752768409375</v>
+        <v>2.0836409343750004</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s">
@@ -4061,7 +4094,7 @@
       </c>
       <c r="F71" s="53">
         <f>M71/C71/100</f>
-        <v>1.5997637972749781</v>
+        <v>1.4397874175474801</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>399</v>
@@ -4107,7 +4140,7 @@
       </c>
       <c r="C72" s="2">
         <f>C65*(1+C53)</f>
-        <v>1.2014760712500003</v>
+        <v>1.1681017359375003</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s">
@@ -4115,7 +4148,7 @@
       </c>
       <c r="F72" s="53">
         <f>M72/C72/100</f>
-        <v>1.5813881320360081</v>
+        <v>1.6265706500941801</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>261</v>
@@ -4219,16 +4252,16 @@
         <v>0.47606999999999999</v>
       </c>
       <c r="T73" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="U73" s="51" t="s">
         <v>476</v>
-      </c>
-      <c r="U73" s="51" t="s">
-        <v>477</v>
       </c>
       <c r="V73" s="10" t="s">
         <v>465</v>
       </c>
       <c r="W73" s="51" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="X73" s="10"/>
       <c r="Y73" s="10"/>
@@ -4256,7 +4289,7 @@
         <v>1.5636323178744218</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H74" s="51">
         <v>1.8</v>
@@ -4294,16 +4327,16 @@
         <v>0.27204</v>
       </c>
       <c r="T74" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="U74" s="12" t="s">
         <v>476</v>
-      </c>
-      <c r="U74" s="12" t="s">
-        <v>477</v>
       </c>
       <c r="V74" s="12" t="s">
         <v>464</v>
       </c>
       <c r="W74" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="X74" s="54"/>
       <c r="Y74" s="12"/>
@@ -4380,9 +4413,9 @@
       <c r="A79" t="s">
         <v>95</v>
       </c>
-      <c r="C79" s="16">
-        <f>(C15/1000/2)</f>
-        <v>7.1619724391352904E-2</v>
+      <c r="C79" s="16" t="e">
+        <f>(#REF!/1000/2)</f>
+        <v>#REF!</v>
       </c>
       <c r="D79" s="16"/>
       <c r="E79" t="s">
@@ -4393,9 +4426,9 @@
       <c r="A80" t="s">
         <v>91</v>
       </c>
-      <c r="C80" s="16">
+      <c r="C80" s="16" t="e">
         <f>C58/C79</f>
-        <v>111.27037373746393</v>
+        <v>#REF!</v>
       </c>
       <c r="D80" s="16"/>
       <c r="E80" t="s">
@@ -4406,9 +4439,9 @@
       <c r="A81" t="s">
         <v>92</v>
       </c>
-      <c r="C81" s="16">
+      <c r="C81" s="16" t="e">
         <f>(C78)*C80*2*PI()</f>
-        <v>699.13237739161468</v>
+        <v>#REF!</v>
       </c>
       <c r="D81" s="16"/>
       <c r="E81" t="s">
@@ -4436,9 +4469,9 @@
       <c r="A85" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="17">
-        <f>(C21/1000/2)</f>
-        <v>3.8197186342054885E-2</v>
+      <c r="C85" s="17" t="e">
+        <f>(#REF!/1000/2)</f>
+        <v>#REF!</v>
       </c>
       <c r="D85" s="17"/>
       <c r="E85" t="s">
@@ -4449,9 +4482,9 @@
       <c r="A86" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="17">
+      <c r="C86" s="17" t="e">
         <f>C59/C85</f>
-        <v>863.20233654744686</v>
+        <v>#REF!</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" t="s">
@@ -4463,9 +4496,9 @@
       <c r="A87" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="17">
+      <c r="C87" s="17" t="e">
         <f>(C84)*C86*2*PI()</f>
-        <v>5423.6602381180064</v>
+        <v>#REF!</v>
       </c>
       <c r="D87" s="17"/>
       <c r="E87" t="s">
@@ -4482,9 +4515,9 @@
       <c r="A90" t="s">
         <v>90</v>
       </c>
-      <c r="C90" s="17">
-        <f>60*C18/C20</f>
-        <v>15</v>
+      <c r="C90" s="17" t="e">
+        <f>60*#REF!/#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="D90" s="17"/>
       <c r="E90" t="s">
@@ -4495,9 +4528,9 @@
       <c r="A91" t="s">
         <v>95</v>
       </c>
-      <c r="C91" s="17">
-        <f>(C25/1000/2)</f>
-        <v>6.3661977236758135E-2</v>
+      <c r="C91" s="17" t="e">
+        <f>(#REF!/1000/2)</f>
+        <v>#REF!</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" t="s">
@@ -4508,9 +4541,9 @@
       <c r="A92" t="s">
         <v>91</v>
       </c>
-      <c r="C92" s="17">
-        <f>C59/(C20/C18)/C91</f>
-        <v>129.48035048211705</v>
+      <c r="C92" s="17" t="e">
+        <f>C59/(#REF!/#REF!)/C91</f>
+        <v>#REF!</v>
       </c>
       <c r="D92" s="17"/>
       <c r="E92" t="s">
@@ -4521,9 +4554,9 @@
       <c r="A93" t="s">
         <v>92</v>
       </c>
-      <c r="C93" s="17">
+      <c r="C93" s="17" t="e">
         <f>(C90/60)*C92*2*PI()</f>
-        <v>203.38725892942526</v>
+        <v>#REF!</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" t="s">
@@ -4545,6 +4578,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>524</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4606,7 +4675,7 @@
         <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G36">
         <v>0.55000000000000004</v>
@@ -4624,7 +4693,7 @@
         <v>30</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G37">
         <f>RADIANS(25-360/C36/2)</f>
@@ -4647,7 +4716,7 @@
         <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G38">
         <f>(2.5-1-2*SIN(RADIANS(20))*0.7)/C37*C38</f>
@@ -4664,7 +4733,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C39" s="2">
         <f>C38-2</f>
@@ -4690,7 +4759,7 @@
         <v>52.905688224779105</v>
       </c>
       <c r="E40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G40">
         <f>2.5-1-2*(SIN(RADIANS(20)))*0.7</f>
@@ -4700,7 +4769,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="E41" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G41">
         <f>G40+SIN(RADIANS(H37))*2*(C37-C38)/2</f>
@@ -4789,7 +4858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
@@ -4811,11 +4880,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -4873,7 +4942,7 @@
         <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -4884,7 +4953,7 @@
         <v>434</v>
       </c>
       <c r="D14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -4917,7 +4986,7 @@
         <v>436</v>
       </c>
       <c r="D17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -4936,7 +5005,7 @@
         <v>441</v>
       </c>
       <c r="B20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4944,7 +5013,7 @@
         <v>444</v>
       </c>
       <c r="B21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C21" t="s">
         <v>460</v>
@@ -4994,7 +5063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
@@ -5071,11 +5140,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="K87" sqref="H86:K87"/>
     </sheetView>
   </sheetViews>
@@ -5471,15 +5540,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O299"/>
+  <dimension ref="A1:O298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C293" sqref="C293"/>
+    <sheetView topLeftCell="A282" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C287" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12171,10 +12240,10 @@
     <row r="272" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B272" s="27"/>
       <c r="C272" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D272" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E272" s="9"/>
       <c r="H272" s="19"/>
@@ -12184,10 +12253,10 @@
     <row r="273" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B273" s="27"/>
       <c r="C273" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D273" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E273" s="9"/>
       <c r="H273" s="19"/>
@@ -12196,28 +12265,28 @@
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C274" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D274" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E274" s="24"/>
       <c r="I274" s="30"/>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C275" t="s">
+        <v>483</v>
+      </c>
+      <c r="D275" t="s">
         <v>484</v>
-      </c>
-      <c r="D275" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C276" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D276" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E276" s="22"/>
       <c r="I276" s="30"/>
@@ -12226,10 +12295,10 @@
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C277" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D277" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E277" s="22"/>
       <c r="I277" s="30"/>
@@ -12238,10 +12307,10 @@
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C278" t="s">
+        <v>492</v>
+      </c>
+      <c r="D278" s="6" t="s">
         <v>493</v>
-      </c>
-      <c r="D278" s="6" t="s">
-        <v>494</v>
       </c>
       <c r="E278" s="22"/>
       <c r="I278" s="30"/>
@@ -12262,7 +12331,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E281" s="24"/>
       <c r="I281" s="30"/>
@@ -12271,7 +12340,7 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E282" s="24"/>
       <c r="I282" s="30"/>
@@ -12279,19 +12348,22 @@
       <c r="K282"/>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B283" t="s">
+        <v>525</v>
+      </c>
       <c r="C283" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B284" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="C284" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D284" s="8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E284" s="21"/>
       <c r="I284" s="30"/>
@@ -12299,87 +12371,98 @@
       <c r="K284"/>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D285" s="8"/>
-      <c r="E285" s="21"/>
+      <c r="B285" t="s">
+        <v>525</v>
+      </c>
+      <c r="C285" t="s">
+        <v>511</v>
+      </c>
+      <c r="D285" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H285" s="19"/>
       <c r="I285" s="30"/>
       <c r="J285"/>
       <c r="K285"/>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A286" t="s">
-        <v>507</v>
-      </c>
-      <c r="E286" s="24"/>
+      <c r="B286" t="s">
+        <v>525</v>
+      </c>
+      <c r="C286" t="s">
+        <v>512</v>
+      </c>
+      <c r="D286" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="H286" s="20"/>
       <c r="I286" s="30"/>
       <c r="J286"/>
       <c r="K286"/>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="C287" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D287" s="8" t="s">
-        <v>515</v>
-      </c>
-      <c r="H287" s="19"/>
-      <c r="I287" s="30"/>
-      <c r="J287"/>
-      <c r="K287"/>
+        <v>516</v>
+      </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B288" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="C288" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D288" s="8" t="s">
-        <v>514</v>
-      </c>
-      <c r="H288" s="20"/>
-      <c r="I288" s="30"/>
-      <c r="J288"/>
-      <c r="K288"/>
+        <v>518</v>
+      </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B289" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="C289" t="s">
-        <v>516</v>
-      </c>
-      <c r="D289" s="8" t="s">
-        <v>517</v>
+        <v>519</v>
+      </c>
+      <c r="D289" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B290" t="s">
-        <v>500</v>
-      </c>
-      <c r="C290" t="s">
-        <v>518</v>
-      </c>
-      <c r="D290" s="8" t="s">
-        <v>519</v>
-      </c>
+      <c r="D290" s="8"/>
+      <c r="E290" s="21"/>
+      <c r="I290" s="30"/>
+      <c r="J290"/>
+      <c r="K290"/>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>506</v>
+      </c>
+      <c r="E291" s="24"/>
+      <c r="I291" s="30"/>
+      <c r="J291"/>
+      <c r="K291"/>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B297" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C297" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D297" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I297" s="30"/>
       <c r="J297"/>
@@ -12387,29 +12470,18 @@
     </row>
     <row r="298" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B298" t="s">
+        <v>499</v>
+      </c>
+      <c r="C298" t="s">
         <v>500</v>
       </c>
-      <c r="C298" t="s">
+      <c r="D298" s="8" t="s">
         <v>501</v>
-      </c>
-      <c r="D298" s="8" t="s">
-        <v>502</v>
       </c>
       <c r="E298" s="22"/>
       <c r="I298" s="30"/>
       <c r="J298"/>
       <c r="K298"/>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B299" t="s">
-        <v>500</v>
-      </c>
-      <c r="C299" t="s">
-        <v>520</v>
-      </c>
-      <c r="D299" t="s">
-        <v>521</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L146 D177:K177 B178:K178 B179:D179 F179:K179 F182:K184 B182:D184 B180:K181 C250 G250:K250 B220:C220 E221 F220:K222 B221:D222 B176 F176:K176 D176 B212:K219 B251:K258 D268:K268 B268 B261:K267 E272:E273 B143:K175 B223:K248 B185:K206 B208:K208 F209:K211 F207:K207 B209:D211 B207:D207 B3:K12 B14:K140">

</xml_diff>

<commit_message>
Trajectory planning now works with movements haveing changes in orientation only
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="3"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -4586,7 +4586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -4868,7 +4868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
introduced automatic retry with timeout after communicaiton failre
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2152,6 +2152,61 @@
         <a:xfrm>
           <a:off x="5569345" y="7277100"/>
           <a:ext cx="2192403" cy="2750820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4" descr="http://img.yunqudao.com/UploadFolder/fecf13ab-0cad-49cd-b400-91041ce0e11c/Default/T2_58.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8046720"/>
+          <a:ext cx="7185660" cy="7185660"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4586,8 +4641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added power supply to the housing
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="6"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="533">
   <si>
     <t>Material</t>
   </si>
@@ -1528,9 +1528,6 @@
     <t>Oberarmmittelblock</t>
   </si>
   <si>
-    <t>Schraublöcher von 8 auf 9mm vergößert damit man bessrer schrauben kann (harmlos)</t>
-  </si>
-  <si>
     <t>loo0</t>
   </si>
   <si>
@@ -1603,10 +1600,31 @@
     <t>gedruckt, nicht montiert</t>
   </si>
   <si>
-    <t>Das Zahnrad sollte auf 14 gehen, die Schulter ist irre Kräftig abr zu langsam.15 ging auch</t>
-  </si>
-  <si>
     <t>ST6018M2008-A</t>
+  </si>
+  <si>
+    <t>Platz ist für bis zu 20Zähne, vermutlich wäre 16 gut</t>
+  </si>
+  <si>
+    <t>Hier ist Platz für bis zu 18Z</t>
+  </si>
+  <si>
+    <t>Das Zahnrad sollte auf 14 gehen, die Schulter ist irre Kräftig abr zu langsam.15 ging auch, Platz ist für 15</t>
+  </si>
+  <si>
+    <t>Am Motor ist Platz für bis zu 18Z</t>
+  </si>
+  <si>
+    <t>An der Zwischenwelle ist Platz für bis zu 15Z</t>
+  </si>
+  <si>
+    <t>Oberarmblock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Platz für Zahnriemenrad auf zwischenwelle auf Z18 vergößert (vorher nur Platz für Z15)</t>
+  </si>
+  <si>
+    <t>Schraublöcher von 8 auf 9mm vergößert damit man bessrer schrauben kann (harmlos). Platz für Zahnriemenrad auf Zwischenwelle Z18 vergößert (vorher nur Platz für Z15)</t>
   </si>
 </sst>
 </file>
@@ -3234,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AE93"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3255,12 +3273,12 @@
     <col min="24" max="24" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3271,7 +3289,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3282,7 +3300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3293,7 +3311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3304,7 +3322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3316,7 +3334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3328,7 +3346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3340,11 +3358,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>397</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f>C14/C12</f>
         <v>9</v>
       </c>
@@ -3352,7 +3370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -3363,7 +3381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -3373,8 +3391,11 @@
       <c r="D12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -3386,7 +3407,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -3397,7 +3418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -3409,7 +3430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3442,6 +3463,9 @@
       <c r="D18" t="s">
         <v>28</v>
       </c>
+      <c r="F18" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -3489,7 +3513,7 @@
         <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3531,7 +3555,7 @@
       <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <f>C30/C28*(C34/C32)</f>
         <v>11.755102040816325</v>
       </c>
@@ -3560,6 +3584,9 @@
       <c r="D28" t="s">
         <v>28</v>
       </c>
+      <c r="F28" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -3605,6 +3632,9 @@
       </c>
       <c r="D32" t="s">
         <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -4158,7 +4188,7 @@
         <v>1.4397874175474801</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H71" s="18">
         <v>1.8</v>
@@ -4649,22 +4679,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H39" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -4677,7 +4707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -5074,7 +5104,7 @@
         <v>443</v>
       </c>
       <c r="B21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C21" t="s">
         <v>459</v>
@@ -5205,7 +5235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="K87" sqref="H86:K87"/>
     </sheetView>
   </sheetViews>
@@ -5606,10 +5636,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O298"/>
+  <dimension ref="A1:O300"/>
   <sheetViews>
-    <sheetView topLeftCell="A282" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C287" sqref="C287"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D299" sqref="D299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12392,7 +12422,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E281" s="24"/>
       <c r="I281" s="30"/>
@@ -12401,7 +12431,7 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E282" s="24"/>
       <c r="I282" s="30"/>
@@ -12410,21 +12440,21 @@
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B283" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C283" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B284" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C284" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D284" s="8" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E284" s="21"/>
       <c r="I284" s="30"/>
@@ -12433,13 +12463,13 @@
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B285" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C285" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D285" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H285" s="19"/>
       <c r="I285" s="30"/>
@@ -12448,13 +12478,13 @@
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B286" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C286" t="s">
+        <v>510</v>
+      </c>
+      <c r="D286" s="8" t="s">
         <v>511</v>
-      </c>
-      <c r="D286" s="8" t="s">
-        <v>512</v>
       </c>
       <c r="H286" s="20"/>
       <c r="I286" s="30"/>
@@ -12463,35 +12493,35 @@
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C287" t="s">
+        <v>513</v>
+      </c>
+      <c r="D287" s="8" t="s">
         <v>514</v>
-      </c>
-      <c r="D287" s="8" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B288" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C288" t="s">
+        <v>515</v>
+      </c>
+      <c r="D288" s="8" t="s">
         <v>516</v>
-      </c>
-      <c r="D288" s="8" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B289" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C289" t="s">
+        <v>517</v>
+      </c>
+      <c r="D289" t="s">
         <v>518</v>
-      </c>
-      <c r="D289" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
@@ -12503,7 +12533,7 @@
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E291" s="24"/>
       <c r="I291" s="30"/>
@@ -12512,7 +12542,7 @@
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
@@ -12523,7 +12553,7 @@
         <v>497</v>
       </c>
       <c r="D297" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I297" s="30"/>
       <c r="J297"/>
@@ -12537,12 +12567,34 @@
         <v>499</v>
       </c>
       <c r="D298" s="8" t="s">
-        <v>500</v>
+        <v>532</v>
       </c>
       <c r="E298" s="22"/>
       <c r="I298" s="30"/>
       <c r="J298"/>
       <c r="K298"/>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B299" t="s">
+        <v>498</v>
+      </c>
+      <c r="C299" t="s">
+        <v>513</v>
+      </c>
+      <c r="D299" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B300" t="s">
+        <v>498</v>
+      </c>
+      <c r="C300" t="s">
+        <v>530</v>
+      </c>
+      <c r="D300" t="s">
+        <v>531</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L146 D177:K177 B178:K178 B179:D179 F179:K179 F182:K184 B182:D184 B180:K181 C250 G250:K250 B220:C220 E221 F220:K222 B221:D222 B176 F176:K176 D176 B212:K219 B251:K258 D268:K268 B268 B261:K267 E272:E273 B143:K175 B223:K248 B185:K206 B208:K208 F209:K211 F207:K207 B209:D211 B207:D207 B3:K12 B14:K140">

</xml_diff>

<commit_message>
configuration changes due to new motor in writs, new gears in upperarm and forearm
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="545">
   <si>
     <t>Material</t>
   </si>
@@ -1604,12 +1604,6 @@
     <t>Hier ist Platz für bis zu 18Z</t>
   </si>
   <si>
-    <t>Das Zahnrad sollte auf 14 gehen, die Schulter ist irre Kräftig abr zu langsam.15 ging auch, Platz ist für 15</t>
-  </si>
-  <si>
-    <t>Am Motor ist Platz für bis zu 18Z</t>
-  </si>
-  <si>
     <t>An der Zwischenwelle ist Platz für bis zu 15Z</t>
   </si>
   <si>
@@ -1640,10 +1634,34 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Schulter ist etwas langsam, so 20% schneller wären gut, 1:17, also aus dem 12Z ein 14Z machen</t>
-  </si>
-  <si>
-    <t>Oberarm ist eigentlich mit 8 mikroschritten ok, 20% schneller wären gut, 1:9, dann könnte man auf 16 mikroschritte gehen, also aus dem 14Z ein 16Z machen</t>
+    <t>montiert</t>
+  </si>
+  <si>
+    <t>Oberarm ist eigentlich mit 8 mikroschritten ok,chneller wären gut, 1:9, dann könnte man auf 16 mikroschritte gehen, also aus dem 14Z ein 15Z machen</t>
+  </si>
+  <si>
+    <t>Zu besorgen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zahnriemenrad T5 Z15 für Oberarm </t>
+  </si>
+  <si>
+    <t>Platz für 15</t>
+  </si>
+  <si>
+    <t>riemen reicht nur fü 15Z, größer geht nicht</t>
+  </si>
+  <si>
+    <t>10 Dioden (sind alle)</t>
+  </si>
+  <si>
+    <t>10 5mm Plastik Hülsen (Platinenverbinder) für Pibot Halterung</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/abstandsbolzen-ohne-gewinde-m3-polystyrol-abstandsmass-5-mm-1-st-526355.html</t>
+  </si>
+  <si>
+    <t>Schulter ist etwas langsamvielleicht  1:17</t>
   </si>
 </sst>
 </file>
@@ -3353,7 +3371,7 @@
   <dimension ref="A2:AE93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3533,13 +3551,13 @@
       </c>
       <c r="C16" s="5">
         <f>C20/C18*(C24/C22)</f>
-        <v>20.571428571428569</v>
+        <v>17.632653061224492</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -3607,13 +3625,13 @@
         <v>34</v>
       </c>
       <c r="C22" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>525</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3622,7 +3640,7 @@
       </c>
       <c r="C23" s="4">
         <f>C22*C17/PI()</f>
-        <v>19.098593171027442</v>
+        <v>22.281692032865347</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
@@ -3657,13 +3675,13 @@
       </c>
       <c r="C26" s="4">
         <f>C30/C28*(C34/C32)</f>
-        <v>11.755102040816325</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3688,7 +3706,7 @@
         <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3731,13 +3749,13 @@
         <v>34</v>
       </c>
       <c r="C32" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
         <v>28</v>
       </c>
       <c r="F32" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3746,7 +3764,7 @@
       </c>
       <c r="C33" s="4">
         <f>C32*C27/PI()</f>
-        <v>22.281692032865347</v>
+        <v>23.8732414637843</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
@@ -3757,7 +3775,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="7">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
@@ -3769,7 +3787,7 @@
       </c>
       <c r="C35" s="4">
         <f>C34*C27/PI()</f>
-        <v>76.394372684109769</v>
+        <v>95.4929658551372</v>
       </c>
       <c r="D35" t="s">
         <v>30</v>
@@ -3790,7 +3808,7 @@
         <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3908,7 +3926,7 @@
         <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -4097,7 +4115,7 @@
       </c>
       <c r="C64" s="2">
         <f>C59/C16</f>
-        <v>1.6028007187500004</v>
+        <v>1.869934171875</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s">
@@ -4110,7 +4128,7 @@
       </c>
       <c r="C65" s="2">
         <f>C60/C26</f>
-        <v>0.89853979687500019</v>
+        <v>0.77017696875000019</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s">
@@ -4286,7 +4304,7 @@
       </c>
       <c r="C71" s="2">
         <f>C64*(1+C53)</f>
-        <v>2.0836409343750004</v>
+        <v>2.4309144234375002</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s">
@@ -4294,7 +4312,7 @@
       </c>
       <c r="F71" s="53">
         <f>M71/C71/100</f>
-        <v>1.4397874175474801</v>
+        <v>1.234103500754983</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>523</v>
@@ -4340,7 +4358,7 @@
       </c>
       <c r="C72" s="2">
         <f>C65*(1+C53)</f>
-        <v>1.1681017359375003</v>
+        <v>1.0012300593750003</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s">
@@ -4348,7 +4366,7 @@
       </c>
       <c r="F72" s="53">
         <f>M72/C72/100</f>
-        <v>1.6265706500941801</v>
+        <v>1.8976657584432097</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>261</v>
@@ -5084,7 +5102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -5352,12 +5370,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -5367,7 +5385,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -5782,10 +5800,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O300"/>
+  <dimension ref="A1:O308"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E195" sqref="E195"/>
+    <sheetView topLeftCell="A286" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D307" sqref="D307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12624,7 +12642,7 @@
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B286" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="C286" t="s">
         <v>509</v>
@@ -12639,7 +12657,7 @@
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="C287" t="s">
         <v>512</v>
@@ -12650,7 +12668,7 @@
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B288" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="C288" t="s">
         <v>514</v>
@@ -12694,7 +12712,7 @@
         <v>497</v>
       </c>
       <c r="D292" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
@@ -12715,7 +12733,7 @@
         <v>499</v>
       </c>
       <c r="D298" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E298" s="22"/>
       <c r="I298" s="30"/>
@@ -12730,7 +12748,7 @@
         <v>512</v>
       </c>
       <c r="D299" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
@@ -12738,10 +12756,31 @@
         <v>498</v>
       </c>
       <c r="C300" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D300" t="s">
-        <v>529</v>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>537</v>
+      </c>
+      <c r="B306" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B307" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B308" t="s">
+        <v>542</v>
+      </c>
+      <c r="D308" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
webserver and planner integrated
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="8"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="566">
   <si>
     <t>Material</t>
   </si>
@@ -1722,6 +1722,9 @@
   </si>
   <si>
     <t>http://www.distrelec.de/de/schrittmotor-mm-65-nm-trinamic-qsh6018-56-28-165/p/15422353</t>
+  </si>
+  <si>
+    <t>Measured value</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1741,7 @@
     <numFmt numFmtId="168" formatCode="0.000\ \V"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2019,7 +2022,7 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2030,7 +2033,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="21">
     <dxf>
       <font>
         <color theme="3"/>
@@ -2129,81 +2132,6 @@
     <dxf>
       <font>
         <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -3589,10 +3517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AL94"/>
+  <dimension ref="A2:AM94"/>
   <sheetViews>
-    <sheetView topLeftCell="B71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="J59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3609,8 +3537,8 @@
     <col min="15" max="18" width="9.77734375" customWidth="1"/>
     <col min="19" max="19" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="16.21875" customWidth="1"/>
-    <col min="31" max="31" width="32.5546875" customWidth="1"/>
+    <col min="25" max="27" width="16.21875" customWidth="1"/>
+    <col min="32" max="32" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4344,7 +4272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -4357,7 +4285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -4370,7 +4298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>128</v>
       </c>
@@ -4383,7 +4311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:38" ht="72" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:39" ht="72" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="F68" t="s">
@@ -4446,19 +4374,22 @@
       </c>
       <c r="Z68" s="51"/>
       <c r="AA68" s="51" t="s">
+        <v>565</v>
+      </c>
+      <c r="AB68" s="51" t="s">
         <v>451</v>
       </c>
-      <c r="AB68" s="51" t="s">
+      <c r="AC68" s="51" t="s">
         <v>452</v>
       </c>
-      <c r="AC68" s="51" t="s">
+      <c r="AD68" s="51" t="s">
         <v>453</v>
       </c>
-      <c r="AD68" s="51" t="s">
+      <c r="AE68" s="51" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="69" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="G69" s="10" t="s">
@@ -4494,7 +4425,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -4563,15 +4494,18 @@
         <v>19.913599999999995</v>
       </c>
       <c r="Y70" s="52">
-        <f>0.6801*N70</f>
+        <f t="shared" ref="Y70:Z74" si="0">0.6801*N70</f>
         <v>1.90428</v>
       </c>
       <c r="Z70" s="52">
-        <f>0.6801*O70</f>
+        <f t="shared" si="0"/>
         <v>2.6930586025558378</v>
       </c>
-    </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AA70" s="52">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -4612,7 +4546,7 @@
         <v>3</v>
       </c>
       <c r="O71" s="57">
-        <f t="shared" ref="O71:O74" si="0">N71*SQRT(2)</f>
+        <f t="shared" ref="O71:O74" si="1">N71*SQRT(2)</f>
         <v>4.2426406871192857</v>
       </c>
       <c r="P71" s="57"/>
@@ -4628,27 +4562,30 @@
         <v>1.4</v>
       </c>
       <c r="V71">
-        <f t="shared" ref="V71:V74" si="1">N71*T71</f>
+        <f t="shared" ref="V71:V74" si="2">N71*T71</f>
         <v>13.11</v>
       </c>
       <c r="W71" s="2">
-        <f t="shared" ref="W71:W74" si="2">V71/24</f>
+        <f t="shared" ref="W71:W74" si="3">V71/24</f>
         <v>0.54625000000000001</v>
       </c>
       <c r="X71" s="2">
-        <f t="shared" ref="X71:X74" si="3">N71*V71*2</f>
+        <f t="shared" ref="X71:X74" si="4">N71*V71*2</f>
         <v>78.66</v>
       </c>
       <c r="Y71" s="52">
-        <f>0.6801*N71</f>
+        <f t="shared" si="0"/>
         <v>2.0403000000000002</v>
       </c>
       <c r="Z71" s="52">
-        <f>0.6801*O71</f>
+        <f t="shared" si="0"/>
         <v>2.8854199313098263</v>
       </c>
-    </row>
-    <row r="72" spans="1:38" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA71" s="52">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:39" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -4689,7 +4626,7 @@
         <v>1.4</v>
       </c>
       <c r="O72" s="57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9798989873223332</v>
       </c>
       <c r="P72" s="60">
@@ -4714,36 +4651,39 @@
         <v>0.77</v>
       </c>
       <c r="V72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9359999999999999</v>
       </c>
       <c r="W72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24733333333333332</v>
       </c>
       <c r="X72" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.620799999999999</v>
       </c>
       <c r="Y72" s="52">
-        <f>0.6801*N72</f>
+        <f t="shared" si="0"/>
         <v>0.95213999999999999</v>
       </c>
       <c r="Z72" s="52">
-        <f>0.6801*O72</f>
+        <f t="shared" si="0"/>
         <v>1.3465293012779189</v>
       </c>
-      <c r="AA72" s="10"/>
+      <c r="AA72" s="52">
+        <v>0.49</v>
+      </c>
       <c r="AB72" s="10"/>
-      <c r="AF72" s="10"/>
+      <c r="AC72" s="10"/>
       <c r="AG72" s="10"/>
       <c r="AH72" s="10"/>
       <c r="AI72" s="10"/>
       <c r="AJ72" s="10"/>
       <c r="AK72" s="10"/>
       <c r="AL72" s="10"/>
-    </row>
-    <row r="73" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AM72" s="10"/>
+    </row>
+    <row r="73" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>379</v>
       </c>
@@ -4784,7 +4724,7 @@
         <v>0.7</v>
       </c>
       <c r="O73" s="57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.98994949366116658</v>
       </c>
       <c r="P73" s="60">
@@ -4809,38 +4749,40 @@
         <v>0.18</v>
       </c>
       <c r="V73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.08</v>
       </c>
       <c r="W73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12833333333333333</v>
       </c>
       <c r="X73" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.3119999999999994</v>
       </c>
       <c r="Y73" s="52">
-        <f>0.6801*N73</f>
+        <f t="shared" si="0"/>
         <v>0.47606999999999999</v>
       </c>
       <c r="Z73" s="52">
-        <f>0.6801*O73</f>
+        <f t="shared" si="0"/>
         <v>0.67326465063895946</v>
       </c>
-      <c r="AA73" s="51" t="s">
+      <c r="AA73" s="52">
+        <v>0.46</v>
+      </c>
+      <c r="AB73" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="AB73" s="51" t="s">
+      <c r="AC73" s="51" t="s">
         <v>466</v>
       </c>
-      <c r="AC73" s="10" t="s">
+      <c r="AD73" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="AD73" s="51" t="s">
+      <c r="AE73" s="51" t="s">
         <v>467</v>
       </c>
-      <c r="AE73" s="10"/>
       <c r="AF73" s="10"/>
       <c r="AG73" s="10"/>
       <c r="AH73" s="10"/>
@@ -4848,8 +4790,9 @@
       <c r="AJ73" s="10"/>
       <c r="AK73" s="10"/>
       <c r="AL73" s="10"/>
-    </row>
-    <row r="74" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AM73" s="10"/>
+    </row>
+    <row r="74" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>129</v>
       </c>
@@ -4890,7 +4833,7 @@
         <v>0.4</v>
       </c>
       <c r="O74" s="57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.56568542494923812</v>
       </c>
       <c r="P74" s="60">
@@ -4915,47 +4858,50 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="V74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="W74" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="X74" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="Y74" s="52">
-        <f>0.6801*N74</f>
+        <f t="shared" si="0"/>
         <v>0.27204</v>
       </c>
       <c r="Z74" s="52">
-        <f>0.6801*O74</f>
+        <f t="shared" si="0"/>
         <v>0.38472265750797685</v>
       </c>
-      <c r="AA74" s="12" t="s">
+      <c r="AA74" s="52">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="AB74" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="AB74" s="12" t="s">
+      <c r="AC74" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="AC74" s="12" t="s">
+      <c r="AD74" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="AD74" s="12" t="s">
+      <c r="AE74" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="AE74" s="54"/>
-      <c r="AF74" s="12"/>
+      <c r="AF74" s="54"/>
       <c r="AG74" s="12"/>
       <c r="AH74" s="12"/>
       <c r="AI74" s="12"/>
       <c r="AJ74" s="12"/>
       <c r="AK74" s="12"/>
       <c r="AL74" s="12"/>
-    </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AM74" s="12"/>
+    </row>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="F75" s="22"/>
@@ -4979,7 +4925,7 @@
       <c r="X75" s="2"/>
       <c r="Y75" s="25"/>
       <c r="Z75" s="51"/>
-      <c r="AA75" s="25"/>
+      <c r="AA75" s="51"/>
       <c r="AB75" s="25"/>
       <c r="AC75" s="25"/>
       <c r="AD75" s="25"/>
@@ -4991,8 +4937,9 @@
       <c r="AJ75" s="25"/>
       <c r="AK75" s="25"/>
       <c r="AL75" s="25"/>
-    </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AM75" s="25"/>
+    </row>
+    <row r="76" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>546</v>
       </c>
@@ -5020,7 +4967,7 @@
         <v>129.10640000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C77" s="58"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -5039,7 +4986,7 @@
       <c r="T77" s="15"/>
       <c r="X77" s="2"/>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>544</v>
       </c>
@@ -5048,11 +4995,11 @@
         <v>129.10640000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C79" s="16"/>
       <c r="D79" s="16"/>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C80" s="16"/>
       <c r="D80" s="16"/>
     </row>
@@ -5691,7 +5638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
@@ -6131,7 +6078,7 @@
   </sheetPr>
   <dimension ref="A1:O321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B296" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B296" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D317" sqref="D317"/>
     </sheetView>
   </sheetViews>
@@ -12852,7 +12799,7 @@
         <v>29.9</v>
       </c>
       <c r="I269" s="31">
-        <f t="shared" ref="I269:I270" si="51">SUMIF(C$1:C$141,"="&amp;C269,B$1:B$141)</f>
+        <f t="shared" ref="I269" si="51">SUMIF(C$1:C$141,"="&amp;C269,B$1:B$141)</f>
         <v>0</v>
       </c>
       <c r="J269" s="32">

</xml_diff>

<commit_message>
new feature: trajectory nodes without a name are given a number
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2029,22 +2029,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="3" builtinId="4"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color theme="3"/>
@@ -2153,21 +2138,6 @@
     <dxf>
       <font>
         <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -5853,8 +5823,8 @@
   </sheetPr>
   <dimension ref="A1:O323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13066,101 +13036,101 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L146 D177:K177 B180:D180 F180:K180 F183:K185 B183:D185 B181:K182 C252 G252:K252 B222:C222 E223 F222:K224 B223:D224 B176 F176:K176 D176 B214:K221 B253:K260 E277:E278 B143:K175 B225:K250 B210:K210 F211:K213 F209:K209 B211:D213 B209:D209 B3:K12 B14:K140 B263:K270 C271:C272 B186:K195 B197:K208 B196:D196 F196:K196 B178:K179">
-    <cfRule type="expression" dxfId="25" priority="465">
+    <cfRule type="expression" dxfId="22" priority="465">
       <formula>$L3=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E224">
-    <cfRule type="expression" dxfId="24" priority="500">
+    <cfRule type="expression" dxfId="21" priority="500">
       <formula>$L222=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E209">
-    <cfRule type="expression" dxfId="23" priority="501">
+    <cfRule type="expression" dxfId="20" priority="501">
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="expression" dxfId="22" priority="502">
+    <cfRule type="expression" dxfId="19" priority="502">
       <formula>$L177=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E183">
-    <cfRule type="expression" dxfId="21" priority="503">
+    <cfRule type="expression" dxfId="18" priority="503">
       <formula>$L177=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E184">
-    <cfRule type="expression" dxfId="20" priority="504">
+    <cfRule type="expression" dxfId="17" priority="504">
       <formula>$L175=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A177 D177:XFD177 A180:D180 F180:XFD180 F183:XFD185 A183:D185 A181:XFD182 C252 G252:L252 A222:C222 E223 A223:D224 F222:XFD224 A176:B176 F176:XFD176 D176 A214:XFD221 A253:XFD260 E277:E278 A143:XFD175 A225:XFD250 A210:XFD210 A211:D213 A209:D209 F211:XFD213 F209:XFD209 A3:XFD12 A14:XFD140 A263:XFD270 C271:C272 A197:XFD208 A196:D196 F196:XFD196 A186:XFD191 A193:XFD195 B192:XFD192 A178:XFD179">
-    <cfRule type="expression" dxfId="19" priority="505">
+    <cfRule type="expression" dxfId="16" priority="505">
       <formula>$L3=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="506">
+    <cfRule type="expression" dxfId="15" priority="506">
       <formula>$L3=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E224">
-    <cfRule type="expression" dxfId="17" priority="569">
+    <cfRule type="expression" dxfId="14" priority="569">
       <formula>$L222=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="570">
+    <cfRule type="expression" dxfId="13" priority="570">
       <formula>$L222=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E209">
-    <cfRule type="expression" dxfId="15" priority="571">
+    <cfRule type="expression" dxfId="12" priority="571">
       <formula>$L223=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="572">
+    <cfRule type="expression" dxfId="11" priority="572">
       <formula>$L223=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="expression" dxfId="13" priority="573">
+    <cfRule type="expression" dxfId="10" priority="573">
       <formula>$L177=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="574">
+    <cfRule type="expression" dxfId="9" priority="574">
       <formula>$L177=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E183">
-    <cfRule type="expression" dxfId="11" priority="575">
+    <cfRule type="expression" dxfId="8" priority="575">
       <formula>$L177=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="576">
+    <cfRule type="expression" dxfId="7" priority="576">
       <formula>$L177=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E184">
-    <cfRule type="expression" dxfId="9" priority="577">
+    <cfRule type="expression" dxfId="6" priority="577">
       <formula>$L175=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="578">
+    <cfRule type="expression" dxfId="5" priority="578">
       <formula>$L175=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:K272">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$L271=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:L272">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$L271=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$L271=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E196">
-    <cfRule type="expression" dxfId="4" priority="581">
+    <cfRule type="expression" dxfId="1" priority="581">
       <formula>$L192=#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="582">
+    <cfRule type="expression" dxfId="0" priority="582">
       <formula>$L192=#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implementation of Towers of Hanoi started
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
+    <workbookView minimized="1" xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -5823,8 +5823,8 @@
   </sheetPr>
   <dimension ref="A1:O323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D280" sqref="D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added freeglut library for windows
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="564">
   <si>
     <t>Material</t>
   </si>
@@ -1715,6 +1715,9 @@
   </si>
   <si>
     <t>Zahnriemenscheibe T5, 15 Zähne (d=23,87)</t>
+  </si>
+  <si>
+    <t>https://www.kugellager-express.de/rillenkugellager-6807-2rs-61807-2rs-35x47x7-mm</t>
   </si>
 </sst>
 </file>
@@ -3294,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AM94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -5813,8 +5816,8 @@
   </sheetPr>
   <dimension ref="A1:O323"/>
   <sheetViews>
-    <sheetView topLeftCell="C248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K276" sqref="K276"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11857,7 +11860,7 @@
         <v>402</v>
       </c>
       <c r="E245" s="9" t="s">
-        <v>69</v>
+        <v>563</v>
       </c>
       <c r="G245">
         <v>1</v>

</xml_diff>

<commit_message>
more or less final
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="7"/>
+    <workbookView xWindow="516" yWindow="516" windowWidth="4380" windowHeight="3396" tabRatio="709" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kräfte" sheetId="3" r:id="rId1"/>
@@ -5098,7 +5098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D99"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
@@ -5816,7 +5816,7 @@
   </sheetPr>
   <dimension ref="A1:O323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>

</xml_diff>